<commit_message>
Eliminato spazio in razionale di applicabilità
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
+++ b/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSE20\medarchiver\it-fse-accreditamento\GATEWAY\S1#111MEDARCHIVER\MEDARCHIVER\MEDARCHIVER_FSE2.0\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C747BD-DD20-41FA-8E79-BF74785FBB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14018B0D-6A27-4234-B950-FFD69ACE9ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="502">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -1890,9 +1890,6 @@
   </si>
   <si>
     <t>2023-03-25T08:54:29Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>555d2cc937e460a3</t>
@@ -2576,7 +2573,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2682,28 +2679,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2785,7 +2760,6 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -2820,6 +2794,28 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4268,10 +4264,10 @@
   <dimension ref="A1:T993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9:XFD9"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4282,11 +4278,11 @@
     <col min="4" max="4" width="63.85546875" customWidth="1"/>
     <col min="5" max="5" width="104.85546875" customWidth="1"/>
     <col min="6" max="8" width="33.140625" style="36" customWidth="1"/>
-    <col min="9" max="9" width="33.140625" style="52" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" style="40" customWidth="1"/>
     <col min="10" max="10" width="27.140625" customWidth="1"/>
     <col min="11" max="11" width="36.42578125" customWidth="1"/>
     <col min="12" max="13" width="36.42578125" style="36" customWidth="1"/>
-    <col min="14" max="14" width="36.42578125" style="52" customWidth="1"/>
+    <col min="14" max="14" width="36.42578125" style="40" customWidth="1"/>
     <col min="15" max="15" width="36.42578125" customWidth="1"/>
     <col min="16" max="16" width="27.140625" customWidth="1"/>
     <col min="17" max="17" width="33.140625" customWidth="1"/>
@@ -4314,14 +4310,14 @@
       <c r="T1" s="35"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="44" t="s">
-        <v>499</v>
-      </c>
-      <c r="D2" s="43"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="82" t="s">
+        <v>498</v>
+      </c>
+      <c r="D2" s="81"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -4339,14 +4335,14 @@
       <c r="T2" s="35"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="51" t="s">
-        <v>500</v>
-      </c>
-      <c r="D3" s="43"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="89" t="s">
+        <v>499</v>
+      </c>
+      <c r="D3" s="81"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -4364,12 +4360,12 @@
       <c r="T3" s="35"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="51" t="s">
-        <v>501</v>
-      </c>
-      <c r="D4" s="43"/>
+      <c r="A4" s="85"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="89" t="s">
+        <v>500</v>
+      </c>
+      <c r="D4" s="81"/>
       <c r="E4" s="2"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -4388,12 +4384,12 @@
       <c r="T4" s="35"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="49"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51" t="s">
-        <v>502</v>
-      </c>
-      <c r="D5" s="43"/>
+      <c r="A5" s="87"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="89" t="s">
+        <v>501</v>
+      </c>
+      <c r="D5" s="81"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -4411,8 +4407,8 @@
       <c r="T5" s="35"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="41"/>
+      <c r="A6" s="78"/>
+      <c r="B6" s="79"/>
       <c r="C6" s="10"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -4467,99 +4463,99 @@
       <c r="S8" s="35"/>
       <c r="T8" s="35"/>
     </row>
-    <row r="9" spans="1:20" s="79" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="80" t="s">
+    <row r="9" spans="1:20" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="81" t="s">
+      <c r="B9" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="81" t="s">
+      <c r="C9" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="81" t="s">
+      <c r="D9" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="81" t="s">
+      <c r="E9" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="81" t="s">
+      <c r="F9" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="81" t="s">
+      <c r="G9" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="81" t="s">
+      <c r="H9" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="81" t="s">
+      <c r="I9" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="81" t="s">
+      <c r="J9" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="81" t="s">
+      <c r="K9" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="82" t="s">
+      <c r="L9" s="69" t="s">
         <v>424</v>
       </c>
-      <c r="M9" s="82" t="s">
+      <c r="M9" s="69" t="s">
         <v>425</v>
       </c>
-      <c r="N9" s="82" t="s">
+      <c r="N9" s="69" t="s">
         <v>426</v>
       </c>
-      <c r="O9" s="82" t="s">
+      <c r="O9" s="69" t="s">
         <v>427</v>
       </c>
-      <c r="P9" s="81" t="s">
+      <c r="P9" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="81" t="s">
+      <c r="Q9" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="R9" s="83" t="s">
+      <c r="R9" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="S9" s="81" t="s">
+      <c r="S9" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="T9" s="84" t="s">
+      <c r="T9" s="71" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="59">
+      <c r="A10" s="47">
         <v>1</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="60" t="s">
+      <c r="C10" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="60" t="s">
+      <c r="D10" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="61" t="s">
+      <c r="E10" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="70"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="62"/>
-      <c r="O10" s="62"/>
-      <c r="P10" s="62"/>
-      <c r="Q10" s="62"/>
-      <c r="R10" s="66"/>
-      <c r="S10" s="67"/>
-      <c r="T10" s="68" t="s">
+      <c r="F10" s="58"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="50"/>
+      <c r="P10" s="50"/>
+      <c r="Q10" s="50"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="55"/>
+      <c r="T10" s="56" t="s">
         <v>429</v>
       </c>
     </row>
@@ -4666,229 +4662,229 @@
       </c>
     </row>
     <row r="14" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="53">
+      <c r="A14" s="41">
         <v>5</v>
       </c>
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="C14" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="D14" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="55" t="s">
+      <c r="E14" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="56"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="58"/>
-      <c r="L14" s="58"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="58"/>
-      <c r="O14" s="58"/>
-      <c r="P14" s="58"/>
-      <c r="Q14" s="58"/>
-      <c r="R14" s="63"/>
-      <c r="S14" s="64"/>
-      <c r="T14" s="65" t="s">
+      <c r="F14" s="44"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="46"/>
+      <c r="N14" s="46"/>
+      <c r="O14" s="46"/>
+      <c r="P14" s="46"/>
+      <c r="Q14" s="46"/>
+      <c r="R14" s="51"/>
+      <c r="S14" s="52"/>
+      <c r="T14" s="53" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="79" customFormat="1" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="85">
+    <row r="15" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="72">
         <v>6</v>
       </c>
-      <c r="B15" s="86" t="s">
+      <c r="B15" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="86" t="s">
+      <c r="C15" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="86" t="s">
+      <c r="D15" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="90" t="s">
+      <c r="E15" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="71">
+      <c r="F15" s="59">
         <v>45010</v>
       </c>
-      <c r="G15" s="72" t="s">
+      <c r="G15" s="60" t="s">
         <v>448</v>
       </c>
-      <c r="H15" s="72" t="s">
+      <c r="H15" s="60" t="s">
         <v>433</v>
       </c>
-      <c r="I15" s="73" t="s">
+      <c r="I15" s="61" t="s">
         <v>434</v>
       </c>
-      <c r="J15" s="72" t="s">
+      <c r="J15" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="K15" s="74"/>
-      <c r="L15" s="72"/>
-      <c r="M15" s="72"/>
-      <c r="N15" s="73"/>
-      <c r="O15" s="75"/>
-      <c r="P15" s="75"/>
-      <c r="Q15" s="75"/>
-      <c r="R15" s="88"/>
-      <c r="S15" s="75"/>
-      <c r="T15" s="89" t="s">
+      <c r="K15" s="62"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="60"/>
+      <c r="N15" s="61"/>
+      <c r="O15" s="63"/>
+      <c r="P15" s="63"/>
+      <c r="Q15" s="63"/>
+      <c r="R15" s="75"/>
+      <c r="S15" s="63"/>
+      <c r="T15" s="76" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="16" spans="1:20" s="79" customFormat="1" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="85">
+    <row r="16" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="72">
         <v>7</v>
       </c>
-      <c r="B16" s="86" t="s">
+      <c r="B16" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="86" t="s">
+      <c r="C16" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="86" t="s">
+      <c r="D16" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="90" t="s">
+      <c r="E16" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="71">
+      <c r="F16" s="59">
         <v>45010</v>
       </c>
-      <c r="G16" s="72" t="s">
+      <c r="G16" s="60" t="s">
         <v>448</v>
       </c>
-      <c r="H16" s="72" t="s">
+      <c r="H16" s="60" t="s">
         <v>435</v>
       </c>
-      <c r="I16" s="73" t="s">
+      <c r="I16" s="61" t="s">
         <v>436</v>
       </c>
-      <c r="J16" s="72" t="s">
+      <c r="J16" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="K16" s="74"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="72"/>
-      <c r="N16" s="73"/>
-      <c r="O16" s="75"/>
-      <c r="P16" s="75"/>
-      <c r="Q16" s="75"/>
-      <c r="R16" s="88"/>
-      <c r="S16" s="75"/>
-      <c r="T16" s="89" t="s">
+      <c r="K16" s="62"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="63"/>
+      <c r="P16" s="63"/>
+      <c r="Q16" s="63"/>
+      <c r="R16" s="75"/>
+      <c r="S16" s="63"/>
+      <c r="T16" s="76" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="79" customFormat="1" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="85">
+    <row r="17" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="72">
         <v>8</v>
       </c>
-      <c r="B17" s="86" t="s">
+      <c r="B17" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="86" t="s">
+      <c r="C17" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="86" t="s">
+      <c r="D17" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="90" t="s">
+      <c r="E17" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="71">
+      <c r="F17" s="59">
         <v>45010</v>
       </c>
-      <c r="G17" s="72" t="s">
+      <c r="G17" s="60" t="s">
         <v>448</v>
       </c>
-      <c r="H17" s="72" t="s">
+      <c r="H17" s="60" t="s">
         <v>437</v>
       </c>
-      <c r="I17" s="73" t="s">
+      <c r="I17" s="61" t="s">
         <v>438</v>
       </c>
-      <c r="J17" s="72" t="s">
+      <c r="J17" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="K17" s="74"/>
-      <c r="L17" s="72"/>
-      <c r="M17" s="72"/>
-      <c r="N17" s="73"/>
-      <c r="O17" s="75"/>
-      <c r="P17" s="75"/>
-      <c r="Q17" s="75"/>
-      <c r="R17" s="88"/>
-      <c r="S17" s="75"/>
-      <c r="T17" s="89" t="s">
+      <c r="K17" s="62"/>
+      <c r="L17" s="60"/>
+      <c r="M17" s="60"/>
+      <c r="N17" s="61"/>
+      <c r="O17" s="63"/>
+      <c r="P17" s="63"/>
+      <c r="Q17" s="63"/>
+      <c r="R17" s="75"/>
+      <c r="S17" s="63"/>
+      <c r="T17" s="76" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="18" spans="1:20" s="79" customFormat="1" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="85">
+    <row r="18" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="72">
         <v>9</v>
       </c>
-      <c r="B18" s="86" t="s">
+      <c r="B18" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="86" t="s">
+      <c r="C18" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="86" t="s">
+      <c r="D18" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="90" t="s">
+      <c r="E18" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="71">
+      <c r="F18" s="59">
         <v>45010</v>
       </c>
-      <c r="G18" s="72" t="s">
+      <c r="G18" s="60" t="s">
         <v>448</v>
       </c>
-      <c r="H18" s="72" t="s">
+      <c r="H18" s="60" t="s">
         <v>439</v>
       </c>
-      <c r="I18" s="73" t="s">
+      <c r="I18" s="61" t="s">
         <v>440</v>
       </c>
-      <c r="J18" s="72" t="s">
+      <c r="J18" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="K18" s="74"/>
-      <c r="L18" s="72"/>
-      <c r="M18" s="72"/>
-      <c r="N18" s="73"/>
-      <c r="O18" s="75"/>
-      <c r="P18" s="75"/>
-      <c r="Q18" s="75"/>
-      <c r="R18" s="88"/>
-      <c r="S18" s="75"/>
-      <c r="T18" s="89" t="s">
+      <c r="K18" s="62"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="63"/>
+      <c r="P18" s="63"/>
+      <c r="Q18" s="63"/>
+      <c r="R18" s="75"/>
+      <c r="S18" s="63"/>
+      <c r="T18" s="76" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="59">
+      <c r="A19" s="47">
         <v>11</v>
       </c>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="60" t="s">
+      <c r="C19" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="60" t="s">
+      <c r="D19" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="61" t="s">
+      <c r="E19" s="49" t="s">
         <v>48</v>
       </c>
       <c r="F19" s="38">
@@ -4908,12 +4904,12 @@
       <c r="N19" t="s">
         <v>443</v>
       </c>
-      <c r="O19" s="62"/>
-      <c r="P19" s="62"/>
-      <c r="Q19" s="62"/>
-      <c r="R19" s="66"/>
-      <c r="S19" s="67"/>
-      <c r="T19" s="68" t="s">
+      <c r="O19" s="50"/>
+      <c r="P19" s="50"/>
+      <c r="Q19" s="50"/>
+      <c r="R19" s="54"/>
+      <c r="S19" s="55"/>
+      <c r="T19" s="56" t="s">
         <v>429</v>
       </c>
     </row>
@@ -5436,107 +5432,107 @@
       </c>
     </row>
     <row r="35" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="53">
+      <c r="A35" s="41">
         <v>28</v>
       </c>
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="54" t="s">
+      <c r="C35" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="54" t="s">
+      <c r="D35" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="E35" s="76" t="s">
+      <c r="E35" s="64" t="s">
         <v>431</v>
       </c>
-      <c r="F35" s="56"/>
-      <c r="G35" s="57"/>
-      <c r="H35" s="57"/>
-      <c r="I35" s="57"/>
-      <c r="J35" s="58"/>
-      <c r="K35" s="58"/>
-      <c r="L35" s="58"/>
-      <c r="M35" s="58"/>
-      <c r="N35" s="58"/>
-      <c r="O35" s="58"/>
-      <c r="P35" s="58"/>
-      <c r="Q35" s="58"/>
-      <c r="R35" s="63"/>
-      <c r="S35" s="64"/>
-      <c r="T35" s="65" t="s">
+      <c r="F35" s="44"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="46"/>
+      <c r="K35" s="46"/>
+      <c r="L35" s="46"/>
+      <c r="M35" s="46"/>
+      <c r="N35" s="46"/>
+      <c r="O35" s="46"/>
+      <c r="P35" s="46"/>
+      <c r="Q35" s="46"/>
+      <c r="R35" s="51"/>
+      <c r="S35" s="52"/>
+      <c r="T35" s="53" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="36" spans="1:20" s="79" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="85">
+    <row r="36" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="72">
         <v>29</v>
       </c>
-      <c r="B36" s="86" t="s">
+      <c r="B36" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="86" t="s">
+      <c r="C36" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="86" t="s">
+      <c r="D36" s="73" t="s">
         <v>84</v>
       </c>
-      <c r="E36" s="87" t="s">
+      <c r="E36" s="74" t="s">
         <v>431</v>
       </c>
-      <c r="F36" s="71">
+      <c r="F36" s="59">
         <v>45010</v>
       </c>
-      <c r="G36" s="72" t="s">
+      <c r="G36" s="60" t="s">
         <v>448</v>
       </c>
-      <c r="H36" s="72" t="s">
+      <c r="H36" s="60" t="s">
         <v>441</v>
       </c>
-      <c r="I36" s="73" t="s">
+      <c r="I36" s="61" t="s">
         <v>442</v>
       </c>
-      <c r="J36" s="72" t="s">
+      <c r="J36" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="K36" s="74"/>
-      <c r="L36" s="72" t="s">
+      <c r="K36" s="62"/>
+      <c r="L36" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="M36" s="72" t="s">
+      <c r="M36" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="N36" s="73" t="s">
-        <v>474</v>
-      </c>
-      <c r="O36" s="75" t="s">
+      <c r="N36" s="61" t="s">
+        <v>473</v>
+      </c>
+      <c r="O36" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="P36" s="75" t="s">
-        <v>487</v>
-      </c>
-      <c r="Q36" s="75"/>
-      <c r="R36" s="88"/>
-      <c r="S36" s="75"/>
-      <c r="T36" s="89" t="s">
+      <c r="P36" s="63" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q36" s="63"/>
+      <c r="R36" s="75"/>
+      <c r="S36" s="63"/>
+      <c r="T36" s="76" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="59">
+      <c r="A37" s="47">
         <v>30</v>
       </c>
-      <c r="B37" s="60" t="s">
+      <c r="B37" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="60" t="s">
+      <c r="C37" s="48" t="s">
         <v>362</v>
       </c>
-      <c r="D37" s="60" t="s">
+      <c r="D37" s="48" t="s">
         <v>363</v>
       </c>
-      <c r="E37" s="77" t="s">
+      <c r="E37" s="65" t="s">
         <v>431</v>
       </c>
       <c r="F37" s="38">
@@ -5556,12 +5552,12 @@
       <c r="N37" t="s">
         <v>445</v>
       </c>
-      <c r="O37" s="62"/>
-      <c r="P37" s="62"/>
-      <c r="Q37" s="62"/>
-      <c r="R37" s="66"/>
-      <c r="S37" s="67"/>
-      <c r="T37" s="68" t="s">
+      <c r="O37" s="50"/>
+      <c r="P37" s="50"/>
+      <c r="Q37" s="50"/>
+      <c r="R37" s="54"/>
+      <c r="S37" s="55"/>
+      <c r="T37" s="56" t="s">
         <v>430</v>
       </c>
     </row>
@@ -5736,124 +5732,124 @@
       </c>
     </row>
     <row r="43" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="53">
+      <c r="A43" s="41">
         <v>36</v>
       </c>
-      <c r="B43" s="54" t="s">
+      <c r="B43" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="C43" s="54" t="s">
+      <c r="C43" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="D43" s="54" t="s">
+      <c r="D43" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="E43" s="76" t="s">
+      <c r="E43" s="64" t="s">
         <v>432</v>
       </c>
-      <c r="F43" s="56"/>
-      <c r="G43" s="57"/>
-      <c r="H43" s="57"/>
-      <c r="I43" s="57"/>
-      <c r="J43" s="58"/>
-      <c r="K43" s="58"/>
-      <c r="L43" s="58"/>
-      <c r="M43" s="58"/>
-      <c r="N43" s="58"/>
-      <c r="O43" s="58"/>
-      <c r="P43" s="58"/>
-      <c r="Q43" s="58"/>
-      <c r="R43" s="63"/>
-      <c r="S43" s="64"/>
-      <c r="T43" s="65" t="s">
+      <c r="F43" s="44"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="45"/>
+      <c r="J43" s="46"/>
+      <c r="K43" s="46"/>
+      <c r="L43" s="46"/>
+      <c r="M43" s="46"/>
+      <c r="N43" s="46"/>
+      <c r="O43" s="46"/>
+      <c r="P43" s="46"/>
+      <c r="Q43" s="46"/>
+      <c r="R43" s="51"/>
+      <c r="S43" s="52"/>
+      <c r="T43" s="53" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="44" spans="1:20" s="79" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="85">
+    <row r="44" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="72">
         <v>37</v>
       </c>
-      <c r="B44" s="86" t="s">
+      <c r="B44" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="86" t="s">
+      <c r="C44" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="D44" s="86" t="s">
+      <c r="D44" s="73" t="s">
         <v>90</v>
       </c>
-      <c r="E44" s="87" t="s">
+      <c r="E44" s="74" t="s">
         <v>432</v>
       </c>
-      <c r="F44" s="71">
+      <c r="F44" s="59">
         <v>45010</v>
       </c>
-      <c r="G44" s="72" t="s">
+      <c r="G44" s="60" t="s">
         <v>448</v>
       </c>
-      <c r="H44" s="72" t="s">
+      <c r="H44" s="60" t="s">
         <v>444</v>
       </c>
-      <c r="I44" s="73" t="s">
+      <c r="I44" s="61" t="s">
         <v>442</v>
       </c>
-      <c r="J44" s="72" t="s">
+      <c r="J44" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="K44" s="74"/>
-      <c r="L44" s="72" t="s">
+      <c r="K44" s="62"/>
+      <c r="L44" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="M44" s="72" t="s">
+      <c r="M44" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="N44" s="73" t="s">
-        <v>473</v>
-      </c>
-      <c r="O44" s="75" t="s">
+      <c r="N44" s="61" t="s">
+        <v>472</v>
+      </c>
+      <c r="O44" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="P44" s="75" t="s">
-        <v>487</v>
-      </c>
-      <c r="Q44" s="75"/>
-      <c r="R44" s="88"/>
-      <c r="S44" s="75"/>
-      <c r="T44" s="89" t="s">
+      <c r="P44" s="63" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q44" s="63"/>
+      <c r="R44" s="75"/>
+      <c r="S44" s="63"/>
+      <c r="T44" s="76" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="45" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="59">
+      <c r="A45" s="47">
         <v>38</v>
       </c>
-      <c r="B45" s="60" t="s">
+      <c r="B45" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="60" t="s">
+      <c r="C45" s="48" t="s">
         <v>362</v>
       </c>
-      <c r="D45" s="60" t="s">
+      <c r="D45" s="48" t="s">
         <v>364</v>
       </c>
-      <c r="E45" s="77" t="s">
+      <c r="E45" s="65" t="s">
         <v>432</v>
       </c>
-      <c r="F45" s="70"/>
-      <c r="G45" s="69"/>
-      <c r="H45" s="69"/>
-      <c r="I45" s="69"/>
-      <c r="J45" s="62"/>
-      <c r="K45" s="62"/>
-      <c r="L45" s="62"/>
-      <c r="M45" s="62"/>
-      <c r="N45" s="62"/>
-      <c r="O45" s="62"/>
-      <c r="P45" s="62"/>
-      <c r="Q45" s="62"/>
-      <c r="R45" s="66"/>
-      <c r="S45" s="67"/>
-      <c r="T45" s="68" t="s">
+      <c r="F45" s="58"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="57"/>
+      <c r="I45" s="57"/>
+      <c r="J45" s="50"/>
+      <c r="K45" s="50"/>
+      <c r="L45" s="50"/>
+      <c r="M45" s="50"/>
+      <c r="N45" s="50"/>
+      <c r="O45" s="50"/>
+      <c r="P45" s="50"/>
+      <c r="Q45" s="50"/>
+      <c r="R45" s="54"/>
+      <c r="S45" s="55"/>
+      <c r="T45" s="56" t="s">
         <v>430</v>
       </c>
     </row>
@@ -6028,120 +6024,120 @@
       </c>
     </row>
     <row r="51" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="53">
+      <c r="A51" s="41">
         <v>44</v>
       </c>
-      <c r="B51" s="54" t="s">
+      <c r="B51" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="C51" s="54" t="s">
+      <c r="C51" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="D51" s="54" t="s">
+      <c r="D51" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="E51" s="55" t="s">
+      <c r="E51" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="F51" s="56"/>
-      <c r="G51" s="57"/>
-      <c r="H51" s="57"/>
-      <c r="I51" s="57"/>
-      <c r="J51" s="58"/>
-      <c r="K51" s="58"/>
-      <c r="L51" s="58"/>
-      <c r="M51" s="58"/>
-      <c r="N51" s="58"/>
-      <c r="O51" s="58"/>
-      <c r="P51" s="58"/>
-      <c r="Q51" s="58"/>
-      <c r="R51" s="63" t="s">
+      <c r="F51" s="44"/>
+      <c r="G51" s="45"/>
+      <c r="H51" s="45"/>
+      <c r="I51" s="45"/>
+      <c r="J51" s="46"/>
+      <c r="K51" s="46"/>
+      <c r="L51" s="46"/>
+      <c r="M51" s="46"/>
+      <c r="N51" s="46"/>
+      <c r="O51" s="46"/>
+      <c r="P51" s="46"/>
+      <c r="Q51" s="46"/>
+      <c r="R51" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="S51" s="64"/>
-      <c r="T51" s="65" t="s">
+      <c r="S51" s="52"/>
+      <c r="T51" s="53" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="52" spans="1:20" s="79" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="85">
+    <row r="52" spans="1:20" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="72">
         <v>45</v>
       </c>
-      <c r="B52" s="86" t="s">
+      <c r="B52" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="C52" s="86" t="s">
+      <c r="C52" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="D52" s="86" t="s">
+      <c r="D52" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="E52" s="90" t="s">
+      <c r="E52" s="77" t="s">
         <v>96</v>
       </c>
-      <c r="F52" s="78"/>
-      <c r="G52" s="78"/>
-      <c r="H52" s="78"/>
-      <c r="I52" s="78"/>
-      <c r="J52" s="72" t="s">
+      <c r="F52" s="66"/>
+      <c r="G52" s="66"/>
+      <c r="H52" s="66"/>
+      <c r="I52" s="66"/>
+      <c r="J52" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="K52" s="75"/>
-      <c r="L52" s="75" t="s">
+      <c r="K52" s="63"/>
+      <c r="L52" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="M52" s="75" t="s">
+      <c r="M52" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="N52" s="75"/>
-      <c r="O52" s="75" t="s">
+      <c r="N52" s="63"/>
+      <c r="O52" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="P52" s="75" t="s">
-        <v>488</v>
-      </c>
-      <c r="Q52" s="75"/>
-      <c r="R52" s="88" t="s">
+      <c r="P52" s="63" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q52" s="63"/>
+      <c r="R52" s="75" t="s">
         <v>83</v>
       </c>
-      <c r="S52" s="75"/>
-      <c r="T52" s="89" t="s">
+      <c r="S52" s="63"/>
+      <c r="T52" s="76" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="53" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="59">
+      <c r="A53" s="47">
         <v>46</v>
       </c>
-      <c r="B53" s="60" t="s">
+      <c r="B53" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="C53" s="60" t="s">
+      <c r="C53" s="48" t="s">
         <v>362</v>
       </c>
-      <c r="D53" s="60" t="s">
+      <c r="D53" s="48" t="s">
         <v>365</v>
       </c>
-      <c r="E53" s="61" t="s">
+      <c r="E53" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="F53" s="70"/>
-      <c r="G53" s="69"/>
-      <c r="H53" s="69"/>
-      <c r="I53" s="69"/>
-      <c r="J53" s="62"/>
-      <c r="K53" s="62"/>
-      <c r="L53" s="62"/>
-      <c r="M53" s="62"/>
-      <c r="N53" s="62"/>
-      <c r="O53" s="62"/>
-      <c r="P53" s="62"/>
-      <c r="Q53" s="62"/>
-      <c r="R53" s="66" t="s">
+      <c r="F53" s="58"/>
+      <c r="G53" s="57"/>
+      <c r="H53" s="57"/>
+      <c r="I53" s="57"/>
+      <c r="J53" s="50"/>
+      <c r="K53" s="50"/>
+      <c r="L53" s="50"/>
+      <c r="M53" s="50"/>
+      <c r="N53" s="50"/>
+      <c r="O53" s="50"/>
+      <c r="P53" s="50"/>
+      <c r="Q53" s="50"/>
+      <c r="R53" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="S53" s="67"/>
-      <c r="T53" s="68" t="s">
+      <c r="S53" s="55"/>
+      <c r="T53" s="56" t="s">
         <v>430</v>
       </c>
     </row>
@@ -6666,766 +6662,742 @@
       </c>
     </row>
     <row r="69" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="53">
+      <c r="A69" s="41">
         <v>62</v>
       </c>
-      <c r="B69" s="54" t="s">
+      <c r="B69" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="C69" s="54" t="s">
+      <c r="C69" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="D69" s="54" t="s">
+      <c r="D69" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="E69" s="55" t="s">
+      <c r="E69" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="F69" s="56"/>
-      <c r="G69" s="57"/>
-      <c r="H69" s="57"/>
-      <c r="I69" s="57"/>
-      <c r="J69" s="58"/>
-      <c r="K69" s="58"/>
-      <c r="L69" s="58"/>
-      <c r="M69" s="58"/>
-      <c r="N69" s="58"/>
-      <c r="O69" s="58"/>
-      <c r="P69" s="58"/>
-      <c r="Q69" s="58"/>
-      <c r="R69" s="63"/>
-      <c r="S69" s="64"/>
-      <c r="T69" s="65" t="s">
+      <c r="F69" s="44"/>
+      <c r="G69" s="45"/>
+      <c r="H69" s="45"/>
+      <c r="I69" s="45"/>
+      <c r="J69" s="46"/>
+      <c r="K69" s="46"/>
+      <c r="L69" s="46"/>
+      <c r="M69" s="46"/>
+      <c r="N69" s="46"/>
+      <c r="O69" s="46"/>
+      <c r="P69" s="46"/>
+      <c r="Q69" s="46"/>
+      <c r="R69" s="51"/>
+      <c r="S69" s="52"/>
+      <c r="T69" s="53" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="70" spans="1:20" s="79" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="85">
+    <row r="70" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="72">
         <v>63</v>
       </c>
-      <c r="B70" s="86" t="s">
+      <c r="B70" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="C70" s="86" t="s">
+      <c r="C70" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="D70" s="86" t="s">
+      <c r="D70" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="E70" s="90" t="s">
+      <c r="E70" s="77" t="s">
         <v>125</v>
       </c>
-      <c r="F70" s="71">
+      <c r="F70" s="59">
         <v>45010</v>
       </c>
-      <c r="G70" s="72" t="s">
+      <c r="G70" s="60" t="s">
         <v>448</v>
       </c>
-      <c r="H70" s="72" t="s">
+      <c r="H70" s="60" t="s">
         <v>446</v>
       </c>
-      <c r="I70" s="73" t="s">
+      <c r="I70" s="61" t="s">
         <v>447</v>
       </c>
-      <c r="J70" s="72" t="s">
+      <c r="J70" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="K70" s="74" t="s">
+      <c r="K70" s="62"/>
+      <c r="L70" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="M70" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="N70" s="61" t="s">
+        <v>474</v>
+      </c>
+      <c r="O70" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="P70" s="63" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q70" s="63"/>
+      <c r="R70" s="75"/>
+      <c r="S70" s="63" t="s">
+        <v>488</v>
+      </c>
+      <c r="T70" s="76" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="72">
+        <v>64</v>
+      </c>
+      <c r="B71" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="C71" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="D71" s="73" t="s">
+        <v>126</v>
+      </c>
+      <c r="E71" s="77" t="s">
+        <v>127</v>
+      </c>
+      <c r="F71" s="59">
+        <v>45010</v>
+      </c>
+      <c r="G71" s="60" t="s">
+        <v>448</v>
+      </c>
+      <c r="H71" s="60" t="s">
         <v>449</v>
       </c>
-      <c r="L70" s="72" t="s">
+      <c r="I71" s="61" t="s">
+        <v>450</v>
+      </c>
+      <c r="J71" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="M70" s="72" t="s">
+      <c r="K71" s="62"/>
+      <c r="L71" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="N70" s="73" t="s">
+      <c r="M71" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="N71" s="61" t="s">
         <v>475</v>
       </c>
-      <c r="O70" s="75" t="s">
+      <c r="O71" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="P70" s="75" t="s">
-        <v>487</v>
-      </c>
-      <c r="Q70" s="75"/>
-      <c r="R70" s="88"/>
-      <c r="S70" s="75" t="s">
+      <c r="P71" s="63" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q71" s="63"/>
+      <c r="R71" s="75"/>
+      <c r="S71" s="63" t="s">
+        <v>495</v>
+      </c>
+      <c r="T71" s="76" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="72">
+        <v>65</v>
+      </c>
+      <c r="B72" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="C72" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="D72" s="73" t="s">
+        <v>128</v>
+      </c>
+      <c r="E72" s="77" t="s">
+        <v>129</v>
+      </c>
+      <c r="F72" s="59">
+        <v>45010</v>
+      </c>
+      <c r="G72" s="60" t="s">
+        <v>448</v>
+      </c>
+      <c r="H72" s="60" t="s">
+        <v>451</v>
+      </c>
+      <c r="I72" s="61" t="s">
+        <v>452</v>
+      </c>
+      <c r="J72" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="K72" s="62"/>
+      <c r="L72" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="M72" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="N72" s="61" t="s">
+        <v>476</v>
+      </c>
+      <c r="O72" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="P72" s="63" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q72" s="63"/>
+      <c r="R72" s="75"/>
+      <c r="S72" s="63" t="s">
+        <v>494</v>
+      </c>
+      <c r="T72" s="76" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="72">
+        <v>66</v>
+      </c>
+      <c r="B73" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="C73" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="D73" s="73" t="s">
+        <v>130</v>
+      </c>
+      <c r="E73" s="77" t="s">
+        <v>131</v>
+      </c>
+      <c r="F73" s="59">
+        <v>45010</v>
+      </c>
+      <c r="G73" s="60" t="s">
+        <v>448</v>
+      </c>
+      <c r="H73" s="60" t="s">
+        <v>453</v>
+      </c>
+      <c r="I73" s="61" t="s">
+        <v>454</v>
+      </c>
+      <c r="J73" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="K73" s="62"/>
+      <c r="L73" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="M73" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="N73" s="61" t="s">
+        <v>477</v>
+      </c>
+      <c r="O73" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="P73" s="63" t="s">
+        <v>471</v>
+      </c>
+      <c r="Q73" s="63"/>
+      <c r="R73" s="75"/>
+      <c r="S73" s="63" t="s">
+        <v>493</v>
+      </c>
+      <c r="T73" s="76" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="72">
+        <v>67</v>
+      </c>
+      <c r="B74" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="C74" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="D74" s="73" t="s">
+        <v>132</v>
+      </c>
+      <c r="E74" s="77" t="s">
+        <v>133</v>
+      </c>
+      <c r="F74" s="59">
+        <v>45010</v>
+      </c>
+      <c r="G74" s="60" t="s">
+        <v>448</v>
+      </c>
+      <c r="H74" s="60" t="s">
+        <v>455</v>
+      </c>
+      <c r="I74" s="61" t="s">
+        <v>456</v>
+      </c>
+      <c r="J74" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="K74" s="62"/>
+      <c r="L74" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="M74" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="N74" s="61" t="s">
+        <v>478</v>
+      </c>
+      <c r="O74" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="P74" s="63" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q74" s="63"/>
+      <c r="R74" s="75"/>
+      <c r="S74" s="63" t="s">
+        <v>492</v>
+      </c>
+      <c r="T74" s="76" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="72">
+        <v>68</v>
+      </c>
+      <c r="B75" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="C75" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="D75" s="73" t="s">
+        <v>134</v>
+      </c>
+      <c r="E75" s="77" t="s">
+        <v>135</v>
+      </c>
+      <c r="F75" s="59">
+        <v>45010</v>
+      </c>
+      <c r="G75" s="60" t="s">
+        <v>448</v>
+      </c>
+      <c r="H75" s="60" t="s">
+        <v>457</v>
+      </c>
+      <c r="I75" s="61" t="s">
+        <v>458</v>
+      </c>
+      <c r="J75" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="K75" s="62"/>
+      <c r="L75" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="M75" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="N75" s="61" t="s">
+        <v>479</v>
+      </c>
+      <c r="O75" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="P75" s="63" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q75" s="63"/>
+      <c r="R75" s="75"/>
+      <c r="S75" s="63" t="s">
+        <v>491</v>
+      </c>
+      <c r="T75" s="76" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="72">
+        <v>69</v>
+      </c>
+      <c r="B76" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="C76" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="D76" s="73" t="s">
+        <v>136</v>
+      </c>
+      <c r="E76" s="77" t="s">
+        <v>137</v>
+      </c>
+      <c r="F76" s="59">
+        <v>45010</v>
+      </c>
+      <c r="G76" s="60" t="s">
+        <v>448</v>
+      </c>
+      <c r="H76" s="60" t="s">
+        <v>459</v>
+      </c>
+      <c r="I76" s="61" t="s">
+        <v>460</v>
+      </c>
+      <c r="J76" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="K76" s="62"/>
+      <c r="L76" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="M76" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="N76" s="61" t="s">
+        <v>480</v>
+      </c>
+      <c r="O76" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="P76" s="63" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q76" s="63"/>
+      <c r="R76" s="75"/>
+      <c r="S76" s="63" t="s">
+        <v>490</v>
+      </c>
+      <c r="T76" s="76" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="72">
+        <v>70</v>
+      </c>
+      <c r="B77" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="C77" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="D77" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="E77" s="77" t="s">
+        <v>139</v>
+      </c>
+      <c r="F77" s="59">
+        <v>45010</v>
+      </c>
+      <c r="G77" s="60" t="s">
+        <v>448</v>
+      </c>
+      <c r="H77" s="60" t="s">
+        <v>461</v>
+      </c>
+      <c r="I77" s="61" t="s">
+        <v>462</v>
+      </c>
+      <c r="J77" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="K77" s="62"/>
+      <c r="L77" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="M77" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="N77" s="61" t="s">
+        <v>481</v>
+      </c>
+      <c r="O77" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="P77" s="63" t="s">
+        <v>471</v>
+      </c>
+      <c r="Q77" s="63"/>
+      <c r="R77" s="75"/>
+      <c r="S77" s="63" t="s">
         <v>489</v>
       </c>
-      <c r="T70" s="89" t="s">
+      <c r="T77" s="76" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="71" spans="1:20" s="79" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="85">
-        <v>64</v>
-      </c>
-      <c r="B71" s="86" t="s">
+    <row r="78" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="72">
+        <v>71</v>
+      </c>
+      <c r="B78" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="C71" s="86" t="s">
+      <c r="C78" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="D71" s="86" t="s">
-        <v>126</v>
-      </c>
-      <c r="E71" s="90" t="s">
-        <v>127</v>
-      </c>
-      <c r="F71" s="71">
+      <c r="D78" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="E78" s="77" t="s">
+        <v>141</v>
+      </c>
+      <c r="F78" s="59">
         <v>45010</v>
       </c>
-      <c r="G71" s="72" t="s">
+      <c r="G78" s="60" t="s">
         <v>448</v>
       </c>
-      <c r="H71" s="72" t="s">
-        <v>450</v>
-      </c>
-      <c r="I71" s="73" t="s">
-        <v>451</v>
-      </c>
-      <c r="J71" s="72" t="s">
+      <c r="H78" s="60" t="s">
+        <v>463</v>
+      </c>
+      <c r="I78" s="61" t="s">
+        <v>464</v>
+      </c>
+      <c r="J78" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="K71" s="74" t="s">
-        <v>449</v>
-      </c>
-      <c r="L71" s="72" t="s">
+      <c r="K78" s="62"/>
+      <c r="L78" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="M71" s="72" t="s">
+      <c r="M78" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="N71" s="73" t="s">
-        <v>476</v>
-      </c>
-      <c r="O71" s="75" t="s">
+      <c r="N78" s="61" t="s">
+        <v>482</v>
+      </c>
+      <c r="O78" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="P71" s="75" t="s">
-        <v>487</v>
-      </c>
-      <c r="Q71" s="75"/>
-      <c r="R71" s="88"/>
-      <c r="S71" s="75" t="s">
+      <c r="P78" s="63" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q78" s="63"/>
+      <c r="R78" s="75"/>
+      <c r="S78" s="63" t="s">
+        <v>489</v>
+      </c>
+      <c r="T78" s="76" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="72">
+        <v>72</v>
+      </c>
+      <c r="B79" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="C79" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="D79" s="73" t="s">
+        <v>142</v>
+      </c>
+      <c r="E79" s="77" t="s">
+        <v>143</v>
+      </c>
+      <c r="F79" s="59">
+        <v>45010</v>
+      </c>
+      <c r="G79" s="60" t="s">
+        <v>448</v>
+      </c>
+      <c r="H79" s="60" t="s">
+        <v>465</v>
+      </c>
+      <c r="I79" s="61" t="s">
+        <v>466</v>
+      </c>
+      <c r="J79" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="K79" s="62"/>
+      <c r="L79" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="M79" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="N79" s="61" t="s">
+        <v>483</v>
+      </c>
+      <c r="O79" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="P79" s="63" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q79" s="63"/>
+      <c r="R79" s="75"/>
+      <c r="S79" s="63" t="s">
         <v>496</v>
       </c>
-      <c r="T71" s="89" t="s">
+      <c r="T79" s="76" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="72" spans="1:20" s="79" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="85">
-        <v>65</v>
-      </c>
-      <c r="B72" s="86" t="s">
+    <row r="80" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="72">
+        <v>73</v>
+      </c>
+      <c r="B80" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="C72" s="86" t="s">
+      <c r="C80" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="D72" s="86" t="s">
-        <v>128</v>
-      </c>
-      <c r="E72" s="90" t="s">
-        <v>129</v>
-      </c>
-      <c r="F72" s="71">
+      <c r="D80" s="73" t="s">
+        <v>144</v>
+      </c>
+      <c r="E80" s="77" t="s">
+        <v>145</v>
+      </c>
+      <c r="F80" s="59">
         <v>45010</v>
       </c>
-      <c r="G72" s="72" t="s">
+      <c r="G80" s="60" t="s">
         <v>448</v>
       </c>
-      <c r="H72" s="72" t="s">
-        <v>452</v>
-      </c>
-      <c r="I72" s="73" t="s">
-        <v>453</v>
-      </c>
-      <c r="J72" s="72" t="s">
+      <c r="H80" s="60" t="s">
+        <v>467</v>
+      </c>
+      <c r="I80" s="61" t="s">
+        <v>468</v>
+      </c>
+      <c r="J80" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="K72" s="74" t="s">
-        <v>449</v>
-      </c>
-      <c r="L72" s="72" t="s">
+      <c r="K80" s="62"/>
+      <c r="L80" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="M72" s="72" t="s">
+      <c r="M80" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="N72" s="73" t="s">
-        <v>477</v>
-      </c>
-      <c r="O72" s="75" t="s">
+      <c r="N80" s="61" t="s">
+        <v>484</v>
+      </c>
+      <c r="O80" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="P72" s="75" t="s">
-        <v>487</v>
-      </c>
-      <c r="Q72" s="75"/>
-      <c r="R72" s="88"/>
-      <c r="S72" s="75" t="s">
-        <v>495</v>
-      </c>
-      <c r="T72" s="89" t="s">
+      <c r="P80" s="63" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q80" s="63"/>
+      <c r="R80" s="75"/>
+      <c r="S80" s="63" t="s">
+        <v>497</v>
+      </c>
+      <c r="T80" s="76" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="73" spans="1:20" s="79" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="85">
-        <v>66</v>
-      </c>
-      <c r="B73" s="86" t="s">
+    <row r="81" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="72">
+        <v>74</v>
+      </c>
+      <c r="B81" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="C73" s="86" t="s">
+      <c r="C81" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="D73" s="86" t="s">
-        <v>130</v>
-      </c>
-      <c r="E73" s="90" t="s">
-        <v>131</v>
-      </c>
-      <c r="F73" s="71">
+      <c r="D81" s="73" t="s">
+        <v>146</v>
+      </c>
+      <c r="E81" s="77" t="s">
+        <v>147</v>
+      </c>
+      <c r="F81" s="59">
         <v>45010</v>
       </c>
-      <c r="G73" s="72" t="s">
+      <c r="G81" s="60" t="s">
         <v>448</v>
       </c>
-      <c r="H73" s="72" t="s">
-        <v>454</v>
-      </c>
-      <c r="I73" s="73" t="s">
-        <v>455</v>
-      </c>
-      <c r="J73" s="72" t="s">
+      <c r="H81" s="60" t="s">
+        <v>469</v>
+      </c>
+      <c r="I81" s="61" t="s">
+        <v>470</v>
+      </c>
+      <c r="J81" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="K73" s="74" t="s">
-        <v>449</v>
-      </c>
-      <c r="L73" s="72" t="s">
+      <c r="K81" s="62"/>
+      <c r="L81" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="M73" s="72" t="s">
+      <c r="M81" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="N73" s="73" t="s">
-        <v>478</v>
-      </c>
-      <c r="O73" s="75" t="s">
+      <c r="N81" s="61" t="s">
+        <v>485</v>
+      </c>
+      <c r="O81" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="P73" s="75" t="s">
-        <v>472</v>
-      </c>
-      <c r="Q73" s="75"/>
-      <c r="R73" s="88"/>
-      <c r="S73" s="75" t="s">
-        <v>494</v>
-      </c>
-      <c r="T73" s="89" t="s">
+      <c r="P81" s="63" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q81" s="63"/>
+      <c r="R81" s="75"/>
+      <c r="S81" s="63" t="s">
+        <v>497</v>
+      </c>
+      <c r="T81" s="76" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="74" spans="1:20" s="79" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="85">
-        <v>67</v>
-      </c>
-      <c r="B74" s="86" t="s">
+    <row r="82" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="47">
+        <v>75</v>
+      </c>
+      <c r="B82" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="C74" s="86" t="s">
-        <v>37</v>
-      </c>
-      <c r="D74" s="86" t="s">
-        <v>132</v>
-      </c>
-      <c r="E74" s="90" t="s">
-        <v>133</v>
-      </c>
-      <c r="F74" s="71">
-        <v>45010</v>
-      </c>
-      <c r="G74" s="72" t="s">
-        <v>448</v>
-      </c>
-      <c r="H74" s="72" t="s">
-        <v>456</v>
-      </c>
-      <c r="I74" s="73" t="s">
-        <v>457</v>
-      </c>
-      <c r="J74" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="K74" s="74" t="s">
-        <v>449</v>
-      </c>
-      <c r="L74" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="M74" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="N74" s="73" t="s">
-        <v>479</v>
-      </c>
-      <c r="O74" s="75" t="s">
-        <v>83</v>
-      </c>
-      <c r="P74" s="75" t="s">
-        <v>487</v>
-      </c>
-      <c r="Q74" s="75"/>
-      <c r="R74" s="88"/>
-      <c r="S74" s="75" t="s">
-        <v>493</v>
-      </c>
-      <c r="T74" s="89" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="75" spans="1:20" s="79" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="85">
-        <v>68</v>
-      </c>
-      <c r="B75" s="86" t="s">
-        <v>25</v>
-      </c>
-      <c r="C75" s="86" t="s">
-        <v>37</v>
-      </c>
-      <c r="D75" s="86" t="s">
-        <v>134</v>
-      </c>
-      <c r="E75" s="90" t="s">
-        <v>135</v>
-      </c>
-      <c r="F75" s="71">
-        <v>45010</v>
-      </c>
-      <c r="G75" s="72" t="s">
-        <v>448</v>
-      </c>
-      <c r="H75" s="72" t="s">
-        <v>458</v>
-      </c>
-      <c r="I75" s="73" t="s">
-        <v>459</v>
-      </c>
-      <c r="J75" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="K75" s="74" t="s">
-        <v>449</v>
-      </c>
-      <c r="L75" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="M75" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="N75" s="73" t="s">
-        <v>480</v>
-      </c>
-      <c r="O75" s="75" t="s">
-        <v>83</v>
-      </c>
-      <c r="P75" s="75" t="s">
-        <v>487</v>
-      </c>
-      <c r="Q75" s="75"/>
-      <c r="R75" s="88"/>
-      <c r="S75" s="75" t="s">
-        <v>492</v>
-      </c>
-      <c r="T75" s="89" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="76" spans="1:20" s="79" customFormat="1" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="85">
-        <v>69</v>
-      </c>
-      <c r="B76" s="86" t="s">
-        <v>25</v>
-      </c>
-      <c r="C76" s="86" t="s">
-        <v>37</v>
-      </c>
-      <c r="D76" s="86" t="s">
-        <v>136</v>
-      </c>
-      <c r="E76" s="90" t="s">
-        <v>137</v>
-      </c>
-      <c r="F76" s="71">
-        <v>45010</v>
-      </c>
-      <c r="G76" s="72" t="s">
-        <v>448</v>
-      </c>
-      <c r="H76" s="72" t="s">
-        <v>460</v>
-      </c>
-      <c r="I76" s="73" t="s">
-        <v>461</v>
-      </c>
-      <c r="J76" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="K76" s="74" t="s">
-        <v>449</v>
-      </c>
-      <c r="L76" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="M76" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="N76" s="73" t="s">
-        <v>481</v>
-      </c>
-      <c r="O76" s="75" t="s">
-        <v>83</v>
-      </c>
-      <c r="P76" s="75" t="s">
-        <v>487</v>
-      </c>
-      <c r="Q76" s="75"/>
-      <c r="R76" s="88"/>
-      <c r="S76" s="75" t="s">
-        <v>491</v>
-      </c>
-      <c r="T76" s="89" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="77" spans="1:20" s="79" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="85">
-        <v>70</v>
-      </c>
-      <c r="B77" s="86" t="s">
-        <v>25</v>
-      </c>
-      <c r="C77" s="86" t="s">
-        <v>37</v>
-      </c>
-      <c r="D77" s="86" t="s">
-        <v>138</v>
-      </c>
-      <c r="E77" s="90" t="s">
-        <v>139</v>
-      </c>
-      <c r="F77" s="71">
-        <v>45010</v>
-      </c>
-      <c r="G77" s="72" t="s">
-        <v>448</v>
-      </c>
-      <c r="H77" s="72" t="s">
-        <v>462</v>
-      </c>
-      <c r="I77" s="73" t="s">
-        <v>463</v>
-      </c>
-      <c r="J77" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="K77" s="74" t="s">
-        <v>449</v>
-      </c>
-      <c r="L77" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="M77" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="N77" s="73" t="s">
-        <v>482</v>
-      </c>
-      <c r="O77" s="75" t="s">
-        <v>83</v>
-      </c>
-      <c r="P77" s="75" t="s">
-        <v>472</v>
-      </c>
-      <c r="Q77" s="75"/>
-      <c r="R77" s="88"/>
-      <c r="S77" s="75" t="s">
-        <v>490</v>
-      </c>
-      <c r="T77" s="89" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="78" spans="1:20" s="79" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="85">
-        <v>71</v>
-      </c>
-      <c r="B78" s="86" t="s">
-        <v>25</v>
-      </c>
-      <c r="C78" s="86" t="s">
-        <v>37</v>
-      </c>
-      <c r="D78" s="86" t="s">
-        <v>140</v>
-      </c>
-      <c r="E78" s="90" t="s">
-        <v>141</v>
-      </c>
-      <c r="F78" s="71">
-        <v>45010</v>
-      </c>
-      <c r="G78" s="72" t="s">
-        <v>448</v>
-      </c>
-      <c r="H78" s="72" t="s">
-        <v>464</v>
-      </c>
-      <c r="I78" s="73" t="s">
-        <v>465</v>
-      </c>
-      <c r="J78" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="K78" s="74" t="s">
-        <v>449</v>
-      </c>
-      <c r="L78" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="M78" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="N78" s="73" t="s">
-        <v>483</v>
-      </c>
-      <c r="O78" s="75" t="s">
-        <v>83</v>
-      </c>
-      <c r="P78" s="75" t="s">
-        <v>487</v>
-      </c>
-      <c r="Q78" s="75"/>
-      <c r="R78" s="88"/>
-      <c r="S78" s="75" t="s">
-        <v>490</v>
-      </c>
-      <c r="T78" s="89" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="79" spans="1:20" s="79" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="85">
-        <v>72</v>
-      </c>
-      <c r="B79" s="86" t="s">
-        <v>25</v>
-      </c>
-      <c r="C79" s="86" t="s">
-        <v>37</v>
-      </c>
-      <c r="D79" s="86" t="s">
-        <v>142</v>
-      </c>
-      <c r="E79" s="90" t="s">
-        <v>143</v>
-      </c>
-      <c r="F79" s="71">
-        <v>45010</v>
-      </c>
-      <c r="G79" s="72" t="s">
-        <v>448</v>
-      </c>
-      <c r="H79" s="72" t="s">
-        <v>466</v>
-      </c>
-      <c r="I79" s="73" t="s">
-        <v>467</v>
-      </c>
-      <c r="J79" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="K79" s="74" t="s">
-        <v>449</v>
-      </c>
-      <c r="L79" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="M79" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="N79" s="73" t="s">
-        <v>484</v>
-      </c>
-      <c r="O79" s="75" t="s">
-        <v>83</v>
-      </c>
-      <c r="P79" s="75" t="s">
-        <v>487</v>
-      </c>
-      <c r="Q79" s="75"/>
-      <c r="R79" s="88"/>
-      <c r="S79" s="75" t="s">
-        <v>497</v>
-      </c>
-      <c r="T79" s="89" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="80" spans="1:20" s="79" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="85">
-        <v>73</v>
-      </c>
-      <c r="B80" s="86" t="s">
-        <v>25</v>
-      </c>
-      <c r="C80" s="86" t="s">
-        <v>37</v>
-      </c>
-      <c r="D80" s="86" t="s">
-        <v>144</v>
-      </c>
-      <c r="E80" s="90" t="s">
-        <v>145</v>
-      </c>
-      <c r="F80" s="71">
-        <v>45010</v>
-      </c>
-      <c r="G80" s="72" t="s">
-        <v>448</v>
-      </c>
-      <c r="H80" s="72" t="s">
-        <v>468</v>
-      </c>
-      <c r="I80" s="73" t="s">
-        <v>469</v>
-      </c>
-      <c r="J80" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="K80" s="74" t="s">
-        <v>449</v>
-      </c>
-      <c r="L80" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="M80" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="N80" s="73" t="s">
-        <v>485</v>
-      </c>
-      <c r="O80" s="75" t="s">
-        <v>83</v>
-      </c>
-      <c r="P80" s="75" t="s">
-        <v>487</v>
-      </c>
-      <c r="Q80" s="75"/>
-      <c r="R80" s="88"/>
-      <c r="S80" s="75" t="s">
-        <v>498</v>
-      </c>
-      <c r="T80" s="89" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="81" spans="1:20" s="79" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="85">
-        <v>74</v>
-      </c>
-      <c r="B81" s="86" t="s">
-        <v>25</v>
-      </c>
-      <c r="C81" s="86" t="s">
-        <v>37</v>
-      </c>
-      <c r="D81" s="86" t="s">
-        <v>146</v>
-      </c>
-      <c r="E81" s="90" t="s">
-        <v>147</v>
-      </c>
-      <c r="F81" s="71">
-        <v>45010</v>
-      </c>
-      <c r="G81" s="72" t="s">
-        <v>448</v>
-      </c>
-      <c r="H81" s="72" t="s">
-        <v>470</v>
-      </c>
-      <c r="I81" s="73" t="s">
-        <v>471</v>
-      </c>
-      <c r="J81" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="K81" s="74" t="s">
-        <v>449</v>
-      </c>
-      <c r="L81" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="M81" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="N81" s="73" t="s">
-        <v>486</v>
-      </c>
-      <c r="O81" s="75" t="s">
-        <v>83</v>
-      </c>
-      <c r="P81" s="75" t="s">
-        <v>487</v>
-      </c>
-      <c r="Q81" s="75"/>
-      <c r="R81" s="88"/>
-      <c r="S81" s="75" t="s">
-        <v>498</v>
-      </c>
-      <c r="T81" s="89" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="82" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="59">
-        <v>75</v>
-      </c>
-      <c r="B82" s="60" t="s">
-        <v>25</v>
-      </c>
-      <c r="C82" s="60" t="s">
+      <c r="C82" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="D82" s="60" t="s">
+      <c r="D82" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="E82" s="61" t="s">
+      <c r="E82" s="49" t="s">
         <v>149</v>
       </c>
-      <c r="F82" s="70"/>
-      <c r="G82" s="69"/>
-      <c r="H82" s="69"/>
-      <c r="I82" s="69"/>
-      <c r="J82" s="62"/>
-      <c r="K82" s="62"/>
-      <c r="L82" s="62"/>
-      <c r="M82" s="62"/>
-      <c r="N82" s="62"/>
-      <c r="O82" s="62"/>
-      <c r="P82" s="62"/>
-      <c r="Q82" s="62"/>
-      <c r="R82" s="66"/>
-      <c r="S82" s="67"/>
-      <c r="T82" s="68" t="s">
+      <c r="F82" s="58"/>
+      <c r="G82" s="57"/>
+      <c r="H82" s="57"/>
+      <c r="I82" s="57"/>
+      <c r="J82" s="50"/>
+      <c r="K82" s="50"/>
+      <c r="L82" s="50"/>
+      <c r="M82" s="50"/>
+      <c r="N82" s="50"/>
+      <c r="O82" s="50"/>
+      <c r="P82" s="50"/>
+      <c r="Q82" s="50"/>
+      <c r="R82" s="54"/>
+      <c r="S82" s="55"/>
+      <c r="T82" s="56" t="s">
         <v>430</v>
       </c>
     </row>
@@ -27135,12 +27107,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -27375,20 +27349,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -27413,18 +27394,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Corrette segnalazioni di errore sul Motivo_Ricovero
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
+++ b/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSE20\medarchiver\it-fse-accreditamento\GATEWAY\S1#111MEDARCHIVER\MEDARCHIVER\MEDARCHIVER_FSE2.0\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14018B0D-6A27-4234-B950-FFD69ACE9ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD9AE97-534F-4D70-95E7-885FA7FCF4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="499">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -1844,30 +1844,6 @@
     </r>
   </si>
   <si>
-    <t>4c966300e4a7e391</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.5187a7c6983155e8ce8a0349302fbf5ed672a64b2432a651aeaa4c11820cfe76.f9777ab0f2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>fcd241d714214d71</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.93079f05d0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>90488801615ce3ac</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.f12a71196e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>75d7c3489c92c304</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.8bbe81b168^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>8b7525e51724add7</t>
   </si>
   <si>
@@ -1883,126 +1859,12 @@
     <t>Il campo action_id non è corretto</t>
   </si>
   <si>
-    <t>3c2faa42df7f821c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.cf4a755127^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-03-25T08:54:29Z</t>
   </si>
   <si>
-    <t>555d2cc937e460a3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.5daaf1b844^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>02d4e67d72b5d6e0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.8f2183046e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>ec6b0d78adb8b044</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.263f4c7c1c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>9570040d112f95aa</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.8324f629b4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>6812efc15706e71e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.5433abb688^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>c89b41b98a283967</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.7b3967fba1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>dfe56abf4fec1f6b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.b6c22208f6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>7936623f68292866</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.65b896431a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>726fc6c594085816</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.5c4e4fecb0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>17feb72f4d2cd60f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.0af3c83814^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>42ff0c812e57d933</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.4e7d761134^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Trattandosi di un errore che non può essere gestito dall'utente, l'applicazione mostra un messaggio di errore di autenticazione e l'errore verrà poi gestito in back-office.</t>
   </si>
   <si>
-    <t>Errore nella validazione del documento. Contattare l'amministratore di sistema. [Il campo action_id non è corretto]</t>
-  </si>
-  <si>
-    <t>Errore nella validazione del documento. Contattare l'amministratore di sistema. [Il campo purpose_of_use non è valorizzato]</t>
-  </si>
-  <si>
-    <t>Errore nella validazione del documento. Contattare l'amministratore di sistema. [ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'languageCode'. One of '{urn:hl7-org:v3":confidentialityCode}' is expected."]</t>
-  </si>
-  <si>
-    <t>Errore nella validazione del documento. Contattare l'amministratore di sistema. [JWT payload: Person id presente nel JWT differente dal codice fiscale del paziente previsto sul CDA]</t>
-  </si>
-  <si>
-    <t>Errore nella validazione del documento. Contattare l'amministratore di sistema.[ERRORE-6| L'elemento 'confidentialityCode' di ClinicalDocument DEVE avere l'attributo @code valorizzato con 'N' o 'V', e il @codeSystem='2.16.840.1.113883.5.25']</t>
-  </si>
-  <si>
-    <t>Errore nella validazione del documento. Contattare l'amministratore di sistema. [ERRORE-11| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi 'country', 'city' e 'streetAddressLine' ]</t>
-  </si>
-  <si>
-    <t>Errore nella validazione del documento. Contattare l'amministratore di sistema. [ERRORE-14| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family']</t>
-  </si>
-  <si>
-    <t>Errore nella validazione del documento. Contattare l'amministratore di sistema. [Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: N]]</t>
-  </si>
-  <si>
-    <t>Errore nella validazione del documento. Contattare l'amministratore di sistema.[[ERRORE-b5| Sezione Condizioni del paziente e diagnosi alla dimissione: la sezione DEVE essere presente],[ERRORE-b6| Sezione Condizioni del paziente e diagnosi alla dimissione: La ]sezione DEVE contenere l'elemento 'text'],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO' contenere l'elemento 'entry' ]</t>
-  </si>
-  <si>
-    <t>Errore nella validazione del documento. Contattare l'amministratore di sistema. [[ERRORE-b3| Sezione Decorso Ospedaliero: la sezione DEVE essere presente],[ERRORE-b4| Sezione Decorso Ospedaliero: La sezione deve contenere l'elemento 'text']]</t>
-  </si>
-  <si>
-    <t>Errore nella validazione del documento. Contattare l'amministratore di sistema.[[ERRORE-b26| Sotto-sezione Anamnesi: l'elemento entry/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato]]</t>
-  </si>
-  <si>
-    <t>Errore nella validazione del documento. Contattare l'amministratore di sistema. [[ERRORE-b94|Sezione Terapia farmacologica alla dimissione: section/entry/substanceAdministration/effectiveTime deve avere l'elemento 'low' valorizzato ]]</t>
-  </si>
-  <si>
-    <t>Errore nella validazione del documento. Contattare l'amministratore di sistema. [Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: xx410.72]]</t>
-  </si>
-  <si>
-    <t>Errore nella validazione del documento. Contattare l'amministratore di sistema. [Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.112 v2.1.0, Codes: xxPO]]</t>
-  </si>
-  <si>
     <t>Trattandosi di un errore che non può essere gestito dall'utente, l'applicazione mostra un messaggio di errore di autenticazione e l'errore verrà poi gestito in back-office. L'errore reale restituito dalla chiamata di validazione può o meno essere mostrato all'utente a seconda della configurazione del sistema.</t>
   </si>
   <si>
@@ -2049,6 +1911,135 @@
   </si>
   <si>
     <t>subject_application_version: 1.0.0.0</t>
+  </si>
+  <si>
+    <t>2023-04-21T18:04:06Z</t>
+  </si>
+  <si>
+    <t>b186c43468e7fe99</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.5187a7c6983155e8ce8a0349302fbf5ed672a64b2432a651aeaa4c11820cfe76.daf987b93c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>29ff771561ed25f3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.fd7263f3a3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>e61919572362204c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.1542a52119^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>4d98f9271a26a796</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.1d0331b465^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>5dfa218167ea8431</t>
+  </si>
+  <si>
+    <t>c4df008884576039</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.7b2ec5bf4f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>4ab2acad4f04d91f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.95e2c00f70^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ec0153ebef48f551</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.9f6574bab0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>563a586ee2ce71d9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.b8bd7d2914^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>00375537684234bb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.dceb415bf8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>c13bdc9a3cbac769</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.b974f490a8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>710e341826ecbba0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.17bf79b3e5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>a5bf10e3010dc43c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.1e2edd104d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>1215e8a417d212d6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.ecb040e473^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>db30aa07a7235dd0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.4c37be04cc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>3788971fec52d857</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.a6a05fe07f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'languageCode'. One of '{urn:hl7-org:v3":confidentialityCode}' is expected."</t>
+  </si>
+  <si>
+    <t>JWT payload: Person id presente nel JWT differente dal codice fiscale del paziente previsto sul CDA</t>
+  </si>
+  <si>
+    <t>[ERRORE-6| L'elemento 'confidentialityCode' di ClinicalDocument DEVE avere l'attributo @code valorizzato con 'N' o 'V', e il @codeSystem='2.16.840.1.113883.5.25']</t>
+  </si>
+  <si>
+    <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: N]</t>
+  </si>
+  <si>
+    <t>[ERRORE-b3| Sezione Decorso Ospedaliero: la sezione DEVE essere presente],[ERRORE-b4| Sezione Decorso Ospedaliero: La sezione deve contenere l'elemento 'text']</t>
+  </si>
+  <si>
+    <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.112 v2.1.0, Codes: xxPO]</t>
+  </si>
+  <si>
+    <t>[ERRORE-b94|Sezione Terapia farmacologica alla dimissione: section/entry/substanceAdministration/effectiveTime deve avere l'elemento 'low' valorizzato ]</t>
+  </si>
+  <si>
+    <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: xx410.72]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ERRORE-b5| Sezione Condizioni del paziente e diagnosi alla dimissione: la sezione DEVE essere presente],[ERRORE-b6| Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione DEVE contenere l'elemento 'text'],[W003|  Sezione Condizioni del </t>
+  </si>
+  <si>
+    <t>[ERRORE-11| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi 'country', 'city' e 'streetAddressLine' ]</t>
+  </si>
+  <si>
+    <t>[ERRORE-14| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family']</t>
   </si>
 </sst>
 </file>
@@ -2178,7 +2169,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -2569,11 +2560,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2736,9 +2766,6 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2816,6 +2843,40 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4263,11 +4324,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T993"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:B5"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4310,14 +4371,14 @@
       <c r="T1" s="35"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="82" t="s">
-        <v>498</v>
-      </c>
-      <c r="D2" s="81"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="81" t="s">
+        <v>452</v>
+      </c>
+      <c r="D2" s="80"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -4335,14 +4396,14 @@
       <c r="T2" s="35"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="89" t="s">
-        <v>499</v>
-      </c>
-      <c r="D3" s="81"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="88" t="s">
+        <v>453</v>
+      </c>
+      <c r="D3" s="80"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -4360,12 +4421,12 @@
       <c r="T3" s="35"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="85"/>
-      <c r="B4" s="86"/>
-      <c r="C4" s="89" t="s">
-        <v>500</v>
-      </c>
-      <c r="D4" s="81"/>
+      <c r="A4" s="84"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="88" t="s">
+        <v>454</v>
+      </c>
+      <c r="D4" s="80"/>
       <c r="E4" s="2"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -4384,12 +4445,12 @@
       <c r="T4" s="35"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="87"/>
-      <c r="B5" s="88"/>
-      <c r="C5" s="89" t="s">
-        <v>501</v>
-      </c>
-      <c r="D5" s="81"/>
+      <c r="A5" s="86"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="88" t="s">
+        <v>455</v>
+      </c>
+      <c r="D5" s="80"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -4407,8 +4468,8 @@
       <c r="T5" s="35"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="78"/>
-      <c r="B6" s="79"/>
+      <c r="A6" s="77"/>
+      <c r="B6" s="78"/>
       <c r="C6" s="10"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -4464,64 +4525,64 @@
       <c r="T8" s="35"/>
     </row>
     <row r="9" spans="1:20" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="68" t="s">
+      <c r="C9" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="68" t="s">
+      <c r="D9" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="68" t="s">
+      <c r="E9" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="68" t="s">
+      <c r="F9" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="68" t="s">
+      <c r="G9" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="68" t="s">
+      <c r="H9" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="68" t="s">
+      <c r="I9" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="68" t="s">
+      <c r="J9" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="68" t="s">
+      <c r="K9" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="69" t="s">
+      <c r="L9" s="68" t="s">
         <v>424</v>
       </c>
-      <c r="M9" s="69" t="s">
+      <c r="M9" s="68" t="s">
         <v>425</v>
       </c>
-      <c r="N9" s="69" t="s">
+      <c r="N9" s="68" t="s">
         <v>426</v>
       </c>
-      <c r="O9" s="69" t="s">
+      <c r="O9" s="68" t="s">
         <v>427</v>
       </c>
-      <c r="P9" s="68" t="s">
+      <c r="P9" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="68" t="s">
+      <c r="Q9" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="R9" s="70" t="s">
+      <c r="R9" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="S9" s="68" t="s">
+      <c r="S9" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="T9" s="71" t="s">
+      <c r="T9" s="70" t="s">
         <v>428</v>
       </c>
     </row>
@@ -4696,178 +4757,178 @@
       </c>
     </row>
     <row r="15" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="72">
+      <c r="A15" s="71">
         <v>6</v>
       </c>
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="73" t="s">
+      <c r="D15" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="77" t="s">
+      <c r="E15" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="59">
-        <v>45010</v>
+      <c r="F15" s="98">
+        <v>45037</v>
       </c>
       <c r="G15" s="60" t="s">
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="H15" s="60" t="s">
-        <v>433</v>
-      </c>
-      <c r="I15" s="61" t="s">
-        <v>434</v>
-      </c>
-      <c r="J15" s="60" t="s">
+        <v>457</v>
+      </c>
+      <c r="I15" s="60" t="s">
+        <v>458</v>
+      </c>
+      <c r="J15" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="K15" s="62"/>
-      <c r="L15" s="60"/>
-      <c r="M15" s="60"/>
-      <c r="N15" s="61"/>
-      <c r="O15" s="63"/>
-      <c r="P15" s="63"/>
-      <c r="Q15" s="63"/>
-      <c r="R15" s="75"/>
-      <c r="S15" s="63"/>
-      <c r="T15" s="76" t="s">
+      <c r="K15" s="61"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="59"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="62"/>
+      <c r="P15" s="62"/>
+      <c r="Q15" s="62"/>
+      <c r="R15" s="74"/>
+      <c r="S15" s="62"/>
+      <c r="T15" s="75" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="72">
+      <c r="A16" s="71">
         <v>7</v>
       </c>
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="73" t="s">
+      <c r="C16" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="73" t="s">
+      <c r="D16" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="77" t="s">
+      <c r="E16" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="59">
-        <v>45010</v>
+      <c r="F16" s="98">
+        <v>45037</v>
       </c>
       <c r="G16" s="60" t="s">
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="H16" s="60" t="s">
-        <v>435</v>
-      </c>
-      <c r="I16" s="61" t="s">
-        <v>436</v>
-      </c>
-      <c r="J16" s="60" t="s">
+        <v>459</v>
+      </c>
+      <c r="I16" s="60" t="s">
+        <v>460</v>
+      </c>
+      <c r="J16" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="K16" s="62"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="60"/>
-      <c r="N16" s="61"/>
-      <c r="O16" s="63"/>
-      <c r="P16" s="63"/>
-      <c r="Q16" s="63"/>
-      <c r="R16" s="75"/>
-      <c r="S16" s="63"/>
-      <c r="T16" s="76" t="s">
+      <c r="K16" s="61"/>
+      <c r="L16" s="59"/>
+      <c r="M16" s="59"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="62"/>
+      <c r="P16" s="62"/>
+      <c r="Q16" s="62"/>
+      <c r="R16" s="74"/>
+      <c r="S16" s="62"/>
+      <c r="T16" s="75" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="72">
+      <c r="A17" s="71">
         <v>8</v>
       </c>
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="73" t="s">
+      <c r="C17" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="73" t="s">
+      <c r="D17" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="77" t="s">
+      <c r="E17" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="59">
-        <v>45010</v>
+      <c r="F17" s="98">
+        <v>45037</v>
       </c>
       <c r="G17" s="60" t="s">
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="H17" s="60" t="s">
-        <v>437</v>
-      </c>
-      <c r="I17" s="61" t="s">
-        <v>438</v>
-      </c>
-      <c r="J17" s="60" t="s">
+        <v>461</v>
+      </c>
+      <c r="I17" s="60" t="s">
+        <v>462</v>
+      </c>
+      <c r="J17" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="K17" s="62"/>
-      <c r="L17" s="60"/>
-      <c r="M17" s="60"/>
-      <c r="N17" s="61"/>
-      <c r="O17" s="63"/>
-      <c r="P17" s="63"/>
-      <c r="Q17" s="63"/>
-      <c r="R17" s="75"/>
-      <c r="S17" s="63"/>
-      <c r="T17" s="76" t="s">
+      <c r="K17" s="61"/>
+      <c r="L17" s="59"/>
+      <c r="M17" s="59"/>
+      <c r="N17" s="60"/>
+      <c r="O17" s="62"/>
+      <c r="P17" s="62"/>
+      <c r="Q17" s="62"/>
+      <c r="R17" s="74"/>
+      <c r="S17" s="62"/>
+      <c r="T17" s="75" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="72">
+      <c r="A18" s="71">
         <v>9</v>
       </c>
-      <c r="B18" s="73" t="s">
+      <c r="B18" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="73" t="s">
+      <c r="C18" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="73" t="s">
+      <c r="D18" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="77" t="s">
+      <c r="E18" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="59">
-        <v>45010</v>
+      <c r="F18" s="98">
+        <v>45037</v>
       </c>
       <c r="G18" s="60" t="s">
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="H18" s="60" t="s">
-        <v>439</v>
-      </c>
-      <c r="I18" s="61" t="s">
-        <v>440</v>
-      </c>
-      <c r="J18" s="60" t="s">
+        <v>463</v>
+      </c>
+      <c r="I18" s="60" t="s">
+        <v>464</v>
+      </c>
+      <c r="J18" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="K18" s="62"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="60"/>
-      <c r="N18" s="61"/>
-      <c r="O18" s="63"/>
-      <c r="P18" s="63"/>
-      <c r="Q18" s="63"/>
-      <c r="R18" s="75"/>
-      <c r="S18" s="63"/>
-      <c r="T18" s="76" t="s">
+      <c r="K18" s="61"/>
+      <c r="L18" s="59"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="60"/>
+      <c r="O18" s="62"/>
+      <c r="P18" s="62"/>
+      <c r="Q18" s="62"/>
+      <c r="R18" s="74"/>
+      <c r="S18" s="62"/>
+      <c r="T18" s="75" t="s">
         <v>429</v>
       </c>
     </row>
@@ -4891,18 +4952,18 @@
         <v>45010</v>
       </c>
       <c r="G19" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
       <c r="H19" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="I19" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="L19"/>
       <c r="M19"/>
       <c r="N19" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="O19" s="50"/>
       <c r="P19" s="50"/>
@@ -4933,18 +4994,18 @@
         <v>45010</v>
       </c>
       <c r="G20" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
       <c r="H20" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="I20" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="L20"/>
       <c r="M20"/>
       <c r="N20" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="O20" s="16"/>
       <c r="P20" s="16"/>
@@ -5444,7 +5505,7 @@
       <c r="D35" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="E35" s="64" t="s">
+      <c r="E35" s="63" t="s">
         <v>431</v>
       </c>
       <c r="F35" s="44"/>
@@ -5466,56 +5527,56 @@
       </c>
     </row>
     <row r="36" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="72">
+      <c r="A36" s="71">
         <v>29</v>
       </c>
-      <c r="B36" s="73" t="s">
+      <c r="B36" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="73" t="s">
+      <c r="C36" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="73" t="s">
+      <c r="D36" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="E36" s="74" t="s">
+      <c r="E36" s="73" t="s">
         <v>431</v>
       </c>
-      <c r="F36" s="59">
+      <c r="F36" s="98">
         <v>45010</v>
       </c>
       <c r="G36" s="60" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
       <c r="H36" s="60" t="s">
-        <v>441</v>
-      </c>
-      <c r="I36" s="61" t="s">
-        <v>442</v>
-      </c>
-      <c r="J36" s="60" t="s">
+        <v>433</v>
+      </c>
+      <c r="I36" s="60" t="s">
+        <v>434</v>
+      </c>
+      <c r="J36" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="K36" s="62"/>
-      <c r="L36" s="60" t="s">
+      <c r="K36" s="61"/>
+      <c r="L36" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="M36" s="60" t="s">
+      <c r="M36" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="N36" s="61" t="s">
-        <v>473</v>
-      </c>
-      <c r="O36" s="63" t="s">
+      <c r="N36" s="60" t="s">
+        <v>435</v>
+      </c>
+      <c r="O36" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="P36" s="63" t="s">
-        <v>486</v>
-      </c>
-      <c r="Q36" s="63"/>
-      <c r="R36" s="75"/>
-      <c r="S36" s="63"/>
-      <c r="T36" s="76" t="s">
+      <c r="P36" s="62" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q36" s="62"/>
+      <c r="R36" s="74"/>
+      <c r="S36" s="62"/>
+      <c r="T36" s="75" t="s">
         <v>430</v>
       </c>
     </row>
@@ -5532,25 +5593,25 @@
       <c r="D37" s="48" t="s">
         <v>363</v>
       </c>
-      <c r="E37" s="65" t="s">
+      <c r="E37" s="64" t="s">
         <v>431</v>
       </c>
       <c r="F37" s="38">
         <v>45010</v>
       </c>
       <c r="G37" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
       <c r="H37" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="I37" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="L37"/>
       <c r="M37"/>
       <c r="N37" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="O37" s="50"/>
       <c r="P37" s="50"/>
@@ -5744,7 +5805,7 @@
       <c r="D43" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="E43" s="64" t="s">
+      <c r="E43" s="63" t="s">
         <v>432</v>
       </c>
       <c r="F43" s="44"/>
@@ -5766,56 +5827,56 @@
       </c>
     </row>
     <row r="44" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="72">
+      <c r="A44" s="71">
         <v>37</v>
       </c>
-      <c r="B44" s="73" t="s">
+      <c r="B44" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="73" t="s">
+      <c r="C44" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="D44" s="73" t="s">
+      <c r="D44" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="E44" s="74" t="s">
+      <c r="E44" s="73" t="s">
         <v>432</v>
       </c>
-      <c r="F44" s="59">
-        <v>45010</v>
+      <c r="F44" s="98">
+        <v>45037</v>
       </c>
       <c r="G44" s="60" t="s">
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="H44" s="60" t="s">
-        <v>444</v>
-      </c>
-      <c r="I44" s="61" t="s">
-        <v>442</v>
-      </c>
-      <c r="J44" s="60" t="s">
+        <v>465</v>
+      </c>
+      <c r="I44" s="60" t="s">
+        <v>434</v>
+      </c>
+      <c r="J44" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="K44" s="62"/>
-      <c r="L44" s="60" t="s">
+      <c r="K44" s="61"/>
+      <c r="L44" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="M44" s="60" t="s">
+      <c r="M44" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="N44" s="61" t="s">
-        <v>472</v>
-      </c>
-      <c r="O44" s="63" t="s">
+      <c r="N44" s="60" t="s">
+        <v>437</v>
+      </c>
+      <c r="O44" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="P44" s="63" t="s">
-        <v>486</v>
-      </c>
-      <c r="Q44" s="63"/>
-      <c r="R44" s="75"/>
-      <c r="S44" s="63"/>
-      <c r="T44" s="76" t="s">
+      <c r="P44" s="62" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q44" s="62"/>
+      <c r="R44" s="74"/>
+      <c r="S44" s="62"/>
+      <c r="T44" s="75" t="s">
         <v>430</v>
       </c>
     </row>
@@ -5832,7 +5893,7 @@
       <c r="D45" s="48" t="s">
         <v>364</v>
       </c>
-      <c r="E45" s="65" t="s">
+      <c r="E45" s="64" t="s">
         <v>432</v>
       </c>
       <c r="F45" s="58"/>
@@ -6060,48 +6121,48 @@
       </c>
     </row>
     <row r="52" spans="1:20" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="72">
+      <c r="A52" s="71">
         <v>45</v>
       </c>
-      <c r="B52" s="73" t="s">
+      <c r="B52" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="C52" s="73" t="s">
+      <c r="C52" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="D52" s="73" t="s">
+      <c r="D52" s="72" t="s">
         <v>97</v>
       </c>
-      <c r="E52" s="77" t="s">
+      <c r="E52" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="F52" s="66"/>
-      <c r="G52" s="66"/>
-      <c r="H52" s="66"/>
-      <c r="I52" s="66"/>
-      <c r="J52" s="60" t="s">
+      <c r="F52" s="65"/>
+      <c r="G52" s="65"/>
+      <c r="H52" s="65"/>
+      <c r="I52" s="65"/>
+      <c r="J52" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="K52" s="63"/>
-      <c r="L52" s="63" t="s">
+      <c r="K52" s="62"/>
+      <c r="L52" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="M52" s="63" t="s">
+      <c r="M52" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="N52" s="63"/>
-      <c r="O52" s="63" t="s">
+      <c r="N52" s="62"/>
+      <c r="O52" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="P52" s="63" t="s">
-        <v>487</v>
-      </c>
-      <c r="Q52" s="63"/>
-      <c r="R52" s="75" t="s">
+      <c r="P52" s="62" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q52" s="62"/>
+      <c r="R52" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="S52" s="63"/>
-      <c r="T52" s="76" t="s">
+      <c r="S52" s="62"/>
+      <c r="T52" s="75" t="s">
         <v>430</v>
       </c>
     </row>
@@ -6696,674 +6757,674 @@
       </c>
     </row>
     <row r="70" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="72">
+      <c r="A70" s="71">
         <v>63</v>
       </c>
-      <c r="B70" s="73" t="s">
+      <c r="B70" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="C70" s="73" t="s">
+      <c r="C70" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="D70" s="73" t="s">
+      <c r="D70" s="72" t="s">
         <v>124</v>
       </c>
-      <c r="E70" s="77" t="s">
+      <c r="E70" s="76" t="s">
         <v>125</v>
       </c>
-      <c r="F70" s="59">
-        <v>45010</v>
+      <c r="F70" s="98">
+        <v>45037</v>
       </c>
       <c r="G70" s="60" t="s">
+        <v>456</v>
+      </c>
+      <c r="H70" s="60" t="s">
+        <v>466</v>
+      </c>
+      <c r="I70" s="60" t="s">
+        <v>467</v>
+      </c>
+      <c r="J70" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="K70" s="61"/>
+      <c r="L70" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="M70" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="N70" t="s">
+        <v>488</v>
+      </c>
+      <c r="O70" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="P70" s="62" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q70" s="62"/>
+      <c r="R70" s="74"/>
+      <c r="S70" s="62" t="s">
+        <v>442</v>
+      </c>
+      <c r="T70" s="75" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="71">
+        <v>64</v>
+      </c>
+      <c r="B71" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="C71" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="D71" s="72" t="s">
+        <v>126</v>
+      </c>
+      <c r="E71" s="76" t="s">
+        <v>127</v>
+      </c>
+      <c r="F71" s="98">
+        <v>45037</v>
+      </c>
+      <c r="G71" s="60" t="s">
+        <v>456</v>
+      </c>
+      <c r="H71" s="60" t="s">
+        <v>468</v>
+      </c>
+      <c r="I71" s="60" t="s">
+        <v>469</v>
+      </c>
+      <c r="J71" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="K71" s="61"/>
+      <c r="L71" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="M71" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="N71" s="60" t="s">
+        <v>489</v>
+      </c>
+      <c r="O71" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="P71" s="62" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q71" s="62"/>
+      <c r="R71" s="74"/>
+      <c r="S71" s="62" t="s">
+        <v>449</v>
+      </c>
+      <c r="T71" s="75" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="71">
+        <v>65</v>
+      </c>
+      <c r="B72" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="C72" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="D72" s="72" t="s">
+        <v>128</v>
+      </c>
+      <c r="E72" s="76" t="s">
+        <v>129</v>
+      </c>
+      <c r="F72" s="98">
+        <v>45037</v>
+      </c>
+      <c r="G72" s="60" t="s">
+        <v>456</v>
+      </c>
+      <c r="H72" s="60" t="s">
+        <v>470</v>
+      </c>
+      <c r="I72" s="60" t="s">
+        <v>471</v>
+      </c>
+      <c r="J72" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="K72" s="61"/>
+      <c r="L72" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="M72" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="N72" s="60" t="s">
+        <v>490</v>
+      </c>
+      <c r="O72" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="P72" s="62" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q72" s="62"/>
+      <c r="R72" s="74"/>
+      <c r="S72" s="62" t="s">
         <v>448</v>
       </c>
-      <c r="H70" s="60" t="s">
+      <c r="T72" s="75" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="71">
+        <v>66</v>
+      </c>
+      <c r="B73" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="C73" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="D73" s="72" t="s">
+        <v>130</v>
+      </c>
+      <c r="E73" s="76" t="s">
+        <v>131</v>
+      </c>
+      <c r="F73" s="98">
+        <v>45037</v>
+      </c>
+      <c r="G73" s="60" t="s">
+        <v>456</v>
+      </c>
+      <c r="H73" s="60" t="s">
+        <v>472</v>
+      </c>
+      <c r="I73" s="60" t="s">
+        <v>473</v>
+      </c>
+      <c r="J73" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="K73" s="61"/>
+      <c r="L73" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="M73" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="N73" s="60" t="s">
+        <v>497</v>
+      </c>
+      <c r="O73" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="P73" s="62" t="s">
+        <v>439</v>
+      </c>
+      <c r="Q73" s="62"/>
+      <c r="R73" s="74"/>
+      <c r="S73" s="62" t="s">
+        <v>447</v>
+      </c>
+      <c r="T73" s="75" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="71">
+        <v>67</v>
+      </c>
+      <c r="B74" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="C74" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="D74" s="72" t="s">
+        <v>132</v>
+      </c>
+      <c r="E74" s="76" t="s">
+        <v>133</v>
+      </c>
+      <c r="F74" s="98">
+        <v>45037</v>
+      </c>
+      <c r="G74" s="60" t="s">
+        <v>456</v>
+      </c>
+      <c r="H74" s="60" t="s">
+        <v>474</v>
+      </c>
+      <c r="I74" s="60" t="s">
+        <v>475</v>
+      </c>
+      <c r="J74" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="K74" s="61"/>
+      <c r="L74" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="M74" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="N74" s="60" t="s">
+        <v>498</v>
+      </c>
+      <c r="O74" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="P74" s="62" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q74" s="62"/>
+      <c r="R74" s="74"/>
+      <c r="S74" s="62" t="s">
         <v>446</v>
       </c>
-      <c r="I70" s="61" t="s">
-        <v>447</v>
-      </c>
-      <c r="J70" s="60" t="s">
+      <c r="T74" s="75" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="71">
+        <v>68</v>
+      </c>
+      <c r="B75" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="C75" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="D75" s="72" t="s">
+        <v>134</v>
+      </c>
+      <c r="E75" s="76" t="s">
+        <v>135</v>
+      </c>
+      <c r="F75" s="98">
+        <v>45037</v>
+      </c>
+      <c r="G75" s="60" t="s">
+        <v>456</v>
+      </c>
+      <c r="H75" s="60" t="s">
+        <v>476</v>
+      </c>
+      <c r="I75" s="60" t="s">
+        <v>477</v>
+      </c>
+      <c r="J75" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="K70" s="62"/>
-      <c r="L70" s="60" t="s">
+      <c r="K75" s="61"/>
+      <c r="L75" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="M70" s="60" t="s">
+      <c r="M75" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="N70" s="61" t="s">
-        <v>474</v>
-      </c>
-      <c r="O70" s="63" t="s">
+      <c r="N75" s="60" t="s">
+        <v>491</v>
+      </c>
+      <c r="O75" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="P70" s="63" t="s">
+      <c r="P75" s="62" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q75" s="62"/>
+      <c r="R75" s="74"/>
+      <c r="S75" s="62" t="s">
+        <v>445</v>
+      </c>
+      <c r="T75" s="75" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="71">
+        <v>69</v>
+      </c>
+      <c r="B76" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="C76" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="D76" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="E76" s="76" t="s">
+        <v>137</v>
+      </c>
+      <c r="F76" s="98">
+        <v>45037</v>
+      </c>
+      <c r="G76" s="60" t="s">
+        <v>456</v>
+      </c>
+      <c r="H76" s="99" t="s">
+        <v>478</v>
+      </c>
+      <c r="I76" s="60" t="s">
+        <v>479</v>
+      </c>
+      <c r="J76" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="K76" s="61"/>
+      <c r="L76" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="M76" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="N76" s="60" t="s">
+        <v>496</v>
+      </c>
+      <c r="O76" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="P76" s="62" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q76" s="62"/>
+      <c r="R76" s="74"/>
+      <c r="S76" s="62" t="s">
+        <v>444</v>
+      </c>
+      <c r="T76" s="75" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="71">
+        <v>70</v>
+      </c>
+      <c r="B77" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="C77" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="D77" s="72" t="s">
+        <v>138</v>
+      </c>
+      <c r="E77" s="76" t="s">
+        <v>139</v>
+      </c>
+      <c r="F77" s="98">
+        <v>45037</v>
+      </c>
+      <c r="G77" s="60" t="s">
+        <v>456</v>
+      </c>
+      <c r="H77" s="60" t="s">
+        <v>480</v>
+      </c>
+      <c r="I77" s="60" t="s">
+        <v>481</v>
+      </c>
+      <c r="J77" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="K77" s="61"/>
+      <c r="L77" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="M77" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="N77" s="60" t="s">
+        <v>492</v>
+      </c>
+      <c r="O77" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="P77" s="62" t="s">
+        <v>439</v>
+      </c>
+      <c r="Q77" s="62"/>
+      <c r="R77" s="74"/>
+      <c r="S77" s="62" t="s">
+        <v>443</v>
+      </c>
+      <c r="T77" s="75" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="71">
+        <v>71</v>
+      </c>
+      <c r="B78" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="C78" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="D78" s="72" t="s">
+        <v>140</v>
+      </c>
+      <c r="E78" s="76" t="s">
+        <v>141</v>
+      </c>
+      <c r="F78" s="98">
+        <v>45037</v>
+      </c>
+      <c r="G78" s="60" t="s">
+        <v>456</v>
+      </c>
+      <c r="H78" s="60" t="s">
+        <v>482</v>
+      </c>
+      <c r="I78" s="60" t="s">
+        <v>483</v>
+      </c>
+      <c r="J78" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="K78" s="61"/>
+      <c r="L78" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="M78" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="N78" s="60" t="s">
+        <v>492</v>
+      </c>
+      <c r="O78" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="P78" s="62" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q78" s="62"/>
+      <c r="R78" s="74"/>
+      <c r="S78" s="62" t="s">
+        <v>443</v>
+      </c>
+      <c r="T78" s="75" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="71">
+        <v>72</v>
+      </c>
+      <c r="B79" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="C79" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="D79" s="72" t="s">
+        <v>142</v>
+      </c>
+      <c r="E79" s="76" t="s">
+        <v>143</v>
+      </c>
+      <c r="F79" s="98">
+        <v>45037</v>
+      </c>
+      <c r="G79" s="60" t="s">
+        <v>456</v>
+      </c>
+      <c r="H79" s="60" t="s">
+        <v>484</v>
+      </c>
+      <c r="I79" s="60" t="s">
+        <v>485</v>
+      </c>
+      <c r="J79" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="K79" s="61"/>
+      <c r="L79" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="M79" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="N79" s="60" t="s">
+        <v>494</v>
+      </c>
+      <c r="O79" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="P79" s="62" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q79" s="62"/>
+      <c r="R79" s="74"/>
+      <c r="S79" s="62" t="s">
+        <v>450</v>
+      </c>
+      <c r="T79" s="75" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="71">
+        <v>73</v>
+      </c>
+      <c r="B80" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="C80" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="D80" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="E80" s="76" t="s">
+        <v>145</v>
+      </c>
+      <c r="F80" s="98">
+        <v>45037</v>
+      </c>
+      <c r="G80" s="60" t="s">
+        <v>456</v>
+      </c>
+      <c r="H80" s="60" t="s">
+        <v>484</v>
+      </c>
+      <c r="I80" s="60" t="s">
+        <v>485</v>
+      </c>
+      <c r="J80" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="K80" s="61"/>
+      <c r="L80" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="M80" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="N80" s="60" t="s">
+        <v>495</v>
+      </c>
+      <c r="O80" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="P80" s="62" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q80" s="62"/>
+      <c r="R80" s="74"/>
+      <c r="S80" s="62" t="s">
+        <v>451</v>
+      </c>
+      <c r="T80" s="75" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="89">
+        <v>74</v>
+      </c>
+      <c r="B81" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="C81" s="90" t="s">
+        <v>37</v>
+      </c>
+      <c r="D81" s="90" t="s">
+        <v>146</v>
+      </c>
+      <c r="E81" s="91" t="s">
+        <v>147</v>
+      </c>
+      <c r="F81" s="100">
+        <v>45037</v>
+      </c>
+      <c r="G81" s="94" t="s">
+        <v>456</v>
+      </c>
+      <c r="H81" s="94" t="s">
         <v>486</v>
       </c>
-      <c r="Q70" s="63"/>
-      <c r="R70" s="75"/>
-      <c r="S70" s="63" t="s">
-        <v>488</v>
-      </c>
-      <c r="T70" s="76" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="72">
-        <v>64</v>
-      </c>
-      <c r="B71" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="C71" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="D71" s="73" t="s">
-        <v>126</v>
-      </c>
-      <c r="E71" s="77" t="s">
-        <v>127</v>
-      </c>
-      <c r="F71" s="59">
-        <v>45010</v>
-      </c>
-      <c r="G71" s="60" t="s">
-        <v>448</v>
-      </c>
-      <c r="H71" s="60" t="s">
-        <v>449</v>
-      </c>
-      <c r="I71" s="61" t="s">
-        <v>450</v>
-      </c>
-      <c r="J71" s="60" t="s">
+      <c r="I81" s="94" t="s">
+        <v>487</v>
+      </c>
+      <c r="J81" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="K71" s="62"/>
-      <c r="L71" s="60" t="s">
+      <c r="K81" s="93"/>
+      <c r="L81" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="M71" s="60" t="s">
+      <c r="M81" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="N71" s="61" t="s">
-        <v>475</v>
-      </c>
-      <c r="O71" s="63" t="s">
+      <c r="N81" s="94" t="s">
+        <v>493</v>
+      </c>
+      <c r="O81" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="P71" s="63" t="s">
-        <v>486</v>
-      </c>
-      <c r="Q71" s="63"/>
-      <c r="R71" s="75"/>
-      <c r="S71" s="63" t="s">
-        <v>495</v>
-      </c>
-      <c r="T71" s="76" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="72">
-        <v>65</v>
-      </c>
-      <c r="B72" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="C72" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="D72" s="73" t="s">
-        <v>128</v>
-      </c>
-      <c r="E72" s="77" t="s">
-        <v>129</v>
-      </c>
-      <c r="F72" s="59">
-        <v>45010</v>
-      </c>
-      <c r="G72" s="60" t="s">
-        <v>448</v>
-      </c>
-      <c r="H72" s="60" t="s">
+      <c r="P81" s="95" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q81" s="95"/>
+      <c r="R81" s="96"/>
+      <c r="S81" s="95" t="s">
         <v>451</v>
       </c>
-      <c r="I72" s="61" t="s">
-        <v>452</v>
-      </c>
-      <c r="J72" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="K72" s="62"/>
-      <c r="L72" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="M72" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="N72" s="61" t="s">
-        <v>476</v>
-      </c>
-      <c r="O72" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="P72" s="63" t="s">
-        <v>486</v>
-      </c>
-      <c r="Q72" s="63"/>
-      <c r="R72" s="75"/>
-      <c r="S72" s="63" t="s">
-        <v>494</v>
-      </c>
-      <c r="T72" s="76" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="72">
-        <v>66</v>
-      </c>
-      <c r="B73" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="C73" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="D73" s="73" t="s">
-        <v>130</v>
-      </c>
-      <c r="E73" s="77" t="s">
-        <v>131</v>
-      </c>
-      <c r="F73" s="59">
-        <v>45010</v>
-      </c>
-      <c r="G73" s="60" t="s">
-        <v>448</v>
-      </c>
-      <c r="H73" s="60" t="s">
-        <v>453</v>
-      </c>
-      <c r="I73" s="61" t="s">
-        <v>454</v>
-      </c>
-      <c r="J73" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="K73" s="62"/>
-      <c r="L73" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="M73" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="N73" s="61" t="s">
-        <v>477</v>
-      </c>
-      <c r="O73" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="P73" s="63" t="s">
-        <v>471</v>
-      </c>
-      <c r="Q73" s="63"/>
-      <c r="R73" s="75"/>
-      <c r="S73" s="63" t="s">
-        <v>493</v>
-      </c>
-      <c r="T73" s="76" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="74" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="72">
-        <v>67</v>
-      </c>
-      <c r="B74" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="C74" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="D74" s="73" t="s">
-        <v>132</v>
-      </c>
-      <c r="E74" s="77" t="s">
-        <v>133</v>
-      </c>
-      <c r="F74" s="59">
-        <v>45010</v>
-      </c>
-      <c r="G74" s="60" t="s">
-        <v>448</v>
-      </c>
-      <c r="H74" s="60" t="s">
-        <v>455</v>
-      </c>
-      <c r="I74" s="61" t="s">
-        <v>456</v>
-      </c>
-      <c r="J74" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="K74" s="62"/>
-      <c r="L74" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="M74" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="N74" s="61" t="s">
-        <v>478</v>
-      </c>
-      <c r="O74" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="P74" s="63" t="s">
-        <v>486</v>
-      </c>
-      <c r="Q74" s="63"/>
-      <c r="R74" s="75"/>
-      <c r="S74" s="63" t="s">
-        <v>492</v>
-      </c>
-      <c r="T74" s="76" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="75" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="72">
-        <v>68</v>
-      </c>
-      <c r="B75" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="C75" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="D75" s="73" t="s">
-        <v>134</v>
-      </c>
-      <c r="E75" s="77" t="s">
-        <v>135</v>
-      </c>
-      <c r="F75" s="59">
-        <v>45010</v>
-      </c>
-      <c r="G75" s="60" t="s">
-        <v>448</v>
-      </c>
-      <c r="H75" s="60" t="s">
-        <v>457</v>
-      </c>
-      <c r="I75" s="61" t="s">
-        <v>458</v>
-      </c>
-      <c r="J75" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="K75" s="62"/>
-      <c r="L75" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="M75" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="N75" s="61" t="s">
-        <v>479</v>
-      </c>
-      <c r="O75" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="P75" s="63" t="s">
-        <v>486</v>
-      </c>
-      <c r="Q75" s="63"/>
-      <c r="R75" s="75"/>
-      <c r="S75" s="63" t="s">
-        <v>491</v>
-      </c>
-      <c r="T75" s="76" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="76" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="72">
-        <v>69</v>
-      </c>
-      <c r="B76" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="C76" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="D76" s="73" t="s">
-        <v>136</v>
-      </c>
-      <c r="E76" s="77" t="s">
-        <v>137</v>
-      </c>
-      <c r="F76" s="59">
-        <v>45010</v>
-      </c>
-      <c r="G76" s="60" t="s">
-        <v>448</v>
-      </c>
-      <c r="H76" s="60" t="s">
-        <v>459</v>
-      </c>
-      <c r="I76" s="61" t="s">
-        <v>460</v>
-      </c>
-      <c r="J76" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="K76" s="62"/>
-      <c r="L76" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="M76" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="N76" s="61" t="s">
-        <v>480</v>
-      </c>
-      <c r="O76" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="P76" s="63" t="s">
-        <v>486</v>
-      </c>
-      <c r="Q76" s="63"/>
-      <c r="R76" s="75"/>
-      <c r="S76" s="63" t="s">
-        <v>490</v>
-      </c>
-      <c r="T76" s="76" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="77" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="72">
-        <v>70</v>
-      </c>
-      <c r="B77" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="C77" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="D77" s="73" t="s">
-        <v>138</v>
-      </c>
-      <c r="E77" s="77" t="s">
-        <v>139</v>
-      </c>
-      <c r="F77" s="59">
-        <v>45010</v>
-      </c>
-      <c r="G77" s="60" t="s">
-        <v>448</v>
-      </c>
-      <c r="H77" s="60" t="s">
-        <v>461</v>
-      </c>
-      <c r="I77" s="61" t="s">
-        <v>462</v>
-      </c>
-      <c r="J77" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="K77" s="62"/>
-      <c r="L77" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="M77" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="N77" s="61" t="s">
-        <v>481</v>
-      </c>
-      <c r="O77" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="P77" s="63" t="s">
-        <v>471</v>
-      </c>
-      <c r="Q77" s="63"/>
-      <c r="R77" s="75"/>
-      <c r="S77" s="63" t="s">
-        <v>489</v>
-      </c>
-      <c r="T77" s="76" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="78" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="72">
-        <v>71</v>
-      </c>
-      <c r="B78" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="C78" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="D78" s="73" t="s">
-        <v>140</v>
-      </c>
-      <c r="E78" s="77" t="s">
-        <v>141</v>
-      </c>
-      <c r="F78" s="59">
-        <v>45010</v>
-      </c>
-      <c r="G78" s="60" t="s">
-        <v>448</v>
-      </c>
-      <c r="H78" s="60" t="s">
-        <v>463</v>
-      </c>
-      <c r="I78" s="61" t="s">
-        <v>464</v>
-      </c>
-      <c r="J78" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="K78" s="62"/>
-      <c r="L78" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="M78" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="N78" s="61" t="s">
-        <v>482</v>
-      </c>
-      <c r="O78" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="P78" s="63" t="s">
-        <v>486</v>
-      </c>
-      <c r="Q78" s="63"/>
-      <c r="R78" s="75"/>
-      <c r="S78" s="63" t="s">
-        <v>489</v>
-      </c>
-      <c r="T78" s="76" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="79" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="72">
-        <v>72</v>
-      </c>
-      <c r="B79" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="C79" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="D79" s="73" t="s">
-        <v>142</v>
-      </c>
-      <c r="E79" s="77" t="s">
-        <v>143</v>
-      </c>
-      <c r="F79" s="59">
-        <v>45010</v>
-      </c>
-      <c r="G79" s="60" t="s">
-        <v>448</v>
-      </c>
-      <c r="H79" s="60" t="s">
-        <v>465</v>
-      </c>
-      <c r="I79" s="61" t="s">
-        <v>466</v>
-      </c>
-      <c r="J79" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="K79" s="62"/>
-      <c r="L79" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="M79" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="N79" s="61" t="s">
-        <v>483</v>
-      </c>
-      <c r="O79" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="P79" s="63" t="s">
-        <v>486</v>
-      </c>
-      <c r="Q79" s="63"/>
-      <c r="R79" s="75"/>
-      <c r="S79" s="63" t="s">
-        <v>496</v>
-      </c>
-      <c r="T79" s="76" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="80" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="72">
-        <v>73</v>
-      </c>
-      <c r="B80" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="C80" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="D80" s="73" t="s">
-        <v>144</v>
-      </c>
-      <c r="E80" s="77" t="s">
-        <v>145</v>
-      </c>
-      <c r="F80" s="59">
-        <v>45010</v>
-      </c>
-      <c r="G80" s="60" t="s">
-        <v>448</v>
-      </c>
-      <c r="H80" s="60" t="s">
-        <v>467</v>
-      </c>
-      <c r="I80" s="61" t="s">
-        <v>468</v>
-      </c>
-      <c r="J80" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="K80" s="62"/>
-      <c r="L80" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="M80" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="N80" s="61" t="s">
-        <v>484</v>
-      </c>
-      <c r="O80" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="P80" s="63" t="s">
-        <v>486</v>
-      </c>
-      <c r="Q80" s="63"/>
-      <c r="R80" s="75"/>
-      <c r="S80" s="63" t="s">
-        <v>497</v>
-      </c>
-      <c r="T80" s="76" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="81" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="72">
-        <v>74</v>
-      </c>
-      <c r="B81" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="C81" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="D81" s="73" t="s">
-        <v>146</v>
-      </c>
-      <c r="E81" s="77" t="s">
-        <v>147</v>
-      </c>
-      <c r="F81" s="59">
-        <v>45010</v>
-      </c>
-      <c r="G81" s="60" t="s">
-        <v>448</v>
-      </c>
-      <c r="H81" s="60" t="s">
-        <v>469</v>
-      </c>
-      <c r="I81" s="61" t="s">
-        <v>470</v>
-      </c>
-      <c r="J81" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="K81" s="62"/>
-      <c r="L81" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="M81" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="N81" s="61" t="s">
-        <v>485</v>
-      </c>
-      <c r="O81" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="P81" s="63" t="s">
-        <v>486</v>
-      </c>
-      <c r="Q81" s="63"/>
-      <c r="R81" s="75"/>
-      <c r="S81" s="63" t="s">
-        <v>497</v>
-      </c>
-      <c r="T81" s="76" t="s">
+      <c r="T81" s="97" t="s">
         <v>430</v>
       </c>
     </row>
@@ -27107,14 +27168,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -27349,27 +27408,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -27394,9 +27446,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Cambiata estensione da .pdf a .PDF nel data.json
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
+++ b/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSE20\medarchiver\it-fse-accreditamento\GATEWAY\S1#111MEDARCHIVER\MEDARCHIVER\MEDARCHIVER_FSE2.0\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3EBFFF-F90A-4E88-84A6-27BEC2EA78CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2787E4-1FFB-4450-B988-1D7D1A49E1FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="501">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -1946,121 +1946,106 @@
     <t>[ERRORE-14| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family']</t>
   </si>
   <si>
-    <t>2023-05-02T08:21:57Z</t>
-  </si>
-  <si>
-    <t>d81eb9cb068222d1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.5187a7c6983155e8ce8a0349302fbf5ed672a64b2432a651aeaa4c11820cfe76.81824f0905^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-02T08:22:08Z</t>
-  </si>
-  <si>
-    <t>e84d110460cf540a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.84e4bec81f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>6b5a57f53c24e29b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.8e7fe7ddcf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-02T08:22:09Z</t>
-  </si>
-  <si>
-    <t>a694954c4410b07d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.b0931cb3b1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-02T08:22:10Z</t>
-  </si>
-  <si>
-    <t>14dc8ecbbafb0a6e</t>
-  </si>
-  <si>
-    <t>1dc437789140c483</t>
-  </si>
-  <si>
-    <t>a30143345ce5188f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.6aa18e2546^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>1ff0af9c46780c2c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.e92d17bd03^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>c91f4d0f966c6793</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.f459f13d64^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>ac492a14a5e9b5e7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.cef086fcf3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>4fb999a87cf0e5ea</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.1d1f6e61cd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-02T08:22:02Z</t>
-  </si>
-  <si>
-    <t>20db3f73ec5c2f15</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.387fcd551b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-02T08:22:03Z</t>
-  </si>
-  <si>
-    <t>f068be4d61d02090</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.3a8a407430^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-02T08:22:07Z</t>
-  </si>
-  <si>
-    <t>5a74715af0fd193b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.9929e4379f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>88ace418c8bedd6d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.8b53dd0a01^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>f53b20ab61b8c3f5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.ec3163db0f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2af1372ce2d90f3a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.1395869099^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-05-04T15:18:32Z</t>
+  </si>
+  <si>
+    <t>76ee3b6ecd2ab383</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.5187a7c6983155e8ce8a0349302fbf5ed672a64b2432a651aeaa4c11820cfe76.28e34df468^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-04T15:18:35Z</t>
+  </si>
+  <si>
+    <t>e5ff9f54e09e262d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.9a34139d20^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>92bec2309e7b30f0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.661868d4a2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>e1b20383be22409b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.2c55a638a9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>9058f73ec861ae77</t>
+  </si>
+  <si>
+    <t>d1ea40d897b386e2</t>
+  </si>
+  <si>
+    <t>12e26db67cc7380d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.954e7a047b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>e407ff19262cddba</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.2adf3f1e94^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>a58325d9ed661d7f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.2a735ea274^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>1c953b1043157210</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.64acce6ef6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>6a7d6ecda5a28e67</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.6e055c4867^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ebd3eaadaf3317b8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.1cabb25788^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>0ba69de3cd0014d4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.935e7895d4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>d040e46ec495ccf1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.e82ca52074^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ecb471b8fe3e8c77</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.3eac321c40^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>bdfbae8f643d14b8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.78cf0a77e8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>8abe3d03467a79a7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.0abb4a1aac^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2190,7 +2175,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -2620,70 +2605,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2939,28 +2865,21 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4408,11 +4327,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T993"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomRight" activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4856,19 +4775,19 @@
       <c r="E15" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="101">
-        <v>45048</v>
-      </c>
-      <c r="G15" s="59" t="s">
+      <c r="F15" s="98">
+        <v>45050</v>
+      </c>
+      <c r="G15" s="60" t="s">
         <v>467</v>
       </c>
-      <c r="H15" s="59" t="s">
+      <c r="H15" s="60" t="s">
         <v>468</v>
       </c>
       <c r="I15" s="60" t="s">
         <v>469</v>
       </c>
-      <c r="J15" s="98" t="s">
+      <c r="J15" s="59" t="s">
         <v>83</v>
       </c>
       <c r="K15" s="61"/>
@@ -4900,19 +4819,19 @@
       <c r="E16" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="101">
-        <v>45048</v>
-      </c>
-      <c r="G16" s="59" t="s">
+      <c r="F16" s="98">
+        <v>45050</v>
+      </c>
+      <c r="G16" s="60" t="s">
         <v>470</v>
       </c>
-      <c r="H16" s="59" t="s">
+      <c r="H16" s="60" t="s">
         <v>471</v>
       </c>
       <c r="I16" s="60" t="s">
         <v>472</v>
       </c>
-      <c r="J16" s="98" t="s">
+      <c r="J16" s="59" t="s">
         <v>83</v>
       </c>
       <c r="K16" s="61"/>
@@ -4944,19 +4863,19 @@
       <c r="E17" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="101">
-        <v>45048</v>
-      </c>
-      <c r="G17" s="59" t="s">
+      <c r="F17" s="98">
+        <v>45050</v>
+      </c>
+      <c r="G17" s="60" t="s">
         <v>470</v>
       </c>
-      <c r="H17" s="59" t="s">
+      <c r="H17" s="60" t="s">
         <v>473</v>
       </c>
       <c r="I17" s="60" t="s">
         <v>474</v>
       </c>
-      <c r="J17" s="98" t="s">
+      <c r="J17" s="59" t="s">
         <v>83</v>
       </c>
       <c r="K17" s="61"/>
@@ -4988,19 +4907,19 @@
       <c r="E18" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="101">
-        <v>45048</v>
-      </c>
-      <c r="G18" s="59" t="s">
+      <c r="F18" s="98">
+        <v>45050</v>
+      </c>
+      <c r="G18" s="60" t="s">
+        <v>470</v>
+      </c>
+      <c r="H18" s="60" t="s">
         <v>475</v>
       </c>
-      <c r="H18" s="59" t="s">
+      <c r="I18" s="60" t="s">
         <v>476</v>
       </c>
-      <c r="I18" s="60" t="s">
-        <v>477</v>
-      </c>
-      <c r="J18" s="98" t="s">
+      <c r="J18" s="59" t="s">
         <v>83</v>
       </c>
       <c r="K18" s="61"/>
@@ -5626,19 +5545,19 @@
       <c r="E36" s="95" t="s">
         <v>431</v>
       </c>
-      <c r="F36" s="101">
-        <v>45048</v>
-      </c>
-      <c r="G36" s="59" t="s">
-        <v>478</v>
-      </c>
-      <c r="H36" s="59" t="s">
-        <v>479</v>
+      <c r="F36" s="98">
+        <v>45050</v>
+      </c>
+      <c r="G36" s="60" t="s">
+        <v>470</v>
+      </c>
+      <c r="H36" s="60" t="s">
+        <v>477</v>
       </c>
       <c r="I36" s="60" t="s">
         <v>434</v>
       </c>
-      <c r="J36" s="98" t="s">
+      <c r="J36" s="59" t="s">
         <v>83</v>
       </c>
       <c r="K36" s="61"/>
@@ -5926,19 +5845,19 @@
       <c r="E44" s="95" t="s">
         <v>432</v>
       </c>
-      <c r="F44" s="101">
-        <v>45048</v>
-      </c>
-      <c r="G44" s="59" t="s">
+      <c r="F44" s="98">
+        <v>45050</v>
+      </c>
+      <c r="G44" s="60" t="s">
+        <v>470</v>
+      </c>
+      <c r="H44" s="60" t="s">
         <v>478</v>
-      </c>
-      <c r="H44" s="59" t="s">
-        <v>480</v>
       </c>
       <c r="I44" s="60" t="s">
         <v>434</v>
       </c>
-      <c r="J44" s="98" t="s">
+      <c r="J44" s="59" t="s">
         <v>83</v>
       </c>
       <c r="K44" s="61"/>
@@ -6224,7 +6143,7 @@
       <c r="G52" s="65"/>
       <c r="H52" s="65"/>
       <c r="I52" s="65"/>
-      <c r="J52" s="98" t="s">
+      <c r="J52" s="59" t="s">
         <v>83</v>
       </c>
       <c r="K52" s="62"/>
@@ -6856,19 +6775,19 @@
       <c r="E70" s="96" t="s">
         <v>125</v>
       </c>
-      <c r="F70" s="101">
-        <v>45048</v>
-      </c>
-      <c r="G70" s="59" t="s">
-        <v>475</v>
-      </c>
-      <c r="H70" s="59" t="s">
-        <v>481</v>
+      <c r="F70" s="98">
+        <v>45050</v>
+      </c>
+      <c r="G70" s="60" t="s">
+        <v>470</v>
+      </c>
+      <c r="H70" s="60" t="s">
+        <v>479</v>
       </c>
       <c r="I70" s="60" t="s">
-        <v>482</v>
-      </c>
-      <c r="J70" s="98" t="s">
+        <v>480</v>
+      </c>
+      <c r="J70" s="59" t="s">
         <v>83</v>
       </c>
       <c r="K70" s="61"/>
@@ -6878,7 +6797,7 @@
       <c r="M70" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="N70" s="100" t="s">
+      <c r="N70" s="61" t="s">
         <v>456</v>
       </c>
       <c r="O70" s="62" t="s">
@@ -6912,19 +6831,19 @@
       <c r="E71" s="96" t="s">
         <v>127</v>
       </c>
-      <c r="F71" s="101">
-        <v>45048</v>
-      </c>
-      <c r="G71" s="59" t="s">
-        <v>475</v>
-      </c>
-      <c r="H71" s="59" t="s">
-        <v>483</v>
+      <c r="F71" s="98">
+        <v>45050</v>
+      </c>
+      <c r="G71" s="60" t="s">
+        <v>470</v>
+      </c>
+      <c r="H71" s="60" t="s">
+        <v>481</v>
       </c>
       <c r="I71" s="60" t="s">
-        <v>484</v>
-      </c>
-      <c r="J71" s="98" t="s">
+        <v>482</v>
+      </c>
+      <c r="J71" s="59" t="s">
         <v>83</v>
       </c>
       <c r="K71" s="61"/>
@@ -6968,19 +6887,19 @@
       <c r="E72" s="96" t="s">
         <v>129</v>
       </c>
-      <c r="F72" s="101">
-        <v>45048</v>
-      </c>
-      <c r="G72" s="59" t="s">
-        <v>475</v>
-      </c>
-      <c r="H72" s="59" t="s">
-        <v>485</v>
+      <c r="F72" s="98">
+        <v>45050</v>
+      </c>
+      <c r="G72" s="60" t="s">
+        <v>470</v>
+      </c>
+      <c r="H72" s="60" t="s">
+        <v>483</v>
       </c>
       <c r="I72" s="60" t="s">
-        <v>486</v>
-      </c>
-      <c r="J72" s="98" t="s">
+        <v>484</v>
+      </c>
+      <c r="J72" s="59" t="s">
         <v>83</v>
       </c>
       <c r="K72" s="61"/>
@@ -7024,19 +6943,19 @@
       <c r="E73" s="96" t="s">
         <v>131</v>
       </c>
-      <c r="F73" s="101">
-        <v>45048</v>
-      </c>
-      <c r="G73" s="59" t="s">
-        <v>475</v>
-      </c>
-      <c r="H73" s="59" t="s">
-        <v>487</v>
+      <c r="F73" s="98">
+        <v>45050</v>
+      </c>
+      <c r="G73" s="60" t="s">
+        <v>470</v>
+      </c>
+      <c r="H73" s="60" t="s">
+        <v>485</v>
       </c>
       <c r="I73" s="60" t="s">
-        <v>488</v>
-      </c>
-      <c r="J73" s="98" t="s">
+        <v>486</v>
+      </c>
+      <c r="J73" s="59" t="s">
         <v>83</v>
       </c>
       <c r="K73" s="61"/>
@@ -7080,19 +6999,19 @@
       <c r="E74" s="96" t="s">
         <v>133</v>
       </c>
-      <c r="F74" s="101">
-        <v>45048</v>
-      </c>
-      <c r="G74" s="59" t="s">
-        <v>478</v>
-      </c>
-      <c r="H74" s="59" t="s">
-        <v>489</v>
+      <c r="F74" s="98">
+        <v>45050</v>
+      </c>
+      <c r="G74" s="60" t="s">
+        <v>470</v>
+      </c>
+      <c r="H74" s="60" t="s">
+        <v>487</v>
       </c>
       <c r="I74" s="60" t="s">
-        <v>490</v>
-      </c>
-      <c r="J74" s="98" t="s">
+        <v>488</v>
+      </c>
+      <c r="J74" s="59" t="s">
         <v>83</v>
       </c>
       <c r="K74" s="61"/>
@@ -7136,19 +7055,19 @@
       <c r="E75" s="96" t="s">
         <v>135</v>
       </c>
-      <c r="F75" s="101">
-        <v>45048</v>
-      </c>
-      <c r="G75" s="59" t="s">
-        <v>491</v>
-      </c>
-      <c r="H75" s="59" t="s">
-        <v>492</v>
+      <c r="F75" s="98">
+        <v>45050</v>
+      </c>
+      <c r="G75" s="60" t="s">
+        <v>470</v>
+      </c>
+      <c r="H75" s="60" t="s">
+        <v>487</v>
       </c>
       <c r="I75" s="60" t="s">
-        <v>493</v>
-      </c>
-      <c r="J75" s="98" t="s">
+        <v>488</v>
+      </c>
+      <c r="J75" s="59" t="s">
         <v>83</v>
       </c>
       <c r="K75" s="61"/>
@@ -7192,19 +7111,19 @@
       <c r="E76" s="96" t="s">
         <v>137</v>
       </c>
-      <c r="F76" s="101">
-        <v>45048</v>
-      </c>
-      <c r="G76" s="59" t="s">
-        <v>494</v>
-      </c>
-      <c r="H76" s="59" t="s">
-        <v>495</v>
+      <c r="F76" s="98">
+        <v>45050</v>
+      </c>
+      <c r="G76" s="60" t="s">
+        <v>470</v>
+      </c>
+      <c r="H76" s="60" t="s">
+        <v>489</v>
       </c>
       <c r="I76" s="60" t="s">
-        <v>496</v>
-      </c>
-      <c r="J76" s="98" t="s">
+        <v>490</v>
+      </c>
+      <c r="J76" s="59" t="s">
         <v>83</v>
       </c>
       <c r="K76" s="61"/>
@@ -7248,19 +7167,19 @@
       <c r="E77" s="96" t="s">
         <v>139</v>
       </c>
-      <c r="F77" s="101">
-        <v>45048</v>
-      </c>
-      <c r="G77" s="59" t="s">
-        <v>497</v>
-      </c>
-      <c r="H77" s="59" t="s">
-        <v>498</v>
+      <c r="F77" s="98">
+        <v>45050</v>
+      </c>
+      <c r="G77" s="60" t="s">
+        <v>470</v>
+      </c>
+      <c r="H77" s="60" t="s">
+        <v>491</v>
       </c>
       <c r="I77" s="60" t="s">
-        <v>499</v>
-      </c>
-      <c r="J77" s="98" t="s">
+        <v>492</v>
+      </c>
+      <c r="J77" s="59" t="s">
         <v>83</v>
       </c>
       <c r="K77" s="61"/>
@@ -7304,19 +7223,19 @@
       <c r="E78" s="96" t="s">
         <v>141</v>
       </c>
-      <c r="F78" s="101">
-        <v>45048</v>
-      </c>
-      <c r="G78" s="59" t="s">
-        <v>497</v>
-      </c>
-      <c r="H78" s="59" t="s">
-        <v>498</v>
+      <c r="F78" s="98">
+        <v>45050</v>
+      </c>
+      <c r="G78" s="60" t="s">
+        <v>470</v>
+      </c>
+      <c r="H78" s="60" t="s">
+        <v>493</v>
       </c>
       <c r="I78" s="60" t="s">
-        <v>499</v>
-      </c>
-      <c r="J78" s="98" t="s">
+        <v>494</v>
+      </c>
+      <c r="J78" s="59" t="s">
         <v>83</v>
       </c>
       <c r="K78" s="61"/>
@@ -7360,19 +7279,19 @@
       <c r="E79" s="96" t="s">
         <v>143</v>
       </c>
-      <c r="F79" s="101">
-        <v>45048</v>
-      </c>
-      <c r="G79" s="59" t="s">
-        <v>497</v>
-      </c>
-      <c r="H79" s="59" t="s">
-        <v>500</v>
+      <c r="F79" s="98">
+        <v>45050</v>
+      </c>
+      <c r="G79" s="60" t="s">
+        <v>470</v>
+      </c>
+      <c r="H79" s="60" t="s">
+        <v>495</v>
       </c>
       <c r="I79" s="60" t="s">
-        <v>501</v>
-      </c>
-      <c r="J79" s="98" t="s">
+        <v>496</v>
+      </c>
+      <c r="J79" s="59" t="s">
         <v>83</v>
       </c>
       <c r="K79" s="61"/>
@@ -7416,19 +7335,19 @@
       <c r="E80" s="96" t="s">
         <v>145</v>
       </c>
-      <c r="F80" s="101">
-        <v>45048</v>
-      </c>
-      <c r="G80" s="59" t="s">
+      <c r="F80" s="98">
+        <v>45050</v>
+      </c>
+      <c r="G80" s="60" t="s">
         <v>470</v>
       </c>
-      <c r="H80" s="59" t="s">
-        <v>502</v>
+      <c r="H80" s="60" t="s">
+        <v>497</v>
       </c>
       <c r="I80" s="60" t="s">
-        <v>503</v>
-      </c>
-      <c r="J80" s="98" t="s">
+        <v>498</v>
+      </c>
+      <c r="J80" s="59" t="s">
         <v>83</v>
       </c>
       <c r="K80" s="61"/>
@@ -7472,19 +7391,19 @@
       <c r="E81" s="97" t="s">
         <v>147</v>
       </c>
-      <c r="F81" s="102">
-        <v>45048</v>
-      </c>
-      <c r="G81" s="77" t="s">
+      <c r="F81" s="99">
+        <v>45050</v>
+      </c>
+      <c r="G81" s="79" t="s">
         <v>470</v>
       </c>
-      <c r="H81" s="77" t="s">
-        <v>504</v>
+      <c r="H81" s="79" t="s">
+        <v>499</v>
       </c>
       <c r="I81" s="79" t="s">
-        <v>505</v>
-      </c>
-      <c r="J81" s="99" t="s">
+        <v>500</v>
+      </c>
+      <c r="J81" s="77" t="s">
         <v>83</v>
       </c>
       <c r="K81" s="78"/>
@@ -27263,6 +27182,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -27493,15 +27421,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
   <ds:schemaRefs>
@@ -27520,6 +27439,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB221413-913B-41FE-97D3-5428BD0403A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27538,14 +27465,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Modificata chiusura del tag code ed eliminati spazi
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
+++ b/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSE20\medarchiver\it-fse-accreditamento\GATEWAY\S1#111MEDARCHIVER\MEDARCHIVER\MEDARCHIVER_FSE2.0\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2787E4-1FFB-4450-B988-1D7D1A49E1FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F3F95F-CA2D-49A1-8F58-68C424645BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="502">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -1946,106 +1946,109 @@
     <t>[ERRORE-14| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family']</t>
   </si>
   <si>
-    <t>2023-05-04T15:18:32Z</t>
-  </si>
-  <si>
-    <t>76ee3b6ecd2ab383</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.5187a7c6983155e8ce8a0349302fbf5ed672a64b2432a651aeaa4c11820cfe76.28e34df468^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-04T15:18:35Z</t>
-  </si>
-  <si>
-    <t>e5ff9f54e09e262d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.9a34139d20^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>92bec2309e7b30f0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.661868d4a2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>e1b20383be22409b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.2c55a638a9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>9058f73ec861ae77</t>
-  </si>
-  <si>
-    <t>d1ea40d897b386e2</t>
-  </si>
-  <si>
-    <t>12e26db67cc7380d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.954e7a047b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>e407ff19262cddba</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.2adf3f1e94^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>a58325d9ed661d7f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.2a735ea274^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>1c953b1043157210</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.64acce6ef6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>6a7d6ecda5a28e67</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.6e055c4867^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>ebd3eaadaf3317b8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.1cabb25788^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>0ba69de3cd0014d4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.935e7895d4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>d040e46ec495ccf1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.e82ca52074^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>ecb471b8fe3e8c77</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.3eac321c40^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>bdfbae8f643d14b8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.78cf0a77e8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>8abe3d03467a79a7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.0abb4a1aac^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-05-12T16:06:34Z</t>
+  </si>
+  <si>
+    <t>307eb1b44e56bef4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.5187a7c6983155e8ce8a0349302fbf5ed672a64b2432a651aeaa4c11820cfe76.65af46f531^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>1d00cf7ad2770b2c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.b7c8bf9275^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>b061926e450d328c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.b8104e2760^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>b4284f412c4e1b9d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.c2d7de8290^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>a285a47da875f9da</t>
+  </si>
+  <si>
+    <t>7d590c53e7ece029</t>
+  </si>
+  <si>
+    <t>aed1275e4e213cd2</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.3463a7935f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>afc6c73f01eef2c7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.4e9de3b4bd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2c872b21ac358d39</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.aaff2cbad1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ad4a14f46bba2d5d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.33a255b313^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>dee16875c91c2480</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.a778079fba^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2466a82a6a4aa343</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.712d99d874^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>07c991cadc35cbdb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.cd8dbee538^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ecb13526c32fca0b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.08d4e4a1de^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>649a98bf77ebc3ea</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.7f9dfda069^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>58c5694c3dd3c4e6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.23c94f9379^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>f4ce77db488f625e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.e8789c638e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>75905654c2996598</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.7d9b713631^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2175,7 +2178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -2566,50 +2569,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2821,26 +2785,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2864,22 +2816,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4327,11 +4263,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T993"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F79" sqref="F79"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15:I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4374,14 +4310,14 @@
       <c r="T1" s="35"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="87" t="s">
+      <c r="B2" s="81"/>
+      <c r="C2" s="82" t="s">
         <v>452</v>
       </c>
-      <c r="D2" s="86"/>
+      <c r="D2" s="81"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -4399,14 +4335,14 @@
       <c r="T2" s="35"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="89"/>
-      <c r="C3" s="94" t="s">
+      <c r="B3" s="84"/>
+      <c r="C3" s="89" t="s">
         <v>453</v>
       </c>
-      <c r="D3" s="86"/>
+      <c r="D3" s="81"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -4424,12 +4360,12 @@
       <c r="T3" s="35"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="90"/>
-      <c r="B4" s="91"/>
-      <c r="C4" s="94" t="s">
+      <c r="A4" s="85"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="89" t="s">
         <v>454</v>
       </c>
-      <c r="D4" s="86"/>
+      <c r="D4" s="81"/>
       <c r="E4" s="2"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -4448,12 +4384,12 @@
       <c r="T4" s="35"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="92"/>
-      <c r="B5" s="93"/>
-      <c r="C5" s="94" t="s">
+      <c r="A5" s="87"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="89" t="s">
         <v>455</v>
       </c>
-      <c r="D5" s="86"/>
+      <c r="D5" s="81"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -4471,8 +4407,8 @@
       <c r="T5" s="35"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="83"/>
-      <c r="B6" s="84"/>
+      <c r="A6" s="78"/>
+      <c r="B6" s="79"/>
       <c r="C6" s="10"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -4772,11 +4708,11 @@
       <c r="D15" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="96" t="s">
+      <c r="E15" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="98">
-        <v>45050</v>
+      <c r="F15" s="77">
+        <v>45058</v>
       </c>
       <c r="G15" s="60" t="s">
         <v>467</v>
@@ -4816,20 +4752,20 @@
       <c r="D16" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="96" t="s">
+      <c r="E16" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="98">
-        <v>45050</v>
+      <c r="F16" s="77">
+        <v>45058</v>
       </c>
       <c r="G16" s="60" t="s">
+        <v>467</v>
+      </c>
+      <c r="H16" s="60" t="s">
         <v>470</v>
       </c>
-      <c r="H16" s="60" t="s">
+      <c r="I16" s="60" t="s">
         <v>471</v>
-      </c>
-      <c r="I16" s="60" t="s">
-        <v>472</v>
       </c>
       <c r="J16" s="59" t="s">
         <v>83</v>
@@ -4860,20 +4796,20 @@
       <c r="D17" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="96" t="s">
+      <c r="E17" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="98">
-        <v>45050</v>
+      <c r="F17" s="77">
+        <v>45058</v>
       </c>
       <c r="G17" s="60" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H17" s="60" t="s">
+        <v>472</v>
+      </c>
+      <c r="I17" s="60" t="s">
         <v>473</v>
-      </c>
-      <c r="I17" s="60" t="s">
-        <v>474</v>
       </c>
       <c r="J17" s="59" t="s">
         <v>83</v>
@@ -4904,20 +4840,20 @@
       <c r="D18" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="96" t="s">
+      <c r="E18" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="98">
-        <v>45050</v>
+      <c r="F18" s="77">
+        <v>45058</v>
       </c>
       <c r="G18" s="60" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H18" s="60" t="s">
+        <v>474</v>
+      </c>
+      <c r="I18" s="60" t="s">
         <v>475</v>
-      </c>
-      <c r="I18" s="60" t="s">
-        <v>476</v>
       </c>
       <c r="J18" s="59" t="s">
         <v>83</v>
@@ -5542,17 +5478,17 @@
       <c r="D36" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="E36" s="95" t="s">
+      <c r="E36" s="75" t="s">
         <v>431</v>
       </c>
-      <c r="F36" s="98">
-        <v>45050</v>
+      <c r="F36" s="77">
+        <v>45058</v>
       </c>
       <c r="G36" s="60" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H36" s="60" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="I36" s="60" t="s">
         <v>434</v>
@@ -5842,17 +5778,17 @@
       <c r="D44" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="E44" s="95" t="s">
+      <c r="E44" s="75" t="s">
         <v>432</v>
       </c>
-      <c r="F44" s="98">
-        <v>45050</v>
+      <c r="F44" s="77">
+        <v>45058</v>
       </c>
       <c r="G44" s="60" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H44" s="60" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I44" s="60" t="s">
         <v>434</v>
@@ -6136,7 +6072,7 @@
       <c r="D52" s="72" t="s">
         <v>97</v>
       </c>
-      <c r="E52" s="96" t="s">
+      <c r="E52" s="76" t="s">
         <v>96</v>
       </c>
       <c r="F52" s="65"/>
@@ -6772,20 +6708,20 @@
       <c r="D70" s="72" t="s">
         <v>124</v>
       </c>
-      <c r="E70" s="96" t="s">
+      <c r="E70" s="76" t="s">
         <v>125</v>
       </c>
-      <c r="F70" s="98">
-        <v>45050</v>
+      <c r="F70" s="77">
+        <v>45058</v>
       </c>
       <c r="G70" s="60" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H70" s="60" t="s">
+        <v>478</v>
+      </c>
+      <c r="I70" s="60" t="s">
         <v>479</v>
-      </c>
-      <c r="I70" s="60" t="s">
-        <v>480</v>
       </c>
       <c r="J70" s="59" t="s">
         <v>83</v>
@@ -6828,20 +6764,20 @@
       <c r="D71" s="72" t="s">
         <v>126</v>
       </c>
-      <c r="E71" s="96" t="s">
+      <c r="E71" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="F71" s="98">
-        <v>45050</v>
+      <c r="F71" s="77">
+        <v>45058</v>
       </c>
       <c r="G71" s="60" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H71" s="60" t="s">
+        <v>480</v>
+      </c>
+      <c r="I71" s="60" t="s">
         <v>481</v>
-      </c>
-      <c r="I71" s="60" t="s">
-        <v>482</v>
       </c>
       <c r="J71" s="59" t="s">
         <v>83</v>
@@ -6884,20 +6820,20 @@
       <c r="D72" s="72" t="s">
         <v>128</v>
       </c>
-      <c r="E72" s="96" t="s">
+      <c r="E72" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="F72" s="98">
-        <v>45050</v>
+      <c r="F72" s="77">
+        <v>45058</v>
       </c>
       <c r="G72" s="60" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H72" s="60" t="s">
+        <v>482</v>
+      </c>
+      <c r="I72" s="60" t="s">
         <v>483</v>
-      </c>
-      <c r="I72" s="60" t="s">
-        <v>484</v>
       </c>
       <c r="J72" s="59" t="s">
         <v>83</v>
@@ -6940,20 +6876,20 @@
       <c r="D73" s="72" t="s">
         <v>130</v>
       </c>
-      <c r="E73" s="96" t="s">
+      <c r="E73" s="76" t="s">
         <v>131</v>
       </c>
-      <c r="F73" s="98">
-        <v>45050</v>
+      <c r="F73" s="77">
+        <v>45058</v>
       </c>
       <c r="G73" s="60" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H73" s="60" t="s">
+        <v>484</v>
+      </c>
+      <c r="I73" s="60" t="s">
         <v>485</v>
-      </c>
-      <c r="I73" s="60" t="s">
-        <v>486</v>
       </c>
       <c r="J73" s="59" t="s">
         <v>83</v>
@@ -6996,20 +6932,20 @@
       <c r="D74" s="72" t="s">
         <v>132</v>
       </c>
-      <c r="E74" s="96" t="s">
+      <c r="E74" s="76" t="s">
         <v>133</v>
       </c>
-      <c r="F74" s="98">
-        <v>45050</v>
+      <c r="F74" s="77">
+        <v>45058</v>
       </c>
       <c r="G74" s="60" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H74" s="60" t="s">
+        <v>486</v>
+      </c>
+      <c r="I74" s="60" t="s">
         <v>487</v>
-      </c>
-      <c r="I74" s="60" t="s">
-        <v>488</v>
       </c>
       <c r="J74" s="59" t="s">
         <v>83</v>
@@ -7052,20 +6988,20 @@
       <c r="D75" s="72" t="s">
         <v>134</v>
       </c>
-      <c r="E75" s="96" t="s">
+      <c r="E75" s="76" t="s">
         <v>135</v>
       </c>
-      <c r="F75" s="98">
-        <v>45050</v>
+      <c r="F75" s="77">
+        <v>45058</v>
       </c>
       <c r="G75" s="60" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H75" s="60" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="I75" s="60" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="J75" s="59" t="s">
         <v>83</v>
@@ -7108,20 +7044,20 @@
       <c r="D76" s="72" t="s">
         <v>136</v>
       </c>
-      <c r="E76" s="96" t="s">
+      <c r="E76" s="76" t="s">
         <v>137</v>
       </c>
-      <c r="F76" s="98">
-        <v>45050</v>
+      <c r="F76" s="77">
+        <v>45058</v>
       </c>
       <c r="G76" s="60" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H76" s="60" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="I76" s="60" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="J76" s="59" t="s">
         <v>83</v>
@@ -7164,20 +7100,20 @@
       <c r="D77" s="72" t="s">
         <v>138</v>
       </c>
-      <c r="E77" s="96" t="s">
+      <c r="E77" s="76" t="s">
         <v>139</v>
       </c>
-      <c r="F77" s="98">
-        <v>45050</v>
+      <c r="F77" s="77">
+        <v>45058</v>
       </c>
       <c r="G77" s="60" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H77" s="60" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="I77" s="60" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="J77" s="59" t="s">
         <v>83</v>
@@ -7220,20 +7156,20 @@
       <c r="D78" s="72" t="s">
         <v>140</v>
       </c>
-      <c r="E78" s="96" t="s">
+      <c r="E78" s="76" t="s">
         <v>141</v>
       </c>
-      <c r="F78" s="98">
-        <v>45050</v>
+      <c r="F78" s="77">
+        <v>45058</v>
       </c>
       <c r="G78" s="60" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H78" s="60" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="I78" s="60" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="J78" s="59" t="s">
         <v>83</v>
@@ -7276,20 +7212,20 @@
       <c r="D79" s="72" t="s">
         <v>142</v>
       </c>
-      <c r="E79" s="96" t="s">
+      <c r="E79" s="76" t="s">
         <v>143</v>
       </c>
-      <c r="F79" s="98">
-        <v>45050</v>
+      <c r="F79" s="77">
+        <v>45058</v>
       </c>
       <c r="G79" s="60" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H79" s="60" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="I79" s="60" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="J79" s="59" t="s">
         <v>83</v>
@@ -7332,20 +7268,20 @@
       <c r="D80" s="72" t="s">
         <v>144</v>
       </c>
-      <c r="E80" s="96" t="s">
+      <c r="E80" s="76" t="s">
         <v>145</v>
       </c>
-      <c r="F80" s="98">
-        <v>45050</v>
+      <c r="F80" s="77">
+        <v>45058</v>
       </c>
       <c r="G80" s="60" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H80" s="60" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="I80" s="60" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="J80" s="59" t="s">
         <v>83</v>
@@ -7376,58 +7312,58 @@
       </c>
     </row>
     <row r="81" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="75">
+      <c r="A81" s="71">
         <v>74</v>
       </c>
-      <c r="B81" s="76" t="s">
+      <c r="B81" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="C81" s="76" t="s">
+      <c r="C81" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="D81" s="76" t="s">
+      <c r="D81" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="E81" s="97" t="s">
+      <c r="E81" s="76" t="s">
         <v>147</v>
       </c>
-      <c r="F81" s="99">
-        <v>45050</v>
-      </c>
-      <c r="G81" s="79" t="s">
-        <v>470</v>
-      </c>
-      <c r="H81" s="79" t="s">
-        <v>499</v>
-      </c>
-      <c r="I81" s="79" t="s">
+      <c r="F81" s="77">
+        <v>45058</v>
+      </c>
+      <c r="G81" s="60" t="s">
+        <v>467</v>
+      </c>
+      <c r="H81" s="60" t="s">
         <v>500</v>
       </c>
-      <c r="J81" s="77" t="s">
+      <c r="I81" s="60" t="s">
+        <v>501</v>
+      </c>
+      <c r="J81" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="K81" s="78"/>
-      <c r="L81" s="77" t="s">
+      <c r="K81" s="61"/>
+      <c r="L81" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="M81" s="77" t="s">
+      <c r="M81" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="N81" s="79" t="s">
+      <c r="N81" s="60" t="s">
         <v>461</v>
       </c>
-      <c r="O81" s="80" t="s">
+      <c r="O81" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="P81" s="80" t="s">
+      <c r="P81" s="62" t="s">
         <v>440</v>
       </c>
-      <c r="Q81" s="80"/>
-      <c r="R81" s="81"/>
-      <c r="S81" s="80" t="s">
+      <c r="Q81" s="62"/>
+      <c r="R81" s="73"/>
+      <c r="S81" s="62" t="s">
         <v>451</v>
       </c>
-      <c r="T81" s="82" t="s">
+      <c r="T81" s="74" t="s">
         <v>430</v>
       </c>
     </row>
@@ -27182,15 +27118,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -27421,6 +27348,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
   <ds:schemaRefs>
@@ -27439,14 +27375,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB221413-913B-41FE-97D3-5428BD0403A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27465,6 +27393,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Modificata descrizione del campo gestione errore
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
+++ b/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSE20\medarchiver\it-fse-accreditamento\GATEWAY\S1#111MEDARCHIVER\MEDARCHIVER\MEDARCHIVER_FSE2.0\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F3F95F-CA2D-49A1-8F58-68C424645BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD25912-5225-401C-B001-5300F7179F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1862,15 +1862,9 @@
     <t>2023-03-25T08:54:29Z</t>
   </si>
   <si>
-    <t>Trattandosi di un errore che non può essere gestito dall'utente, l'applicazione mostra un messaggio di errore di autenticazione e l'errore verrà poi gestito in back-office.</t>
-  </si>
-  <si>
     <t>Trattandosi di un errore che non può essere gestito dall'utente, l'applicazione mostra un messaggio di errore di autenticazione e l'errore verrà poi gestito in back-office. L'errore reale restituito dalla chiamata di validazione può o meno essere mostrato all'utente a seconda della configurazione del sistema.</t>
   </si>
   <si>
-    <t>Errore nella validazione del documento. Contattare l'amministratore di sistema. [Timeout durante la validazione]</t>
-  </si>
-  <si>
     <t>Per eseguire il test sono stati disattivati i controlli applicativi normalmente presenti (normalmente non è possibile non specificare il confidentialityCode)</t>
   </si>
   <si>
@@ -2049,6 +2043,12 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.7d9b713631^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Errore nella validazione del documento. Contattare l'amministratore di sistema. [Timeout durante la validazione]. L'applicazione consente di effettuare n tentativi con n configurabile. Al fallimento degli n tentativi, il record viene messo in una coda per la gestione in back-office e l'invio dovrà essere effettuato manualmente dall'operatore.</t>
+  </si>
+  <si>
+    <t>Trattandosi di un errore che non può essere gestito dall'utente, l'applicazione visualizza un messaggio di errore di validazione e l'errore verrà notificato all'amministratore di sistema per la sua gestione. Per effettuare nuovamente l'invio dopo la correzione dell'errore, l'utente dispone di una lista di documenti da riprocessare manualmente. L'errore restituito dalla chiamata di validazione può o meno essere mostrato all'utente o sostituito con un errore parlante a seconda della configurazione richiesta dal cliente.</t>
   </si>
 </sst>
 </file>
@@ -4263,11 +4263,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T993"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="I80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F15" sqref="F15:I81"/>
+      <selection pane="bottomRight" activeCell="P81" sqref="P81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4315,7 +4315,7 @@
       </c>
       <c r="B2" s="81"/>
       <c r="C2" s="82" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D2" s="81"/>
       <c r="F2" s="7"/>
@@ -4340,7 +4340,7 @@
       </c>
       <c r="B3" s="84"/>
       <c r="C3" s="89" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D3" s="81"/>
       <c r="F3" s="7"/>
@@ -4363,7 +4363,7 @@
       <c r="A4" s="85"/>
       <c r="B4" s="86"/>
       <c r="C4" s="89" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D4" s="81"/>
       <c r="E4" s="2"/>
@@ -4387,7 +4387,7 @@
       <c r="A5" s="87"/>
       <c r="B5" s="88"/>
       <c r="C5" s="89" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D5" s="81"/>
       <c r="F5" s="7"/>
@@ -4715,13 +4715,13 @@
         <v>45058</v>
       </c>
       <c r="G15" s="60" t="s">
+        <v>465</v>
+      </c>
+      <c r="H15" s="60" t="s">
+        <v>466</v>
+      </c>
+      <c r="I15" s="60" t="s">
         <v>467</v>
-      </c>
-      <c r="H15" s="60" t="s">
-        <v>468</v>
-      </c>
-      <c r="I15" s="60" t="s">
-        <v>469</v>
       </c>
       <c r="J15" s="59" t="s">
         <v>83</v>
@@ -4759,13 +4759,13 @@
         <v>45058</v>
       </c>
       <c r="G16" s="60" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H16" s="60" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="I16" s="60" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="J16" s="59" t="s">
         <v>83</v>
@@ -4803,13 +4803,13 @@
         <v>45058</v>
       </c>
       <c r="G17" s="60" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H17" s="60" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="I17" s="60" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="J17" s="59" t="s">
         <v>83</v>
@@ -4847,13 +4847,13 @@
         <v>45058</v>
       </c>
       <c r="G18" s="60" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H18" s="60" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="I18" s="60" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="J18" s="59" t="s">
         <v>83</v>
@@ -5485,10 +5485,10 @@
         <v>45058</v>
       </c>
       <c r="G36" s="60" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H36" s="60" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="I36" s="60" t="s">
         <v>434</v>
@@ -5510,7 +5510,7 @@
         <v>83</v>
       </c>
       <c r="P36" s="62" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="Q36" s="62"/>
       <c r="R36" s="73"/>
@@ -5785,10 +5785,10 @@
         <v>45058</v>
       </c>
       <c r="G44" s="60" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H44" s="60" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="I44" s="60" t="s">
         <v>434</v>
@@ -5810,7 +5810,7 @@
         <v>83</v>
       </c>
       <c r="P44" s="62" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="Q44" s="62"/>
       <c r="R44" s="73"/>
@@ -6059,7 +6059,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="71">
         <v>45</v>
       </c>
@@ -6094,7 +6094,7 @@
         <v>83</v>
       </c>
       <c r="P52" s="62" t="s">
-        <v>441</v>
+        <v>500</v>
       </c>
       <c r="Q52" s="62"/>
       <c r="R52" s="73" t="s">
@@ -6661,7 +6661,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" ht="47.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="41">
         <v>62</v>
       </c>
@@ -6695,7 +6695,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" ht="275.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="71">
         <v>63</v>
       </c>
@@ -6715,13 +6715,13 @@
         <v>45058</v>
       </c>
       <c r="G70" s="60" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H70" s="60" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="I70" s="60" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="J70" s="59" t="s">
         <v>83</v>
@@ -6734,24 +6734,24 @@
         <v>83</v>
       </c>
       <c r="N70" s="61" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="O70" s="62" t="s">
         <v>83</v>
       </c>
       <c r="P70" s="62" t="s">
-        <v>440</v>
+        <v>501</v>
       </c>
       <c r="Q70" s="62"/>
       <c r="R70" s="73"/>
       <c r="S70" s="62" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="T70" s="74" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="71">
         <v>64</v>
       </c>
@@ -6771,13 +6771,13 @@
         <v>45058</v>
       </c>
       <c r="G71" s="60" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H71" s="60" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="I71" s="60" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="J71" s="59" t="s">
         <v>83</v>
@@ -6790,24 +6790,24 @@
         <v>83</v>
       </c>
       <c r="N71" s="60" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="O71" s="62" t="s">
         <v>83</v>
       </c>
       <c r="P71" s="62" t="s">
-        <v>440</v>
+        <v>501</v>
       </c>
       <c r="Q71" s="62"/>
       <c r="R71" s="73"/>
       <c r="S71" s="62" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="T71" s="74" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="71">
         <v>65</v>
       </c>
@@ -6827,13 +6827,13 @@
         <v>45058</v>
       </c>
       <c r="G72" s="60" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H72" s="60" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I72" s="60" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="J72" s="59" t="s">
         <v>83</v>
@@ -6846,24 +6846,24 @@
         <v>83</v>
       </c>
       <c r="N72" s="60" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="O72" s="62" t="s">
         <v>83</v>
       </c>
       <c r="P72" s="62" t="s">
-        <v>440</v>
+        <v>501</v>
       </c>
       <c r="Q72" s="62"/>
       <c r="R72" s="73"/>
       <c r="S72" s="62" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="T72" s="74" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="71">
         <v>66</v>
       </c>
@@ -6883,13 +6883,13 @@
         <v>45058</v>
       </c>
       <c r="G73" s="60" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H73" s="60" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="I73" s="60" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="J73" s="59" t="s">
         <v>83</v>
@@ -6902,24 +6902,24 @@
         <v>83</v>
       </c>
       <c r="N73" s="60" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="O73" s="62" t="s">
         <v>83</v>
       </c>
       <c r="P73" s="62" t="s">
-        <v>439</v>
+        <v>501</v>
       </c>
       <c r="Q73" s="62"/>
       <c r="R73" s="73"/>
       <c r="S73" s="62" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="T73" s="74" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="71">
         <v>67</v>
       </c>
@@ -6939,13 +6939,13 @@
         <v>45058</v>
       </c>
       <c r="G74" s="60" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H74" s="60" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="I74" s="60" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="J74" s="59" t="s">
         <v>83</v>
@@ -6958,24 +6958,24 @@
         <v>83</v>
       </c>
       <c r="N74" s="60" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="O74" s="62" t="s">
         <v>83</v>
       </c>
       <c r="P74" s="62" t="s">
-        <v>440</v>
+        <v>501</v>
       </c>
       <c r="Q74" s="62"/>
       <c r="R74" s="73"/>
       <c r="S74" s="62" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="T74" s="74" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="71">
         <v>68</v>
       </c>
@@ -6995,13 +6995,13 @@
         <v>45058</v>
       </c>
       <c r="G75" s="60" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H75" s="60" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="I75" s="60" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="J75" s="59" t="s">
         <v>83</v>
@@ -7014,24 +7014,24 @@
         <v>83</v>
       </c>
       <c r="N75" s="60" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="O75" s="62" t="s">
         <v>83</v>
       </c>
       <c r="P75" s="62" t="s">
-        <v>440</v>
+        <v>501</v>
       </c>
       <c r="Q75" s="62"/>
       <c r="R75" s="73"/>
       <c r="S75" s="62" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="T75" s="74" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="71">
         <v>69</v>
       </c>
@@ -7051,13 +7051,13 @@
         <v>45058</v>
       </c>
       <c r="G76" s="60" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H76" s="60" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="I76" s="60" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="J76" s="59" t="s">
         <v>83</v>
@@ -7070,24 +7070,24 @@
         <v>83</v>
       </c>
       <c r="N76" s="60" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="O76" s="62" t="s">
         <v>83</v>
       </c>
       <c r="P76" s="62" t="s">
-        <v>440</v>
+        <v>501</v>
       </c>
       <c r="Q76" s="62"/>
       <c r="R76" s="73"/>
       <c r="S76" s="62" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="T76" s="74" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="71">
         <v>70</v>
       </c>
@@ -7107,13 +7107,13 @@
         <v>45058</v>
       </c>
       <c r="G77" s="60" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H77" s="60" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="I77" s="60" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="J77" s="59" t="s">
         <v>83</v>
@@ -7126,24 +7126,24 @@
         <v>83</v>
       </c>
       <c r="N77" s="60" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="O77" s="62" t="s">
         <v>83</v>
       </c>
       <c r="P77" s="62" t="s">
-        <v>439</v>
+        <v>501</v>
       </c>
       <c r="Q77" s="62"/>
       <c r="R77" s="73"/>
       <c r="S77" s="62" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="T77" s="74" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="71">
         <v>71</v>
       </c>
@@ -7163,13 +7163,13 @@
         <v>45058</v>
       </c>
       <c r="G78" s="60" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H78" s="60" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="I78" s="60" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="J78" s="59" t="s">
         <v>83</v>
@@ -7182,24 +7182,24 @@
         <v>83</v>
       </c>
       <c r="N78" s="60" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="O78" s="62" t="s">
         <v>83</v>
       </c>
       <c r="P78" s="62" t="s">
-        <v>440</v>
+        <v>501</v>
       </c>
       <c r="Q78" s="62"/>
       <c r="R78" s="73"/>
       <c r="S78" s="62" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="T78" s="74" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="71">
         <v>72</v>
       </c>
@@ -7219,13 +7219,13 @@
         <v>45058</v>
       </c>
       <c r="G79" s="60" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H79" s="60" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I79" s="60" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J79" s="59" t="s">
         <v>83</v>
@@ -7238,24 +7238,24 @@
         <v>83</v>
       </c>
       <c r="N79" s="60" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="O79" s="62" t="s">
         <v>83</v>
       </c>
       <c r="P79" s="62" t="s">
-        <v>440</v>
+        <v>501</v>
       </c>
       <c r="Q79" s="62"/>
       <c r="R79" s="73"/>
       <c r="S79" s="62" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="T79" s="74" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="71">
         <v>73</v>
       </c>
@@ -7275,13 +7275,13 @@
         <v>45058</v>
       </c>
       <c r="G80" s="60" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H80" s="60" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="I80" s="60" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="J80" s="59" t="s">
         <v>83</v>
@@ -7294,24 +7294,24 @@
         <v>83</v>
       </c>
       <c r="N80" s="60" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="O80" s="62" t="s">
         <v>83</v>
       </c>
       <c r="P80" s="62" t="s">
-        <v>440</v>
+        <v>501</v>
       </c>
       <c r="Q80" s="62"/>
       <c r="R80" s="73"/>
       <c r="S80" s="62" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="T80" s="74" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="71">
         <v>74</v>
       </c>
@@ -7331,13 +7331,13 @@
         <v>45058</v>
       </c>
       <c r="G81" s="60" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H81" s="60" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="I81" s="60" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="J81" s="59" t="s">
         <v>83</v>
@@ -7350,18 +7350,18 @@
         <v>83</v>
       </c>
       <c r="N81" s="60" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="O81" s="62" t="s">
         <v>83</v>
       </c>
       <c r="P81" s="62" t="s">
-        <v>440</v>
+        <v>501</v>
       </c>
       <c r="Q81" s="62"/>
       <c r="R81" s="73"/>
       <c r="S81" s="62" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="T81" s="74" t="s">
         <v>430</v>
@@ -27118,6 +27118,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -27348,15 +27357,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
   <ds:schemaRefs>
@@ -27375,6 +27375,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB221413-913B-41FE-97D3-5428BD0403A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27393,14 +27401,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Aggiornamento accreditamento per S1#111MEDARCHIVER
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
+++ b/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSE20\medarchiver\it-fse-accreditamento\GATEWAY\S1#111MEDARCHIVER\MEDARCHIVER\MEDARCHIVER_FSE2.0\1.0.0.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gzamparo\Documents\FSE 2.0\it-fse-accreditamento\GATEWAY\S1#111MEDARCHIVER\MEDARCHIVER\MEDARCHIVER_FSE2.0\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD25912-5225-401C-B001-5300F7179F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900D3E44-3BFD-4E56-858E-B6877C988A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="509">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -2049,6 +2049,27 @@
   </si>
   <si>
     <t>Trattandosi di un errore che non può essere gestito dall'utente, l'applicazione visualizza un messaggio di errore di validazione e l'errore verrà notificato all'amministratore di sistema per la sua gestione. Per effettuare nuovamente l'invio dopo la correzione dell'errore, l'utente dispone di una lista di documenti da riprocessare manualmente. L'errore restituito dalla chiamata di validazione può o meno essere mostrato all'utente o sostituito con un errore parlante a seconda della configurazione richiesta dal cliente.</t>
+  </si>
+  <si>
+    <t>2023-09-08T15:15:45Z</t>
+  </si>
+  <si>
+    <t>b2f9a08800ec68e0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.bb61a94250ccedcbb320afd3e9903df362179d04d7c7dfe90a1ceaf3144621be.713f387389^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2b38f154fb3200cb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c9cf13c411a40543c41310886420256438189d40bbec51216e7d6905038273c8.e61d7e13b7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>8d8ba4f93c29df72</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ea9bc6690db4bab486666fc38ef5de05188118e04583f2d832ac39eed72c3e54.fcf85e24ce^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4260,14 +4281,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:T993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="I80" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="P81" sqref="P81"/>
+      <selection pane="bottomRight" activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4525,7 +4545,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="47">
         <v>1</v>
       </c>
@@ -4559,7 +4579,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>2</v>
       </c>
@@ -4593,7 +4613,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>3</v>
       </c>
@@ -4627,7 +4647,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>4</v>
       </c>
@@ -4661,7 +4681,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="41">
         <v>5</v>
       </c>
@@ -4871,7 +4891,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="47">
         <v>11</v>
       </c>
@@ -4913,7 +4933,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11">
         <v>12</v>
       </c>
@@ -4955,7 +4975,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
         <v>13</v>
       </c>
@@ -4989,7 +5009,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11">
         <v>14</v>
       </c>
@@ -5023,7 +5043,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11">
         <v>16</v>
       </c>
@@ -5057,7 +5077,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11">
         <v>17</v>
       </c>
@@ -5091,7 +5111,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
         <v>18</v>
       </c>
@@ -5125,7 +5145,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11">
         <v>19</v>
       </c>
@@ -5159,7 +5179,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <v>20</v>
       </c>
@@ -5193,7 +5213,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11">
         <v>21</v>
       </c>
@@ -5227,7 +5247,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11">
         <v>22</v>
       </c>
@@ -5261,7 +5281,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <v>23</v>
       </c>
@@ -5295,7 +5315,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
         <v>24</v>
       </c>
@@ -5329,7 +5349,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11">
         <v>25</v>
       </c>
@@ -5363,7 +5383,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11">
         <v>26</v>
       </c>
@@ -5397,7 +5417,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11">
         <v>27</v>
       </c>
@@ -5431,7 +5451,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="41">
         <v>28</v>
       </c>
@@ -5519,7 +5539,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="47">
         <v>30</v>
       </c>
@@ -5561,7 +5581,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11">
         <v>31</v>
       </c>
@@ -5595,7 +5615,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="22">
         <v>32</v>
       </c>
@@ -5629,7 +5649,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11">
         <v>33</v>
       </c>
@@ -5663,7 +5683,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11">
         <v>34</v>
       </c>
@@ -5697,7 +5717,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11">
         <v>35</v>
       </c>
@@ -5731,7 +5751,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="41">
         <v>36</v>
       </c>
@@ -5819,7 +5839,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="47">
         <v>38</v>
       </c>
@@ -5853,7 +5873,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="11">
         <v>39</v>
       </c>
@@ -5887,7 +5907,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="22">
         <v>40</v>
       </c>
@@ -5921,7 +5941,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11">
         <v>41</v>
       </c>
@@ -5955,7 +5975,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11">
         <v>42</v>
       </c>
@@ -5989,7 +6009,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="11">
         <v>43</v>
       </c>
@@ -6023,7 +6043,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="41">
         <v>44</v>
       </c>
@@ -6105,7 +6125,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="47">
         <v>46</v>
       </c>
@@ -6141,7 +6161,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="11">
         <v>47</v>
       </c>
@@ -6177,7 +6197,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11">
         <v>48</v>
       </c>
@@ -6213,7 +6233,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11">
         <v>49</v>
       </c>
@@ -6249,7 +6269,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="11">
         <v>50</v>
       </c>
@@ -6285,7 +6305,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="11">
         <v>51</v>
       </c>
@@ -6321,7 +6341,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="11">
         <v>52</v>
       </c>
@@ -6355,7 +6375,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="11">
         <v>53</v>
       </c>
@@ -6389,7 +6409,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="11">
         <v>54</v>
       </c>
@@ -6423,7 +6443,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="11">
         <v>55</v>
       </c>
@@ -6457,7 +6477,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="11">
         <v>56</v>
       </c>
@@ -6491,7 +6511,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="11">
         <v>57</v>
       </c>
@@ -6525,7 +6545,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="11">
         <v>58</v>
       </c>
@@ -6559,7 +6579,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="11">
         <v>59</v>
       </c>
@@ -6593,7 +6613,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="11">
         <v>60</v>
       </c>
@@ -6627,7 +6647,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="11">
         <v>61</v>
       </c>
@@ -6661,7 +6681,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="47.25" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="41">
         <v>62</v>
       </c>
@@ -7367,7 +7387,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="47">
         <v>75</v>
       </c>
@@ -7401,7 +7421,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="11">
         <v>76</v>
       </c>
@@ -7435,7 +7455,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="11">
         <v>77</v>
       </c>
@@ -7469,7 +7489,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="11">
         <v>78</v>
       </c>
@@ -7503,7 +7523,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="11">
         <v>79</v>
       </c>
@@ -7537,7 +7557,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="11">
         <v>80</v>
       </c>
@@ -7571,7 +7591,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="11">
         <v>81</v>
       </c>
@@ -7605,7 +7625,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="11">
         <v>82</v>
       </c>
@@ -7639,7 +7659,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="11">
         <v>83</v>
       </c>
@@ -7673,7 +7693,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="11">
         <v>84</v>
       </c>
@@ -7707,7 +7727,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="11">
         <v>85</v>
       </c>
@@ -7741,7 +7761,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="11">
         <v>86</v>
       </c>
@@ -7775,7 +7795,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="11">
         <v>87</v>
       </c>
@@ -7809,7 +7829,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="11">
         <v>88</v>
       </c>
@@ -7843,7 +7863,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="11">
         <v>89</v>
       </c>
@@ -7877,7 +7897,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="11">
         <v>90</v>
       </c>
@@ -7911,7 +7931,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="11">
         <v>91</v>
       </c>
@@ -7945,7 +7965,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="11">
         <v>92</v>
       </c>
@@ -7979,7 +7999,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="11">
         <v>93</v>
       </c>
@@ -8013,7 +8033,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="11">
         <v>94</v>
       </c>
@@ -8047,7 +8067,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="11">
         <v>95</v>
       </c>
@@ -8081,7 +8101,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="11">
         <v>96</v>
       </c>
@@ -8115,7 +8135,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="11">
         <v>97</v>
       </c>
@@ -8149,7 +8169,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="11">
         <v>98</v>
       </c>
@@ -8183,7 +8203,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="11">
         <v>99</v>
       </c>
@@ -8217,7 +8237,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="11">
         <v>100</v>
       </c>
@@ -8251,7 +8271,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="11">
         <v>101</v>
       </c>
@@ -8285,7 +8305,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="11">
         <v>102</v>
       </c>
@@ -8319,7 +8339,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="11">
         <v>103</v>
       </c>
@@ -8353,7 +8373,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="11">
         <v>104</v>
       </c>
@@ -8387,7 +8407,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="11">
         <v>105</v>
       </c>
@@ -8421,7 +8441,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="11">
         <v>106</v>
       </c>
@@ -8455,7 +8475,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="11">
         <v>107</v>
       </c>
@@ -8489,7 +8509,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="11">
         <v>108</v>
       </c>
@@ -8523,7 +8543,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="11">
         <v>109</v>
       </c>
@@ -8557,7 +8577,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="11">
         <v>110</v>
       </c>
@@ -8591,7 +8611,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="11">
         <v>111</v>
       </c>
@@ -8625,7 +8645,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="11">
         <v>112</v>
       </c>
@@ -8659,7 +8679,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="11">
         <v>113</v>
       </c>
@@ -8693,7 +8713,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="11">
         <v>114</v>
       </c>
@@ -8727,7 +8747,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="11">
         <v>115</v>
       </c>
@@ -8761,7 +8781,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="11">
         <v>116</v>
       </c>
@@ -8795,7 +8815,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="11">
         <v>117</v>
       </c>
@@ -8829,7 +8849,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="11">
         <v>118</v>
       </c>
@@ -8863,7 +8883,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="11">
         <v>119</v>
       </c>
@@ -8897,7 +8917,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="11">
         <v>120</v>
       </c>
@@ -8931,7 +8951,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="11">
         <v>121</v>
       </c>
@@ -8965,7 +8985,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="11">
         <v>122</v>
       </c>
@@ -8999,7 +9019,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="11">
         <v>123</v>
       </c>
@@ -9033,7 +9053,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="11">
         <v>124</v>
       </c>
@@ -9067,7 +9087,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="11">
         <v>125</v>
       </c>
@@ -9101,7 +9121,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="11">
         <v>126</v>
       </c>
@@ -9135,7 +9155,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="11">
         <v>127</v>
       </c>
@@ -9169,7 +9189,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="11">
         <v>128</v>
       </c>
@@ -9203,7 +9223,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="11">
         <v>129</v>
       </c>
@@ -9237,7 +9257,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="11">
         <v>130</v>
       </c>
@@ -9271,7 +9291,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="11">
         <v>131</v>
       </c>
@@ -9305,7 +9325,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="11">
         <v>132</v>
       </c>
@@ -9339,7 +9359,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="11">
         <v>133</v>
       </c>
@@ -9373,7 +9393,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="11">
         <v>134</v>
       </c>
@@ -9407,7 +9427,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="11">
         <v>135</v>
       </c>
@@ -9441,7 +9461,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="11">
         <v>136</v>
       </c>
@@ -9475,7 +9495,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="11">
         <v>137</v>
       </c>
@@ -9509,7 +9529,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="11">
         <v>138</v>
       </c>
@@ -9543,7 +9563,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="11">
         <v>139</v>
       </c>
@@ -9577,7 +9597,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="11">
         <v>140</v>
       </c>
@@ -9611,7 +9631,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="148" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="11">
         <v>141</v>
       </c>
@@ -9645,7 +9665,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="149" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="11">
         <v>142</v>
       </c>
@@ -9679,7 +9699,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="11">
         <v>143</v>
       </c>
@@ -9713,7 +9733,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="151" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="11">
         <v>144</v>
       </c>
@@ -9747,7 +9767,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="152" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="11">
         <v>145</v>
       </c>
@@ -9781,7 +9801,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="153" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="11">
         <v>146</v>
       </c>
@@ -9815,7 +9835,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="11">
         <v>147</v>
       </c>
@@ -9831,11 +9851,21 @@
       <c r="E154" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="F154" s="14"/>
-      <c r="G154" s="15"/>
-      <c r="H154" s="15"/>
-      <c r="I154" s="15"/>
-      <c r="J154" s="16"/>
+      <c r="F154" s="14">
+        <v>45177</v>
+      </c>
+      <c r="G154" s="15" t="s">
+        <v>502</v>
+      </c>
+      <c r="H154" s="15" t="s">
+        <v>503</v>
+      </c>
+      <c r="I154" s="15" t="s">
+        <v>504</v>
+      </c>
+      <c r="J154" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="K154" s="16"/>
       <c r="L154" s="16"/>
       <c r="M154" s="16"/>
@@ -9849,7 +9879,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="11">
         <v>148</v>
       </c>
@@ -9865,10 +9895,18 @@
       <c r="E155" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="F155" s="14"/>
-      <c r="G155" s="15"/>
-      <c r="H155" s="15"/>
-      <c r="I155" s="15"/>
+      <c r="F155" s="14">
+        <v>45177</v>
+      </c>
+      <c r="G155" s="15" t="s">
+        <v>502</v>
+      </c>
+      <c r="H155" s="15" t="s">
+        <v>505</v>
+      </c>
+      <c r="I155" s="15" t="s">
+        <v>506</v>
+      </c>
       <c r="J155" s="16"/>
       <c r="K155" s="16"/>
       <c r="L155" s="16"/>
@@ -9883,7 +9921,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="11">
         <v>149</v>
       </c>
@@ -9899,10 +9937,18 @@
       <c r="E156" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="F156" s="14"/>
-      <c r="G156" s="15"/>
-      <c r="H156" s="15"/>
-      <c r="I156" s="15"/>
+      <c r="F156" s="14">
+        <v>45177</v>
+      </c>
+      <c r="G156" s="15" t="s">
+        <v>502</v>
+      </c>
+      <c r="H156" s="15" t="s">
+        <v>507</v>
+      </c>
+      <c r="I156" s="15" t="s">
+        <v>508</v>
+      </c>
       <c r="J156" s="16"/>
       <c r="K156" s="16"/>
       <c r="L156" s="16"/>
@@ -9917,7 +9963,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="11">
         <v>150</v>
       </c>
@@ -9951,7 +9997,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="158" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="11">
         <v>151</v>
       </c>
@@ -9985,7 +10031,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="11">
         <v>152</v>
       </c>
@@ -10019,7 +10065,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="11">
         <v>153</v>
       </c>
@@ -10053,7 +10099,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="11">
         <v>154</v>
       </c>
@@ -10087,7 +10133,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="11">
         <v>155</v>
       </c>
@@ -10121,7 +10167,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="11">
         <v>156</v>
       </c>
@@ -10155,7 +10201,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="11">
         <v>157</v>
       </c>
@@ -10189,7 +10235,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="11">
         <v>158</v>
       </c>
@@ -10223,7 +10269,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="11">
         <v>159</v>
       </c>
@@ -10257,7 +10303,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="11">
         <v>160</v>
       </c>
@@ -10291,7 +10337,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="11">
         <v>161</v>
       </c>
@@ -10325,7 +10371,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="11">
         <v>162</v>
       </c>
@@ -10359,7 +10405,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="11">
         <v>163</v>
       </c>
@@ -10393,7 +10439,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="11">
         <v>164</v>
       </c>
@@ -10427,7 +10473,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="11">
         <v>165</v>
       </c>
@@ -10461,7 +10507,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="11">
         <v>166</v>
       </c>
@@ -10495,7 +10541,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="11">
         <v>167</v>
       </c>
@@ -10529,7 +10575,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="11">
         <v>168</v>
       </c>
@@ -10563,7 +10609,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="129.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:20" ht="129.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="11">
         <v>169</v>
       </c>
@@ -10597,7 +10643,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="177" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="11">
         <v>170</v>
       </c>
@@ -10631,7 +10677,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="178" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="11">
         <v>171</v>
       </c>
@@ -10665,7 +10711,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="179" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="11">
         <v>172</v>
       </c>
@@ -10699,7 +10745,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="11">
         <v>173</v>
       </c>
@@ -10733,7 +10779,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="11">
         <v>174</v>
       </c>
@@ -10767,7 +10813,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="11">
         <v>175</v>
       </c>
@@ -10801,7 +10847,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="11">
         <v>176</v>
       </c>
@@ -10835,7 +10881,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="11">
         <v>177</v>
       </c>
@@ -10869,7 +10915,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="11">
         <v>178</v>
       </c>
@@ -10903,7 +10949,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="186" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="11">
         <v>179</v>
       </c>
@@ -10937,7 +10983,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="187" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="11">
         <v>180</v>
       </c>
@@ -10971,7 +11017,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="188" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="11">
         <v>181</v>
       </c>
@@ -11005,7 +11051,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="189" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="11">
         <v>182</v>
       </c>
@@ -11039,7 +11085,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="190" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="11">
         <v>183</v>
       </c>
@@ -11073,7 +11119,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="11">
         <v>184</v>
       </c>
@@ -11107,7 +11153,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="11">
         <v>185</v>
       </c>
@@ -11141,7 +11187,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="11">
         <v>186</v>
       </c>
@@ -11175,7 +11221,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="11">
         <v>187</v>
       </c>
@@ -11209,7 +11255,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="195" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="11">
         <v>188</v>
       </c>
@@ -11243,7 +11289,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="196" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="11">
         <v>189</v>
       </c>
@@ -11277,7 +11323,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="197" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="11">
         <v>190</v>
       </c>
@@ -11311,7 +11357,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:20" ht="150" x14ac:dyDescent="0.25">
       <c r="A198" s="11">
         <v>191</v>
       </c>
@@ -24861,13 +24907,7 @@
       <c r="T993" s="35"/>
     </row>
   </sheetData>
-  <autoFilter ref="A9:T198" xr:uid="{00000000-0001-0000-0100-000000000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="LDO"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A9:T198" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
@@ -27107,26 +27147,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -27357,32 +27377,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB221413-913B-41FE-97D3-5428BD0403A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27401,6 +27416,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Aggiornamento accreditamento per S1#111MEDARCHIVER tutti i test v.2
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
+++ b/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gzamparo\Documents\FSE 2.0\it-fse-accreditamento\GATEWAY\S1#111MEDARCHIVER\MEDARCHIVER\MEDARCHIVER_FSE2.0\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB822E35-D62F-4B9B-95C5-7CBDC9935CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1CB9AD-80F9-4407-9931-E40951B86944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="567">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -4413,10 +4413,10 @@
   <dimension ref="A1:T993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="I39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B172" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J158" sqref="J158:J198"/>
+      <selection pane="bottomRight" activeCell="M162" sqref="M162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5775,12 +5775,8 @@
       <c r="J39" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K39" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L39" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
       <c r="M39" s="16" t="s">
         <v>435</v>
       </c>
@@ -6087,12 +6083,8 @@
       <c r="J47" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K47" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L47" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
       <c r="M47" s="16" t="s">
         <v>437</v>
       </c>
@@ -9334,7 +9326,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="11">
         <v>127</v>
       </c>
@@ -9368,7 +9360,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="11">
         <v>128</v>
       </c>
@@ -9402,7 +9394,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="11">
         <v>129</v>
       </c>
@@ -9436,7 +9428,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="11">
         <v>130</v>
       </c>
@@ -9470,7 +9462,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="11">
         <v>131</v>
       </c>
@@ -9504,7 +9496,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="11">
         <v>132</v>
       </c>
@@ -9538,7 +9530,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="11">
         <v>133</v>
       </c>
@@ -9572,7 +9564,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="11">
         <v>134</v>
       </c>
@@ -9606,7 +9598,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="11">
         <v>135</v>
       </c>
@@ -9640,7 +9632,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="11">
         <v>136</v>
       </c>
@@ -9674,7 +9666,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="11">
         <v>137</v>
       </c>
@@ -9708,7 +9700,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="11">
         <v>138</v>
       </c>
@@ -9742,7 +9734,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="11">
         <v>139</v>
       </c>
@@ -9776,7 +9768,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="11">
         <v>140</v>
       </c>
@@ -9810,7 +9802,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="148" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="11">
         <v>141</v>
       </c>
@@ -9844,7 +9836,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="149" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="11">
         <v>142</v>
       </c>
@@ -9878,7 +9870,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="11">
         <v>143</v>
       </c>
@@ -9912,7 +9904,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="151" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="11">
         <v>144</v>
       </c>
@@ -9946,7 +9938,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="152" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="11">
         <v>145</v>
       </c>
@@ -9980,7 +9972,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="153" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="11">
         <v>146</v>
       </c>
@@ -10221,12 +10213,8 @@
       <c r="J158" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K158" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L158" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K158" s="16"/>
+      <c r="L158" s="16"/>
       <c r="M158" s="16" t="s">
         <v>509</v>
       </c>
@@ -10273,15 +10261,9 @@
       <c r="J159" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K159" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L159" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="M159" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K159" s="16"/>
+      <c r="L159" s="16"/>
+      <c r="M159" s="16"/>
       <c r="N159" s="16" t="s">
         <v>455</v>
       </c>
@@ -10325,15 +10307,9 @@
       <c r="J160" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K160" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L160" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="M160" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K160" s="16"/>
+      <c r="L160" s="16"/>
+      <c r="M160" s="16"/>
       <c r="N160" s="16"/>
       <c r="O160" s="16"/>
       <c r="P160" s="16"/>
@@ -10375,15 +10351,9 @@
       <c r="J161" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K161" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L161" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="M161" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K161" s="16"/>
+      <c r="L161" s="16"/>
+      <c r="M161" s="16"/>
       <c r="N161" s="16" t="s">
         <v>463</v>
       </c>
@@ -10427,15 +10397,9 @@
       <c r="J162" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K162" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L162" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="M162" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K162" s="16"/>
+      <c r="L162" s="16"/>
+      <c r="M162" s="16"/>
       <c r="N162" s="16" t="s">
         <v>464</v>
       </c>
@@ -10479,15 +10443,9 @@
       <c r="J163" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K163" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L163" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="M163" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K163" s="16"/>
+      <c r="L163" s="16"/>
+      <c r="M163" s="16"/>
       <c r="N163" s="16" t="s">
         <v>510</v>
       </c>
@@ -10531,15 +10489,9 @@
       <c r="J164" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K164" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L164" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="M164" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K164" s="16"/>
+      <c r="L164" s="16"/>
+      <c r="M164" s="16"/>
       <c r="N164" s="16" t="s">
         <v>511</v>
       </c>
@@ -10583,15 +10535,9 @@
       <c r="J165" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K165" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L165" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="M165" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K165" s="16"/>
+      <c r="L165" s="16"/>
+      <c r="M165" s="16"/>
       <c r="N165" s="16" t="s">
         <v>512</v>
       </c>
@@ -10635,15 +10581,9 @@
       <c r="J166" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K166" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L166" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="M166" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K166" s="16"/>
+      <c r="L166" s="16"/>
+      <c r="M166" s="16"/>
       <c r="N166" s="16" t="s">
         <v>513</v>
       </c>
@@ -10687,15 +10627,9 @@
       <c r="J167" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K167" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L167" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="M167" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K167" s="16"/>
+      <c r="L167" s="16"/>
+      <c r="M167" s="16"/>
       <c r="N167" s="16" t="s">
         <v>514</v>
       </c>
@@ -10739,15 +10673,9 @@
       <c r="J168" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K168" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L168" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="M168" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K168" s="16"/>
+      <c r="L168" s="16"/>
+      <c r="M168" s="16"/>
       <c r="N168" s="16" t="s">
         <v>515</v>
       </c>
@@ -10791,15 +10719,9 @@
       <c r="J169" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K169" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L169" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="M169" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K169" s="16"/>
+      <c r="L169" s="16"/>
+      <c r="M169" s="16"/>
       <c r="N169" s="16" t="s">
         <v>516</v>
       </c>
@@ -10843,15 +10765,9 @@
       <c r="J170" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K170" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L170" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="M170" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K170" s="16"/>
+      <c r="L170" s="16"/>
+      <c r="M170" s="16"/>
       <c r="N170" s="16" t="s">
         <v>517</v>
       </c>
@@ -10895,15 +10811,9 @@
       <c r="J171" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K171" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L171" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="M171" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K171" s="16"/>
+      <c r="L171" s="16"/>
+      <c r="M171" s="16"/>
       <c r="N171" s="16" t="s">
         <v>518</v>
       </c>
@@ -10947,15 +10857,9 @@
       <c r="J172" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K172" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L172" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="M172" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K172" s="16"/>
+      <c r="L172" s="16"/>
+      <c r="M172" s="16"/>
       <c r="N172" s="16" t="s">
         <v>519</v>
       </c>
@@ -10999,15 +10903,9 @@
       <c r="J173" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K173" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L173" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="M173" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K173" s="16"/>
+      <c r="L173" s="16"/>
+      <c r="M173" s="16"/>
       <c r="N173" s="16" t="s">
         <v>520</v>
       </c>
@@ -11051,15 +10949,9 @@
       <c r="J174" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K174" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L174" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="M174" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K174" s="16"/>
+      <c r="L174" s="16"/>
+      <c r="M174" s="16"/>
       <c r="N174" s="16" t="s">
         <v>521</v>
       </c>
@@ -11103,15 +10995,9 @@
       <c r="J175" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K175" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L175" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="M175" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K175" s="16"/>
+      <c r="L175" s="16"/>
+      <c r="M175" s="16"/>
       <c r="N175" s="16" t="s">
         <v>522</v>
       </c>
@@ -11155,15 +11041,9 @@
       <c r="J176" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="K176" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="L176" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="M176" s="16" t="s">
-        <v>509</v>
-      </c>
+      <c r="K176" s="16"/>
+      <c r="L176" s="16"/>
+      <c r="M176" s="16"/>
       <c r="N176" s="16" t="s">
         <v>523</v>
       </c>

</xml_diff>

<commit_message>
Aggiornamento accreditamento per S1#111MEDARCHIVER tutti i test v.3 - Update Checklist
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
+++ b/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gzamparo\Documents\FSE 2.0\it-fse-accreditamento\GATEWAY\S1#111MEDARCHIVER\MEDARCHIVER\MEDARCHIVER_FSE2.0\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1CB9AD-80F9-4407-9931-E40951B86944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9D070E-6B95-434C-A42D-76E0F78BDF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="574">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -2072,9 +2072,6 @@
     <t>2.16.840.1.113883.2.9.2.190.4.4.ea9bc6690db4bab486666fc38ef5de05188118e04583f2d832ac39eed72c3e54.fcf85e24ce^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: X]</t>
   </si>
   <si>
@@ -2244,6 +2241,30 @@
   </si>
   <si>
     <t>59ab2b74d0827505</t>
+  </si>
+  <si>
+    <t>Per eseguire i test sono state modificate le codifiche in quanto non è possibile inserire un codice diverso da quelli previsti</t>
+  </si>
+  <si>
+    <t>Per eseguire il test sono stati disattivati i controlli applicativi normalmente presenti (normalmente non è possibile non specificare l'identificativo della prescrizione se in regime SSN)</t>
+  </si>
+  <si>
+    <t>Per eseguire il test sono stati disattivati i controlli applicativi normalmente presenti (normalmente la codifica per la prestazione prevede tutti i codici necessari)</t>
+  </si>
+  <si>
+    <t>Per eseguire i test sono state modificate le codifiche in quanto non è possibile proseguire se non è stato inserito un referto</t>
+  </si>
+  <si>
+    <t>Per eseguire i test sono state modificate le codifiche in quanto non è possibile proseguire se non è stato inserito un quesito diagnostico</t>
+  </si>
+  <si>
+    <t>Per eseguire i test sono state modificate le codifiche in quanto non è possibile proseguire se non è stato inserito il dato</t>
+  </si>
+  <si>
+    <t>Per eseguire i test sono stati cancellati i codici normalmente obbligatori in fase di codifica delle voci</t>
+  </si>
+  <si>
+    <t>Per eseguire i test sono state modificate le codifiche in quanto valori non inseribili da utente o in fase di configurazione</t>
   </si>
 </sst>
 </file>
@@ -4413,10 +4434,10 @@
   <dimension ref="A1:T993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B172" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="K168" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="M162" sqref="M162"/>
+      <selection pane="bottomRight" activeCell="N166" sqref="N166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4844,7 +4865,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="65">
         <v>6</v>
       </c>
@@ -4888,7 +4909,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="65">
         <v>7</v>
       </c>
@@ -4932,7 +4953,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="65">
         <v>8</v>
       </c>
@@ -4976,7 +4997,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="65">
         <v>9</v>
       </c>
@@ -5614,7 +5635,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="65">
         <v>29</v>
       </c>
@@ -5760,17 +5781,17 @@
       <c r="E39" s="32" t="s">
         <v>431</v>
       </c>
-      <c r="F39" s="14" t="s">
-        <v>524</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>566</v>
+      <c r="F39" s="71">
+        <v>45183</v>
+      </c>
+      <c r="G39" s="14" t="s">
+        <v>523</v>
       </c>
       <c r="H39" s="15" t="s">
+        <v>565</v>
+      </c>
+      <c r="I39" s="15" t="s">
         <v>434</v>
-      </c>
-      <c r="I39" s="15" t="s">
-        <v>509</v>
       </c>
       <c r="J39" s="16" t="s">
         <v>83</v>
@@ -5783,7 +5804,9 @@
       <c r="N39" s="16" t="s">
         <v>435</v>
       </c>
-      <c r="O39" s="16"/>
+      <c r="O39" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="P39" s="16" t="s">
         <v>439</v>
       </c>
@@ -5930,7 +5953,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="65">
         <v>37</v>
       </c>
@@ -6068,25 +6091,27 @@
       <c r="E47" s="32" t="s">
         <v>432</v>
       </c>
-      <c r="F47" s="14" t="s">
-        <v>524</v>
+      <c r="F47" s="14">
+        <v>45183</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>565</v>
+        <v>523</v>
       </c>
       <c r="H47" s="15" t="s">
+        <v>564</v>
+      </c>
+      <c r="I47" s="15" t="s">
         <v>434</v>
-      </c>
-      <c r="I47" s="15" t="s">
-        <v>509</v>
       </c>
       <c r="J47" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K47" s="16"/>
-      <c r="L47" s="16"/>
+      <c r="L47" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="M47" s="16" t="s">
-        <v>437</v>
+        <v>83</v>
       </c>
       <c r="N47" s="16" t="s">
         <v>437</v>
@@ -6242,7 +6267,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="210.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="65">
         <v>45</v>
       </c>
@@ -6886,7 +6911,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="275.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" ht="275.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="65">
         <v>63</v>
       </c>
@@ -6942,7 +6967,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="65">
         <v>64</v>
       </c>
@@ -6998,7 +7023,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="65">
         <v>65</v>
       </c>
@@ -7054,7 +7079,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="65">
         <v>66</v>
       </c>
@@ -7110,7 +7135,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="65">
         <v>67</v>
       </c>
@@ -7166,7 +7191,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="65">
         <v>68</v>
       </c>
@@ -7222,7 +7247,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="65">
         <v>69</v>
       </c>
@@ -7278,7 +7303,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="65">
         <v>70</v>
       </c>
@@ -7334,7 +7359,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="65">
         <v>71</v>
       </c>
@@ -7390,7 +7415,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="65">
         <v>72</v>
       </c>
@@ -7446,7 +7471,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="65">
         <v>73</v>
       </c>
@@ -7502,7 +7527,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="65">
         <v>74</v>
       </c>
@@ -10158,13 +10183,13 @@
         <v>45183</v>
       </c>
       <c r="G157" s="15" t="s">
+        <v>523</v>
+      </c>
+      <c r="H157" s="15" t="s">
         <v>524</v>
       </c>
-      <c r="H157" s="15" t="s">
+      <c r="I157" s="15" t="s">
         <v>525</v>
-      </c>
-      <c r="I157" s="15" t="s">
-        <v>526</v>
       </c>
       <c r="J157" s="16" t="s">
         <v>83</v>
@@ -10182,7 +10207,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="158" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="11">
         <v>151</v>
       </c>
@@ -10202,35 +10227,43 @@
         <v>45183</v>
       </c>
       <c r="G158" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H158" s="15" t="s">
+        <v>526</v>
+      </c>
+      <c r="I158" s="15" t="s">
         <v>527</v>
-      </c>
-      <c r="I158" s="15" t="s">
-        <v>528</v>
       </c>
       <c r="J158" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K158" s="16"/>
-      <c r="L158" s="16"/>
+      <c r="L158" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="M158" s="16" t="s">
-        <v>509</v>
+        <v>83</v>
       </c>
       <c r="N158" s="16" t="s">
         <v>454</v>
       </c>
-      <c r="O158" s="16"/>
-      <c r="P158" s="16"/>
+      <c r="O158" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P158" s="16" t="s">
+        <v>501</v>
+      </c>
       <c r="Q158" s="16"/>
       <c r="R158" s="17"/>
-      <c r="S158" s="18"/>
+      <c r="S158" s="18" t="s">
+        <v>440</v>
+      </c>
       <c r="T158" s="29" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="11">
         <v>152</v>
       </c>
@@ -10250,25 +10283,33 @@
         <v>45183</v>
       </c>
       <c r="G159" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H159" s="15" t="s">
+        <v>528</v>
+      </c>
+      <c r="I159" s="15" t="s">
         <v>529</v>
-      </c>
-      <c r="I159" s="15" t="s">
-        <v>530</v>
       </c>
       <c r="J159" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K159" s="16"/>
-      <c r="L159" s="16"/>
-      <c r="M159" s="16"/>
+      <c r="L159" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M159" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="N159" s="16" t="s">
         <v>455</v>
       </c>
-      <c r="O159" s="16"/>
-      <c r="P159" s="16"/>
+      <c r="O159" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P159" s="16" t="s">
+        <v>501</v>
+      </c>
       <c r="Q159" s="16"/>
       <c r="R159" s="17"/>
       <c r="S159" s="18"/>
@@ -10276,7 +10317,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="11">
         <v>153</v>
       </c>
@@ -10296,23 +10337,33 @@
         <v>45183</v>
       </c>
       <c r="G160" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H160" s="15" t="s">
+        <v>530</v>
+      </c>
+      <c r="I160" s="15" t="s">
         <v>531</v>
-      </c>
-      <c r="I160" s="15" t="s">
-        <v>532</v>
       </c>
       <c r="J160" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K160" s="16"/>
-      <c r="L160" s="16"/>
-      <c r="M160" s="16"/>
-      <c r="N160" s="16"/>
-      <c r="O160" s="16"/>
-      <c r="P160" s="16"/>
+      <c r="L160" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M160" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="N160" s="16" t="s">
+        <v>456</v>
+      </c>
+      <c r="O160" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P160" s="16" t="s">
+        <v>501</v>
+      </c>
       <c r="Q160" s="16"/>
       <c r="R160" s="17"/>
       <c r="S160" s="18"/>
@@ -10320,7 +10371,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="11">
         <v>154</v>
       </c>
@@ -10340,33 +10391,43 @@
         <v>45183</v>
       </c>
       <c r="G161" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H161" s="15" t="s">
+        <v>532</v>
+      </c>
+      <c r="I161" s="15" t="s">
         <v>533</v>
-      </c>
-      <c r="I161" s="15" t="s">
-        <v>534</v>
       </c>
       <c r="J161" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K161" s="16"/>
-      <c r="L161" s="16"/>
-      <c r="M161" s="16"/>
+      <c r="L161" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M161" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="N161" s="16" t="s">
         <v>463</v>
       </c>
-      <c r="O161" s="16"/>
-      <c r="P161" s="16"/>
+      <c r="O161" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P161" s="16" t="s">
+        <v>501</v>
+      </c>
       <c r="Q161" s="16"/>
       <c r="R161" s="17"/>
-      <c r="S161" s="18"/>
+      <c r="S161" s="18" t="s">
+        <v>445</v>
+      </c>
       <c r="T161" s="29" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="11">
         <v>155</v>
       </c>
@@ -10386,33 +10447,43 @@
         <v>45183</v>
       </c>
       <c r="G162" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H162" s="15" t="s">
+        <v>534</v>
+      </c>
+      <c r="I162" s="15" t="s">
         <v>535</v>
-      </c>
-      <c r="I162" s="15" t="s">
-        <v>536</v>
       </c>
       <c r="J162" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K162" s="16"/>
-      <c r="L162" s="16"/>
-      <c r="M162" s="16"/>
+      <c r="L162" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M162" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="N162" s="16" t="s">
         <v>464</v>
       </c>
-      <c r="O162" s="16"/>
-      <c r="P162" s="16"/>
+      <c r="O162" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P162" s="16" t="s">
+        <v>501</v>
+      </c>
       <c r="Q162" s="16"/>
       <c r="R162" s="17"/>
-      <c r="S162" s="18"/>
+      <c r="S162" s="18" t="s">
+        <v>444</v>
+      </c>
       <c r="T162" s="29" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="11">
         <v>156</v>
       </c>
@@ -10432,33 +10503,43 @@
         <v>45183</v>
       </c>
       <c r="G163" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H163" s="15" t="s">
+        <v>536</v>
+      </c>
+      <c r="I163" s="15" t="s">
         <v>537</v>
-      </c>
-      <c r="I163" s="15" t="s">
-        <v>538</v>
       </c>
       <c r="J163" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K163" s="16"/>
-      <c r="L163" s="16"/>
-      <c r="M163" s="16"/>
+      <c r="L163" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M163" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="N163" s="16" t="s">
-        <v>510</v>
-      </c>
-      <c r="O163" s="16"/>
-      <c r="P163" s="16"/>
+        <v>509</v>
+      </c>
+      <c r="O163" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P163" s="16" t="s">
+        <v>501</v>
+      </c>
       <c r="Q163" s="16"/>
       <c r="R163" s="17"/>
-      <c r="S163" s="18"/>
+      <c r="S163" s="18" t="s">
+        <v>443</v>
+      </c>
       <c r="T163" s="29" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="11">
         <v>157</v>
       </c>
@@ -10478,33 +10559,43 @@
         <v>45183</v>
       </c>
       <c r="G164" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H164" s="15" t="s">
+        <v>538</v>
+      </c>
+      <c r="I164" s="15" t="s">
         <v>539</v>
-      </c>
-      <c r="I164" s="15" t="s">
-        <v>540</v>
       </c>
       <c r="J164" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K164" s="16"/>
-      <c r="L164" s="16"/>
-      <c r="M164" s="16"/>
+      <c r="L164" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M164" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="N164" s="16" t="s">
-        <v>511</v>
-      </c>
-      <c r="O164" s="16"/>
-      <c r="P164" s="16"/>
+        <v>510</v>
+      </c>
+      <c r="O164" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P164" s="16" t="s">
+        <v>501</v>
+      </c>
       <c r="Q164" s="16"/>
       <c r="R164" s="17"/>
-      <c r="S164" s="18"/>
+      <c r="S164" s="18" t="s">
+        <v>566</v>
+      </c>
       <c r="T164" s="29" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="11">
         <v>158</v>
       </c>
@@ -10524,25 +10615,33 @@
         <v>45183</v>
       </c>
       <c r="G165" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H165" s="15" t="s">
+        <v>540</v>
+      </c>
+      <c r="I165" s="15" t="s">
         <v>541</v>
-      </c>
-      <c r="I165" s="15" t="s">
-        <v>542</v>
       </c>
       <c r="J165" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K165" s="16"/>
-      <c r="L165" s="16"/>
-      <c r="M165" s="16"/>
+      <c r="L165" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M165" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="N165" s="16" t="s">
-        <v>512</v>
-      </c>
-      <c r="O165" s="16"/>
-      <c r="P165" s="16"/>
+        <v>511</v>
+      </c>
+      <c r="O165" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P165" s="16" t="s">
+        <v>501</v>
+      </c>
       <c r="Q165" s="16"/>
       <c r="R165" s="17"/>
       <c r="S165" s="18"/>
@@ -10550,7 +10649,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="11">
         <v>159</v>
       </c>
@@ -10570,33 +10669,43 @@
         <v>45183</v>
       </c>
       <c r="G166" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H166" s="15" t="s">
+        <v>542</v>
+      </c>
+      <c r="I166" s="15" t="s">
         <v>543</v>
-      </c>
-      <c r="I166" s="15" t="s">
-        <v>544</v>
       </c>
       <c r="J166" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K166" s="16"/>
-      <c r="L166" s="16"/>
-      <c r="M166" s="16"/>
+      <c r="L166" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M166" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="N166" s="16" t="s">
-        <v>513</v>
-      </c>
-      <c r="O166" s="16"/>
-      <c r="P166" s="16"/>
+        <v>512</v>
+      </c>
+      <c r="O166" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P166" s="16" t="s">
+        <v>501</v>
+      </c>
       <c r="Q166" s="16"/>
       <c r="R166" s="17"/>
-      <c r="S166" s="18"/>
+      <c r="S166" s="18" t="s">
+        <v>567</v>
+      </c>
       <c r="T166" s="29" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="11">
         <v>160</v>
       </c>
@@ -10616,33 +10725,43 @@
         <v>45183</v>
       </c>
       <c r="G167" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H167" s="15" t="s">
+        <v>544</v>
+      </c>
+      <c r="I167" s="15" t="s">
         <v>545</v>
-      </c>
-      <c r="I167" s="15" t="s">
-        <v>546</v>
       </c>
       <c r="J167" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K167" s="16"/>
-      <c r="L167" s="16"/>
-      <c r="M167" s="16"/>
+      <c r="L167" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M167" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="N167" s="16" t="s">
-        <v>514</v>
-      </c>
-      <c r="O167" s="16"/>
-      <c r="P167" s="16"/>
+        <v>513</v>
+      </c>
+      <c r="O167" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P167" s="16" t="s">
+        <v>501</v>
+      </c>
       <c r="Q167" s="16"/>
       <c r="R167" s="17"/>
-      <c r="S167" s="18"/>
+      <c r="S167" s="18" t="s">
+        <v>568</v>
+      </c>
       <c r="T167" s="29" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="11">
         <v>161</v>
       </c>
@@ -10662,33 +10781,43 @@
         <v>45183</v>
       </c>
       <c r="G168" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H168" s="15" t="s">
+        <v>546</v>
+      </c>
+      <c r="I168" s="15" t="s">
         <v>547</v>
-      </c>
-      <c r="I168" s="15" t="s">
-        <v>548</v>
       </c>
       <c r="J168" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K168" s="16"/>
-      <c r="L168" s="16"/>
-      <c r="M168" s="16"/>
+      <c r="L168" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M168" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="N168" s="16" t="s">
-        <v>515</v>
-      </c>
-      <c r="O168" s="16"/>
-      <c r="P168" s="16"/>
+        <v>514</v>
+      </c>
+      <c r="O168" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P168" s="16" t="s">
+        <v>501</v>
+      </c>
       <c r="Q168" s="16"/>
       <c r="R168" s="17"/>
-      <c r="S168" s="18"/>
+      <c r="S168" s="18" t="s">
+        <v>569</v>
+      </c>
       <c r="T168" s="29" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="11">
         <v>162</v>
       </c>
@@ -10708,33 +10837,43 @@
         <v>45183</v>
       </c>
       <c r="G169" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H169" s="15" t="s">
+        <v>548</v>
+      </c>
+      <c r="I169" s="15" t="s">
         <v>549</v>
-      </c>
-      <c r="I169" s="15" t="s">
-        <v>550</v>
       </c>
       <c r="J169" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K169" s="16"/>
-      <c r="L169" s="16"/>
-      <c r="M169" s="16"/>
+      <c r="L169" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M169" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="N169" s="16" t="s">
-        <v>516</v>
-      </c>
-      <c r="O169" s="16"/>
-      <c r="P169" s="16"/>
+        <v>515</v>
+      </c>
+      <c r="O169" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P169" s="16" t="s">
+        <v>501</v>
+      </c>
       <c r="Q169" s="16"/>
       <c r="R169" s="17"/>
-      <c r="S169" s="18"/>
+      <c r="S169" s="18" t="s">
+        <v>570</v>
+      </c>
       <c r="T169" s="29" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="11">
         <v>163</v>
       </c>
@@ -10754,25 +10893,33 @@
         <v>45183</v>
       </c>
       <c r="G170" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H170" s="15" t="s">
+        <v>550</v>
+      </c>
+      <c r="I170" s="15" t="s">
         <v>551</v>
-      </c>
-      <c r="I170" s="15" t="s">
-        <v>552</v>
       </c>
       <c r="J170" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K170" s="16"/>
-      <c r="L170" s="16"/>
-      <c r="M170" s="16"/>
+      <c r="L170" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M170" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="N170" s="16" t="s">
-        <v>517</v>
-      </c>
-      <c r="O170" s="16"/>
-      <c r="P170" s="16"/>
+        <v>516</v>
+      </c>
+      <c r="O170" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P170" s="16" t="s">
+        <v>501</v>
+      </c>
       <c r="Q170" s="16"/>
       <c r="R170" s="17"/>
       <c r="S170" s="18"/>
@@ -10780,7 +10927,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="11">
         <v>164</v>
       </c>
@@ -10800,33 +10947,43 @@
         <v>45183</v>
       </c>
       <c r="G171" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H171" s="15" t="s">
+        <v>552</v>
+      </c>
+      <c r="I171" s="15" t="s">
         <v>553</v>
-      </c>
-      <c r="I171" s="15" t="s">
-        <v>554</v>
       </c>
       <c r="J171" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K171" s="16"/>
-      <c r="L171" s="16"/>
-      <c r="M171" s="16"/>
+      <c r="L171" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M171" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="N171" s="16" t="s">
-        <v>518</v>
-      </c>
-      <c r="O171" s="16"/>
-      <c r="P171" s="16"/>
+        <v>517</v>
+      </c>
+      <c r="O171" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P171" s="16" t="s">
+        <v>501</v>
+      </c>
       <c r="Q171" s="16"/>
       <c r="R171" s="17"/>
-      <c r="S171" s="18"/>
+      <c r="S171" s="18" t="s">
+        <v>571</v>
+      </c>
       <c r="T171" s="29" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="11">
         <v>165</v>
       </c>
@@ -10846,33 +11003,43 @@
         <v>45183</v>
       </c>
       <c r="G172" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H172" s="15" t="s">
+        <v>554</v>
+      </c>
+      <c r="I172" s="15" t="s">
         <v>555</v>
-      </c>
-      <c r="I172" s="15" t="s">
-        <v>556</v>
       </c>
       <c r="J172" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K172" s="16"/>
-      <c r="L172" s="16"/>
-      <c r="M172" s="16"/>
+      <c r="L172" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M172" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="N172" s="16" t="s">
-        <v>519</v>
-      </c>
-      <c r="O172" s="16"/>
-      <c r="P172" s="16"/>
+        <v>518</v>
+      </c>
+      <c r="O172" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P172" s="16" t="s">
+        <v>501</v>
+      </c>
       <c r="Q172" s="16"/>
       <c r="R172" s="17"/>
-      <c r="S172" s="18"/>
+      <c r="S172" s="18" t="s">
+        <v>571</v>
+      </c>
       <c r="T172" s="29" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="11">
         <v>166</v>
       </c>
@@ -10892,33 +11059,43 @@
         <v>45183</v>
       </c>
       <c r="G173" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H173" s="15" t="s">
+        <v>556</v>
+      </c>
+      <c r="I173" s="15" t="s">
         <v>557</v>
-      </c>
-      <c r="I173" s="15" t="s">
-        <v>558</v>
       </c>
       <c r="J173" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K173" s="16"/>
-      <c r="L173" s="16"/>
-      <c r="M173" s="16"/>
+      <c r="L173" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M173" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="N173" s="16" t="s">
-        <v>520</v>
-      </c>
-      <c r="O173" s="16"/>
-      <c r="P173" s="16"/>
+        <v>519</v>
+      </c>
+      <c r="O173" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P173" s="16" t="s">
+        <v>501</v>
+      </c>
       <c r="Q173" s="16"/>
       <c r="R173" s="17"/>
-      <c r="S173" s="18"/>
+      <c r="S173" s="18" t="s">
+        <v>571</v>
+      </c>
       <c r="T173" s="29" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="11">
         <v>167</v>
       </c>
@@ -10938,33 +11115,43 @@
         <v>45183</v>
       </c>
       <c r="G174" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H174" s="15" t="s">
+        <v>558</v>
+      </c>
+      <c r="I174" s="15" t="s">
         <v>559</v>
-      </c>
-      <c r="I174" s="15" t="s">
-        <v>560</v>
       </c>
       <c r="J174" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K174" s="16"/>
-      <c r="L174" s="16"/>
-      <c r="M174" s="16"/>
+      <c r="L174" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M174" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="N174" s="16" t="s">
-        <v>521</v>
-      </c>
-      <c r="O174" s="16"/>
-      <c r="P174" s="16"/>
+        <v>520</v>
+      </c>
+      <c r="O174" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P174" s="16" t="s">
+        <v>501</v>
+      </c>
       <c r="Q174" s="16"/>
       <c r="R174" s="17"/>
-      <c r="S174" s="18"/>
+      <c r="S174" s="18" t="s">
+        <v>571</v>
+      </c>
       <c r="T174" s="29" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="11">
         <v>168</v>
       </c>
@@ -10984,28 +11171,38 @@
         <v>45183</v>
       </c>
       <c r="G175" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H175" s="15" t="s">
+        <v>560</v>
+      </c>
+      <c r="I175" s="15" t="s">
         <v>561</v>
-      </c>
-      <c r="I175" s="15" t="s">
-        <v>562</v>
       </c>
       <c r="J175" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K175" s="16"/>
-      <c r="L175" s="16"/>
-      <c r="M175" s="16"/>
+      <c r="L175" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M175" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="N175" s="16" t="s">
-        <v>522</v>
-      </c>
-      <c r="O175" s="16"/>
-      <c r="P175" s="16"/>
+        <v>521</v>
+      </c>
+      <c r="O175" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P175" s="16" t="s">
+        <v>501</v>
+      </c>
       <c r="Q175" s="16"/>
       <c r="R175" s="17"/>
-      <c r="S175" s="18"/>
+      <c r="S175" s="18" t="s">
+        <v>572</v>
+      </c>
       <c r="T175" s="29" t="s">
         <v>430</v>
       </c>
@@ -11030,28 +11227,38 @@
         <v>45183</v>
       </c>
       <c r="G176" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H176" s="15" t="s">
+        <v>562</v>
+      </c>
+      <c r="I176" s="15" t="s">
         <v>563</v>
-      </c>
-      <c r="I176" s="15" t="s">
-        <v>564</v>
       </c>
       <c r="J176" s="16" t="s">
         <v>83</v>
       </c>
       <c r="K176" s="16"/>
-      <c r="L176" s="16"/>
-      <c r="M176" s="16"/>
+      <c r="L176" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="M176" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="N176" s="16" t="s">
-        <v>523</v>
-      </c>
-      <c r="O176" s="16"/>
-      <c r="P176" s="16"/>
+        <v>522</v>
+      </c>
+      <c r="O176" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="P176" s="16" t="s">
+        <v>501</v>
+      </c>
       <c r="Q176" s="16"/>
       <c r="R176" s="17"/>
-      <c r="S176" s="18"/>
+      <c r="S176" s="18" t="s">
+        <v>573</v>
+      </c>
       <c r="T176" s="29" t="s">
         <v>430</v>
       </c>
@@ -25323,6 +25530,7 @@
   <autoFilter ref="A9:T198" xr:uid="{00000000-0001-0000-0100-000000000000}">
     <filterColumn colId="2">
       <filters>
+        <filter val="LDO"/>
         <filter val="RSA"/>
       </filters>
     </filterColumn>
@@ -25358,7 +25566,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>L1:M8 O1:O8 L40:L43 L10:L35 O10:O1048576 L37:L38 L45:L46 M10:M1048576 L48:L1048576</xm:sqref>
+          <xm:sqref>L1:M8 O1:O8 L40:L43 L10:L35 L48:L1048576 L37:L38 L45:L46 M10:M1048576 O10:O1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -27566,6 +27774,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -27796,41 +28024,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB221413-913B-41FE-97D3-5428BD0403A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -27853,9 +28050,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB221413-913B-41FE-97D3-5428BD0403A1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Aggiornamento accreditamento per S1#111MEDARCHIVER tutti i test v.4 - Update Checklist
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
+++ b/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gzamparo\Documents\FSE 2.0\it-fse-accreditamento\GATEWAY\S1#111MEDARCHIVER\MEDARCHIVER\MEDARCHIVER_FSE2.0\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9D070E-6B95-434C-A42D-76E0F78BDF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A1620E-8716-4DDD-AB16-C57063CFB95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="574">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -4434,10 +4434,10 @@
   <dimension ref="A1:T993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="K168" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="K39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="N166" sqref="N166"/>
+      <selection pane="bottomRight" activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4865,7 +4865,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="65">
         <v>6</v>
       </c>
@@ -4909,7 +4909,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="65">
         <v>7</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="65">
         <v>8</v>
       </c>
@@ -4997,7 +4997,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="65">
         <v>9</v>
       </c>
@@ -5635,7 +5635,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="65">
         <v>29</v>
       </c>
@@ -5797,7 +5797,9 @@
         <v>83</v>
       </c>
       <c r="K39" s="16"/>
-      <c r="L39" s="16"/>
+      <c r="L39" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="M39" s="16" t="s">
         <v>435</v>
       </c>
@@ -5953,7 +5955,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="65">
         <v>37</v>
       </c>
@@ -6075,7 +6077,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="22">
         <v>40</v>
       </c>
@@ -6267,7 +6269,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" ht="210.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="65">
         <v>45</v>
       </c>
@@ -6385,7 +6387,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" ht="210.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11">
         <v>48</v>
       </c>
@@ -6911,7 +6913,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="275.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" ht="275.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="65">
         <v>63</v>
       </c>
@@ -6967,7 +6969,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="65">
         <v>64</v>
       </c>
@@ -7023,7 +7025,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="65">
         <v>65</v>
       </c>
@@ -7079,7 +7081,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="65">
         <v>66</v>
       </c>
@@ -7135,7 +7137,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="65">
         <v>67</v>
       </c>
@@ -7191,7 +7193,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="65">
         <v>68</v>
       </c>
@@ -7247,7 +7249,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="65">
         <v>69</v>
       </c>
@@ -7303,7 +7305,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="65">
         <v>70</v>
       </c>
@@ -7359,7 +7361,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="65">
         <v>71</v>
       </c>
@@ -7415,7 +7417,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="65">
         <v>72</v>
       </c>
@@ -7471,7 +7473,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="65">
         <v>73</v>
       </c>
@@ -7527,7 +7529,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="65">
         <v>74</v>
       </c>
@@ -7583,7 +7585,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="42">
         <v>75</v>
       </c>
@@ -7617,7 +7619,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11">
         <v>76</v>
       </c>
@@ -7651,7 +7653,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11">
         <v>77</v>
       </c>
@@ -7685,7 +7687,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11">
         <v>78</v>
       </c>
@@ -7719,7 +7721,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="11">
         <v>79</v>
       </c>
@@ -7753,7 +7755,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="11">
         <v>80</v>
       </c>
@@ -7787,7 +7789,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="11">
         <v>81</v>
       </c>
@@ -7821,7 +7823,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="11">
         <v>82</v>
       </c>
@@ -7855,7 +7857,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="11">
         <v>83</v>
       </c>
@@ -7889,7 +7891,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="11">
         <v>84</v>
       </c>
@@ -7923,7 +7925,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="11">
         <v>85</v>
       </c>
@@ -7957,7 +7959,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="11">
         <v>86</v>
       </c>
@@ -7991,7 +7993,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="11">
         <v>87</v>
       </c>
@@ -8025,7 +8027,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="11">
         <v>88</v>
       </c>
@@ -8059,7 +8061,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="11">
         <v>89</v>
       </c>
@@ -8093,7 +8095,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="11">
         <v>90</v>
       </c>
@@ -8127,7 +8129,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="11">
         <v>91</v>
       </c>
@@ -8161,7 +8163,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="11">
         <v>92</v>
       </c>
@@ -8195,7 +8197,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="11">
         <v>93</v>
       </c>
@@ -8229,7 +8231,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="11">
         <v>94</v>
       </c>
@@ -8263,7 +8265,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="11">
         <v>95</v>
       </c>
@@ -8297,7 +8299,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="11">
         <v>96</v>
       </c>
@@ -8331,7 +8333,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="11">
         <v>97</v>
       </c>
@@ -8365,7 +8367,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="11">
         <v>98</v>
       </c>
@@ -8399,7 +8401,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="11">
         <v>99</v>
       </c>
@@ -8433,7 +8435,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="11">
         <v>100</v>
       </c>
@@ -8467,7 +8469,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="11">
         <v>101</v>
       </c>
@@ -8501,7 +8503,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="11">
         <v>102</v>
       </c>
@@ -8535,7 +8537,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="11">
         <v>103</v>
       </c>
@@ -8569,7 +8571,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="11">
         <v>104</v>
       </c>
@@ -8603,7 +8605,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="11">
         <v>105</v>
       </c>
@@ -8637,7 +8639,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="11">
         <v>106</v>
       </c>
@@ -8671,7 +8673,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="11">
         <v>107</v>
       </c>
@@ -8705,7 +8707,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="11">
         <v>108</v>
       </c>
@@ -8739,7 +8741,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="11">
         <v>109</v>
       </c>
@@ -8773,7 +8775,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="11">
         <v>110</v>
       </c>
@@ -8807,7 +8809,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="11">
         <v>111</v>
       </c>
@@ -8841,7 +8843,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="11">
         <v>112</v>
       </c>
@@ -8875,7 +8877,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="11">
         <v>113</v>
       </c>
@@ -8909,7 +8911,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="11">
         <v>114</v>
       </c>
@@ -8943,7 +8945,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="11">
         <v>115</v>
       </c>
@@ -8977,7 +8979,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="11">
         <v>116</v>
       </c>
@@ -9011,7 +9013,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="11">
         <v>117</v>
       </c>
@@ -9045,7 +9047,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="11">
         <v>118</v>
       </c>
@@ -9079,7 +9081,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="11">
         <v>119</v>
       </c>
@@ -9113,7 +9115,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="11">
         <v>120</v>
       </c>
@@ -9147,7 +9149,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="11">
         <v>121</v>
       </c>
@@ -9181,7 +9183,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="11">
         <v>122</v>
       </c>
@@ -9215,7 +9217,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="11">
         <v>123</v>
       </c>
@@ -9249,7 +9251,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="11">
         <v>124</v>
       </c>
@@ -9283,7 +9285,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="11">
         <v>125</v>
       </c>
@@ -9317,7 +9319,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="11">
         <v>126</v>
       </c>
@@ -9351,7 +9353,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="11">
         <v>127</v>
       </c>
@@ -9385,7 +9387,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="11">
         <v>128</v>
       </c>
@@ -9419,7 +9421,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="11">
         <v>129</v>
       </c>
@@ -9453,7 +9455,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="11">
         <v>130</v>
       </c>
@@ -9487,7 +9489,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="11">
         <v>131</v>
       </c>
@@ -9521,7 +9523,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="11">
         <v>132</v>
       </c>
@@ -9555,7 +9557,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="11">
         <v>133</v>
       </c>
@@ -9589,7 +9591,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="11">
         <v>134</v>
       </c>
@@ -9623,7 +9625,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="11">
         <v>135</v>
       </c>
@@ -9657,7 +9659,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="11">
         <v>136</v>
       </c>
@@ -9691,7 +9693,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="11">
         <v>137</v>
       </c>
@@ -9725,7 +9727,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="11">
         <v>138</v>
       </c>
@@ -9759,7 +9761,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="11">
         <v>139</v>
       </c>
@@ -9793,7 +9795,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="11">
         <v>140</v>
       </c>
@@ -9827,7 +9829,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="148" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="11">
         <v>141</v>
       </c>
@@ -9861,7 +9863,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="149" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="11">
         <v>142</v>
       </c>
@@ -9895,7 +9897,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="11">
         <v>143</v>
       </c>
@@ -9929,7 +9931,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="151" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="11">
         <v>144</v>
       </c>
@@ -9963,7 +9965,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="152" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="11">
         <v>145</v>
       </c>
@@ -9997,7 +9999,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="153" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="11">
         <v>146</v>
       </c>
@@ -10031,7 +10033,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:20" ht="165" x14ac:dyDescent="0.25">
       <c r="A154" s="11">
         <v>147</v>
       </c>
@@ -10075,7 +10077,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="11">
         <v>148</v>
       </c>
@@ -10119,7 +10121,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="11">
         <v>149</v>
       </c>
@@ -10163,7 +10165,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="11">
         <v>150</v>
       </c>
@@ -10207,7 +10209,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="158" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="11">
         <v>151</v>
       </c>
@@ -10263,7 +10265,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="11">
         <v>152</v>
       </c>
@@ -10317,7 +10319,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="11">
         <v>153</v>
       </c>
@@ -10371,7 +10373,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="11">
         <v>154</v>
       </c>
@@ -10427,7 +10429,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="11">
         <v>155</v>
       </c>
@@ -10483,7 +10485,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="11">
         <v>156</v>
       </c>
@@ -10539,7 +10541,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="11">
         <v>157</v>
       </c>
@@ -10595,7 +10597,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="11">
         <v>158</v>
       </c>
@@ -10649,7 +10651,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="11">
         <v>159</v>
       </c>
@@ -10705,7 +10707,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="11">
         <v>160</v>
       </c>
@@ -10761,7 +10763,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="11">
         <v>161</v>
       </c>
@@ -10817,7 +10819,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="11">
         <v>162</v>
       </c>
@@ -10873,7 +10875,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="11">
         <v>163</v>
       </c>
@@ -10927,7 +10929,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="11">
         <v>164</v>
       </c>
@@ -10983,7 +10985,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="11">
         <v>165</v>
       </c>
@@ -11039,7 +11041,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="11">
         <v>166</v>
       </c>
@@ -11095,7 +11097,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="11">
         <v>167</v>
       </c>
@@ -11151,7 +11153,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="11">
         <v>168</v>
       </c>
@@ -11207,7 +11209,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="129.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:20" ht="129.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="11">
         <v>169</v>
       </c>
@@ -25528,9 +25530,14 @@
     </row>
   </sheetData>
   <autoFilter ref="A9:T198" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="32"/>
+        <filter val="147"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="2">
       <filters>
-        <filter val="LDO"/>
         <filter val="RSA"/>
       </filters>
     </filterColumn>
@@ -27774,26 +27781,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -28024,10 +28011,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB221413-913B-41FE-97D3-5428BD0403A1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28050,20 +28068,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB221413-913B-41FE-97D3-5428BD0403A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Accreditamento LDA, RSA v.2
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
+++ b/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gzamparo\Documents\FSE 2.0\it-fse-accreditamento\GATEWAY\S1#111MEDARCHIVER\MEDARCHIVER\MEDARCHIVER_FSE2.0\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72258A6B-EBF8-4D0B-95EC-32520FC640A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A40EF4-8CF4-44E2-B155-C3519C814E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="577">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -2171,30 +2171,6 @@
     <t>2023-09-29T17:08:21Z</t>
   </si>
   <si>
-    <t>f1e394c476bdfed1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.5187a7c6983155e8ce8a0349302fbf5ed672a64b2432a651aeaa4c11820cfe76.641f4c5d49^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>4ddb1731acd44ab3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.1998839e5b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>689b5b02e3ae1b22</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.bf4176332d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>219402d661e12b0b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.2765776584^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>28e7a17d1c0405db</t>
   </si>
   <si>
@@ -2207,12 +2183,6 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.ba793e02e9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>a1d7be0d897d8130</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.e7a5c56c46^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2b0a7449c52e5692</t>
   </si>
   <si>
@@ -2271,6 +2241,39 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.be7c0457b7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-10-06T10:46:17Z</t>
+  </si>
+  <si>
+    <t>c93432e4e8d64071</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.5187a7c6983155e8ce8a0349302fbf5ed672a64b2432a651aeaa4c11820cfe76.f8226cb04e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>c0c0dccb76b24d9a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.04dc0e44cd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>4514c4807392a10b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.4214c51452^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>6689a674e30b1c2e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.8ba1287cb4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>1accc88dfcbdb5f5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.508c27f438^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4359,10 +4362,10 @@
   <dimension ref="A1:T993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="K15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="O55" sqref="O55"/>
+      <selection pane="bottomRight" activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4790,7 +4793,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>6</v>
       </c>
@@ -4807,16 +4810,16 @@
         <v>39</v>
       </c>
       <c r="F15" s="14">
-        <v>45198</v>
+        <v>45205</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>541</v>
+        <v>566</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>542</v>
+        <v>567</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>543</v>
+        <v>568</v>
       </c>
       <c r="J15" s="16" t="s">
         <v>83</v>
@@ -4834,7 +4837,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
         <v>7</v>
       </c>
@@ -4851,16 +4854,16 @@
         <v>41</v>
       </c>
       <c r="F16" s="14">
-        <v>45198</v>
+        <v>45205</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>541</v>
+        <v>566</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>544</v>
+        <v>569</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>545</v>
+        <v>570</v>
       </c>
       <c r="J16" s="16" t="s">
         <v>83</v>
@@ -4878,7 +4881,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>8</v>
       </c>
@@ -4895,16 +4898,16 @@
         <v>43</v>
       </c>
       <c r="F17" s="14">
-        <v>45198</v>
+        <v>45205</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>541</v>
+        <v>566</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>546</v>
+        <v>571</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="J17" s="16" t="s">
         <v>83</v>
@@ -4922,7 +4925,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>9</v>
       </c>
@@ -4939,16 +4942,16 @@
         <v>45</v>
       </c>
       <c r="F18" s="14">
-        <v>45198</v>
+        <v>45205</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>541</v>
+        <v>566</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>548</v>
+        <v>573</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>549</v>
+        <v>574</v>
       </c>
       <c r="J18" s="16" t="s">
         <v>83</v>
@@ -4983,10 +4986,10 @@
         <v>48</v>
       </c>
       <c r="F19" s="14">
-        <v>45010</v>
+        <v>45205</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>438</v>
+        <v>566</v>
       </c>
       <c r="H19" s="15" t="s">
         <v>433</v>
@@ -5587,7 +5590,7 @@
         <v>541</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="I36" s="15" t="s">
         <v>434</v>
@@ -5909,7 +5912,7 @@
         <v>541</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
       <c r="I44" s="15" t="s">
         <v>434</v>
@@ -6200,7 +6203,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" ht="210.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="11">
         <v>45</v>
       </c>
@@ -6318,7 +6321,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="210" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" ht="210.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11">
         <v>48</v>
       </c>
@@ -6364,7 +6367,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11">
         <v>49</v>
       </c>
@@ -6400,7 +6403,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="11">
         <v>50</v>
       </c>
@@ -6436,7 +6439,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="11">
         <v>51</v>
       </c>
@@ -6472,7 +6475,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="11">
         <v>52</v>
       </c>
@@ -6506,7 +6509,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="11">
         <v>53</v>
       </c>
@@ -6540,7 +6543,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="11">
         <v>54</v>
       </c>
@@ -6574,7 +6577,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="11">
         <v>55</v>
       </c>
@@ -6608,7 +6611,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="11">
         <v>56</v>
       </c>
@@ -6642,7 +6645,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="11">
         <v>57</v>
       </c>
@@ -6676,7 +6679,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="11">
         <v>58</v>
       </c>
@@ -6710,7 +6713,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="11">
         <v>59</v>
       </c>
@@ -6744,7 +6747,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="11">
         <v>60</v>
       </c>
@@ -6778,7 +6781,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="11">
         <v>61</v>
       </c>
@@ -6812,7 +6815,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="11">
         <v>62</v>
       </c>
@@ -6846,7 +6849,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="11">
         <v>63</v>
       </c>
@@ -6869,10 +6872,10 @@
         <v>541</v>
       </c>
       <c r="H70" s="15" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="I70" s="15" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="J70" s="16" t="s">
         <v>83</v>
@@ -6902,7 +6905,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" ht="300" x14ac:dyDescent="0.25">
       <c r="A71" s="11">
         <v>64</v>
       </c>
@@ -6919,16 +6922,16 @@
         <v>127</v>
       </c>
       <c r="F71" s="14">
-        <v>45198</v>
+        <v>45205</v>
       </c>
       <c r="G71" s="15" t="s">
-        <v>541</v>
+        <v>566</v>
       </c>
       <c r="H71" s="15" t="s">
-        <v>554</v>
+        <v>575</v>
       </c>
       <c r="I71" s="15" t="s">
-        <v>555</v>
+        <v>576</v>
       </c>
       <c r="J71" s="16" t="s">
         <v>83</v>
@@ -6981,10 +6984,10 @@
         <v>541</v>
       </c>
       <c r="H72" s="15" t="s">
-        <v>556</v>
+        <v>546</v>
       </c>
       <c r="I72" s="15" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
       <c r="J72" s="16" t="s">
         <v>83</v>
@@ -7037,10 +7040,10 @@
         <v>541</v>
       </c>
       <c r="H73" s="15" t="s">
-        <v>558</v>
+        <v>548</v>
       </c>
       <c r="I73" s="15" t="s">
-        <v>559</v>
+        <v>549</v>
       </c>
       <c r="J73" s="16" t="s">
         <v>83</v>
@@ -7093,10 +7096,10 @@
         <v>541</v>
       </c>
       <c r="H74" s="15" t="s">
-        <v>560</v>
+        <v>550</v>
       </c>
       <c r="I74" s="15" t="s">
-        <v>561</v>
+        <v>551</v>
       </c>
       <c r="J74" s="16" t="s">
         <v>83</v>
@@ -7149,10 +7152,10 @@
         <v>541</v>
       </c>
       <c r="H75" s="15" t="s">
-        <v>562</v>
+        <v>552</v>
       </c>
       <c r="I75" s="15" t="s">
-        <v>563</v>
+        <v>553</v>
       </c>
       <c r="J75" s="16" t="s">
         <v>83</v>
@@ -7205,10 +7208,10 @@
         <v>541</v>
       </c>
       <c r="H76" s="15" t="s">
-        <v>564</v>
+        <v>554</v>
       </c>
       <c r="I76" s="15" t="s">
-        <v>565</v>
+        <v>555</v>
       </c>
       <c r="J76" s="16" t="s">
         <v>83</v>
@@ -7261,10 +7264,10 @@
         <v>541</v>
       </c>
       <c r="H77" s="15" t="s">
-        <v>566</v>
+        <v>556</v>
       </c>
       <c r="I77" s="15" t="s">
-        <v>567</v>
+        <v>557</v>
       </c>
       <c r="J77" s="16" t="s">
         <v>83</v>
@@ -7317,10 +7320,10 @@
         <v>541</v>
       </c>
       <c r="H78" s="15" t="s">
-        <v>568</v>
+        <v>558</v>
       </c>
       <c r="I78" s="15" t="s">
-        <v>569</v>
+        <v>559</v>
       </c>
       <c r="J78" s="16" t="s">
         <v>83</v>
@@ -7373,10 +7376,10 @@
         <v>541</v>
       </c>
       <c r="H79" s="15" t="s">
-        <v>570</v>
+        <v>560</v>
       </c>
       <c r="I79" s="15" t="s">
-        <v>571</v>
+        <v>561</v>
       </c>
       <c r="J79" s="16" t="s">
         <v>83</v>
@@ -7429,10 +7432,10 @@
         <v>541</v>
       </c>
       <c r="H80" s="15" t="s">
-        <v>572</v>
+        <v>562</v>
       </c>
       <c r="I80" s="15" t="s">
-        <v>573</v>
+        <v>563</v>
       </c>
       <c r="J80" s="16" t="s">
         <v>83</v>
@@ -7485,10 +7488,10 @@
         <v>541</v>
       </c>
       <c r="H81" s="15" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
       <c r="I81" s="15" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="J81" s="16" t="s">
         <v>83</v>
@@ -25463,16 +25466,20 @@
     </row>
   </sheetData>
   <autoFilter ref="A9:T198" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="6"/>
+        <filter val="64"/>
+        <filter val="7"/>
+        <filter val="8"/>
+        <filter val="9"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="2">
       <filters>
         <filter val="LDO"/>
         <filter val="RSA"/>
       </filters>
-    </filterColumn>
-    <filterColumn colId="17">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
     </filterColumn>
   </autoFilter>
   <mergeCells count="7">
@@ -27714,26 +27721,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -27964,10 +27951,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB221413-913B-41FE-97D3-5428BD0403A1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -27990,20 +28008,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB221413-913B-41FE-97D3-5428BD0403A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Accreditamento LDO, RSA v.2.2
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
+++ b/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gzamparo\Documents\FSE 2.0\it-fse-accreditamento\GATEWAY\S1#111MEDARCHIVER\MEDARCHIVER\MEDARCHIVER_FSE2.0\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A40EF4-8CF4-44E2-B155-C3519C814E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE95ECDD-96B5-4616-87BA-C461D2A860B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="582">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -2126,12 +2126,6 @@
     <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.76c16e90ae^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>7fc072b0eee91338</t>
-  </si>
-  <si>
-    <t>59ab2b74d0827505</t>
-  </si>
-  <si>
     <t>Per eseguire i test sono state modificate le codifiche in quanto non è possibile inserire un codice diverso da quelli previsti</t>
   </si>
   <si>
@@ -2171,12 +2165,6 @@
     <t>2023-09-29T17:08:21Z</t>
   </si>
   <si>
-    <t>28e7a17d1c0405db</t>
-  </si>
-  <si>
-    <t>dc185264a2dac3b3</t>
-  </si>
-  <si>
     <t>a5a655b0b9480217</t>
   </si>
   <si>
@@ -2270,10 +2258,37 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.8ba1287cb4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>1accc88dfcbdb5f5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.508c27f438^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-10-26T10:10:48Z</t>
+  </si>
+  <si>
+    <t>5a1c35de62eca011</t>
+  </si>
+  <si>
+    <t>2023-10-26T10:26:51Z</t>
+  </si>
+  <si>
+    <t>740b7f55a5e7aa8a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.1d809278a5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-10-26T10:49:32Z</t>
+  </si>
+  <si>
+    <t>78ad9e3fd2955bc0</t>
+  </si>
+  <si>
+    <t>2023-10-26T11:00:04Z</t>
+  </si>
+  <si>
+    <t>b6161e1e5fcd8c50</t>
+  </si>
+  <si>
+    <t>2023-10-26T11:04:28Z</t>
+  </si>
+  <si>
+    <t>3d7aac25df1cbfe4</t>
   </si>
 </sst>
 </file>
@@ -4362,10 +4377,10 @@
   <dimension ref="A1:T993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I71" sqref="I71"/>
+      <selection pane="bottomRight" activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4793,7 +4808,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>6</v>
       </c>
@@ -4813,13 +4828,13 @@
         <v>45205</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="J15" s="16" t="s">
         <v>83</v>
@@ -4837,7 +4852,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
         <v>7</v>
       </c>
@@ -4857,13 +4872,13 @@
         <v>45205</v>
       </c>
       <c r="G16" s="15" t="s">
+        <v>562</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>565</v>
+      </c>
+      <c r="I16" s="15" t="s">
         <v>566</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>569</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>570</v>
       </c>
       <c r="J16" s="16" t="s">
         <v>83</v>
@@ -4881,7 +4896,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>8</v>
       </c>
@@ -4901,13 +4916,13 @@
         <v>45205</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="J17" s="16" t="s">
         <v>83</v>
@@ -4925,7 +4940,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>9</v>
       </c>
@@ -4945,13 +4960,13 @@
         <v>45205</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="J18" s="16" t="s">
         <v>83</v>
@@ -4989,7 +5004,7 @@
         <v>45205</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="H19" s="15" t="s">
         <v>433</v>
@@ -5584,13 +5599,13 @@
         <v>431</v>
       </c>
       <c r="F36" s="14">
-        <v>45198</v>
+        <v>45225</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>541</v>
+        <v>576</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>542</v>
+        <v>577</v>
       </c>
       <c r="I36" s="15" t="s">
         <v>434</v>
@@ -5699,7 +5714,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11">
         <v>32</v>
       </c>
@@ -5716,13 +5731,13 @@
         <v>431</v>
       </c>
       <c r="F39" s="14">
-        <v>45183</v>
+        <v>45225</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>488</v>
+        <v>580</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>528</v>
+        <v>581</v>
       </c>
       <c r="I39" s="15" t="s">
         <v>434</v>
@@ -5753,7 +5768,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11">
         <v>33</v>
       </c>
@@ -5787,7 +5802,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
         <v>34</v>
       </c>
@@ -5821,7 +5836,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11">
         <v>35</v>
       </c>
@@ -5855,7 +5870,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
         <v>36</v>
       </c>
@@ -5889,7 +5904,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11">
         <v>37</v>
       </c>
@@ -5906,13 +5921,13 @@
         <v>432</v>
       </c>
       <c r="F44" s="14">
-        <v>45198</v>
+        <v>45225</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>541</v>
+        <v>571</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>543</v>
+        <v>572</v>
       </c>
       <c r="I44" s="15" t="s">
         <v>434</v>
@@ -5943,7 +5958,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
         <v>38</v>
       </c>
@@ -5977,7 +5992,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
         <v>39</v>
       </c>
@@ -6011,7 +6026,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" ht="180" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
         <v>40</v>
       </c>
@@ -6028,13 +6043,13 @@
         <v>432</v>
       </c>
       <c r="F47" s="14">
-        <v>45183</v>
+        <v>45225</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>488</v>
+        <v>578</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>527</v>
+        <v>579</v>
       </c>
       <c r="I47" s="15" t="s">
         <v>434</v>
@@ -6065,7 +6080,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
         <v>41</v>
       </c>
@@ -6099,7 +6114,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
         <v>42</v>
       </c>
@@ -6133,7 +6148,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <v>43</v>
       </c>
@@ -6167,7 +6182,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11">
         <v>44</v>
       </c>
@@ -6203,7 +6218,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="210.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="11">
         <v>45</v>
       </c>
@@ -6249,7 +6264,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="11">
         <v>46</v>
       </c>
@@ -6285,7 +6300,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="11">
         <v>47</v>
       </c>
@@ -6321,7 +6336,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="210.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
         <v>48</v>
       </c>
@@ -6367,7 +6382,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="11">
         <v>49</v>
       </c>
@@ -6403,7 +6418,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
         <v>50</v>
       </c>
@@ -6439,7 +6454,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="11">
         <v>51</v>
       </c>
@@ -6475,7 +6490,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
         <v>52</v>
       </c>
@@ -6509,7 +6524,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="11">
         <v>53</v>
       </c>
@@ -6543,7 +6558,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
         <v>54</v>
       </c>
@@ -6577,7 +6592,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>55</v>
       </c>
@@ -6611,7 +6626,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
         <v>56</v>
       </c>
@@ -6645,7 +6660,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="11">
         <v>57</v>
       </c>
@@ -6679,7 +6694,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="11">
         <v>58</v>
       </c>
@@ -6713,7 +6728,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="11">
         <v>59</v>
       </c>
@@ -6747,7 +6762,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11">
         <v>60</v>
       </c>
@@ -6781,7 +6796,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11">
         <v>61</v>
       </c>
@@ -6815,7 +6830,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11">
         <v>62</v>
       </c>
@@ -6849,7 +6864,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="11">
         <v>63</v>
       </c>
@@ -6869,13 +6884,13 @@
         <v>45198</v>
       </c>
       <c r="G70" s="15" t="s">
+        <v>539</v>
+      </c>
+      <c r="H70" s="15" t="s">
+        <v>540</v>
+      </c>
+      <c r="I70" s="15" t="s">
         <v>541</v>
-      </c>
-      <c r="H70" s="15" t="s">
-        <v>544</v>
-      </c>
-      <c r="I70" s="15" t="s">
-        <v>545</v>
       </c>
       <c r="J70" s="16" t="s">
         <v>83</v>
@@ -6905,7 +6920,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="300" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="11">
         <v>64</v>
       </c>
@@ -6922,16 +6937,16 @@
         <v>127</v>
       </c>
       <c r="F71" s="14">
-        <v>45205</v>
+        <v>45225</v>
       </c>
       <c r="G71" s="15" t="s">
-        <v>566</v>
+        <v>573</v>
       </c>
       <c r="H71" s="15" t="s">
+        <v>574</v>
+      </c>
+      <c r="I71" s="15" t="s">
         <v>575</v>
-      </c>
-      <c r="I71" s="15" t="s">
-        <v>576</v>
       </c>
       <c r="J71" s="16" t="s">
         <v>83</v>
@@ -6981,13 +6996,13 @@
         <v>45198</v>
       </c>
       <c r="G72" s="15" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="H72" s="15" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="I72" s="15" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="J72" s="16" t="s">
         <v>83</v>
@@ -7037,13 +7052,13 @@
         <v>45198</v>
       </c>
       <c r="G73" s="15" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="H73" s="15" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="I73" s="15" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="J73" s="16" t="s">
         <v>83</v>
@@ -7093,13 +7108,13 @@
         <v>45198</v>
       </c>
       <c r="G74" s="15" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="H74" s="15" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="I74" s="15" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="J74" s="16" t="s">
         <v>83</v>
@@ -7149,13 +7164,13 @@
         <v>45198</v>
       </c>
       <c r="G75" s="15" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="H75" s="15" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="I75" s="15" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="J75" s="16" t="s">
         <v>83</v>
@@ -7205,13 +7220,13 @@
         <v>45198</v>
       </c>
       <c r="G76" s="15" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="H76" s="15" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="I76" s="15" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="J76" s="16" t="s">
         <v>83</v>
@@ -7261,13 +7276,13 @@
         <v>45198</v>
       </c>
       <c r="G77" s="15" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="H77" s="15" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="I77" s="15" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="J77" s="16" t="s">
         <v>83</v>
@@ -7317,13 +7332,13 @@
         <v>45198</v>
       </c>
       <c r="G78" s="15" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="H78" s="15" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="I78" s="15" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="J78" s="16" t="s">
         <v>83</v>
@@ -7373,13 +7388,13 @@
         <v>45198</v>
       </c>
       <c r="G79" s="15" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="H79" s="15" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="I79" s="15" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="J79" s="16" t="s">
         <v>83</v>
@@ -7429,13 +7444,13 @@
         <v>45198</v>
       </c>
       <c r="G80" s="15" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="H80" s="15" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="I80" s="15" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="J80" s="16" t="s">
         <v>83</v>
@@ -7485,13 +7500,13 @@
         <v>45198</v>
       </c>
       <c r="G81" s="15" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="H81" s="15" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="I81" s="15" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="J81" s="16" t="s">
         <v>83</v>
@@ -10275,13 +10290,13 @@
         <v>45198</v>
       </c>
       <c r="G160" s="15" t="s">
+        <v>535</v>
+      </c>
+      <c r="H160" s="15" t="s">
+        <v>536</v>
+      </c>
+      <c r="I160" s="15" t="s">
         <v>537</v>
-      </c>
-      <c r="H160" s="15" t="s">
-        <v>538</v>
-      </c>
-      <c r="I160" s="15" t="s">
-        <v>539</v>
       </c>
       <c r="J160" s="16" t="s">
         <v>83</v>
@@ -10294,7 +10309,7 @@
         <v>83</v>
       </c>
       <c r="N160" s="16" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="O160" s="16" t="s">
         <v>83</v>
@@ -10527,7 +10542,7 @@
       <c r="Q164" s="16"/>
       <c r="R164" s="17"/>
       <c r="S164" s="18" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="T164" s="27" t="s">
         <v>430</v>
@@ -10637,7 +10652,7 @@
       <c r="Q166" s="16"/>
       <c r="R166" s="17"/>
       <c r="S166" s="18" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="T166" s="27" t="s">
         <v>430</v>
@@ -10693,7 +10708,7 @@
       <c r="Q167" s="16"/>
       <c r="R167" s="17"/>
       <c r="S167" s="18" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="T167" s="27" t="s">
         <v>430</v>
@@ -10749,7 +10764,7 @@
       <c r="Q168" s="16"/>
       <c r="R168" s="17"/>
       <c r="S168" s="18" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="T168" s="27" t="s">
         <v>430</v>
@@ -10805,7 +10820,7 @@
       <c r="Q169" s="16"/>
       <c r="R169" s="17"/>
       <c r="S169" s="18" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="T169" s="27" t="s">
         <v>430</v>
@@ -10915,7 +10930,7 @@
       <c r="Q171" s="16"/>
       <c r="R171" s="17"/>
       <c r="S171" s="18" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="T171" s="27" t="s">
         <v>430</v>
@@ -10971,7 +10986,7 @@
       <c r="Q172" s="16"/>
       <c r="R172" s="17"/>
       <c r="S172" s="18" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="T172" s="27" t="s">
         <v>430</v>
@@ -11027,7 +11042,7 @@
       <c r="Q173" s="16"/>
       <c r="R173" s="17"/>
       <c r="S173" s="18" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="T173" s="27" t="s">
         <v>430</v>
@@ -11083,7 +11098,7 @@
       <c r="Q174" s="16"/>
       <c r="R174" s="17"/>
       <c r="S174" s="18" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="T174" s="27" t="s">
         <v>430</v>
@@ -11139,7 +11154,7 @@
       <c r="Q175" s="16"/>
       <c r="R175" s="17"/>
       <c r="S175" s="18" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="T175" s="27" t="s">
         <v>430</v>
@@ -11195,7 +11210,7 @@
       <c r="Q176" s="16"/>
       <c r="R176" s="17"/>
       <c r="S176" s="18" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="T176" s="27" t="s">
         <v>430</v>
@@ -25468,17 +25483,8 @@
   <autoFilter ref="A9:T198" xr:uid="{00000000-0001-0000-0100-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="6"/>
-        <filter val="64"/>
-        <filter val="7"/>
-        <filter val="8"/>
-        <filter val="9"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="LDO"/>
-        <filter val="RSA"/>
+        <filter val="32"/>
+        <filter val="40"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -27721,6 +27727,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -27951,41 +27977,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB221413-913B-41FE-97D3-5428BD0403A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28008,9 +28003,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB221413-913B-41FE-97D3-5428BD0403A1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Accreditamento LDO, RSA v.2.2.1
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
+++ b/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gzamparo\Documents\FSE 2.0\it-fse-accreditamento\GATEWAY\S1#111MEDARCHIVER\MEDARCHIVER\MEDARCHIVER_FSE2.0\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE95ECDD-96B5-4616-87BA-C461D2A860B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E293FC-FA56-43D7-8F0D-275FF3754A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="584">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -2138,9 +2138,6 @@
     <t>Per eseguire i test sono state modificate le codifiche in quanto non è possibile proseguire se non è stato inserito un referto</t>
   </si>
   <si>
-    <t>Per eseguire i test sono state modificate le codifiche in quanto non è possibile proseguire se non è stato inserito un quesito diagnostico</t>
-  </si>
-  <si>
     <t>Per eseguire i test sono state modificate le codifiche in quanto non è possibile proseguire se non è stato inserito il dato</t>
   </si>
   <si>
@@ -2289,6 +2286,15 @@
   </si>
   <si>
     <t>3d7aac25df1cbfe4</t>
+  </si>
+  <si>
+    <t>Per eseguire il test sono stati disattivati i controlli applicativi normalmente presenti (normalmente non è possibile non completare la sezione decorso) per cui se il CDA2 non dovesse contenere il dato, si tratta di un problema tecnico, il problema viene segnalato all'amministratore di sistema che provvede alla correzione; una volta risolto l'utente (compilatore) dispone di una lista dei documenti da rifirmare.</t>
+  </si>
+  <si>
+    <t>Trattandosi di un errore che non può essere gestito dall'utente (compilatore) poichè l'applicativo non permette di lasciare il campo vuoto, l'applicazione visualizza un messaggio di errore di validazione e l'errore verrà notificato all'amministratore di sistema per la sua gestione. Per effettuare nuovamente l'invio dopo la correzione dell'errore, l'utente dispone di una lista di documenti da riprocessare manualmente. L'errore restituito dalla chiamata di validazione può o meno essere mostrato all'utente o sostituito con un errore parlante a seconda della configurazione richiesta dal cliente.</t>
+  </si>
+  <si>
+    <t>Per eseguire il test sono stati disattivati i controlli applicativi normalmente presenti (normalmente non è possibile non completare la sezione quesito diagnostico) per cui se il CDA2 non dovesse contenere il dato, si tratta di un problema tecnico, il problema viene segnalato all'amministratore di sistema che provvede alla correzione; una volta risolto l'utente (compilatore) dispone di una lista dei documenti da rifirmare.</t>
   </si>
 </sst>
 </file>
@@ -4377,10 +4383,10 @@
   <dimension ref="A1:T993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="J77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I39" sqref="I39"/>
+      <selection pane="bottomRight" activeCell="K169" sqref="K169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4828,13 +4834,13 @@
         <v>45205</v>
       </c>
       <c r="G15" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="H15" s="15" t="s">
         <v>562</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="I15" s="15" t="s">
         <v>563</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>564</v>
       </c>
       <c r="J15" s="16" t="s">
         <v>83</v>
@@ -4872,13 +4878,13 @@
         <v>45205</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H16" s="15" t="s">
+        <v>564</v>
+      </c>
+      <c r="I16" s="15" t="s">
         <v>565</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>566</v>
       </c>
       <c r="J16" s="16" t="s">
         <v>83</v>
@@ -4916,13 +4922,13 @@
         <v>45205</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H17" s="15" t="s">
+        <v>566</v>
+      </c>
+      <c r="I17" s="15" t="s">
         <v>567</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>568</v>
       </c>
       <c r="J17" s="16" t="s">
         <v>83</v>
@@ -4960,13 +4966,13 @@
         <v>45205</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H18" s="15" t="s">
+        <v>568</v>
+      </c>
+      <c r="I18" s="15" t="s">
         <v>569</v>
-      </c>
-      <c r="I18" s="15" t="s">
-        <v>570</v>
       </c>
       <c r="J18" s="16" t="s">
         <v>83</v>
@@ -5004,7 +5010,7 @@
         <v>45205</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H19" s="15" t="s">
         <v>433</v>
@@ -5602,10 +5608,10 @@
         <v>45225</v>
       </c>
       <c r="G36" s="15" t="s">
+        <v>575</v>
+      </c>
+      <c r="H36" s="15" t="s">
         <v>576</v>
-      </c>
-      <c r="H36" s="15" t="s">
-        <v>577</v>
       </c>
       <c r="I36" s="15" t="s">
         <v>434</v>
@@ -5714,7 +5720,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11">
         <v>32</v>
       </c>
@@ -5734,10 +5740,10 @@
         <v>45225</v>
       </c>
       <c r="G39" s="15" t="s">
+        <v>579</v>
+      </c>
+      <c r="H39" s="15" t="s">
         <v>580</v>
-      </c>
-      <c r="H39" s="15" t="s">
-        <v>581</v>
       </c>
       <c r="I39" s="15" t="s">
         <v>434</v>
@@ -5768,7 +5774,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11">
         <v>33</v>
       </c>
@@ -5802,7 +5808,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11">
         <v>34</v>
       </c>
@@ -5836,7 +5842,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11">
         <v>35</v>
       </c>
@@ -5870,7 +5876,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11">
         <v>36</v>
       </c>
@@ -5904,7 +5910,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11">
         <v>37</v>
       </c>
@@ -5924,10 +5930,10 @@
         <v>45225</v>
       </c>
       <c r="G44" s="15" t="s">
+        <v>570</v>
+      </c>
+      <c r="H44" s="15" t="s">
         <v>571</v>
-      </c>
-      <c r="H44" s="15" t="s">
-        <v>572</v>
       </c>
       <c r="I44" s="15" t="s">
         <v>434</v>
@@ -5958,7 +5964,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11">
         <v>38</v>
       </c>
@@ -5992,7 +5998,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="11">
         <v>39</v>
       </c>
@@ -6026,7 +6032,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="180" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="11">
         <v>40</v>
       </c>
@@ -6046,10 +6052,10 @@
         <v>45225</v>
       </c>
       <c r="G47" s="15" t="s">
+        <v>577</v>
+      </c>
+      <c r="H47" s="15" t="s">
         <v>578</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>579</v>
       </c>
       <c r="I47" s="15" t="s">
         <v>434</v>
@@ -6080,7 +6086,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11">
         <v>41</v>
       </c>
@@ -6114,7 +6120,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11">
         <v>42</v>
       </c>
@@ -6148,7 +6154,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="11">
         <v>43</v>
       </c>
@@ -6182,7 +6188,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="11">
         <v>44</v>
       </c>
@@ -6218,7 +6224,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" ht="210.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="11">
         <v>45</v>
       </c>
@@ -6264,7 +6270,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="11">
         <v>46</v>
       </c>
@@ -6300,7 +6306,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="11">
         <v>47</v>
       </c>
@@ -6336,7 +6342,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" ht="210.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11">
         <v>48</v>
       </c>
@@ -6382,7 +6388,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11">
         <v>49</v>
       </c>
@@ -6418,7 +6424,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="11">
         <v>50</v>
       </c>
@@ -6454,7 +6460,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="11">
         <v>51</v>
       </c>
@@ -6490,7 +6496,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="11">
         <v>52</v>
       </c>
@@ -6524,7 +6530,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="11">
         <v>53</v>
       </c>
@@ -6558,7 +6564,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="11">
         <v>54</v>
       </c>
@@ -6592,7 +6598,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="11">
         <v>55</v>
       </c>
@@ -6626,7 +6632,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="11">
         <v>56</v>
       </c>
@@ -6660,7 +6666,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="11">
         <v>57</v>
       </c>
@@ -6694,7 +6700,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="11">
         <v>58</v>
       </c>
@@ -6728,7 +6734,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="11">
         <v>59</v>
       </c>
@@ -6762,7 +6768,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="11">
         <v>60</v>
       </c>
@@ -6796,7 +6802,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="11">
         <v>61</v>
       </c>
@@ -6830,7 +6836,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="11">
         <v>62</v>
       </c>
@@ -6864,7 +6870,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="11">
         <v>63</v>
       </c>
@@ -6884,13 +6890,13 @@
         <v>45198</v>
       </c>
       <c r="G70" s="15" t="s">
+        <v>538</v>
+      </c>
+      <c r="H70" s="15" t="s">
         <v>539</v>
       </c>
-      <c r="H70" s="15" t="s">
+      <c r="I70" s="15" t="s">
         <v>540</v>
-      </c>
-      <c r="I70" s="15" t="s">
-        <v>541</v>
       </c>
       <c r="J70" s="16" t="s">
         <v>83</v>
@@ -6920,7 +6926,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="11">
         <v>64</v>
       </c>
@@ -6940,13 +6946,13 @@
         <v>45225</v>
       </c>
       <c r="G71" s="15" t="s">
+        <v>572</v>
+      </c>
+      <c r="H71" s="15" t="s">
         <v>573</v>
       </c>
-      <c r="H71" s="15" t="s">
+      <c r="I71" s="15" t="s">
         <v>574</v>
-      </c>
-      <c r="I71" s="15" t="s">
-        <v>575</v>
       </c>
       <c r="J71" s="16" t="s">
         <v>83</v>
@@ -6976,7 +6982,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="11">
         <v>65</v>
       </c>
@@ -6996,13 +7002,13 @@
         <v>45198</v>
       </c>
       <c r="G72" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H72" s="15" t="s">
+        <v>541</v>
+      </c>
+      <c r="I72" s="15" t="s">
         <v>542</v>
-      </c>
-      <c r="I72" s="15" t="s">
-        <v>543</v>
       </c>
       <c r="J72" s="16" t="s">
         <v>83</v>
@@ -7032,7 +7038,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="11">
         <v>66</v>
       </c>
@@ -7052,13 +7058,13 @@
         <v>45198</v>
       </c>
       <c r="G73" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H73" s="15" t="s">
+        <v>543</v>
+      </c>
+      <c r="I73" s="15" t="s">
         <v>544</v>
-      </c>
-      <c r="I73" s="15" t="s">
-        <v>545</v>
       </c>
       <c r="J73" s="16" t="s">
         <v>83</v>
@@ -7088,7 +7094,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="11">
         <v>67</v>
       </c>
@@ -7108,13 +7114,13 @@
         <v>45198</v>
       </c>
       <c r="G74" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H74" s="15" t="s">
+        <v>545</v>
+      </c>
+      <c r="I74" s="15" t="s">
         <v>546</v>
-      </c>
-      <c r="I74" s="15" t="s">
-        <v>547</v>
       </c>
       <c r="J74" s="16" t="s">
         <v>83</v>
@@ -7144,7 +7150,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="11">
         <v>68</v>
       </c>
@@ -7164,13 +7170,13 @@
         <v>45198</v>
       </c>
       <c r="G75" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H75" s="15" t="s">
+        <v>547</v>
+      </c>
+      <c r="I75" s="15" t="s">
         <v>548</v>
-      </c>
-      <c r="I75" s="15" t="s">
-        <v>549</v>
       </c>
       <c r="J75" s="16" t="s">
         <v>83</v>
@@ -7200,7 +7206,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="11">
         <v>69</v>
       </c>
@@ -7220,13 +7226,13 @@
         <v>45198</v>
       </c>
       <c r="G76" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H76" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="I76" s="15" t="s">
         <v>550</v>
-      </c>
-      <c r="I76" s="15" t="s">
-        <v>551</v>
       </c>
       <c r="J76" s="16" t="s">
         <v>83</v>
@@ -7256,7 +7262,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" ht="345.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="11">
         <v>70</v>
       </c>
@@ -7276,13 +7282,13 @@
         <v>45198</v>
       </c>
       <c r="G77" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H77" s="15" t="s">
+        <v>551</v>
+      </c>
+      <c r="I77" s="15" t="s">
         <v>552</v>
-      </c>
-      <c r="I77" s="15" t="s">
-        <v>553</v>
       </c>
       <c r="J77" s="16" t="s">
         <v>83</v>
@@ -7301,12 +7307,12 @@
         <v>83</v>
       </c>
       <c r="P77" s="16" t="s">
-        <v>466</v>
+        <v>582</v>
       </c>
       <c r="Q77" s="16"/>
       <c r="R77" s="17"/>
       <c r="S77" s="18" t="s">
-        <v>441</v>
+        <v>581</v>
       </c>
       <c r="T77" s="27" t="s">
         <v>430</v>
@@ -7332,13 +7338,13 @@
         <v>45198</v>
       </c>
       <c r="G78" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H78" s="15" t="s">
+        <v>553</v>
+      </c>
+      <c r="I78" s="15" t="s">
         <v>554</v>
-      </c>
-      <c r="I78" s="15" t="s">
-        <v>555</v>
       </c>
       <c r="J78" s="16" t="s">
         <v>83</v>
@@ -7388,13 +7394,13 @@
         <v>45198</v>
       </c>
       <c r="G79" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H79" s="15" t="s">
+        <v>555</v>
+      </c>
+      <c r="I79" s="15" t="s">
         <v>556</v>
-      </c>
-      <c r="I79" s="15" t="s">
-        <v>557</v>
       </c>
       <c r="J79" s="16" t="s">
         <v>83</v>
@@ -7444,13 +7450,13 @@
         <v>45198</v>
       </c>
       <c r="G80" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H80" s="15" t="s">
+        <v>557</v>
+      </c>
+      <c r="I80" s="15" t="s">
         <v>558</v>
-      </c>
-      <c r="I80" s="15" t="s">
-        <v>559</v>
       </c>
       <c r="J80" s="16" t="s">
         <v>83</v>
@@ -7500,13 +7506,13 @@
         <v>45198</v>
       </c>
       <c r="G81" s="15" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H81" s="15" t="s">
+        <v>559</v>
+      </c>
+      <c r="I81" s="15" t="s">
         <v>560</v>
-      </c>
-      <c r="I81" s="15" t="s">
-        <v>561</v>
       </c>
       <c r="J81" s="16" t="s">
         <v>83</v>
@@ -10290,13 +10296,13 @@
         <v>45198</v>
       </c>
       <c r="G160" s="15" t="s">
+        <v>534</v>
+      </c>
+      <c r="H160" s="15" t="s">
         <v>535</v>
       </c>
-      <c r="H160" s="15" t="s">
+      <c r="I160" s="15" t="s">
         <v>536</v>
-      </c>
-      <c r="I160" s="15" t="s">
-        <v>537</v>
       </c>
       <c r="J160" s="16" t="s">
         <v>83</v>
@@ -10309,7 +10315,7 @@
         <v>83</v>
       </c>
       <c r="N160" s="16" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="O160" s="16" t="s">
         <v>83</v>
@@ -10770,7 +10776,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:20" ht="345" x14ac:dyDescent="0.25">
       <c r="A169" s="11">
         <v>162</v>
       </c>
@@ -10815,12 +10821,12 @@
         <v>83</v>
       </c>
       <c r="P169" s="16" t="s">
-        <v>466</v>
+        <v>582</v>
       </c>
       <c r="Q169" s="16"/>
       <c r="R169" s="17"/>
       <c r="S169" s="18" t="s">
-        <v>531</v>
+        <v>583</v>
       </c>
       <c r="T169" s="27" t="s">
         <v>430</v>
@@ -10930,7 +10936,7 @@
       <c r="Q171" s="16"/>
       <c r="R171" s="17"/>
       <c r="S171" s="18" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="T171" s="27" t="s">
         <v>430</v>
@@ -10986,7 +10992,7 @@
       <c r="Q172" s="16"/>
       <c r="R172" s="17"/>
       <c r="S172" s="18" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="T172" s="27" t="s">
         <v>430</v>
@@ -11042,7 +11048,7 @@
       <c r="Q173" s="16"/>
       <c r="R173" s="17"/>
       <c r="S173" s="18" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="T173" s="27" t="s">
         <v>430</v>
@@ -11098,7 +11104,7 @@
       <c r="Q174" s="16"/>
       <c r="R174" s="17"/>
       <c r="S174" s="18" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="T174" s="27" t="s">
         <v>430</v>
@@ -11154,7 +11160,7 @@
       <c r="Q175" s="16"/>
       <c r="R175" s="17"/>
       <c r="S175" s="18" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="T175" s="27" t="s">
         <v>430</v>
@@ -11210,7 +11216,7 @@
       <c r="Q176" s="16"/>
       <c r="R176" s="17"/>
       <c r="S176" s="18" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="T176" s="27" t="s">
         <v>430</v>
@@ -25483,8 +25489,8 @@
   <autoFilter ref="A9:T198" xr:uid="{00000000-0001-0000-0100-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="32"/>
-        <filter val="40"/>
+        <filter val="70"/>
+        <filter val="162"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -27727,26 +27733,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -27977,10 +27963,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB221413-913B-41FE-97D3-5428BD0403A1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28003,20 +28020,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB221413-913B-41FE-97D3-5428BD0403A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Accreditamento VPS, RSA, LDO v.1.1
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
+++ b/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gzamparo\Documents\FSE 2.0\it-fse-accreditamento\GATEWAY\S1#111MEDARCHIVER\MEDARCHIVER\MEDARCHIVER_FSE2.0\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02512D3-BCD6-4ECB-9D47-FACEACEE038F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB83E3B-2BA5-43F2-9C62-49B1B7885741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -22,8 +22,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$198</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mhXj7RfszpgZKzxg8oD/Tet7lb94w=="/>
     </ext>
@@ -62,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1725" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1725" uniqueCount="677">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -2024,30 +2035,6 @@
     <t>2024-02-05T10:26:33Z</t>
   </si>
   <si>
-    <t>6959c4c61ccbaf77</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.901a974f5334d085fad6c1d59a37bdb959baf7f480569d531dcdabc96e298dc6.982ca62d83^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>e68aa98a61a52fec</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.abe0d581c3345ebacde561969b7d6923b33947d9c04b0843343fc2f304b2fcec.1419197252^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>6321d5334d965dd5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.112f695949^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>81b33b3393cbd444</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.ffee57db6b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>1fe878c76d035327</t>
   </si>
   <si>
@@ -2312,12 +2299,6 @@
     <t>f05ab6a93b35903e</t>
   </si>
   <si>
-    <t>787aac772838ac52</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.5637c76296^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>90f9c086fd26bc6c</t>
   </si>
   <si>
@@ -2531,15 +2512,6 @@
     <t>1e710e7ad4cfe2f3</t>
   </si>
   <si>
-    <t>2024-02-05T15:13:42Z</t>
-  </si>
-  <si>
-    <t>91698d44adec9344</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.a9cade2f8c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2024-02-05T15:15:28Z</t>
   </si>
   <si>
@@ -2562,6 +2534,57 @@
   </si>
   <si>
     <t>7ba9006f241ad450</t>
+  </si>
+  <si>
+    <t>2024-02-07T09:36:58Z</t>
+  </si>
+  <si>
+    <t>28ef5a0883564fa8</t>
+  </si>
+  <si>
+    <t>2024-02-07T12:41:47Z</t>
+  </si>
+  <si>
+    <t>45ee3f384cbbd1e1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.641ee0751dad17117e6d991886171890720f9552821beaa685cd6afaba60610f.d3e2e6e48d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-02-07T15:50:24Z</t>
+  </si>
+  <si>
+    <t>77af659f65ae706b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.641ee0751dad17117e6d991886171890720f9552821beaa685cd6afaba60610f.9936634cd2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-02-08T12:02:15Z</t>
+  </si>
+  <si>
+    <t>74aeaf03be14ac04</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.641ee0751dad17117e6d991886171890720f9552821beaa685cd6afaba60610f.50dce8c006^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-02-08T12:12:20Z</t>
+  </si>
+  <si>
+    <t>8d9bd613b992b3c4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.641ee0751dad17117e6d991886171890720f9552821beaa685cd6afaba60610f.04e34a52df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-02-08T12:15:21Z</t>
+  </si>
+  <si>
+    <t>867f398fb2b840ee</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.bad2ea390c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4650,10 +4673,10 @@
   <dimension ref="A1:T993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="D160" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J55" sqref="J55"/>
+      <selection pane="bottomRight" activeCell="F160" sqref="F160:I160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5101,13 +5124,13 @@
         <v>45327</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>625</v>
+        <v>615</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>624</v>
+        <v>614</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>623</v>
+        <v>613</v>
       </c>
       <c r="J15" s="16" t="s">
         <v>83</v>
@@ -5145,13 +5168,13 @@
         <v>45327</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>628</v>
+        <v>618</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>632</v>
+        <v>622</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>631</v>
+        <v>621</v>
       </c>
       <c r="J16" s="16" t="s">
         <v>83</v>
@@ -5189,13 +5212,13 @@
         <v>45327</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>628</v>
+        <v>618</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>630</v>
+        <v>620</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>629</v>
+        <v>619</v>
       </c>
       <c r="J17" s="16" t="s">
         <v>83</v>
@@ -5233,13 +5256,13 @@
         <v>45327</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>628</v>
+        <v>618</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>627</v>
+        <v>617</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>626</v>
+        <v>616</v>
       </c>
       <c r="J18" s="16" t="s">
         <v>83</v>
@@ -5702,16 +5725,16 @@
         <v>75</v>
       </c>
       <c r="F31" s="14">
-        <v>45327</v>
+        <v>45329</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>492</v>
+        <v>662</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>493</v>
+        <v>663</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>494</v>
+        <v>664</v>
       </c>
       <c r="J31" s="16" t="s">
         <v>83</v>
@@ -5746,16 +5769,16 @@
         <v>77</v>
       </c>
       <c r="F32" s="14">
-        <v>45327</v>
+        <v>45329</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>492</v>
+        <v>665</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>495</v>
+        <v>666</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>496</v>
+        <v>667</v>
       </c>
       <c r="J32" s="16" t="s">
         <v>83</v>
@@ -5790,16 +5813,16 @@
         <v>79</v>
       </c>
       <c r="F33" s="14">
-        <v>45327</v>
+        <v>45330</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>492</v>
+        <v>668</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>497</v>
+        <v>669</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>498</v>
+        <v>670</v>
       </c>
       <c r="J33" s="16" t="s">
         <v>83</v>
@@ -5834,16 +5857,16 @@
         <v>81</v>
       </c>
       <c r="F34" s="14">
-        <v>45327</v>
+        <v>45330</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>492</v>
+        <v>671</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>499</v>
+        <v>672</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>500</v>
+        <v>673</v>
       </c>
       <c r="J34" s="16" t="s">
         <v>83</v>
@@ -5915,10 +5938,10 @@
         <v>45327</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>665</v>
+        <v>652</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>666</v>
+        <v>653</v>
       </c>
       <c r="I36" s="15" t="s">
         <v>434</v>
@@ -6044,16 +6067,16 @@
         <v>431</v>
       </c>
       <c r="F39" s="14">
-        <v>45327</v>
+        <v>45329</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="I39" s="15" t="s">
-        <v>664</v>
+        <v>434</v>
       </c>
       <c r="J39" s="16" t="s">
         <v>83</v>
@@ -6169,10 +6192,10 @@
         <v>45327</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>660</v>
+        <v>650</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>661</v>
+        <v>651</v>
       </c>
       <c r="I42" s="15" t="s">
         <v>434</v>
@@ -6257,10 +6280,10 @@
         <v>45327</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>672</v>
+        <v>659</v>
       </c>
       <c r="I44" s="15" t="s">
         <v>434</v>
@@ -6379,10 +6402,10 @@
         <v>45327</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>669</v>
+        <v>656</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>670</v>
+        <v>657</v>
       </c>
       <c r="I47" s="15" t="s">
         <v>434</v>
@@ -6501,10 +6524,10 @@
         <v>45327</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>667</v>
+        <v>654</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>668</v>
+        <v>655</v>
       </c>
       <c r="I50" s="15" t="s">
         <v>434</v>
@@ -7247,13 +7270,13 @@
         <v>45327</v>
       </c>
       <c r="G70" s="15" t="s">
-        <v>628</v>
+        <v>618</v>
       </c>
       <c r="H70" s="15" t="s">
-        <v>634</v>
+        <v>624</v>
       </c>
       <c r="I70" s="15" t="s">
-        <v>633</v>
+        <v>623</v>
       </c>
       <c r="J70" s="16" t="s">
         <v>83</v>
@@ -7303,13 +7326,13 @@
         <v>45327</v>
       </c>
       <c r="G71" s="15" t="s">
-        <v>657</v>
+        <v>647</v>
       </c>
       <c r="H71" s="15" t="s">
-        <v>658</v>
+        <v>648</v>
       </c>
       <c r="I71" s="15" t="s">
-        <v>659</v>
+        <v>649</v>
       </c>
       <c r="J71" s="16" t="s">
         <v>83</v>
@@ -7359,13 +7382,13 @@
         <v>45327</v>
       </c>
       <c r="G72" s="15" t="s">
-        <v>628</v>
+        <v>618</v>
       </c>
       <c r="H72" s="15" t="s">
-        <v>635</v>
+        <v>625</v>
       </c>
       <c r="I72" s="15" t="s">
-        <v>636</v>
+        <v>626</v>
       </c>
       <c r="J72" s="16" t="s">
         <v>83</v>
@@ -7415,13 +7438,13 @@
         <v>45327</v>
       </c>
       <c r="G73" s="15" t="s">
+        <v>618</v>
+      </c>
+      <c r="H73" s="15" t="s">
+        <v>627</v>
+      </c>
+      <c r="I73" s="15" t="s">
         <v>628</v>
-      </c>
-      <c r="H73" s="15" t="s">
-        <v>637</v>
-      </c>
-      <c r="I73" s="15" t="s">
-        <v>638</v>
       </c>
       <c r="J73" s="16" t="s">
         <v>83</v>
@@ -7471,13 +7494,13 @@
         <v>45327</v>
       </c>
       <c r="G74" s="15" t="s">
-        <v>628</v>
+        <v>618</v>
       </c>
       <c r="H74" s="15" t="s">
-        <v>639</v>
+        <v>629</v>
       </c>
       <c r="I74" s="15" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="J74" s="16" t="s">
         <v>83</v>
@@ -7527,13 +7550,13 @@
         <v>45327</v>
       </c>
       <c r="G75" s="15" t="s">
-        <v>625</v>
+        <v>615</v>
       </c>
       <c r="H75" s="15" t="s">
-        <v>654</v>
+        <v>644</v>
       </c>
       <c r="I75" s="15" t="s">
-        <v>653</v>
+        <v>643</v>
       </c>
       <c r="J75" s="16" t="s">
         <v>83</v>
@@ -7583,13 +7606,13 @@
         <v>45327</v>
       </c>
       <c r="G76" s="15" t="s">
-        <v>625</v>
+        <v>615</v>
       </c>
       <c r="H76" s="15" t="s">
-        <v>652</v>
+        <v>642</v>
       </c>
       <c r="I76" s="15" t="s">
-        <v>651</v>
+        <v>641</v>
       </c>
       <c r="J76" s="16" t="s">
         <v>83</v>
@@ -7602,7 +7625,7 @@
         <v>83</v>
       </c>
       <c r="N76" s="16" t="s">
-        <v>655</v>
+        <v>645</v>
       </c>
       <c r="O76" s="16" t="s">
         <v>83</v>
@@ -7639,13 +7662,13 @@
         <v>45327</v>
       </c>
       <c r="G77" s="15" t="s">
-        <v>625</v>
+        <v>615</v>
       </c>
       <c r="H77" s="15" t="s">
-        <v>650</v>
+        <v>640</v>
       </c>
       <c r="I77" s="15" t="s">
-        <v>649</v>
+        <v>639</v>
       </c>
       <c r="J77" s="16" t="s">
         <v>83</v>
@@ -7695,13 +7718,13 @@
         <v>45327</v>
       </c>
       <c r="G78" s="15" t="s">
-        <v>625</v>
+        <v>615</v>
       </c>
       <c r="H78" s="15" t="s">
-        <v>648</v>
+        <v>638</v>
       </c>
       <c r="I78" s="15" t="s">
-        <v>647</v>
+        <v>637</v>
       </c>
       <c r="J78" s="16" t="s">
         <v>83</v>
@@ -7714,7 +7737,7 @@
         <v>83</v>
       </c>
       <c r="N78" s="16" t="s">
-        <v>656</v>
+        <v>646</v>
       </c>
       <c r="O78" s="16" t="s">
         <v>83</v>
@@ -7751,13 +7774,13 @@
         <v>45327</v>
       </c>
       <c r="G79" s="15" t="s">
-        <v>625</v>
+        <v>615</v>
       </c>
       <c r="H79" s="15" t="s">
-        <v>646</v>
+        <v>636</v>
       </c>
       <c r="I79" s="15" t="s">
-        <v>645</v>
+        <v>635</v>
       </c>
       <c r="J79" s="16" t="s">
         <v>83</v>
@@ -7807,13 +7830,13 @@
         <v>45327</v>
       </c>
       <c r="G80" s="15" t="s">
-        <v>625</v>
+        <v>615</v>
       </c>
       <c r="H80" s="15" t="s">
-        <v>644</v>
+        <v>634</v>
       </c>
       <c r="I80" s="15" t="s">
-        <v>643</v>
+        <v>633</v>
       </c>
       <c r="J80" s="16" t="s">
         <v>83</v>
@@ -7863,13 +7886,13 @@
         <v>45327</v>
       </c>
       <c r="G81" s="15" t="s">
-        <v>625</v>
+        <v>615</v>
       </c>
       <c r="H81" s="15" t="s">
-        <v>642</v>
+        <v>632</v>
       </c>
       <c r="I81" s="15" t="s">
-        <v>641</v>
+        <v>631</v>
       </c>
       <c r="J81" s="16" t="s">
         <v>83</v>
@@ -9520,10 +9543,10 @@
         <v>492</v>
       </c>
       <c r="H129" s="15" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="I129" s="15" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="J129" s="16" t="s">
         <v>83</v>
@@ -9574,10 +9597,10 @@
         <v>492</v>
       </c>
       <c r="H130" s="15" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="I130" s="15" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="J130" s="16" t="s">
         <v>83</v>
@@ -9630,10 +9653,10 @@
         <v>492</v>
       </c>
       <c r="H131" s="15" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="I131" s="15" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="J131" s="16" t="s">
         <v>83</v>
@@ -9686,10 +9709,10 @@
         <v>492</v>
       </c>
       <c r="H132" s="15" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="I132" s="15" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="J132" s="16" t="s">
         <v>83</v>
@@ -9702,7 +9725,7 @@
         <v>83</v>
       </c>
       <c r="N132" s="16" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="O132" s="16" t="s">
         <v>83</v>
@@ -9713,7 +9736,7 @@
       <c r="Q132" s="16"/>
       <c r="R132" s="17"/>
       <c r="S132" s="18" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="T132" s="16" t="s">
         <v>430</v>
@@ -9742,10 +9765,10 @@
         <v>492</v>
       </c>
       <c r="H133" s="15" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="I133" s="15" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="J133" s="16" t="s">
         <v>83</v>
@@ -9758,7 +9781,7 @@
         <v>83</v>
       </c>
       <c r="N133" s="16" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="O133" s="16" t="s">
         <v>83</v>
@@ -9769,7 +9792,7 @@
       <c r="Q133" s="16"/>
       <c r="R133" s="17"/>
       <c r="S133" s="18" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="T133" s="16" t="s">
         <v>430</v>
@@ -9798,10 +9821,10 @@
         <v>492</v>
       </c>
       <c r="H134" s="15" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="I134" s="15" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="J134" s="16" t="s">
         <v>83</v>
@@ -9814,7 +9837,7 @@
         <v>83</v>
       </c>
       <c r="N134" s="16" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="O134" s="16" t="s">
         <v>83</v>
@@ -9825,7 +9848,7 @@
       <c r="Q134" s="16"/>
       <c r="R134" s="17"/>
       <c r="S134" s="18" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="T134" s="16" t="s">
         <v>430</v>
@@ -9854,10 +9877,10 @@
         <v>492</v>
       </c>
       <c r="H135" s="15" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="I135" s="15" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="J135" s="16" t="s">
         <v>83</v>
@@ -9870,7 +9893,7 @@
         <v>83</v>
       </c>
       <c r="N135" s="16" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="O135" s="16" t="s">
         <v>83</v>
@@ -9881,7 +9904,7 @@
       <c r="Q135" s="16"/>
       <c r="R135" s="17"/>
       <c r="S135" s="18" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="T135" s="16" t="s">
         <v>430</v>
@@ -9910,10 +9933,10 @@
         <v>492</v>
       </c>
       <c r="H136" s="15" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="I136" s="15" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="J136" s="16" t="s">
         <v>83</v>
@@ -9926,7 +9949,7 @@
         <v>83</v>
       </c>
       <c r="N136" s="16" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="O136" s="16" t="s">
         <v>83</v>
@@ -9966,10 +9989,10 @@
         <v>492</v>
       </c>
       <c r="H137" s="15" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="I137" s="15" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="J137" s="16" t="s">
         <v>83</v>
@@ -9982,7 +10005,7 @@
         <v>83</v>
       </c>
       <c r="N137" s="16" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="O137" s="16" t="s">
         <v>83</v>
@@ -9993,7 +10016,7 @@
       <c r="Q137" s="16"/>
       <c r="R137" s="17"/>
       <c r="S137" s="18" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="T137" s="16" t="s">
         <v>430</v>
@@ -10022,10 +10045,10 @@
         <v>492</v>
       </c>
       <c r="H138" s="15" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="I138" s="15" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="J138" s="16" t="s">
         <v>83</v>
@@ -10038,7 +10061,7 @@
         <v>83</v>
       </c>
       <c r="N138" s="16" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="O138" s="16" t="s">
         <v>83</v>
@@ -10076,10 +10099,10 @@
         <v>492</v>
       </c>
       <c r="H139" s="15" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="I139" s="15" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="J139" s="16" t="s">
         <v>83</v>
@@ -10092,7 +10115,7 @@
         <v>83</v>
       </c>
       <c r="N139" s="16" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="O139" s="16" t="s">
         <v>83</v>
@@ -10132,10 +10155,10 @@
         <v>492</v>
       </c>
       <c r="H140" s="15" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="I140" s="15" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="J140" s="16" t="s">
         <v>83</v>
@@ -10148,7 +10171,7 @@
         <v>83</v>
       </c>
       <c r="N140" s="16" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="O140" s="16" t="s">
         <v>83</v>
@@ -10188,10 +10211,10 @@
         <v>492</v>
       </c>
       <c r="H141" s="15" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="I141" s="15" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="J141" s="16" t="s">
         <v>83</v>
@@ -10204,7 +10227,7 @@
         <v>83</v>
       </c>
       <c r="N141" s="16" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="O141" s="16" t="s">
         <v>83</v>
@@ -10215,7 +10238,7 @@
       <c r="Q141" s="16"/>
       <c r="R141" s="17"/>
       <c r="S141" s="18" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="T141" s="16" t="s">
         <v>430</v>
@@ -10244,10 +10267,10 @@
         <v>492</v>
       </c>
       <c r="H142" s="15" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="I142" s="15" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="J142" s="16" t="s">
         <v>83</v>
@@ -10260,7 +10283,7 @@
         <v>83</v>
       </c>
       <c r="N142" s="16" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="O142" s="16" t="s">
         <v>83</v>
@@ -10300,10 +10323,10 @@
         <v>492</v>
       </c>
       <c r="H143" s="15" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="I143" s="15" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="J143" s="16" t="s">
         <v>83</v>
@@ -10316,7 +10339,7 @@
         <v>83</v>
       </c>
       <c r="N143" s="16" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="O143" s="16" t="s">
         <v>83</v>
@@ -10327,7 +10350,7 @@
       <c r="Q143" s="16"/>
       <c r="R143" s="17"/>
       <c r="S143" s="18" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="T143" s="16" t="s">
         <v>430</v>
@@ -10356,10 +10379,10 @@
         <v>492</v>
       </c>
       <c r="H144" s="15" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="I144" s="15" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="J144" s="16" t="s">
         <v>83</v>
@@ -10372,7 +10395,7 @@
         <v>83</v>
       </c>
       <c r="N144" s="16" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="O144" s="16" t="s">
         <v>83</v>
@@ -10383,7 +10406,7 @@
       <c r="Q144" s="16"/>
       <c r="R144" s="17"/>
       <c r="S144" s="18" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="T144" s="16" t="s">
         <v>430</v>
@@ -10412,10 +10435,10 @@
         <v>492</v>
       </c>
       <c r="H145" s="15" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="I145" s="15" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="J145" s="16" t="s">
         <v>83</v>
@@ -10428,7 +10451,7 @@
         <v>83</v>
       </c>
       <c r="N145" s="16" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="O145" s="16" t="s">
         <v>83</v>
@@ -10468,10 +10491,10 @@
         <v>492</v>
       </c>
       <c r="H146" s="15" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="I146" s="15" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="J146" s="16" t="s">
         <v>83</v>
@@ -10484,7 +10507,7 @@
         <v>83</v>
       </c>
       <c r="N146" s="16" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="O146" s="16" t="s">
         <v>83</v>
@@ -10524,10 +10547,10 @@
         <v>492</v>
       </c>
       <c r="H147" s="15" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
       <c r="I147" s="15" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="J147" s="16" t="s">
         <v>83</v>
@@ -10540,7 +10563,7 @@
         <v>83</v>
       </c>
       <c r="N147" s="16" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="O147" s="16" t="s">
         <v>83</v>
@@ -10580,10 +10603,10 @@
         <v>492</v>
       </c>
       <c r="H148" s="15" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="I148" s="15" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
       <c r="J148" s="16" t="s">
         <v>83</v>
@@ -10596,7 +10619,7 @@
         <v>83</v>
       </c>
       <c r="N148" s="16" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="O148" s="16" t="s">
         <v>83</v>
@@ -10636,10 +10659,10 @@
         <v>492</v>
       </c>
       <c r="H149" s="15" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
       <c r="I149" s="15" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
       <c r="J149" s="16" t="s">
         <v>83</v>
@@ -10652,7 +10675,7 @@
         <v>83</v>
       </c>
       <c r="N149" s="16" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="O149" s="16" t="s">
         <v>83</v>
@@ -10692,10 +10715,10 @@
         <v>492</v>
       </c>
       <c r="H150" s="15" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="I150" s="15" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="J150" s="16" t="s">
         <v>83</v>
@@ -10708,7 +10731,7 @@
         <v>83</v>
       </c>
       <c r="N150" s="16" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="O150" s="16" t="s">
         <v>83</v>
@@ -10748,10 +10771,10 @@
         <v>492</v>
       </c>
       <c r="H151" s="15" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="I151" s="15" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="J151" s="16" t="s">
         <v>83</v>
@@ -10764,7 +10787,7 @@
         <v>83</v>
       </c>
       <c r="N151" s="16" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="O151" s="16" t="s">
         <v>83</v>
@@ -10804,10 +10827,10 @@
         <v>492</v>
       </c>
       <c r="H152" s="15" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="I152" s="15" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="J152" s="16" t="s">
         <v>83</v>
@@ -10820,7 +10843,7 @@
         <v>83</v>
       </c>
       <c r="N152" s="16" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="O152" s="16" t="s">
         <v>83</v>
@@ -10860,10 +10883,10 @@
         <v>492</v>
       </c>
       <c r="H153" s="15" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="I153" s="15" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="J153" s="16" t="s">
         <v>83</v>
@@ -10876,7 +10899,7 @@
         <v>83</v>
       </c>
       <c r="N153" s="16" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
       <c r="O153" s="16" t="s">
         <v>83</v>
@@ -10913,13 +10936,13 @@
         <v>45327</v>
       </c>
       <c r="G154" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H154" s="15" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="I154" s="15" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="J154" s="16" t="s">
         <v>83</v>
@@ -10957,13 +10980,13 @@
         <v>45327</v>
       </c>
       <c r="G155" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H155" s="15" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="I155" s="15" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
       <c r="J155" s="16" t="s">
         <v>83</v>
@@ -11001,13 +11024,13 @@
         <v>45327</v>
       </c>
       <c r="G156" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H156" s="15" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="I156" s="15" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="J156" s="16" t="s">
         <v>83</v>
@@ -11045,13 +11068,13 @@
         <v>45327</v>
       </c>
       <c r="G157" s="15" t="s">
+        <v>568</v>
+      </c>
+      <c r="H157" s="15" t="s">
         <v>576</v>
       </c>
-      <c r="H157" s="15" t="s">
-        <v>584</v>
-      </c>
       <c r="I157" s="15" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
       <c r="J157" s="16" t="s">
         <v>83</v>
@@ -11089,13 +11112,13 @@
         <v>45327</v>
       </c>
       <c r="G158" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H158" s="15" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="I158" s="15" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
       <c r="J158" s="16" t="s">
         <v>83</v>
@@ -11145,13 +11168,13 @@
         <v>45327</v>
       </c>
       <c r="G159" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H159" s="15" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="I159" s="15" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
       <c r="J159" s="16" t="s">
         <v>83</v>
@@ -11196,16 +11219,16 @@
         <v>341</v>
       </c>
       <c r="F160" s="14">
-        <v>45327</v>
+        <v>45330</v>
       </c>
       <c r="G160" s="15" t="s">
-        <v>576</v>
+        <v>674</v>
       </c>
       <c r="H160" s="15" t="s">
-        <v>589</v>
+        <v>675</v>
       </c>
       <c r="I160" s="15" t="s">
-        <v>590</v>
+        <v>676</v>
       </c>
       <c r="J160" s="16" t="s">
         <v>83</v>
@@ -11253,13 +11276,13 @@
         <v>45327</v>
       </c>
       <c r="G161" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H161" s="15" t="s">
-        <v>591</v>
+        <v>581</v>
       </c>
       <c r="I161" s="15" t="s">
-        <v>592</v>
+        <v>582</v>
       </c>
       <c r="J161" s="16" t="s">
         <v>83</v>
@@ -11309,13 +11332,13 @@
         <v>45327</v>
       </c>
       <c r="G162" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H162" s="15" t="s">
-        <v>593</v>
+        <v>583</v>
       </c>
       <c r="I162" s="15" t="s">
-        <v>594</v>
+        <v>584</v>
       </c>
       <c r="J162" s="16" t="s">
         <v>83</v>
@@ -11365,13 +11388,13 @@
         <v>45327</v>
       </c>
       <c r="G163" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H163" s="15" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
       <c r="I163" s="15" t="s">
-        <v>613</v>
+        <v>603</v>
       </c>
       <c r="J163" s="16" t="s">
         <v>83</v>
@@ -11421,13 +11444,13 @@
         <v>45327</v>
       </c>
       <c r="G164" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H164" s="15" t="s">
-        <v>612</v>
+        <v>602</v>
       </c>
       <c r="I164" s="15" t="s">
-        <v>611</v>
+        <v>601</v>
       </c>
       <c r="J164" s="16" t="s">
         <v>83</v>
@@ -11477,13 +11500,13 @@
         <v>45327</v>
       </c>
       <c r="G165" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H165" s="15" t="s">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="I165" s="15" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
       <c r="J165" s="16" t="s">
         <v>83</v>
@@ -11531,13 +11554,13 @@
         <v>45327</v>
       </c>
       <c r="G166" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H166" s="15" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="I166" s="15" t="s">
-        <v>607</v>
+        <v>597</v>
       </c>
       <c r="J166" s="16" t="s">
         <v>83</v>
@@ -11587,13 +11610,13 @@
         <v>45327</v>
       </c>
       <c r="G167" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H167" s="15" t="s">
-        <v>606</v>
+        <v>596</v>
       </c>
       <c r="I167" s="15" t="s">
-        <v>605</v>
+        <v>595</v>
       </c>
       <c r="J167" s="16" t="s">
         <v>83</v>
@@ -11643,13 +11666,13 @@
         <v>45327</v>
       </c>
       <c r="G168" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H168" s="15" t="s">
-        <v>604</v>
+        <v>594</v>
       </c>
       <c r="I168" s="15" t="s">
-        <v>603</v>
+        <v>593</v>
       </c>
       <c r="J168" s="16" t="s">
         <v>83</v>
@@ -11699,13 +11722,13 @@
         <v>45327</v>
       </c>
       <c r="G169" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H169" s="15" t="s">
-        <v>602</v>
+        <v>592</v>
       </c>
       <c r="I169" s="15" t="s">
-        <v>601</v>
+        <v>591</v>
       </c>
       <c r="J169" s="16" t="s">
         <v>83</v>
@@ -11755,13 +11778,13 @@
         <v>45327</v>
       </c>
       <c r="G170" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H170" s="15" t="s">
-        <v>600</v>
+        <v>590</v>
       </c>
       <c r="I170" s="15" t="s">
-        <v>599</v>
+        <v>589</v>
       </c>
       <c r="J170" s="16" t="s">
         <v>83</v>
@@ -11809,13 +11832,13 @@
         <v>45327</v>
       </c>
       <c r="G171" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H171" s="15" t="s">
-        <v>598</v>
+        <v>588</v>
       </c>
       <c r="I171" s="15" t="s">
-        <v>597</v>
+        <v>587</v>
       </c>
       <c r="J171" s="16" t="s">
         <v>83</v>
@@ -11865,13 +11888,13 @@
         <v>45327</v>
       </c>
       <c r="G172" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H172" s="15" t="s">
-        <v>596</v>
+        <v>586</v>
       </c>
       <c r="I172" s="15" t="s">
-        <v>595</v>
+        <v>585</v>
       </c>
       <c r="J172" s="16" t="s">
         <v>83</v>
@@ -11921,13 +11944,13 @@
         <v>45327</v>
       </c>
       <c r="G173" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H173" s="15" t="s">
-        <v>615</v>
+        <v>605</v>
       </c>
       <c r="I173" s="15" t="s">
-        <v>616</v>
+        <v>606</v>
       </c>
       <c r="J173" s="16" t="s">
         <v>83</v>
@@ -11977,13 +12000,13 @@
         <v>45327</v>
       </c>
       <c r="G174" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H174" s="15" t="s">
-        <v>617</v>
+        <v>607</v>
       </c>
       <c r="I174" s="15" t="s">
-        <v>618</v>
+        <v>608</v>
       </c>
       <c r="J174" s="16" t="s">
         <v>83</v>
@@ -12033,13 +12056,13 @@
         <v>45327</v>
       </c>
       <c r="G175" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H175" s="15" t="s">
-        <v>619</v>
+        <v>609</v>
       </c>
       <c r="I175" s="15" t="s">
-        <v>620</v>
+        <v>610</v>
       </c>
       <c r="J175" s="16" t="s">
         <v>83</v>
@@ -12089,13 +12112,13 @@
         <v>45327</v>
       </c>
       <c r="G176" s="15" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="H176" s="15" t="s">
-        <v>621</v>
+        <v>611</v>
       </c>
       <c r="I176" s="15" t="s">
-        <v>622</v>
+        <v>612</v>
       </c>
       <c r="J176" s="16" t="s">
         <v>83</v>
@@ -28637,15 +28660,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
@@ -28654,6 +28668,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28888,14 +28911,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
@@ -28908,6 +28923,14 @@
     <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Accreditamento VPS, RSA, LDO v.1.1.1
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
+++ b/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gzamparo\Documents\FSE 2.0\it-fse-accreditamento\GATEWAY\S1#111MEDARCHIVER\MEDARCHIVER\MEDARCHIVER_FSE2.0\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB83E3B-2BA5-43F2-9C62-49B1B7885741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1AC3E3-991A-4908-B6C9-483C81C0E927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1725" uniqueCount="677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1725" uniqueCount="676">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -2536,12 +2536,6 @@
     <t>7ba9006f241ad450</t>
   </si>
   <si>
-    <t>2024-02-07T09:36:58Z</t>
-  </si>
-  <si>
-    <t>28ef5a0883564fa8</t>
-  </si>
-  <si>
     <t>2024-02-07T12:41:47Z</t>
   </si>
   <si>
@@ -2560,24 +2554,6 @@
     <t>2.16.840.1.113883.2.9.2.190.4.4.641ee0751dad17117e6d991886171890720f9552821beaa685cd6afaba60610f.9936634cd2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2024-02-08T12:02:15Z</t>
-  </si>
-  <si>
-    <t>74aeaf03be14ac04</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.641ee0751dad17117e6d991886171890720f9552821beaa685cd6afaba60610f.50dce8c006^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-02-08T12:12:20Z</t>
-  </si>
-  <si>
-    <t>8d9bd613b992b3c4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.641ee0751dad17117e6d991886171890720f9552821beaa685cd6afaba60610f.04e34a52df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2024-02-08T12:15:21Z</t>
   </si>
   <si>
@@ -2585,6 +2561,27 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.bad2ea390c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-02-09T09:42:23Z</t>
+  </si>
+  <si>
+    <t>ead3dbfb6af3f70e</t>
+  </si>
+  <si>
+    <t>2024-02-09T09:44:49Z</t>
+  </si>
+  <si>
+    <t>ee6be17d5472120f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.641ee0751dad17117e6d991886171890720f9552821beaa685cd6afaba60610f.2e5ce6545d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>8140b5168e1c97eb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.641ee0751dad17117e6d991886171890720f9552821beaa685cd6afaba60610f.fc38989166^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4673,10 +4670,10 @@
   <dimension ref="A1:T993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D160" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F160" sqref="F160:I160"/>
+      <selection pane="bottomRight" activeCell="F33" sqref="F33:I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5728,13 +5725,13 @@
         <v>45329</v>
       </c>
       <c r="G31" s="15" t="s">
+        <v>660</v>
+      </c>
+      <c r="H31" s="15" t="s">
+        <v>661</v>
+      </c>
+      <c r="I31" s="15" t="s">
         <v>662</v>
-      </c>
-      <c r="H31" s="15" t="s">
-        <v>663</v>
-      </c>
-      <c r="I31" s="15" t="s">
-        <v>664</v>
       </c>
       <c r="J31" s="16" t="s">
         <v>83</v>
@@ -5772,13 +5769,13 @@
         <v>45329</v>
       </c>
       <c r="G32" s="15" t="s">
+        <v>663</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>664</v>
+      </c>
+      <c r="I32" s="15" t="s">
         <v>665</v>
-      </c>
-      <c r="H32" s="15" t="s">
-        <v>666</v>
-      </c>
-      <c r="I32" s="15" t="s">
-        <v>667</v>
       </c>
       <c r="J32" s="16" t="s">
         <v>83</v>
@@ -5813,16 +5810,16 @@
         <v>79</v>
       </c>
       <c r="F33" s="14">
-        <v>45330</v>
+        <v>45331</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="J33" s="16" t="s">
         <v>83</v>
@@ -5857,16 +5854,16 @@
         <v>81</v>
       </c>
       <c r="F34" s="14">
-        <v>45330</v>
+        <v>45331</v>
       </c>
       <c r="G34" s="15" t="s">
         <v>671</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="J34" s="16" t="s">
         <v>83</v>
@@ -6067,13 +6064,13 @@
         <v>431</v>
       </c>
       <c r="F39" s="14">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>660</v>
+        <v>669</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>661</v>
+        <v>670</v>
       </c>
       <c r="I39" s="15" t="s">
         <v>434</v>
@@ -11222,13 +11219,13 @@
         <v>45330</v>
       </c>
       <c r="G160" s="15" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="H160" s="15" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
       <c r="I160" s="15" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
       <c r="J160" s="16" t="s">
         <v>83</v>
@@ -28660,26 +28657,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -28910,32 +28887,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB221413-913B-41FE-97D3-5428BD0403A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28954,6 +28926,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Accreditamento VPS, RSA, LDO v.1.1.2
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
+++ b/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gzamparo\Documents\FSE 2.0\it-fse-accreditamento\GATEWAY\S1#111MEDARCHIVER\MEDARCHIVER\MEDARCHIVER_FSE2.0\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1AC3E3-991A-4908-B6C9-483C81C0E927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E17EA3-AF5B-4194-B287-2EF21BA48525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -2563,12 +2563,6 @@
     <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.bad2ea390c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2024-02-09T09:42:23Z</t>
-  </si>
-  <si>
-    <t>ead3dbfb6af3f70e</t>
-  </si>
-  <si>
     <t>2024-02-09T09:44:49Z</t>
   </si>
   <si>
@@ -2582,6 +2576,12 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.190.4.4.641ee0751dad17117e6d991886171890720f9552821beaa685cd6afaba60610f.fc38989166^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-03-21T17:33:31Z</t>
+  </si>
+  <si>
+    <t>2454aa4be2e3176d</t>
   </si>
 </sst>
 </file>
@@ -4670,10 +4670,10 @@
   <dimension ref="A1:T993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F33" sqref="F33:I34"/>
+      <selection pane="bottomRight" activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5813,13 +5813,13 @@
         <v>45331</v>
       </c>
       <c r="G33" s="15" t="s">
+        <v>669</v>
+      </c>
+      <c r="H33" s="15" t="s">
+        <v>670</v>
+      </c>
+      <c r="I33" s="15" t="s">
         <v>671</v>
-      </c>
-      <c r="H33" s="15" t="s">
-        <v>672</v>
-      </c>
-      <c r="I33" s="15" t="s">
-        <v>673</v>
       </c>
       <c r="J33" s="16" t="s">
         <v>83</v>
@@ -5857,13 +5857,13 @@
         <v>45331</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="J34" s="16" t="s">
         <v>83</v>
@@ -6064,13 +6064,13 @@
         <v>431</v>
       </c>
       <c r="F39" s="14">
-        <v>45331</v>
+        <v>45372</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>669</v>
+        <v>674</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>670</v>
+        <v>675</v>
       </c>
       <c r="I39" s="15" t="s">
         <v>434</v>
@@ -28657,6 +28657,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -28887,27 +28907,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB221413-913B-41FE-97D3-5428BD0403A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28926,31 +28951,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Accreditamento VPS, RSA, LDO v.1.1.3
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
+++ b/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gzamparo\Documents\FSE 2.0\it-fse-accreditamento\GATEWAY\S1#111MEDARCHIVER\MEDARCHIVER\MEDARCHIVER_FSE2.0\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E17EA3-AF5B-4194-B287-2EF21BA48525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECA6BDD-7AF3-488F-86BA-D562D8770417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1725" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1726" uniqueCount="674">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -2032,219 +2032,66 @@
     <t>Per eseguire il test sono stati disattivati i controlli applicativi normalmente presenti (normalmente non è possibile non completare la sezione quesito diagnostico) per cui se il CDA2 non dovesse contenere il dato, si tratta di un problema tecnico, il problema viene segnalato all'amministratore di sistema che provvede alla correzione; una volta risolto l'utente (compilatore) dispone di una lista dei documenti da rifirmare.</t>
   </si>
   <si>
-    <t>2024-02-05T10:26:33Z</t>
-  </si>
-  <si>
-    <t>1fe878c76d035327</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.464a695e13^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>e87b9880412237ef</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.6c2dc01ea3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>a3df8856082de854</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.4ad79442c3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>a67fdeee1fad943d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.98a18a46fb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>[ERRORE-12| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi 'country', 'city' e 'streetAddressLine' ]</t>
   </si>
   <si>
-    <t>411238b3e94c3b50</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.99da795ff6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>[ERRORE-15| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family']</t>
   </si>
   <si>
     <t>[ERRORE-b132| Sezione Allergie: l'elemento entry/act/entryRelationship/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato ]</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.104c8f7698^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>9b4a21ace276509d</t>
-  </si>
-  <si>
     <t>[ERRORE-b114| Sotto-sezione Anamnesi: l'elemento entry/organizer/subject/relatedSubject deve avere l'attributo @classCode='PRS' e deve contenere l'elemento 'code']</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.05c8910cdf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>57e722a4ed87998f</t>
-  </si>
-  <si>
     <t>[ERRORE-b104| Sotto-sezione Anamnesi: l'elemento entry/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato]</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.f7fcf3b4ba^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>1f5a7269c55ceb14</t>
-  </si>
-  <si>
     <t>[ERRORE-b83| Sezione Triage: l'elemento entry/observation/value DEVE essere valorizzato col value set CodiceTriage_VPS]</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.cf4e390e61^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>24e3ebc6c0130e31</t>
-  </si>
-  <si>
     <t>[ERRORE-b11| Sezione Motivo della visita: l'elemento entry/observation/value relativo al Problema Principale" DEVE essere valorizzato col value set ProblemaPrincipale_VPS]"</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.a3fde444f2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>5bdf3b1fcab566d4</t>
-  </si>
-  <si>
     <t>[ERRORE-b6| Sezione Motivo della Visita: la sezione DEVE contenere l'elemento 'text']</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.2646b4291d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>afcd91db35db88bf</t>
-  </si>
-  <si>
     <t>[ERRORE-b1| Sezione Modalità di Trasporto: la sezione DEVE essere presente],[ERRORE-b2| Sezione Modalità di Trasporto: la sezione deve contenere l'elemento templateId valorizzato con l'attributo @root='2.16.840.1.113883.2.9.10.1.6.20'],[ERRORE-b3| Sezione Modalità di Trasporto: la sezione DEVE contenere un elemento 'text' e un solo elemento 'entry']</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.8696aa70f2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>af4cbe425c1c28e7</t>
-  </si>
-  <si>
     <t>ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element 'assignedPerson'. One of '{urn:hl7-org:v3":realmCode, "urn:hl7-org:v3":typeId, "urn:hl7-org:v3":templateId, "urn:hl7-org:v3":id}' is expected."</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.b548c0a6b5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>ece1b5da0597232c</t>
-  </si>
-  <si>
     <t>[ERRORE-b3| Sezione Modalità di Trasporto: la sezione DEVE contenere un elemento 'text' e un solo elemento 'entry']</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.95dfd92b2a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>3969e4d11c81670b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.636e21b739^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>577ea12a92b832e4</t>
-  </si>
-  <si>
-    <t>e375c4c44063a553</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.8cfdcea6e2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>[ERRORE-b154| Sezione Encounters: L'elemento entry/encounters/effectiveTime deve essere presente e deve avere gli elementi 'low' e 'high' valorizzati.]</t>
   </si>
   <si>
-    <t>0980735f6398e00e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.cbacae1b73^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>[ERRORE-b168| Sezione Complicanze: l'elemento entry/observation/value DEVE essere valorizzato con l'attributo @xsi:type=CD.]</t>
   </si>
   <si>
-    <t>b32d311f84935e69</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.7ffc2fcfbe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>[ERRORE-b28| Sezione Dimissione: l'entry/act/performer/assignedEntity/assignedPerson/name DEVE contenere gli elementi 'family' e 'given']</t>
   </si>
   <si>
-    <t>058619352f9591a0</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.16ac540399^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>[ERRORE-b30| Sezione Dimissione: l'entry/act Dimissione" DEVE contenere un solo elemento 'entryRelationship' relativo all'Esito],[ERRORE-b31| Sezione Dimissione: l'entry/act/entryRelationship relativo all'Esito DEVE contenere  un elemento 'templateId' valorizzato con @root='2.16.840.1.113883.2.9.10.1.6.69'.],[ERRORE-b32| Sezione Dimissione: l'entry/act/entryRelationship relativo all'Esito DEVE contenere  un elemento 'statusCode' valorizzato con @code='completed'],[ERRORE-b33| Sezione Dimissione: l'entry/act/entryRelationship relativo all'Esito DEVE contenere  un elemento 'value' valorizzato secondo il value set "EsitoTrattamento_VPS" - @codeSystem='2.16.840.1.113883.2.9.6.1.54.5']"</t>
   </si>
   <si>
-    <t>f56a57863c88abd3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.44cdcf0c83^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>[ERRORE-b252|Sezione Terapia farmacologica alla dimissione: entry/substanceAdministration/effectiveTime deve avere l'elemento 'low' valorizzato ]</t>
   </si>
   <si>
-    <t>31d6b7cc88c14299</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.3bfd7d77bc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.2.9.6.1.54.6, Codes: 145]</t>
   </si>
   <si>
-    <t>5af077f42c097b73</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.867a816860^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.2.9.6.1.54.4, Codes: 36]</t>
   </si>
   <si>
-    <t>bf5b1a1499fdb412</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.f5cea9e71f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>[ERRORE-b237| Sezione Dimissione - Diagnosi di Dimissione": l'elemento entry/act/entryRelationship/observation deve contenere l'elemento 'code' con attributi @code='29308-4' e @codeSystem='2.16.840.1.113883.6.1']"</t>
   </si>
   <si>
-    <t>813ab0c255f8a6ba</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.60f8eb44ca^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.2.9.6.1.5, Codes: 04323348022], [CodeSystem: 2.16.840.1.113883.6.73, Codes: C0238CA01]</t>
   </si>
   <si>
-    <t>3422c70ba86ae19a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.91b354610a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>[ERRORE-b136| Sezione Allergie: entry/act/entryRelationship/observation deve contenere almeno un elemento 'participant']</t>
   </si>
   <si>
@@ -2260,328 +2107,475 @@
     <t>Per eseguire il test sono stati disattivati i controlli applicativi normalmente presenti</t>
   </si>
   <si>
-    <t>2024-02-05T12:11:37Z</t>
-  </si>
-  <si>
-    <t>bbfa0d5e928509eb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.bb61a94250ccedcbb320afd3e9903df362179d04d7c7dfe90a1ceaf3144621be.3e7f03fb57^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.c9cf13c411a40543c41310886420256438189d40bbec51216e7d6905038273c8.3099b57c26^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>083eda47536df7aa</t>
-  </si>
-  <si>
-    <t>da97af9758711ba5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.ea9bc6690db4bab486666fc38ef5de05188118e04583f2d832ac39eed72c3e54.e303888f03^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.3831350bd3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>8676b7e2fcb39b6e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.da293ca52a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>eec9e44f38349634</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.87bde3d630^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>f05ab6a93b35903e</t>
-  </si>
-  <si>
-    <t>90f9c086fd26bc6c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.2a1f491796^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>f84422bf4212af99</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.80d579092a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.1f7d374a80^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>ba3dd7ad0076f81b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.0259661471^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>1a480c8bd7bfc4fb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.59147492e6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>286ae817d8d2d826</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.fb21e139d9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>bc00602762962f23</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.6637902e75^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>4c75669c3d00efeb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.ada7b16f24^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>4985c6f72148d05a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.ab30239d12^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>ec723d69baf4c49f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.cf44ea978a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>3dbd520632e75164</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.20614f6c7d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>607a4b6b5fcb4625</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.0ed8864235^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>ccda156df5213590</t>
-  </si>
-  <si>
-    <t>98c03ef715ce6e0b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.4ba651c979^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>fa8f71de38cb4b68</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.4ed8323469^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>384b9f99267896d6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.39ddbe066b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>8b94ce28ad2a87f3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.7e59f4e268^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.5187a7c6983155e8ce8a0349302fbf5ed672a64b2432a651aeaa4c11820cfe76.0ca66cf94f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>6f3e8797b3fd2876</t>
-  </si>
-  <si>
-    <t>2024-02-05T12:42:07Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.bf369a51d1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>5583a88fb6db72d3</t>
-  </si>
-  <si>
-    <t>2024-02-05T12:42:08Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.2619803088^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>3aa2237a23c3529f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.e73e7675ad^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>06f1b548c8f82880</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.1d74b80802^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>9508e662ef2aa8a7</t>
-  </si>
-  <si>
-    <t>4e8078d581f611c7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.59dd059110^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>64099188b00f9cd4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.d5f264a6e3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>82114ca975115823</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.22d43196f9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.e589b421fd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>e2175233eb6adbe6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.b844d960c7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>21869c6193fde2f3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.45c347ba2b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>6ec966b019948737</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.b7ce7a0879^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>72ff13fadb3adb40</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.36b3cfa48b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>d17d68e79656d1a6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.3f2f9363a5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>6919fbdec238f904</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.8fbd45b638^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>a75313cd5b7c6dd8</t>
-  </si>
-  <si>
     <t>[ERRORE-b5| Sezione Condizioni del paziente e diagnosi alla dimissione: la sezione DEVE essere presente],[ERRORE-b6| Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione DEVE contenere l'elemento 'text'],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO' contenere l'elemento 'entry' ]</t>
   </si>
   <si>
     <t>[ERRORE-b26| Sotto-sezione Anamnesi: l'elemento entry/observation/effectiveTime deve essere presente e deve avere l'elemento 'low' valorizzato]</t>
   </si>
   <si>
-    <t>2024-02-05T14:46:51Z</t>
-  </si>
-  <si>
-    <t>a4bbb5457be48c44</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.b1a8d20080^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-02-05T15:11:46Z</t>
-  </si>
-  <si>
     <t>1e710e7ad4cfe2f3</t>
   </si>
   <si>
-    <t>2024-02-05T15:15:28Z</t>
-  </si>
-  <si>
-    <t>12d03116438bbf4d</t>
-  </si>
-  <si>
-    <t>2024-02-05T15:20:00Z</t>
-  </si>
-  <si>
-    <t>f00f0189431b24ac</t>
-  </si>
-  <si>
-    <t>2024-02-05T15:21:36Z</t>
-  </si>
-  <si>
-    <t>fac612db15ae23eb</t>
-  </si>
-  <si>
-    <t>2024-02-05T15:22:37Z</t>
-  </si>
-  <si>
-    <t>7ba9006f241ad450</t>
-  </si>
-  <si>
-    <t>2024-02-07T12:41:47Z</t>
-  </si>
-  <si>
-    <t>45ee3f384cbbd1e1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.641ee0751dad17117e6d991886171890720f9552821beaa685cd6afaba60610f.d3e2e6e48d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-02-07T15:50:24Z</t>
-  </si>
-  <si>
-    <t>77af659f65ae706b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.641ee0751dad17117e6d991886171890720f9552821beaa685cd6afaba60610f.9936634cd2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-02-08T12:15:21Z</t>
-  </si>
-  <si>
-    <t>867f398fb2b840ee</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.bad2ea390c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-02-09T09:44:49Z</t>
-  </si>
-  <si>
-    <t>ee6be17d5472120f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.641ee0751dad17117e6d991886171890720f9552821beaa685cd6afaba60610f.2e5ce6545d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>8140b5168e1c97eb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.641ee0751dad17117e6d991886171890720f9552821beaa685cd6afaba60610f.fc38989166^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-03-21T17:33:31Z</t>
-  </si>
-  <si>
-    <t>2454aa4be2e3176d</t>
+    <t>2025-11-20T12:47:38Z</t>
+  </si>
+  <si>
+    <t>3bdc46d9fa3b1def2c3de9ee1aec4555</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.5187a7c6983155e8ce8a0349302fbf5ed672a64b2432a651aeaa4c11820cfe76.72c26016f6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>2025-11-20T12:47:40Z</t>
+  </si>
+  <si>
+    <t>777c7c126637b7d71b9562ffd3d2255a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.ca561ad88f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>3d91962a12eea35d84e97fa8bf4d72d2</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.c2407bf6ab^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>520e94bd16e7c141c727fa122a205584</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.cc36565ef7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>9bfbc972eac1918dbd3b633c8f5ba409</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.bd65c34714^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>1395872f67c3c0f21c2153c0ade2ee5a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.6cf530952a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>1432363d7299bd9cdf5e930b656e31b0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.2c174aa86d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>db73a3543da36bb6a58e058e7316ff6a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.6747b1c2df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>a68b1f36ee6a338d9cb1d6d6f35212f7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.689a2a5c01^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ERROR: -1,-1 cvc-complex-type.2.4.a: Invalid content was found starting with element '{urn:hl7-org:v3":languageCode}'. One of '{"urn:hl7-org:v3":confidentialityCode}' is expected."</t>
+  </si>
+  <si>
+    <t>71c4bfc911226254afa034995a8e3214</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.fdc40c0fd8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>f672a6a37c98ab51a8aa6f645a510daa</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.18bb942f10^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>30ffa5b54935f29275242e5f8926765a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.b1880617e3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>430f5aa474cfd34fe4f1a5d5aa2259e4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.83e7f242b3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>45b147ec5697949c68b8f4921a607f20</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.a2cbe4b1d7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>b1c8cd86dc837372034029f25de324d1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.bf73ad49f7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>e0b87c56d1154eedf848932c0c7a4659</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.3578ff9ecd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-11-20T12:56:19Z</t>
+  </si>
+  <si>
+    <t>05c3770d6d7c7c81f87a59a073c52cb4</t>
+  </si>
+  <si>
+    <t>2025-11-20T12:58:39Z</t>
+  </si>
+  <si>
+    <t>f735afe1d5dcc83cba3bfdf27c6bb5c6</t>
+  </si>
+  <si>
+    <t>2025-11-20T15:52:26Z</t>
+  </si>
+  <si>
+    <t>93e068b41cd64de0b69ca406dcbfe36a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.5187a7c6983155e8ce8a0349302fbf5ed672a64b2432a651aeaa4c11820cfe76.1e28b728db^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.5187a7c6983155e8ce8a0349302fbf5ed672a64b2432a651aeaa4c11820cfe76.1bb3fcbe4e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>19f64c6fc20ef2a606eec45300e83bc5</t>
+  </si>
+  <si>
+    <t>2025-11-20T15:52:28Z</t>
+  </si>
+  <si>
+    <t>151e3dd88636aeac24462451badade3e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.ea9bc6690db4bab486666fc38ef5de05188118e04583f2d832ac39eed72c3e54.539d4098e9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>4f859b28d2717bcc31944a8fa53f9db9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.ad0ebc0a67^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>c4b2bcf0a9945456ad7693cc631eebbe</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.e091d90021^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ade53cfb7da4f601f396685045379a85</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.c01dd23245^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>255efd6cc29f3ef117950ea195e3193b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.27c19df039^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>b2872940ff67d98852223793ab0a4597</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.44120f57b9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>b20e64054e190648c78144f0894ccd4c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.d126558ca4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>e0eef2340f4cf5598e987d2e276b60a8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.a1ec775ce3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>3ff18c73f47dc95410c5aab818c0edde</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.d610f31865^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>7ab3955152796a8124c477bf692a8c2f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.19071eea3a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2921087e4d75863a4ef58670e774a0eb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.433349ba5a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>435dc949b7f4a6e2f5b0d0a931f0c052</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.36d249ceeb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>528b463262240ae78ac6ea547c543b99</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.e87a2a3099^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>8e81da9ffdaadd354452dd9c51a57113</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.3b2467304f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>866b5ada131a0d846f170b78c26eec17</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.bd3f00204d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>d51c630722e71cbb2d4d323e75c4c3a7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.3f8e4bf644^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ebfed4cf2c74df8ab8e475b6a7b44c0e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.7bd205abbf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>4895865b77b3bd4c52dd199cd0879c33</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.8a48b57ece^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>5703faecd14f8f582d436f28e5b88450</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.aa87d0db98^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>e7a3bd232ac7a8861956d067a88b4cb4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.5eda6ea0ae^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>f15cea80f19bd4c919382dfc5c6c6e66</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.5e0978cad15caf367542a1f71b81987fc8384e5878a20f12e394ae6d0d849b45.6137f11d40^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-11-20T15:58:04Z</t>
+  </si>
+  <si>
+    <t>1270ad9bfc34b3c33edcda1b3400913e</t>
+  </si>
+  <si>
+    <t>2025-11-20T15:59:53Z</t>
+  </si>
+  <si>
+    <t>b6b66f3615cc9747a9c46e7d6c1e5648</t>
+  </si>
+  <si>
+    <t>2025-11-20T16:52:21Z</t>
+  </si>
+  <si>
+    <t>32e7a3ca2db9a0ba1ee93b40b529f268</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.641ee0751dad17117e6d991886171890720f9552821beaa685cd6afaba60610f.3358f60165^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.641ee0751dad17117e6d991886171890720f9552821beaa685cd6afaba60610f.d8d4b08251^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>9d2bf27072600500989d1a7a38b2746c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.641ee0751dad17117e6d991886171890720f9552821beaa685cd6afaba60610f.eb2a54c0c9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>935b7e24e3354196dbbce10e053931f8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.641ee0751dad17117e6d991886171890720f9552821beaa685cd6afaba60610f.24c42508f8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>88c0d3895088badf3c35091fe5256857</t>
+  </si>
+  <si>
+    <t>ad68ca4fa0f0b62445cb8435f0775aa9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.32dcaf8ec8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>1f58d0669c65b98cf46f083a11b4a241</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.d06744e466^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>84f23e17a608c23b0427f98b1fecadc1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.e67707fd73^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>95f1256522659d7e6643af52e21574c7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.dc2e9bae2b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2d7fb3e3f1f89ebf399c51f6fbfcde7d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.85d4927f06^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.130b7dce44^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>f246fd71b035ed7a76dcbf519707a957</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.acb2734420^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>e71ad6960d70d697ebb381ff4cd7621c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.02f07bffe1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>480f26a315ed51add00e35d3b9855a7d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.ede14c5534^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>464def2f3c4e85d7ce199cccb8eba8ef</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.9908740a54^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>dfe9b1e968576ae3f029d1beb7747dc8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.82795c818e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>a7e851c0537de0fef5783dda9cec4442</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.ff8731eed7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>0038faf27da177ec2d9e11af70587abc</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.ffa57acb2c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>978a399322be258fe2a9d92fd7e2ae09</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.c25d96f6aa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>7085a0946baa29ff42d445562fd91989</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.e7548ce03e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>f5e876bff433277b9ea2ba700ae183ae</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.8bb48f0c0c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>89c40196bcd437878356b3bbd9cc083f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.dc90508308^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>1879e9174f6b9341a9140f75dc3fa108</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.73e09694df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>b68ede0c40d3ef028487be0eace01f05</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.1c89b0f74d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>f0e9b43f32648405b59981de7d200af9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.34b0fedbd0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>1e98d275bbab1885fde22add152cb805</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.588abe3d61^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>a3996bb866aa50fdf85c17ec0b75bcf0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.0e96fd3c22^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>3974c5eadb260dab3edc52a979afd831</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.1fe16f5faf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>729ce38451943bdcaefa53eb6564d812</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.22eaedbfbe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>a38633eb379732e814fa9419545e6890</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.c989ef1360f348ac94738a0369e02bd448abbc5e05a36452b5e142875a66eacc.7ae37bb126^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>66cf3f4fc48dc9ed671a4343e5dd1121</t>
+  </si>
+  <si>
+    <t>2025-11-20T16:57:56Z</t>
+  </si>
+  <si>
+    <t>8383971c41ed47ecaf2e79de67048c98</t>
+  </si>
+  <si>
+    <t>2025-11-20T16:59:45Z</t>
   </si>
 </sst>
 </file>
@@ -3048,7 +3042,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -3223,6 +3217,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -4670,10 +4666,10 @@
   <dimension ref="A1:T993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="K39" sqref="K39"/>
+      <selection pane="bottomRight" activeCell="F42" sqref="F42:I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5101,7 +5097,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>6</v>
       </c>
@@ -5117,25 +5113,31 @@
       <c r="E15" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>615</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>614</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>613</v>
-      </c>
-      <c r="J15" s="16" t="s">
+      <c r="F15" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G15" t="s">
+        <v>520</v>
+      </c>
+      <c r="H15" t="s">
+        <v>521</v>
+      </c>
+      <c r="I15" t="s">
+        <v>522</v>
+      </c>
+      <c r="J15" t="s">
         <v>83</v>
       </c>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
+      <c r="K15" t="s">
+        <v>523</v>
+      </c>
+      <c r="L15" t="s">
+        <v>523</v>
+      </c>
+      <c r="M15" t="s">
+        <v>523</v>
+      </c>
+      <c r="N15"/>
       <c r="O15" s="16"/>
       <c r="P15" s="16"/>
       <c r="Q15" s="16"/>
@@ -5145,7 +5147,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
         <v>7</v>
       </c>
@@ -5161,17 +5163,17 @@
       <c r="E16" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>618</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>622</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>621</v>
+      <c r="F16" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G16" t="s">
+        <v>524</v>
+      </c>
+      <c r="H16" t="s">
+        <v>525</v>
+      </c>
+      <c r="I16" t="s">
+        <v>526</v>
       </c>
       <c r="J16" s="16" t="s">
         <v>83</v>
@@ -5189,7 +5191,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>8</v>
       </c>
@@ -5205,17 +5207,17 @@
       <c r="E17" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>618</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>620</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>619</v>
+      <c r="F17" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G17" t="s">
+        <v>524</v>
+      </c>
+      <c r="H17" t="s">
+        <v>527</v>
+      </c>
+      <c r="I17" t="s">
+        <v>528</v>
       </c>
       <c r="J17" s="16" t="s">
         <v>83</v>
@@ -5233,7 +5235,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>9</v>
       </c>
@@ -5249,17 +5251,17 @@
       <c r="E18" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>618</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>617</v>
-      </c>
-      <c r="I18" s="15" t="s">
-        <v>616</v>
+      <c r="F18" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G18" t="s">
+        <v>524</v>
+      </c>
+      <c r="H18" t="s">
+        <v>529</v>
+      </c>
+      <c r="I18" t="s">
+        <v>530</v>
       </c>
       <c r="J18" s="16" t="s">
         <v>83</v>
@@ -5721,17 +5723,17 @@
       <c r="E31" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="F31" s="14">
-        <v>45329</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>660</v>
-      </c>
-      <c r="H31" s="15" t="s">
-        <v>661</v>
-      </c>
-      <c r="I31" s="15" t="s">
-        <v>662</v>
+      <c r="F31" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G31" t="s">
+        <v>612</v>
+      </c>
+      <c r="H31" t="s">
+        <v>613</v>
+      </c>
+      <c r="I31" t="s">
+        <v>614</v>
       </c>
       <c r="J31" s="16" t="s">
         <v>83</v>
@@ -5765,17 +5767,17 @@
       <c r="E32" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F32" s="14">
-        <v>45329</v>
-      </c>
-      <c r="G32" s="15" t="s">
-        <v>663</v>
-      </c>
-      <c r="H32" s="15" t="s">
-        <v>664</v>
-      </c>
-      <c r="I32" s="15" t="s">
-        <v>665</v>
+      <c r="F32" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G32" t="s">
+        <v>612</v>
+      </c>
+      <c r="H32" t="s">
+        <v>616</v>
+      </c>
+      <c r="I32" t="s">
+        <v>615</v>
       </c>
       <c r="J32" s="16" t="s">
         <v>83</v>
@@ -5809,17 +5811,17 @@
       <c r="E33" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="F33" s="14">
-        <v>45331</v>
-      </c>
-      <c r="G33" s="15" t="s">
-        <v>669</v>
-      </c>
-      <c r="H33" s="15" t="s">
-        <v>670</v>
-      </c>
-      <c r="I33" s="15" t="s">
-        <v>671</v>
+      <c r="F33" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G33" t="s">
+        <v>612</v>
+      </c>
+      <c r="H33" t="s">
+        <v>620</v>
+      </c>
+      <c r="I33" t="s">
+        <v>619</v>
       </c>
       <c r="J33" s="16" t="s">
         <v>83</v>
@@ -5853,17 +5855,17 @@
       <c r="E34" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F34" s="14">
-        <v>45331</v>
-      </c>
-      <c r="G34" s="15" t="s">
-        <v>669</v>
-      </c>
-      <c r="H34" s="15" t="s">
-        <v>672</v>
-      </c>
-      <c r="I34" s="15" t="s">
-        <v>673</v>
+      <c r="F34" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G34" t="s">
+        <v>612</v>
+      </c>
+      <c r="H34" t="s">
+        <v>618</v>
+      </c>
+      <c r="I34" t="s">
+        <v>617</v>
       </c>
       <c r="J34" s="16" t="s">
         <v>83</v>
@@ -5915,7 +5917,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11">
         <v>29</v>
       </c>
@@ -5931,16 +5933,16 @@
       <c r="E36" s="13" t="s">
         <v>431</v>
       </c>
-      <c r="F36" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G36" s="15" t="s">
-        <v>652</v>
-      </c>
-      <c r="H36" s="15" t="s">
-        <v>653</v>
-      </c>
-      <c r="I36" s="15" t="s">
+      <c r="F36" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G36" t="s">
+        <v>558</v>
+      </c>
+      <c r="H36" t="s">
+        <v>559</v>
+      </c>
+      <c r="I36" t="s">
         <v>434</v>
       </c>
       <c r="J36" s="16" t="s">
@@ -6047,7 +6049,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11">
         <v>32</v>
       </c>
@@ -6063,16 +6065,16 @@
       <c r="E39" s="13" t="s">
         <v>431</v>
       </c>
-      <c r="F39" s="14">
-        <v>45372</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>674</v>
-      </c>
-      <c r="H39" s="15" t="s">
-        <v>675</v>
-      </c>
-      <c r="I39" s="15" t="s">
+      <c r="F39" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G39" t="s">
+        <v>610</v>
+      </c>
+      <c r="H39" t="s">
+        <v>611</v>
+      </c>
+      <c r="I39" t="s">
         <v>434</v>
       </c>
       <c r="J39" s="16" t="s">
@@ -6185,16 +6187,16 @@
       <c r="E42" s="13" t="s">
         <v>431</v>
       </c>
-      <c r="F42" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G42" s="15" t="s">
-        <v>650</v>
-      </c>
-      <c r="H42" s="15" t="s">
-        <v>651</v>
-      </c>
-      <c r="I42" s="15" t="s">
+      <c r="F42" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G42" t="s">
+        <v>673</v>
+      </c>
+      <c r="H42" s="68" t="s">
+        <v>519</v>
+      </c>
+      <c r="I42" t="s">
         <v>434</v>
       </c>
       <c r="J42" s="16" t="s">
@@ -6257,7 +6259,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11">
         <v>37</v>
       </c>
@@ -6273,16 +6275,16 @@
       <c r="E44" s="13" t="s">
         <v>432</v>
       </c>
-      <c r="F44" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G44" s="15" t="s">
-        <v>658</v>
-      </c>
-      <c r="H44" s="15" t="s">
-        <v>659</v>
-      </c>
-      <c r="I44" s="15" t="s">
+      <c r="F44" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G44" t="s">
+        <v>556</v>
+      </c>
+      <c r="H44" t="s">
+        <v>557</v>
+      </c>
+      <c r="I44" t="s">
         <v>434</v>
       </c>
       <c r="J44" s="16" t="s">
@@ -6379,7 +6381,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="11">
         <v>40</v>
       </c>
@@ -6395,16 +6397,16 @@
       <c r="E47" s="13" t="s">
         <v>432</v>
       </c>
-      <c r="F47" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G47" s="15" t="s">
-        <v>656</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>657</v>
-      </c>
-      <c r="I47" s="15" t="s">
+      <c r="F47" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G47" t="s">
+        <v>608</v>
+      </c>
+      <c r="H47" t="s">
+        <v>609</v>
+      </c>
+      <c r="I47" t="s">
         <v>434</v>
       </c>
       <c r="J47" s="16" t="s">
@@ -6517,16 +6519,16 @@
       <c r="E50" s="13" t="s">
         <v>432</v>
       </c>
-      <c r="F50" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G50" s="15" t="s">
-        <v>654</v>
-      </c>
-      <c r="H50" s="15" t="s">
-        <v>655</v>
-      </c>
-      <c r="I50" s="15" t="s">
+      <c r="F50" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G50" t="s">
+        <v>671</v>
+      </c>
+      <c r="H50" t="s">
+        <v>672</v>
+      </c>
+      <c r="I50" t="s">
         <v>434</v>
       </c>
       <c r="J50" s="16" t="s">
@@ -6591,7 +6593,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" ht="210.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="11">
         <v>45</v>
       </c>
@@ -6709,7 +6711,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" ht="210.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11">
         <v>48</v>
       </c>
@@ -7247,7 +7249,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="11">
         <v>63</v>
       </c>
@@ -7263,17 +7265,17 @@
       <c r="E70" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="F70" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G70" s="15" t="s">
-        <v>618</v>
-      </c>
-      <c r="H70" s="15" t="s">
-        <v>624</v>
-      </c>
-      <c r="I70" s="15" t="s">
-        <v>623</v>
+      <c r="F70" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G70" t="s">
+        <v>524</v>
+      </c>
+      <c r="H70" t="s">
+        <v>531</v>
+      </c>
+      <c r="I70" t="s">
+        <v>532</v>
       </c>
       <c r="J70" s="16" t="s">
         <v>83</v>
@@ -7285,8 +7287,8 @@
       <c r="M70" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="N70" s="16" t="s">
-        <v>454</v>
+      <c r="N70" t="s">
+        <v>541</v>
       </c>
       <c r="O70" s="16" t="s">
         <v>83</v>
@@ -7303,7 +7305,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="11">
         <v>64</v>
       </c>
@@ -7319,17 +7321,17 @@
       <c r="E71" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="F71" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G71" s="15" t="s">
-        <v>647</v>
-      </c>
-      <c r="H71" s="15" t="s">
-        <v>648</v>
-      </c>
-      <c r="I71" s="15" t="s">
-        <v>649</v>
+      <c r="F71" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G71" t="s">
+        <v>524</v>
+      </c>
+      <c r="H71" t="s">
+        <v>533</v>
+      </c>
+      <c r="I71" t="s">
+        <v>534</v>
       </c>
       <c r="J71" s="16" t="s">
         <v>83</v>
@@ -7341,9 +7343,7 @@
       <c r="M71" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="N71" s="16" t="s">
-        <v>455</v>
-      </c>
+      <c r="N71"/>
       <c r="O71" s="16" t="s">
         <v>83</v>
       </c>
@@ -7359,7 +7359,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="11">
         <v>65</v>
       </c>
@@ -7375,17 +7375,17 @@
       <c r="E72" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="F72" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G72" s="15" t="s">
-        <v>618</v>
-      </c>
-      <c r="H72" s="15" t="s">
-        <v>625</v>
-      </c>
-      <c r="I72" s="15" t="s">
-        <v>626</v>
+      <c r="F72" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G72" t="s">
+        <v>524</v>
+      </c>
+      <c r="H72" t="s">
+        <v>535</v>
+      </c>
+      <c r="I72" t="s">
+        <v>536</v>
       </c>
       <c r="J72" s="16" t="s">
         <v>83</v>
@@ -7397,9 +7397,7 @@
       <c r="M72" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="N72" s="16" t="s">
-        <v>456</v>
-      </c>
+      <c r="N72"/>
       <c r="O72" s="16" t="s">
         <v>83</v>
       </c>
@@ -7415,7 +7413,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="11">
         <v>66</v>
       </c>
@@ -7431,17 +7429,17 @@
       <c r="E73" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="F73" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G73" s="15" t="s">
-        <v>618</v>
-      </c>
-      <c r="H73" s="15" t="s">
-        <v>627</v>
-      </c>
-      <c r="I73" s="15" t="s">
-        <v>628</v>
+      <c r="F73" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G73" t="s">
+        <v>524</v>
+      </c>
+      <c r="H73" t="s">
+        <v>537</v>
+      </c>
+      <c r="I73" t="s">
+        <v>538</v>
       </c>
       <c r="J73" s="16" t="s">
         <v>83</v>
@@ -7453,7 +7451,7 @@
       <c r="M73" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="N73" s="16" t="s">
+      <c r="N73" t="s">
         <v>462</v>
       </c>
       <c r="O73" s="16" t="s">
@@ -7471,7 +7469,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="11">
         <v>67</v>
       </c>
@@ -7487,17 +7485,17 @@
       <c r="E74" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="F74" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G74" s="15" t="s">
-        <v>618</v>
-      </c>
-      <c r="H74" s="15" t="s">
-        <v>629</v>
-      </c>
-      <c r="I74" s="15" t="s">
-        <v>630</v>
+      <c r="F74" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G74" t="s">
+        <v>524</v>
+      </c>
+      <c r="H74" t="s">
+        <v>539</v>
+      </c>
+      <c r="I74" t="s">
+        <v>540</v>
       </c>
       <c r="J74" s="16" t="s">
         <v>83</v>
@@ -7509,7 +7507,7 @@
       <c r="M74" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="N74" s="16" t="s">
+      <c r="N74" t="s">
         <v>463</v>
       </c>
       <c r="O74" s="16" t="s">
@@ -7527,7 +7525,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="11">
         <v>68</v>
       </c>
@@ -7543,17 +7541,17 @@
       <c r="E75" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="F75" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G75" s="15" t="s">
-        <v>615</v>
-      </c>
-      <c r="H75" s="15" t="s">
-        <v>644</v>
-      </c>
-      <c r="I75" s="15" t="s">
-        <v>643</v>
+      <c r="F75" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G75" t="s">
+        <v>524</v>
+      </c>
+      <c r="H75" t="s">
+        <v>542</v>
+      </c>
+      <c r="I75" t="s">
+        <v>543</v>
       </c>
       <c r="J75" s="16" t="s">
         <v>83</v>
@@ -7565,7 +7563,7 @@
       <c r="M75" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="N75" s="16" t="s">
+      <c r="N75" t="s">
         <v>457</v>
       </c>
       <c r="O75" s="16" t="s">
@@ -7583,7 +7581,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="11">
         <v>69</v>
       </c>
@@ -7599,17 +7597,17 @@
       <c r="E76" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="F76" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G76" s="15" t="s">
-        <v>615</v>
-      </c>
-      <c r="H76" s="15" t="s">
-        <v>642</v>
-      </c>
-      <c r="I76" s="15" t="s">
-        <v>641</v>
+      <c r="F76" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G76" t="s">
+        <v>524</v>
+      </c>
+      <c r="H76" t="s">
+        <v>544</v>
+      </c>
+      <c r="I76" t="s">
+        <v>545</v>
       </c>
       <c r="J76" s="16" t="s">
         <v>83</v>
@@ -7621,8 +7619,8 @@
       <c r="M76" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="N76" s="16" t="s">
-        <v>645</v>
+      <c r="N76" t="s">
+        <v>517</v>
       </c>
       <c r="O76" s="16" t="s">
         <v>83</v>
@@ -7639,7 +7637,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="345.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" ht="345.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="11">
         <v>70</v>
       </c>
@@ -7655,17 +7653,17 @@
       <c r="E77" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="F77" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G77" s="15" t="s">
-        <v>615</v>
-      </c>
-      <c r="H77" s="15" t="s">
-        <v>640</v>
-      </c>
-      <c r="I77" s="15" t="s">
-        <v>639</v>
+      <c r="F77" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G77" t="s">
+        <v>524</v>
+      </c>
+      <c r="H77" t="s">
+        <v>546</v>
+      </c>
+      <c r="I77" t="s">
+        <v>547</v>
       </c>
       <c r="J77" s="16" t="s">
         <v>83</v>
@@ -7677,7 +7675,7 @@
       <c r="M77" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="N77" s="16" t="s">
+      <c r="N77" t="s">
         <v>458</v>
       </c>
       <c r="O77" s="16" t="s">
@@ -7695,7 +7693,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="11">
         <v>71</v>
       </c>
@@ -7711,17 +7709,17 @@
       <c r="E78" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="F78" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G78" s="15" t="s">
-        <v>615</v>
-      </c>
-      <c r="H78" s="15" t="s">
-        <v>638</v>
-      </c>
-      <c r="I78" s="15" t="s">
-        <v>637</v>
+      <c r="F78" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G78" t="s">
+        <v>524</v>
+      </c>
+      <c r="H78" t="s">
+        <v>548</v>
+      </c>
+      <c r="I78" t="s">
+        <v>549</v>
       </c>
       <c r="J78" s="16" t="s">
         <v>83</v>
@@ -7733,8 +7731,8 @@
       <c r="M78" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="N78" s="16" t="s">
-        <v>646</v>
+      <c r="N78" t="s">
+        <v>518</v>
       </c>
       <c r="O78" s="16" t="s">
         <v>83</v>
@@ -7751,7 +7749,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="11">
         <v>72</v>
       </c>
@@ -7767,17 +7765,17 @@
       <c r="E79" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="F79" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G79" s="15" t="s">
-        <v>615</v>
-      </c>
-      <c r="H79" s="15" t="s">
-        <v>636</v>
-      </c>
-      <c r="I79" s="15" t="s">
-        <v>635</v>
+      <c r="F79" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G79" t="s">
+        <v>524</v>
+      </c>
+      <c r="H79" t="s">
+        <v>550</v>
+      </c>
+      <c r="I79" t="s">
+        <v>551</v>
       </c>
       <c r="J79" s="16" t="s">
         <v>83</v>
@@ -7789,7 +7787,7 @@
       <c r="M79" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="N79" s="16" t="s">
+      <c r="N79" t="s">
         <v>460</v>
       </c>
       <c r="O79" s="16" t="s">
@@ -7807,7 +7805,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="11">
         <v>73</v>
       </c>
@@ -7823,17 +7821,17 @@
       <c r="E80" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="F80" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G80" s="15" t="s">
-        <v>615</v>
-      </c>
-      <c r="H80" s="15" t="s">
-        <v>634</v>
-      </c>
-      <c r="I80" s="15" t="s">
-        <v>633</v>
+      <c r="F80" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G80" t="s">
+        <v>524</v>
+      </c>
+      <c r="H80" t="s">
+        <v>552</v>
+      </c>
+      <c r="I80" t="s">
+        <v>553</v>
       </c>
       <c r="J80" s="16" t="s">
         <v>83</v>
@@ -7845,7 +7843,7 @@
       <c r="M80" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="N80" s="16" t="s">
+      <c r="N80" t="s">
         <v>461</v>
       </c>
       <c r="O80" s="16" t="s">
@@ -7863,7 +7861,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="11">
         <v>74</v>
       </c>
@@ -7879,17 +7877,17 @@
       <c r="E81" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="F81" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G81" s="15" t="s">
-        <v>615</v>
-      </c>
-      <c r="H81" s="15" t="s">
-        <v>632</v>
-      </c>
-      <c r="I81" s="15" t="s">
-        <v>631</v>
+      <c r="F81" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G81" t="s">
+        <v>524</v>
+      </c>
+      <c r="H81" t="s">
+        <v>554</v>
+      </c>
+      <c r="I81" t="s">
+        <v>555</v>
       </c>
       <c r="J81" s="16" t="s">
         <v>83</v>
@@ -7901,7 +7899,7 @@
       <c r="M81" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="N81" s="16" t="s">
+      <c r="N81" t="s">
         <v>459</v>
       </c>
       <c r="O81" s="16" t="s">
@@ -9533,17 +9531,17 @@
       <c r="E129" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="F129" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G129" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H129" s="15" t="s">
-        <v>493</v>
-      </c>
-      <c r="I129" s="15" t="s">
-        <v>494</v>
+      <c r="F129" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G129" t="s">
+        <v>612</v>
+      </c>
+      <c r="H129" t="s">
+        <v>621</v>
+      </c>
+      <c r="I129" t="s">
+        <v>622</v>
       </c>
       <c r="J129" s="16" t="s">
         <v>83</v>
@@ -9587,17 +9585,17 @@
       <c r="E130" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="F130" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G130" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H130" s="15" t="s">
-        <v>495</v>
-      </c>
-      <c r="I130" s="15" t="s">
-        <v>496</v>
+      <c r="F130" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G130" t="s">
+        <v>612</v>
+      </c>
+      <c r="H130" t="s">
+        <v>623</v>
+      </c>
+      <c r="I130" t="s">
+        <v>624</v>
       </c>
       <c r="J130" s="16" t="s">
         <v>83</v>
@@ -9643,17 +9641,17 @@
       <c r="E131" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="F131" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G131" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H131" s="15" t="s">
-        <v>497</v>
-      </c>
-      <c r="I131" s="15" t="s">
-        <v>498</v>
+      <c r="F131" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G131" t="s">
+        <v>612</v>
+      </c>
+      <c r="H131" t="s">
+        <v>625</v>
+      </c>
+      <c r="I131" t="s">
+        <v>626</v>
       </c>
       <c r="J131" s="16" t="s">
         <v>83</v>
@@ -9699,17 +9697,17 @@
       <c r="E132" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="F132" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G132" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H132" s="15" t="s">
-        <v>499</v>
-      </c>
-      <c r="I132" s="15" t="s">
-        <v>500</v>
+      <c r="F132" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G132" t="s">
+        <v>612</v>
+      </c>
+      <c r="H132" t="s">
+        <v>627</v>
+      </c>
+      <c r="I132" t="s">
+        <v>628</v>
       </c>
       <c r="J132" s="16" t="s">
         <v>83</v>
@@ -9722,7 +9720,7 @@
         <v>83</v>
       </c>
       <c r="N132" s="16" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="O132" s="16" t="s">
         <v>83</v>
@@ -9733,7 +9731,7 @@
       <c r="Q132" s="16"/>
       <c r="R132" s="17"/>
       <c r="S132" s="18" t="s">
-        <v>564</v>
+        <v>513</v>
       </c>
       <c r="T132" s="16" t="s">
         <v>430</v>
@@ -9755,17 +9753,17 @@
       <c r="E133" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="F133" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G133" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H133" s="15" t="s">
-        <v>502</v>
-      </c>
-      <c r="I133" s="15" t="s">
-        <v>503</v>
+      <c r="F133" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G133" t="s">
+        <v>612</v>
+      </c>
+      <c r="H133" t="s">
+        <v>629</v>
+      </c>
+      <c r="I133" t="s">
+        <v>630</v>
       </c>
       <c r="J133" s="16" t="s">
         <v>83</v>
@@ -9778,7 +9776,7 @@
         <v>83</v>
       </c>
       <c r="N133" s="16" t="s">
-        <v>504</v>
+        <v>493</v>
       </c>
       <c r="O133" s="16" t="s">
         <v>83</v>
@@ -9789,7 +9787,7 @@
       <c r="Q133" s="16"/>
       <c r="R133" s="17"/>
       <c r="S133" s="18" t="s">
-        <v>564</v>
+        <v>513</v>
       </c>
       <c r="T133" s="16" t="s">
         <v>430</v>
@@ -9811,17 +9809,17 @@
       <c r="E134" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="F134" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G134" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H134" s="15" t="s">
-        <v>533</v>
-      </c>
-      <c r="I134" s="15" t="s">
-        <v>532</v>
+      <c r="F134" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G134" t="s">
+        <v>612</v>
+      </c>
+      <c r="H134" t="s">
+        <v>650</v>
+      </c>
+      <c r="I134" t="s">
+        <v>649</v>
       </c>
       <c r="J134" s="16" t="s">
         <v>83</v>
@@ -9834,7 +9832,7 @@
         <v>83</v>
       </c>
       <c r="N134" s="16" t="s">
-        <v>529</v>
+        <v>502</v>
       </c>
       <c r="O134" s="16" t="s">
         <v>83</v>
@@ -9845,7 +9843,7 @@
       <c r="Q134" s="16"/>
       <c r="R134" s="17"/>
       <c r="S134" s="18" t="s">
-        <v>565</v>
+        <v>514</v>
       </c>
       <c r="T134" s="16" t="s">
         <v>430</v>
@@ -9867,17 +9865,17 @@
       <c r="E135" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="F135" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G135" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H135" s="15" t="s">
-        <v>531</v>
-      </c>
-      <c r="I135" s="15" t="s">
-        <v>530</v>
+      <c r="F135" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G135" t="s">
+        <v>612</v>
+      </c>
+      <c r="H135" t="s">
+        <v>648</v>
+      </c>
+      <c r="I135" t="s">
+        <v>647</v>
       </c>
       <c r="J135" s="16" t="s">
         <v>83</v>
@@ -9890,7 +9888,7 @@
         <v>83</v>
       </c>
       <c r="N135" s="16" t="s">
-        <v>529</v>
+        <v>502</v>
       </c>
       <c r="O135" s="16" t="s">
         <v>83</v>
@@ -9901,7 +9899,7 @@
       <c r="Q135" s="16"/>
       <c r="R135" s="17"/>
       <c r="S135" s="18" t="s">
-        <v>565</v>
+        <v>514</v>
       </c>
       <c r="T135" s="16" t="s">
         <v>430</v>
@@ -9923,17 +9921,17 @@
       <c r="E136" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="F136" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G136" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H136" s="15" t="s">
-        <v>528</v>
-      </c>
-      <c r="I136" s="15" t="s">
-        <v>527</v>
+      <c r="F136" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G136" t="s">
+        <v>612</v>
+      </c>
+      <c r="H136" t="s">
+        <v>646</v>
+      </c>
+      <c r="I136" t="s">
+        <v>645</v>
       </c>
       <c r="J136" s="16" t="s">
         <v>83</v>
@@ -9946,7 +9944,7 @@
         <v>83</v>
       </c>
       <c r="N136" s="16" t="s">
-        <v>526</v>
+        <v>501</v>
       </c>
       <c r="O136" s="16" t="s">
         <v>83</v>
@@ -9979,17 +9977,17 @@
       <c r="E137" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="F137" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G137" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H137" s="15" t="s">
-        <v>525</v>
-      </c>
-      <c r="I137" s="15" t="s">
-        <v>524</v>
+      <c r="F137" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G137" t="s">
+        <v>612</v>
+      </c>
+      <c r="H137" t="s">
+        <v>644</v>
+      </c>
+      <c r="I137" t="s">
+        <v>643</v>
       </c>
       <c r="J137" s="16" t="s">
         <v>83</v>
@@ -10002,7 +10000,7 @@
         <v>83</v>
       </c>
       <c r="N137" s="16" t="s">
-        <v>523</v>
+        <v>500</v>
       </c>
       <c r="O137" s="16" t="s">
         <v>83</v>
@@ -10013,7 +10011,7 @@
       <c r="Q137" s="16"/>
       <c r="R137" s="17"/>
       <c r="S137" s="18" t="s">
-        <v>565</v>
+        <v>514</v>
       </c>
       <c r="T137" s="16" t="s">
         <v>430</v>
@@ -10035,17 +10033,17 @@
       <c r="E138" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="F138" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G138" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H138" s="15" t="s">
-        <v>522</v>
-      </c>
-      <c r="I138" s="15" t="s">
-        <v>521</v>
+      <c r="F138" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G138" t="s">
+        <v>612</v>
+      </c>
+      <c r="H138" t="s">
+        <v>642</v>
+      </c>
+      <c r="I138" t="s">
+        <v>641</v>
       </c>
       <c r="J138" s="16" t="s">
         <v>83</v>
@@ -10058,7 +10056,7 @@
         <v>83</v>
       </c>
       <c r="N138" s="16" t="s">
-        <v>520</v>
+        <v>499</v>
       </c>
       <c r="O138" s="16" t="s">
         <v>83</v>
@@ -10089,17 +10087,17 @@
       <c r="E139" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="F139" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G139" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H139" s="15" t="s">
-        <v>519</v>
-      </c>
-      <c r="I139" s="15" t="s">
-        <v>518</v>
+      <c r="F139" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G139" t="s">
+        <v>612</v>
+      </c>
+      <c r="H139" t="s">
+        <v>640</v>
+      </c>
+      <c r="I139" t="s">
+        <v>639</v>
       </c>
       <c r="J139" s="16" t="s">
         <v>83</v>
@@ -10112,7 +10110,7 @@
         <v>83</v>
       </c>
       <c r="N139" s="16" t="s">
-        <v>517</v>
+        <v>498</v>
       </c>
       <c r="O139" s="16" t="s">
         <v>83</v>
@@ -10145,17 +10143,17 @@
       <c r="E140" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="F140" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G140" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H140" s="15" t="s">
-        <v>516</v>
-      </c>
-      <c r="I140" s="15" t="s">
-        <v>515</v>
+      <c r="F140" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G140" t="s">
+        <v>612</v>
+      </c>
+      <c r="H140" t="s">
+        <v>638</v>
+      </c>
+      <c r="I140" t="s">
+        <v>637</v>
       </c>
       <c r="J140" s="16" t="s">
         <v>83</v>
@@ -10168,7 +10166,7 @@
         <v>83</v>
       </c>
       <c r="N140" s="16" t="s">
-        <v>514</v>
+        <v>497</v>
       </c>
       <c r="O140" s="16" t="s">
         <v>83</v>
@@ -10201,17 +10199,17 @@
       <c r="E141" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="F141" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G141" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H141" s="15" t="s">
-        <v>513</v>
-      </c>
-      <c r="I141" s="15" t="s">
-        <v>512</v>
+      <c r="F141" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G141" t="s">
+        <v>612</v>
+      </c>
+      <c r="H141" t="s">
+        <v>636</v>
+      </c>
+      <c r="I141" t="s">
+        <v>635</v>
       </c>
       <c r="J141" s="16" t="s">
         <v>83</v>
@@ -10224,7 +10222,7 @@
         <v>83</v>
       </c>
       <c r="N141" s="16" t="s">
-        <v>511</v>
+        <v>496</v>
       </c>
       <c r="O141" s="16" t="s">
         <v>83</v>
@@ -10235,7 +10233,7 @@
       <c r="Q141" s="16"/>
       <c r="R141" s="17"/>
       <c r="S141" s="18" t="s">
-        <v>566</v>
+        <v>515</v>
       </c>
       <c r="T141" s="16" t="s">
         <v>430</v>
@@ -10257,17 +10255,17 @@
       <c r="E142" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="F142" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G142" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H142" s="15" t="s">
-        <v>510</v>
-      </c>
-      <c r="I142" s="15" t="s">
-        <v>509</v>
+      <c r="F142" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G142" t="s">
+        <v>612</v>
+      </c>
+      <c r="H142" t="s">
+        <v>634</v>
+      </c>
+      <c r="I142" t="s">
+        <v>633</v>
       </c>
       <c r="J142" s="16" t="s">
         <v>83</v>
@@ -10280,7 +10278,7 @@
         <v>83</v>
       </c>
       <c r="N142" s="16" t="s">
-        <v>508</v>
+        <v>495</v>
       </c>
       <c r="O142" s="16" t="s">
         <v>83</v>
@@ -10313,17 +10311,17 @@
       <c r="E143" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F143" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G143" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H143" s="15" t="s">
-        <v>507</v>
-      </c>
-      <c r="I143" s="15" t="s">
-        <v>506</v>
+      <c r="F143" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G143" t="s">
+        <v>612</v>
+      </c>
+      <c r="H143" t="s">
+        <v>632</v>
+      </c>
+      <c r="I143" t="s">
+        <v>631</v>
       </c>
       <c r="J143" s="16" t="s">
         <v>83</v>
@@ -10336,7 +10334,7 @@
         <v>83</v>
       </c>
       <c r="N143" s="16" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="O143" s="16" t="s">
         <v>83</v>
@@ -10347,7 +10345,7 @@
       <c r="Q143" s="16"/>
       <c r="R143" s="17"/>
       <c r="S143" s="18" t="s">
-        <v>567</v>
+        <v>516</v>
       </c>
       <c r="T143" s="16" t="s">
         <v>430</v>
@@ -10369,17 +10367,17 @@
       <c r="E144" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="F144" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G144" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H144" s="15" t="s">
-        <v>534</v>
-      </c>
-      <c r="I144" s="15" t="s">
-        <v>535</v>
+      <c r="F144" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G144" t="s">
+        <v>612</v>
+      </c>
+      <c r="H144" t="s">
+        <v>670</v>
+      </c>
+      <c r="I144" t="s">
+        <v>669</v>
       </c>
       <c r="J144" s="16" t="s">
         <v>83</v>
@@ -10392,7 +10390,7 @@
         <v>83</v>
       </c>
       <c r="N144" s="16" t="s">
-        <v>536</v>
+        <v>503</v>
       </c>
       <c r="O144" s="16" t="s">
         <v>83</v>
@@ -10403,7 +10401,7 @@
       <c r="Q144" s="16"/>
       <c r="R144" s="17"/>
       <c r="S144" s="18" t="s">
-        <v>567</v>
+        <v>516</v>
       </c>
       <c r="T144" s="16" t="s">
         <v>430</v>
@@ -10425,17 +10423,17 @@
       <c r="E145" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="F145" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G145" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H145" s="15" t="s">
-        <v>537</v>
-      </c>
-      <c r="I145" s="15" t="s">
-        <v>538</v>
+      <c r="F145" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G145" t="s">
+        <v>612</v>
+      </c>
+      <c r="H145" t="s">
+        <v>668</v>
+      </c>
+      <c r="I145" t="s">
+        <v>667</v>
       </c>
       <c r="J145" s="16" t="s">
         <v>83</v>
@@ -10448,7 +10446,7 @@
         <v>83</v>
       </c>
       <c r="N145" s="16" t="s">
-        <v>539</v>
+        <v>504</v>
       </c>
       <c r="O145" s="16" t="s">
         <v>83</v>
@@ -10481,17 +10479,17 @@
       <c r="E146" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="F146" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G146" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H146" s="15" t="s">
-        <v>540</v>
-      </c>
-      <c r="I146" s="15" t="s">
-        <v>541</v>
+      <c r="F146" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G146" t="s">
+        <v>612</v>
+      </c>
+      <c r="H146" t="s">
+        <v>666</v>
+      </c>
+      <c r="I146" t="s">
+        <v>665</v>
       </c>
       <c r="J146" s="16" t="s">
         <v>83</v>
@@ -10504,7 +10502,7 @@
         <v>83</v>
       </c>
       <c r="N146" s="16" t="s">
-        <v>542</v>
+        <v>505</v>
       </c>
       <c r="O146" s="16" t="s">
         <v>83</v>
@@ -10537,17 +10535,17 @@
       <c r="E147" s="13" t="s">
         <v>279</v>
       </c>
-      <c r="F147" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G147" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H147" s="15" t="s">
-        <v>543</v>
-      </c>
-      <c r="I147" s="15" t="s">
-        <v>544</v>
+      <c r="F147" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G147" t="s">
+        <v>612</v>
+      </c>
+      <c r="H147" t="s">
+        <v>664</v>
+      </c>
+      <c r="I147" t="s">
+        <v>663</v>
       </c>
       <c r="J147" s="16" t="s">
         <v>83</v>
@@ -10560,7 +10558,7 @@
         <v>83</v>
       </c>
       <c r="N147" s="16" t="s">
-        <v>545</v>
+        <v>506</v>
       </c>
       <c r="O147" s="16" t="s">
         <v>83</v>
@@ -10593,17 +10591,17 @@
       <c r="E148" s="13" t="s">
         <v>281</v>
       </c>
-      <c r="F148" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G148" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H148" s="15" t="s">
-        <v>546</v>
-      </c>
-      <c r="I148" s="15" t="s">
-        <v>547</v>
+      <c r="F148" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G148" t="s">
+        <v>612</v>
+      </c>
+      <c r="H148" t="s">
+        <v>662</v>
+      </c>
+      <c r="I148" t="s">
+        <v>661</v>
       </c>
       <c r="J148" s="16" t="s">
         <v>83</v>
@@ -10616,7 +10614,7 @@
         <v>83</v>
       </c>
       <c r="N148" s="16" t="s">
-        <v>548</v>
+        <v>507</v>
       </c>
       <c r="O148" s="16" t="s">
         <v>83</v>
@@ -10649,17 +10647,17 @@
       <c r="E149" s="13" t="s">
         <v>283</v>
       </c>
-      <c r="F149" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G149" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H149" s="15" t="s">
-        <v>549</v>
-      </c>
-      <c r="I149" s="15" t="s">
-        <v>550</v>
+      <c r="F149" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G149" t="s">
+        <v>612</v>
+      </c>
+      <c r="H149" t="s">
+        <v>660</v>
+      </c>
+      <c r="I149" t="s">
+        <v>659</v>
       </c>
       <c r="J149" s="16" t="s">
         <v>83</v>
@@ -10672,7 +10670,7 @@
         <v>83</v>
       </c>
       <c r="N149" s="16" t="s">
-        <v>551</v>
+        <v>508</v>
       </c>
       <c r="O149" s="16" t="s">
         <v>83</v>
@@ -10705,17 +10703,17 @@
       <c r="E150" s="13" t="s">
         <v>285</v>
       </c>
-      <c r="F150" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G150" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H150" s="15" t="s">
-        <v>552</v>
-      </c>
-      <c r="I150" s="15" t="s">
-        <v>553</v>
+      <c r="F150" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G150" t="s">
+        <v>612</v>
+      </c>
+      <c r="H150" t="s">
+        <v>658</v>
+      </c>
+      <c r="I150" t="s">
+        <v>657</v>
       </c>
       <c r="J150" s="16" t="s">
         <v>83</v>
@@ -10728,7 +10726,7 @@
         <v>83</v>
       </c>
       <c r="N150" s="16" t="s">
-        <v>554</v>
+        <v>509</v>
       </c>
       <c r="O150" s="16" t="s">
         <v>83</v>
@@ -10761,17 +10759,17 @@
       <c r="E151" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="F151" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G151" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H151" s="15" t="s">
-        <v>555</v>
-      </c>
-      <c r="I151" s="15" t="s">
-        <v>556</v>
+      <c r="F151" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G151" t="s">
+        <v>612</v>
+      </c>
+      <c r="H151" t="s">
+        <v>656</v>
+      </c>
+      <c r="I151" t="s">
+        <v>655</v>
       </c>
       <c r="J151" s="16" t="s">
         <v>83</v>
@@ -10784,7 +10782,7 @@
         <v>83</v>
       </c>
       <c r="N151" s="16" t="s">
-        <v>557</v>
+        <v>510</v>
       </c>
       <c r="O151" s="16" t="s">
         <v>83</v>
@@ -10817,17 +10815,17 @@
       <c r="E152" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="F152" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G152" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H152" s="15" t="s">
-        <v>558</v>
-      </c>
-      <c r="I152" s="15" t="s">
-        <v>559</v>
+      <c r="F152" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G152" t="s">
+        <v>612</v>
+      </c>
+      <c r="H152" s="68" t="s">
+        <v>654</v>
+      </c>
+      <c r="I152" t="s">
+        <v>653</v>
       </c>
       <c r="J152" s="16" t="s">
         <v>83</v>
@@ -10840,7 +10838,7 @@
         <v>83</v>
       </c>
       <c r="N152" s="16" t="s">
-        <v>560</v>
+        <v>511</v>
       </c>
       <c r="O152" s="16" t="s">
         <v>83</v>
@@ -10857,7 +10855,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="153" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:20" ht="300" x14ac:dyDescent="0.25">
       <c r="A153" s="11">
         <v>146</v>
       </c>
@@ -10873,17 +10871,17 @@
       <c r="E153" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="F153" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G153" s="15" t="s">
-        <v>492</v>
-      </c>
-      <c r="H153" s="15" t="s">
-        <v>561</v>
-      </c>
-      <c r="I153" s="15" t="s">
-        <v>562</v>
+      <c r="F153" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G153" t="s">
+        <v>612</v>
+      </c>
+      <c r="H153" t="s">
+        <v>652</v>
+      </c>
+      <c r="I153" t="s">
+        <v>651</v>
       </c>
       <c r="J153" s="16" t="s">
         <v>83</v>
@@ -10896,7 +10894,7 @@
         <v>83</v>
       </c>
       <c r="N153" s="16" t="s">
-        <v>563</v>
+        <v>512</v>
       </c>
       <c r="O153" s="16" t="s">
         <v>83</v>
@@ -10913,7 +10911,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="154" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="11">
         <v>147</v>
       </c>
@@ -10929,17 +10927,17 @@
       <c r="E154" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="F154" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G154" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H154" s="15" t="s">
-        <v>569</v>
-      </c>
-      <c r="I154" s="15" t="s">
-        <v>570</v>
+      <c r="F154" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G154" t="s">
+        <v>560</v>
+      </c>
+      <c r="H154" t="s">
+        <v>561</v>
+      </c>
+      <c r="I154" t="s">
+        <v>562</v>
       </c>
       <c r="J154" s="16" t="s">
         <v>83</v>
@@ -10957,7 +10955,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="155" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="11">
         <v>148</v>
       </c>
@@ -10973,17 +10971,17 @@
       <c r="E155" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="F155" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G155" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H155" s="15" t="s">
-        <v>572</v>
-      </c>
-      <c r="I155" s="15" t="s">
-        <v>571</v>
+      <c r="F155" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G155" t="s">
+        <v>565</v>
+      </c>
+      <c r="H155" t="s">
+        <v>564</v>
+      </c>
+      <c r="I155" t="s">
+        <v>563</v>
       </c>
       <c r="J155" s="16" t="s">
         <v>83</v>
@@ -11001,7 +10999,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="11">
         <v>149</v>
       </c>
@@ -11017,17 +11015,17 @@
       <c r="E156" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="F156" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G156" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H156" s="15" t="s">
-        <v>573</v>
-      </c>
-      <c r="I156" s="15" t="s">
-        <v>574</v>
+      <c r="F156" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G156" t="s">
+        <v>565</v>
+      </c>
+      <c r="H156" t="s">
+        <v>566</v>
+      </c>
+      <c r="I156" t="s">
+        <v>567</v>
       </c>
       <c r="J156" s="16" t="s">
         <v>83</v>
@@ -11045,7 +11043,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="11">
         <v>150</v>
       </c>
@@ -11061,17 +11059,17 @@
       <c r="E157" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="F157" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G157" s="15" t="s">
+      <c r="F157" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G157" t="s">
+        <v>565</v>
+      </c>
+      <c r="H157" t="s">
         <v>568</v>
       </c>
-      <c r="H157" s="15" t="s">
-        <v>576</v>
-      </c>
-      <c r="I157" s="15" t="s">
-        <v>575</v>
+      <c r="I157" t="s">
+        <v>569</v>
       </c>
       <c r="J157" s="16" t="s">
         <v>83</v>
@@ -11089,7 +11087,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="158" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="11">
         <v>151</v>
       </c>
@@ -11105,17 +11103,17 @@
       <c r="E158" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="F158" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G158" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H158" s="15" t="s">
-        <v>580</v>
-      </c>
-      <c r="I158" s="15" t="s">
-        <v>579</v>
+      <c r="F158" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G158" t="s">
+        <v>565</v>
+      </c>
+      <c r="H158" t="s">
+        <v>570</v>
+      </c>
+      <c r="I158" t="s">
+        <v>571</v>
       </c>
       <c r="J158" s="16" t="s">
         <v>83</v>
@@ -11145,7 +11143,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="11">
         <v>152</v>
       </c>
@@ -11161,17 +11159,17 @@
       <c r="E159" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="F159" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G159" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H159" s="15" t="s">
-        <v>578</v>
-      </c>
-      <c r="I159" s="15" t="s">
-        <v>577</v>
+      <c r="F159" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G159" t="s">
+        <v>565</v>
+      </c>
+      <c r="H159" t="s">
+        <v>572</v>
+      </c>
+      <c r="I159" t="s">
+        <v>573</v>
       </c>
       <c r="J159" s="16" t="s">
         <v>83</v>
@@ -11199,7 +11197,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="160" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="11">
         <v>153</v>
       </c>
@@ -11215,17 +11213,17 @@
       <c r="E160" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="F160" s="14">
-        <v>45330</v>
-      </c>
-      <c r="G160" s="15" t="s">
-        <v>666</v>
-      </c>
-      <c r="H160" s="15" t="s">
-        <v>667</v>
-      </c>
-      <c r="I160" s="15" t="s">
-        <v>668</v>
+      <c r="F160" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G160" t="s">
+        <v>565</v>
+      </c>
+      <c r="H160" t="s">
+        <v>574</v>
+      </c>
+      <c r="I160" t="s">
+        <v>575</v>
       </c>
       <c r="J160" s="16" t="s">
         <v>83</v>
@@ -11253,7 +11251,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="11">
         <v>154</v>
       </c>
@@ -11269,17 +11267,17 @@
       <c r="E161" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="F161" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G161" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H161" s="15" t="s">
-        <v>581</v>
-      </c>
-      <c r="I161" s="15" t="s">
-        <v>582</v>
+      <c r="F161" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G161" t="s">
+        <v>565</v>
+      </c>
+      <c r="H161" t="s">
+        <v>576</v>
+      </c>
+      <c r="I161" t="s">
+        <v>577</v>
       </c>
       <c r="J161" s="16" t="s">
         <v>83</v>
@@ -11309,7 +11307,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="11">
         <v>155</v>
       </c>
@@ -11325,17 +11323,17 @@
       <c r="E162" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="F162" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G162" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H162" s="15" t="s">
-        <v>583</v>
-      </c>
-      <c r="I162" s="15" t="s">
-        <v>584</v>
+      <c r="F162" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G162" t="s">
+        <v>565</v>
+      </c>
+      <c r="H162" t="s">
+        <v>578</v>
+      </c>
+      <c r="I162" t="s">
+        <v>579</v>
       </c>
       <c r="J162" s="16" t="s">
         <v>83</v>
@@ -11365,7 +11363,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="11">
         <v>156</v>
       </c>
@@ -11381,17 +11379,17 @@
       <c r="E163" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="F163" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G163" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H163" s="15" t="s">
-        <v>604</v>
-      </c>
-      <c r="I163" s="15" t="s">
-        <v>603</v>
+      <c r="F163" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G163" t="s">
+        <v>565</v>
+      </c>
+      <c r="H163" t="s">
+        <v>580</v>
+      </c>
+      <c r="I163" t="s">
+        <v>581</v>
       </c>
       <c r="J163" s="16" t="s">
         <v>83</v>
@@ -11421,7 +11419,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="11">
         <v>157</v>
       </c>
@@ -11437,17 +11435,17 @@
       <c r="E164" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="F164" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G164" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H164" s="15" t="s">
-        <v>602</v>
-      </c>
-      <c r="I164" s="15" t="s">
-        <v>601</v>
+      <c r="F164" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G164" t="s">
+        <v>565</v>
+      </c>
+      <c r="H164" t="s">
+        <v>582</v>
+      </c>
+      <c r="I164" t="s">
+        <v>583</v>
       </c>
       <c r="J164" s="16" t="s">
         <v>83</v>
@@ -11477,7 +11475,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="11">
         <v>158</v>
       </c>
@@ -11493,17 +11491,17 @@
       <c r="E165" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="F165" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G165" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H165" s="15" t="s">
-        <v>600</v>
-      </c>
-      <c r="I165" s="15" t="s">
-        <v>599</v>
+      <c r="F165" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G165" t="s">
+        <v>565</v>
+      </c>
+      <c r="H165" t="s">
+        <v>584</v>
+      </c>
+      <c r="I165" t="s">
+        <v>585</v>
       </c>
       <c r="J165" s="16" t="s">
         <v>83</v>
@@ -11531,7 +11529,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="11">
         <v>159</v>
       </c>
@@ -11547,17 +11545,17 @@
       <c r="E166" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="F166" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G166" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H166" s="15" t="s">
-        <v>598</v>
-      </c>
-      <c r="I166" s="15" t="s">
-        <v>597</v>
+      <c r="F166" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G166" t="s">
+        <v>565</v>
+      </c>
+      <c r="H166" t="s">
+        <v>586</v>
+      </c>
+      <c r="I166" t="s">
+        <v>587</v>
       </c>
       <c r="J166" s="16" t="s">
         <v>83</v>
@@ -11587,7 +11585,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="11">
         <v>160</v>
       </c>
@@ -11603,17 +11601,17 @@
       <c r="E167" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="F167" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G167" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H167" s="15" t="s">
-        <v>596</v>
-      </c>
-      <c r="I167" s="15" t="s">
-        <v>595</v>
+      <c r="F167" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G167" t="s">
+        <v>565</v>
+      </c>
+      <c r="H167" t="s">
+        <v>588</v>
+      </c>
+      <c r="I167" t="s">
+        <v>589</v>
       </c>
       <c r="J167" s="16" t="s">
         <v>83</v>
@@ -11643,7 +11641,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="11">
         <v>161</v>
       </c>
@@ -11659,17 +11657,17 @@
       <c r="E168" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="F168" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G168" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H168" s="15" t="s">
-        <v>594</v>
-      </c>
-      <c r="I168" s="15" t="s">
-        <v>593</v>
+      <c r="F168" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G168" t="s">
+        <v>565</v>
+      </c>
+      <c r="H168" t="s">
+        <v>590</v>
+      </c>
+      <c r="I168" t="s">
+        <v>591</v>
       </c>
       <c r="J168" s="16" t="s">
         <v>83</v>
@@ -11699,7 +11697,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="345.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:20" ht="345" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="11">
         <v>162</v>
       </c>
@@ -11715,17 +11713,17 @@
       <c r="E169" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="F169" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G169" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H169" s="15" t="s">
+      <c r="F169" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G169" t="s">
+        <v>565</v>
+      </c>
+      <c r="H169" t="s">
         <v>592</v>
       </c>
-      <c r="I169" s="15" t="s">
-        <v>591</v>
+      <c r="I169" t="s">
+        <v>593</v>
       </c>
       <c r="J169" s="16" t="s">
         <v>83</v>
@@ -11755,7 +11753,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="11">
         <v>163</v>
       </c>
@@ -11771,17 +11769,17 @@
       <c r="E170" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="F170" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G170" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H170" s="15" t="s">
-        <v>590</v>
-      </c>
-      <c r="I170" s="15" t="s">
-        <v>589</v>
+      <c r="F170" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G170" t="s">
+        <v>565</v>
+      </c>
+      <c r="H170" t="s">
+        <v>594</v>
+      </c>
+      <c r="I170" t="s">
+        <v>595</v>
       </c>
       <c r="J170" s="16" t="s">
         <v>83</v>
@@ -11809,7 +11807,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="11">
         <v>164</v>
       </c>
@@ -11825,17 +11823,17 @@
       <c r="E171" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="F171" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G171" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H171" s="15" t="s">
-        <v>588</v>
-      </c>
-      <c r="I171" s="15" t="s">
-        <v>587</v>
+      <c r="F171" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G171" t="s">
+        <v>565</v>
+      </c>
+      <c r="H171" t="s">
+        <v>596</v>
+      </c>
+      <c r="I171" t="s">
+        <v>597</v>
       </c>
       <c r="J171" s="16" t="s">
         <v>83</v>
@@ -11865,7 +11863,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="11">
         <v>165</v>
       </c>
@@ -11881,17 +11879,17 @@
       <c r="E172" s="13" t="s">
         <v>353</v>
       </c>
-      <c r="F172" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G172" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H172" s="15" t="s">
-        <v>586</v>
-      </c>
-      <c r="I172" s="15" t="s">
-        <v>585</v>
+      <c r="F172" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G172" t="s">
+        <v>565</v>
+      </c>
+      <c r="H172" t="s">
+        <v>598</v>
+      </c>
+      <c r="I172" t="s">
+        <v>599</v>
       </c>
       <c r="J172" s="16" t="s">
         <v>83</v>
@@ -11921,7 +11919,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="11">
         <v>166</v>
       </c>
@@ -11937,17 +11935,17 @@
       <c r="E173" s="13" t="s">
         <v>354</v>
       </c>
-      <c r="F173" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G173" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H173" s="15" t="s">
-        <v>605</v>
-      </c>
-      <c r="I173" s="15" t="s">
-        <v>606</v>
+      <c r="F173" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G173" t="s">
+        <v>565</v>
+      </c>
+      <c r="H173" t="s">
+        <v>600</v>
+      </c>
+      <c r="I173" t="s">
+        <v>601</v>
       </c>
       <c r="J173" s="16" t="s">
         <v>83</v>
@@ -11977,7 +11975,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="11">
         <v>167</v>
       </c>
@@ -11993,17 +11991,17 @@
       <c r="E174" s="13" t="s">
         <v>355</v>
       </c>
-      <c r="F174" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G174" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H174" s="15" t="s">
-        <v>607</v>
-      </c>
-      <c r="I174" s="15" t="s">
-        <v>608</v>
+      <c r="F174" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G174" t="s">
+        <v>565</v>
+      </c>
+      <c r="H174" t="s">
+        <v>602</v>
+      </c>
+      <c r="I174" t="s">
+        <v>603</v>
       </c>
       <c r="J174" s="16" t="s">
         <v>83</v>
@@ -12033,7 +12031,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="11">
         <v>168</v>
       </c>
@@ -12049,17 +12047,17 @@
       <c r="E175" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="F175" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G175" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H175" s="15" t="s">
-        <v>609</v>
-      </c>
-      <c r="I175" s="15" t="s">
-        <v>610</v>
+      <c r="F175" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G175" t="s">
+        <v>565</v>
+      </c>
+      <c r="H175" t="s">
+        <v>604</v>
+      </c>
+      <c r="I175" t="s">
+        <v>605</v>
       </c>
       <c r="J175" s="16" t="s">
         <v>83</v>
@@ -12089,7 +12087,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="129.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:20" ht="129.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="11">
         <v>169</v>
       </c>
@@ -12105,17 +12103,17 @@
       <c r="E176" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="F176" s="14">
-        <v>45327</v>
-      </c>
-      <c r="G176" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="H176" s="15" t="s">
-        <v>611</v>
-      </c>
-      <c r="I176" s="15" t="s">
-        <v>612</v>
+      <c r="F176" s="67">
+        <v>45981</v>
+      </c>
+      <c r="G176" t="s">
+        <v>565</v>
+      </c>
+      <c r="H176" t="s">
+        <v>606</v>
+      </c>
+      <c r="I176" t="s">
+        <v>607</v>
       </c>
       <c r="J176" s="16" t="s">
         <v>83</v>
@@ -26412,11 +26410,12 @@
   <autoFilter ref="A9:T198" xr:uid="{00000000-0001-0000-0100-000000000000}">
     <filterColumn colId="2">
       <filters>
-        <filter val="LDO"/>
-        <filter val="RSA"/>
         <filter val="VPS"/>
       </filters>
     </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A39:T176">
+      <sortCondition ref="A9:A198"/>
+    </sortState>
   </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
@@ -28657,26 +28656,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -28907,32 +28886,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB221413-913B-41FE-97D3-5428BD0403A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28951,6 +28925,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Accreditamento VPS, RSA, LDO v.3.0.1
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
+++ b/GATEWAY/S1#111MEDARCHIVER/MEDARCHIVER/MEDARCHIVER_FSE2.0/1.0.0.0/accreditamento-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gzamparo\Documents\FSE 2.0\it-fse-accreditamento\GATEWAY\S1#111MEDARCHIVER\MEDARCHIVER\MEDARCHIVER_FSE2.0\1.0.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBA9D9C-4D92-44A6-8543-DD31C02D673F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78439749-9497-4907-92C8-68914BC07692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1661" uniqueCount="628">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1726,9 +1726,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.0b94b867385907ec26d38994ebb6a3c258644486124e50ecf9ff0dc20b97a316.32741491de^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>[ERRORE-11| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i sotto-elementi 'country', 'city' e 'streetAddressLine' ]</t>
@@ -4390,10 +4387,10 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D94" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="O12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H99" sqref="H99"/>
+      <selection pane="bottomRight" activeCell="V28" sqref="V28:V43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4440,7 +4437,7 @@
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="51" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D2" s="50"/>
       <c r="F2" s="6"/>
@@ -4468,7 +4465,7 @@
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="58" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D3" s="50"/>
       <c r="F3" s="6"/>
@@ -4494,7 +4491,7 @@
       <c r="A4" s="54"/>
       <c r="B4" s="55"/>
       <c r="C4" s="58" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D4" s="50"/>
       <c r="E4" s="4"/>
@@ -4521,7 +4518,7 @@
       <c r="A5" s="56"/>
       <c r="B5" s="57"/>
       <c r="C5" s="58" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D5" s="50"/>
       <c r="F5" s="6"/>
@@ -4774,13 +4771,13 @@
         <v>45985</v>
       </c>
       <c r="G12" s="37" t="s">
+        <v>481</v>
+      </c>
+      <c r="H12" s="37" t="s">
         <v>482</v>
       </c>
-      <c r="H12" s="37" t="s">
-        <v>483</v>
-      </c>
       <c r="I12" s="42" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J12" s="38" t="s">
         <v>64</v>
@@ -4794,7 +4791,7 @@
         <v>64</v>
       </c>
       <c r="O12" s="38" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="P12" s="38" t="s">
         <v>64</v>
@@ -4802,12 +4799,12 @@
       <c r="Q12" s="38"/>
       <c r="R12" s="38"/>
       <c r="S12" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T12" s="38"/>
       <c r="U12" s="39"/>
       <c r="V12" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W12" s="38" t="s">
         <v>44</v>
@@ -4907,13 +4904,13 @@
         <v>45985</v>
       </c>
       <c r="G15" s="37" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="H15" s="37" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I15" s="42" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J15" s="38" t="s">
         <v>64</v>
@@ -4927,7 +4924,7 @@
         <v>64</v>
       </c>
       <c r="O15" s="38" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="P15" s="38" t="s">
         <v>64</v>
@@ -4935,12 +4932,12 @@
       <c r="Q15" s="38"/>
       <c r="R15" s="38"/>
       <c r="S15" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T15" s="38"/>
       <c r="U15" s="39"/>
       <c r="V15" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W15" s="38" t="s">
         <v>44</v>
@@ -5040,13 +5037,13 @@
         <v>45986</v>
       </c>
       <c r="G18" s="37" t="s">
+        <v>547</v>
+      </c>
+      <c r="H18" s="37" t="s">
         <v>548</v>
       </c>
-      <c r="H18" s="37" t="s">
-        <v>549</v>
-      </c>
       <c r="I18" s="42" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J18" s="38" t="s">
         <v>64</v>
@@ -5060,7 +5057,7 @@
         <v>64</v>
       </c>
       <c r="O18" s="38" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="P18" s="38" t="s">
         <v>64</v>
@@ -5068,12 +5065,12 @@
       <c r="Q18" s="38"/>
       <c r="R18" s="38"/>
       <c r="S18" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T18" s="38"/>
       <c r="U18" s="39"/>
       <c r="V18" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W18" s="38" t="s">
         <v>44</v>
@@ -5136,13 +5133,13 @@
         <v>45985</v>
       </c>
       <c r="G20" s="37" t="s">
+        <v>478</v>
+      </c>
+      <c r="H20" s="37" t="s">
         <v>479</v>
       </c>
-      <c r="H20" s="37" t="s">
-        <v>480</v>
-      </c>
       <c r="I20" s="42" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J20" s="38" t="s">
         <v>64</v>
@@ -5156,7 +5153,7 @@
         <v>64</v>
       </c>
       <c r="O20" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="P20" s="38" t="s">
         <v>64</v>
@@ -5164,12 +5161,12 @@
       <c r="Q20" s="38"/>
       <c r="R20" s="38"/>
       <c r="S20" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T20" s="38"/>
       <c r="U20" s="39"/>
       <c r="V20" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W20" s="38" t="s">
         <v>44</v>
@@ -5269,23 +5266,19 @@
         <v>45985</v>
       </c>
       <c r="G23" s="37" t="s">
+        <v>542</v>
+      </c>
+      <c r="H23" s="37" t="s">
         <v>543</v>
       </c>
-      <c r="H23" s="37" t="s">
-        <v>544</v>
-      </c>
       <c r="I23" s="42" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J23" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K23" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="L23" s="38" t="s">
-        <v>442</v>
-      </c>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
       <c r="M23" s="38" t="s">
         <v>64</v>
       </c>
@@ -5293,7 +5286,7 @@
         <v>64</v>
       </c>
       <c r="O23" s="38" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="P23" s="38" t="s">
         <v>64</v>
@@ -5301,12 +5294,12 @@
       <c r="Q23" s="38"/>
       <c r="R23" s="38"/>
       <c r="S23" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T23" s="38"/>
       <c r="U23" s="39"/>
       <c r="V23" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W23" s="38" t="s">
         <v>44</v>
@@ -5406,13 +5399,13 @@
         <v>45986</v>
       </c>
       <c r="G26" s="37" t="s">
+        <v>545</v>
+      </c>
+      <c r="H26" s="37" t="s">
         <v>546</v>
       </c>
-      <c r="H26" s="37" t="s">
-        <v>547</v>
-      </c>
       <c r="I26" s="42" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J26" s="38" t="s">
         <v>64</v>
@@ -5426,7 +5419,7 @@
         <v>64</v>
       </c>
       <c r="O26" s="38" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="P26" s="38" t="s">
         <v>64</v>
@@ -5434,12 +5427,12 @@
       <c r="Q26" s="38"/>
       <c r="R26" s="38"/>
       <c r="S26" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T26" s="38"/>
       <c r="U26" s="39"/>
       <c r="V26" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W26" s="38" t="s">
         <v>44</v>
@@ -5516,7 +5509,7 @@
         <v>64</v>
       </c>
       <c r="O28" s="38" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="P28" s="38" t="s">
         <v>64</v>
@@ -5524,7 +5517,7 @@
       <c r="Q28" s="38"/>
       <c r="R28" s="38"/>
       <c r="S28" s="45" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="T28" s="38"/>
       <c r="U28" s="39" t="s">
@@ -5645,7 +5638,7 @@
         <v>64</v>
       </c>
       <c r="O31" s="38" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="P31" s="38" t="s">
         <v>64</v>
@@ -5653,7 +5646,7 @@
       <c r="Q31" s="38"/>
       <c r="R31" s="38"/>
       <c r="S31" s="45" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="T31" s="38"/>
       <c r="U31" s="39" t="s">
@@ -5774,7 +5767,7 @@
         <v>64</v>
       </c>
       <c r="O34" s="38" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="P34" s="38" t="s">
         <v>64</v>
@@ -5782,7 +5775,7 @@
       <c r="Q34" s="38"/>
       <c r="R34" s="38"/>
       <c r="S34" s="45" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="T34" s="38"/>
       <c r="U34" s="39" t="s">
@@ -6129,7 +6122,7 @@
         <v>64</v>
       </c>
       <c r="O43" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P43" s="38" t="s">
         <v>64</v>
@@ -6137,7 +6130,7 @@
       <c r="Q43" s="38"/>
       <c r="R43" s="38"/>
       <c r="S43" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T43" s="38"/>
       <c r="U43" s="39"/>
@@ -6177,20 +6170,16 @@
       <c r="J44" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="K44" s="38" t="s">
+      <c r="K44" s="38"/>
+      <c r="L44" s="38"/>
+      <c r="M44" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="N44" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="O44" s="38" t="s">
         <v>442</v>
-      </c>
-      <c r="L44" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="M44" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="N44" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="O44" s="38" t="s">
-        <v>443</v>
       </c>
       <c r="P44" s="45" t="s">
         <v>64</v>
@@ -6198,12 +6187,12 @@
       <c r="Q44" s="38"/>
       <c r="R44" s="38"/>
       <c r="S44" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T44" s="38"/>
       <c r="U44" s="39"/>
       <c r="V44" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W44" s="38" t="s">
         <v>44</v>
@@ -6232,28 +6221,24 @@
         <v>437</v>
       </c>
       <c r="H45" s="37" t="s">
+        <v>443</v>
+      </c>
+      <c r="I45" s="42" t="s">
         <v>444</v>
       </c>
-      <c r="I45" s="42" t="s">
+      <c r="J45" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="K45" s="38"/>
+      <c r="L45" s="38"/>
+      <c r="M45" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="N45" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="O45" s="38" t="s">
         <v>445</v>
-      </c>
-      <c r="J45" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="K45" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="L45" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="M45" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="N45" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="O45" s="38" t="s">
-        <v>446</v>
       </c>
       <c r="P45" s="45" t="s">
         <v>64</v>
@@ -6261,12 +6246,12 @@
       <c r="Q45" s="38"/>
       <c r="R45" s="38"/>
       <c r="S45" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T45" s="38"/>
       <c r="U45" s="39"/>
       <c r="V45" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W45" s="38" t="s">
         <v>44</v>
@@ -6295,28 +6280,24 @@
         <v>437</v>
       </c>
       <c r="H46" s="37" t="s">
+        <v>446</v>
+      </c>
+      <c r="I46" s="42" t="s">
         <v>447</v>
       </c>
-      <c r="I46" s="42" t="s">
+      <c r="J46" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="K46" s="38"/>
+      <c r="L46" s="38"/>
+      <c r="M46" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="N46" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="O46" s="38" t="s">
         <v>448</v>
-      </c>
-      <c r="J46" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="K46" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="L46" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="M46" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="N46" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="O46" s="38" t="s">
-        <v>449</v>
       </c>
       <c r="P46" s="45" t="s">
         <v>64</v>
@@ -6324,12 +6305,12 @@
       <c r="Q46" s="38"/>
       <c r="R46" s="38"/>
       <c r="S46" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T46" s="38"/>
       <c r="U46" s="39"/>
       <c r="V46" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W46" s="38" t="s">
         <v>44</v>
@@ -6358,28 +6339,24 @@
         <v>437</v>
       </c>
       <c r="H47" s="37" t="s">
+        <v>449</v>
+      </c>
+      <c r="I47" s="42" t="s">
         <v>450</v>
       </c>
-      <c r="I47" s="42" t="s">
+      <c r="J47" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="K47" s="38"/>
+      <c r="L47" s="38"/>
+      <c r="M47" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="N47" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="O47" s="38" t="s">
         <v>451</v>
-      </c>
-      <c r="J47" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="K47" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="L47" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="M47" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="N47" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="O47" s="38" t="s">
-        <v>452</v>
       </c>
       <c r="P47" s="45" t="s">
         <v>64</v>
@@ -6387,12 +6364,12 @@
       <c r="Q47" s="38"/>
       <c r="R47" s="38"/>
       <c r="S47" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T47" s="38"/>
       <c r="U47" s="39"/>
       <c r="V47" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W47" s="38" t="s">
         <v>44</v>
@@ -6421,28 +6398,24 @@
         <v>437</v>
       </c>
       <c r="H48" s="37" t="s">
+        <v>452</v>
+      </c>
+      <c r="I48" s="42" t="s">
         <v>453</v>
       </c>
-      <c r="I48" s="42" t="s">
+      <c r="J48" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="K48" s="38"/>
+      <c r="L48" s="38"/>
+      <c r="M48" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="N48" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="O48" s="38" t="s">
         <v>454</v>
-      </c>
-      <c r="J48" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="K48" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="L48" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="M48" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="N48" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="O48" s="38" t="s">
-        <v>455</v>
       </c>
       <c r="P48" s="45" t="s">
         <v>64</v>
@@ -6450,12 +6423,12 @@
       <c r="Q48" s="38"/>
       <c r="R48" s="38"/>
       <c r="S48" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T48" s="38"/>
       <c r="U48" s="39"/>
       <c r="V48" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W48" s="38" t="s">
         <v>44</v>
@@ -6484,28 +6457,24 @@
         <v>437</v>
       </c>
       <c r="H49" s="37" t="s">
+        <v>455</v>
+      </c>
+      <c r="I49" s="42" t="s">
         <v>456</v>
       </c>
-      <c r="I49" s="42" t="s">
+      <c r="J49" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="K49" s="38"/>
+      <c r="L49" s="38"/>
+      <c r="M49" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="N49" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="O49" s="38" t="s">
         <v>457</v>
-      </c>
-      <c r="J49" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="K49" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="L49" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="M49" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="N49" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="O49" s="38" t="s">
-        <v>458</v>
       </c>
       <c r="P49" s="45" t="s">
         <v>64</v>
@@ -6513,12 +6482,12 @@
       <c r="Q49" s="38"/>
       <c r="R49" s="38"/>
       <c r="S49" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T49" s="38"/>
       <c r="U49" s="39"/>
       <c r="V49" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W49" s="38" t="s">
         <v>44</v>
@@ -6547,28 +6516,24 @@
         <v>437</v>
       </c>
       <c r="H50" s="37" t="s">
+        <v>458</v>
+      </c>
+      <c r="I50" s="42" t="s">
         <v>459</v>
       </c>
-      <c r="I50" s="42" t="s">
+      <c r="J50" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="K50" s="38"/>
+      <c r="L50" s="38"/>
+      <c r="M50" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="N50" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="O50" s="38" t="s">
         <v>460</v>
-      </c>
-      <c r="J50" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="K50" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="L50" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="M50" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="N50" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="O50" s="38" t="s">
-        <v>461</v>
       </c>
       <c r="P50" s="45" t="s">
         <v>64</v>
@@ -6576,12 +6541,12 @@
       <c r="Q50" s="38"/>
       <c r="R50" s="38"/>
       <c r="S50" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T50" s="38"/>
       <c r="U50" s="39"/>
       <c r="V50" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W50" s="38" t="s">
         <v>44</v>
@@ -6610,28 +6575,24 @@
         <v>437</v>
       </c>
       <c r="H51" s="37" t="s">
+        <v>461</v>
+      </c>
+      <c r="I51" s="42" t="s">
         <v>462</v>
       </c>
-      <c r="I51" s="42" t="s">
+      <c r="J51" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="K51" s="38"/>
+      <c r="L51" s="38"/>
+      <c r="M51" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="N51" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="O51" s="38" t="s">
         <v>463</v>
-      </c>
-      <c r="J51" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="K51" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="L51" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="M51" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="N51" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="O51" s="38" t="s">
-        <v>464</v>
       </c>
       <c r="P51" s="45" t="s">
         <v>64</v>
@@ -6639,12 +6600,12 @@
       <c r="Q51" s="38"/>
       <c r="R51" s="38"/>
       <c r="S51" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T51" s="38"/>
       <c r="U51" s="39"/>
       <c r="V51" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W51" s="38" t="s">
         <v>44</v>
@@ -6673,28 +6634,24 @@
         <v>437</v>
       </c>
       <c r="H52" s="37" t="s">
+        <v>464</v>
+      </c>
+      <c r="I52" s="42" t="s">
         <v>465</v>
       </c>
-      <c r="I52" s="42" t="s">
+      <c r="J52" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="K52" s="38"/>
+      <c r="L52" s="38"/>
+      <c r="M52" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="N52" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="O52" s="38" t="s">
         <v>466</v>
-      </c>
-      <c r="J52" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="K52" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="L52" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="M52" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="N52" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="O52" s="38" t="s">
-        <v>467</v>
       </c>
       <c r="P52" s="45" t="s">
         <v>64</v>
@@ -6702,12 +6659,12 @@
       <c r="Q52" s="38"/>
       <c r="R52" s="38"/>
       <c r="S52" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T52" s="38"/>
       <c r="U52" s="39"/>
       <c r="V52" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W52" s="38" t="s">
         <v>44</v>
@@ -8213,13 +8170,13 @@
         <v>45986</v>
       </c>
       <c r="G93" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H93" s="37" t="s">
+        <v>615</v>
+      </c>
+      <c r="I93" s="42" t="s">
         <v>616</v>
-      </c>
-      <c r="I93" s="42" t="s">
-        <v>617</v>
       </c>
       <c r="J93" s="38" t="s">
         <v>64</v>
@@ -8233,7 +8190,7 @@
         <v>64</v>
       </c>
       <c r="O93" s="38" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P93" s="45" t="s">
         <v>64</v>
@@ -8241,12 +8198,12 @@
       <c r="Q93" s="38"/>
       <c r="R93" s="38"/>
       <c r="S93" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T93" s="38"/>
       <c r="U93" s="39"/>
       <c r="V93" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W93" s="38" t="s">
         <v>44</v>
@@ -8272,13 +8229,13 @@
         <v>45986</v>
       </c>
       <c r="G94" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H94" s="37" t="s">
+        <v>617</v>
+      </c>
+      <c r="I94" s="42" t="s">
         <v>618</v>
-      </c>
-      <c r="I94" s="42" t="s">
-        <v>619</v>
       </c>
       <c r="J94" s="38" t="s">
         <v>64</v>
@@ -8292,7 +8249,7 @@
         <v>64</v>
       </c>
       <c r="O94" s="38" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="P94" s="45" t="s">
         <v>64</v>
@@ -8300,12 +8257,12 @@
       <c r="Q94" s="38"/>
       <c r="R94" s="38"/>
       <c r="S94" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T94" s="38"/>
       <c r="U94" s="39"/>
       <c r="V94" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W94" s="38" t="s">
         <v>44</v>
@@ -8331,13 +8288,13 @@
         <v>45986</v>
       </c>
       <c r="G95" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H95" s="37" t="s">
+        <v>619</v>
+      </c>
+      <c r="I95" s="42" t="s">
         <v>620</v>
-      </c>
-      <c r="I95" s="42" t="s">
-        <v>621</v>
       </c>
       <c r="J95" s="38" t="s">
         <v>64</v>
@@ -8351,7 +8308,7 @@
         <v>64</v>
       </c>
       <c r="O95" s="38" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="P95" s="45" t="s">
         <v>64</v>
@@ -8359,12 +8316,12 @@
       <c r="Q95" s="38"/>
       <c r="R95" s="38"/>
       <c r="S95" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T95" s="38"/>
       <c r="U95" s="39"/>
       <c r="V95" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W95" s="38" t="s">
         <v>44</v>
@@ -8390,13 +8347,13 @@
         <v>45986</v>
       </c>
       <c r="G96" s="37" t="s">
+        <v>549</v>
+      </c>
+      <c r="H96" s="37" t="s">
         <v>550</v>
       </c>
-      <c r="H96" s="37" t="s">
+      <c r="I96" s="42" t="s">
         <v>551</v>
-      </c>
-      <c r="I96" s="42" t="s">
-        <v>552</v>
       </c>
       <c r="J96" s="38" t="s">
         <v>64</v>
@@ -8410,7 +8367,7 @@
         <v>64</v>
       </c>
       <c r="O96" s="38" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="P96" s="45" t="s">
         <v>64</v>
@@ -8418,12 +8375,12 @@
       <c r="Q96" s="38"/>
       <c r="R96" s="38"/>
       <c r="S96" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T96" s="38"/>
       <c r="U96" s="39"/>
       <c r="V96" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W96" s="38" t="s">
         <v>44</v>
@@ -8449,13 +8406,13 @@
         <v>45986</v>
       </c>
       <c r="G97" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H97" s="37" t="s">
+        <v>552</v>
+      </c>
+      <c r="I97" s="42" t="s">
         <v>553</v>
-      </c>
-      <c r="I97" s="42" t="s">
-        <v>554</v>
       </c>
       <c r="J97" s="38" t="s">
         <v>64</v>
@@ -8469,7 +8426,7 @@
         <v>64</v>
       </c>
       <c r="O97" s="38" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="P97" s="45" t="s">
         <v>64</v>
@@ -8477,12 +8434,12 @@
       <c r="Q97" s="38"/>
       <c r="R97" s="38"/>
       <c r="S97" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T97" s="38"/>
       <c r="U97" s="39"/>
       <c r="V97" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W97" s="38" t="s">
         <v>44</v>
@@ -8508,13 +8465,13 @@
         <v>45986</v>
       </c>
       <c r="G98" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H98" s="37" t="s">
+        <v>554</v>
+      </c>
+      <c r="I98" s="42" t="s">
         <v>555</v>
-      </c>
-      <c r="I98" s="42" t="s">
-        <v>556</v>
       </c>
       <c r="J98" s="38" t="s">
         <v>64</v>
@@ -8528,7 +8485,7 @@
         <v>64</v>
       </c>
       <c r="O98" s="38" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="P98" s="45" t="s">
         <v>64</v>
@@ -8536,12 +8493,12 @@
       <c r="Q98" s="38"/>
       <c r="R98" s="38"/>
       <c r="S98" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T98" s="38"/>
       <c r="U98" s="39"/>
       <c r="V98" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W98" s="38" t="s">
         <v>44</v>
@@ -8567,13 +8524,13 @@
         <v>45986</v>
       </c>
       <c r="G99" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H99" s="37" t="s">
+        <v>556</v>
+      </c>
+      <c r="I99" s="42" t="s">
         <v>557</v>
-      </c>
-      <c r="I99" s="42" t="s">
-        <v>558</v>
       </c>
       <c r="J99" s="38" t="s">
         <v>64</v>
@@ -8587,7 +8544,7 @@
         <v>64</v>
       </c>
       <c r="O99" s="38" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="P99" s="45" t="s">
         <v>64</v>
@@ -8595,12 +8552,12 @@
       <c r="Q99" s="38"/>
       <c r="R99" s="38"/>
       <c r="S99" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T99" s="38"/>
       <c r="U99" s="39"/>
       <c r="V99" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W99" s="38" t="s">
         <v>44</v>
@@ -8626,13 +8583,13 @@
         <v>45986</v>
       </c>
       <c r="G100" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H100" s="37" t="s">
+        <v>558</v>
+      </c>
+      <c r="I100" s="42" t="s">
         <v>559</v>
-      </c>
-      <c r="I100" s="42" t="s">
-        <v>560</v>
       </c>
       <c r="J100" s="38" t="s">
         <v>64</v>
@@ -8646,7 +8603,7 @@
         <v>64</v>
       </c>
       <c r="O100" s="38" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="P100" s="45" t="s">
         <v>64</v>
@@ -8654,12 +8611,12 @@
       <c r="Q100" s="38"/>
       <c r="R100" s="38"/>
       <c r="S100" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T100" s="38"/>
       <c r="U100" s="39"/>
       <c r="V100" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W100" s="38" t="s">
         <v>44</v>
@@ -8685,13 +8642,13 @@
         <v>45986</v>
       </c>
       <c r="G101" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H101" s="37" t="s">
+        <v>560</v>
+      </c>
+      <c r="I101" s="42" t="s">
         <v>561</v>
-      </c>
-      <c r="I101" s="42" t="s">
-        <v>562</v>
       </c>
       <c r="J101" s="38" t="s">
         <v>64</v>
@@ -8705,7 +8662,7 @@
         <v>64</v>
       </c>
       <c r="O101" s="38" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="P101" s="45" t="s">
         <v>64</v>
@@ -8713,12 +8670,12 @@
       <c r="Q101" s="38"/>
       <c r="R101" s="38"/>
       <c r="S101" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T101" s="38"/>
       <c r="U101" s="39"/>
       <c r="V101" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W101" s="38" t="s">
         <v>44</v>
@@ -8744,13 +8701,13 @@
         <v>45986</v>
       </c>
       <c r="G102" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H102" s="37" t="s">
+        <v>562</v>
+      </c>
+      <c r="I102" s="42" t="s">
         <v>563</v>
-      </c>
-      <c r="I102" s="42" t="s">
-        <v>564</v>
       </c>
       <c r="J102" s="38" t="s">
         <v>64</v>
@@ -8764,7 +8721,7 @@
         <v>64</v>
       </c>
       <c r="O102" s="38" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="P102" s="45" t="s">
         <v>64</v>
@@ -8772,12 +8729,12 @@
       <c r="Q102" s="38"/>
       <c r="R102" s="38"/>
       <c r="S102" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T102" s="38"/>
       <c r="U102" s="39"/>
       <c r="V102" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W102" s="38" t="s">
         <v>44</v>
@@ -8803,13 +8760,13 @@
         <v>45986</v>
       </c>
       <c r="G103" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H103" s="37" t="s">
+        <v>564</v>
+      </c>
+      <c r="I103" s="42" t="s">
         <v>565</v>
-      </c>
-      <c r="I103" s="42" t="s">
-        <v>566</v>
       </c>
       <c r="J103" s="38" t="s">
         <v>64</v>
@@ -8823,7 +8780,7 @@
         <v>64</v>
       </c>
       <c r="O103" s="38" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="P103" s="45" t="s">
         <v>64</v>
@@ -8831,12 +8788,12 @@
       <c r="Q103" s="38"/>
       <c r="R103" s="38"/>
       <c r="S103" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T103" s="38"/>
       <c r="U103" s="39"/>
       <c r="V103" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W103" s="38" t="s">
         <v>44</v>
@@ -8862,13 +8819,13 @@
         <v>45986</v>
       </c>
       <c r="G104" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H104" s="37" t="s">
+        <v>566</v>
+      </c>
+      <c r="I104" s="42" t="s">
         <v>567</v>
-      </c>
-      <c r="I104" s="42" t="s">
-        <v>568</v>
       </c>
       <c r="J104" s="38" t="s">
         <v>64</v>
@@ -8882,7 +8839,7 @@
         <v>64</v>
       </c>
       <c r="O104" s="38" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="P104" s="45" t="s">
         <v>64</v>
@@ -8890,12 +8847,12 @@
       <c r="Q104" s="38"/>
       <c r="R104" s="38"/>
       <c r="S104" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T104" s="38"/>
       <c r="U104" s="39"/>
       <c r="V104" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W104" s="38" t="s">
         <v>44</v>
@@ -8921,13 +8878,13 @@
         <v>45986</v>
       </c>
       <c r="G105" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H105" s="37" t="s">
+        <v>568</v>
+      </c>
+      <c r="I105" s="42" t="s">
         <v>569</v>
-      </c>
-      <c r="I105" s="42" t="s">
-        <v>570</v>
       </c>
       <c r="J105" s="38" t="s">
         <v>64</v>
@@ -8941,7 +8898,7 @@
         <v>64</v>
       </c>
       <c r="O105" s="38" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="P105" s="45" t="s">
         <v>64</v>
@@ -8949,12 +8906,12 @@
       <c r="Q105" s="38"/>
       <c r="R105" s="38"/>
       <c r="S105" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T105" s="38"/>
       <c r="U105" s="39"/>
       <c r="V105" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W105" s="38" t="s">
         <v>44</v>
@@ -8980,13 +8937,13 @@
         <v>45986</v>
       </c>
       <c r="G106" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H106" s="37" t="s">
+        <v>570</v>
+      </c>
+      <c r="I106" s="42" t="s">
         <v>571</v>
-      </c>
-      <c r="I106" s="42" t="s">
-        <v>572</v>
       </c>
       <c r="J106" s="38" t="s">
         <v>64</v>
@@ -9000,7 +8957,7 @@
         <v>64</v>
       </c>
       <c r="O106" s="38" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="P106" s="45" t="s">
         <v>64</v>
@@ -9008,12 +8965,12 @@
       <c r="Q106" s="38"/>
       <c r="R106" s="38"/>
       <c r="S106" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T106" s="38"/>
       <c r="U106" s="39"/>
       <c r="V106" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W106" s="38" t="s">
         <v>44</v>
@@ -9039,13 +8996,13 @@
         <v>45986</v>
       </c>
       <c r="G107" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H107" s="37" t="s">
+        <v>572</v>
+      </c>
+      <c r="I107" s="42" t="s">
         <v>573</v>
-      </c>
-      <c r="I107" s="42" t="s">
-        <v>574</v>
       </c>
       <c r="J107" s="38" t="s">
         <v>64</v>
@@ -9059,7 +9016,7 @@
         <v>64</v>
       </c>
       <c r="O107" s="38" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="P107" s="45" t="s">
         <v>64</v>
@@ -9067,12 +9024,12 @@
       <c r="Q107" s="38"/>
       <c r="R107" s="38"/>
       <c r="S107" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T107" s="38"/>
       <c r="U107" s="39"/>
       <c r="V107" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W107" s="38" t="s">
         <v>44</v>
@@ -9098,13 +9055,13 @@
         <v>45986</v>
       </c>
       <c r="G108" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H108" s="37" t="s">
+        <v>574</v>
+      </c>
+      <c r="I108" s="42" t="s">
         <v>575</v>
-      </c>
-      <c r="I108" s="42" t="s">
-        <v>576</v>
       </c>
       <c r="J108" s="38" t="s">
         <v>64</v>
@@ -9118,7 +9075,7 @@
         <v>64</v>
       </c>
       <c r="O108" s="38" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="P108" s="45" t="s">
         <v>64</v>
@@ -9126,12 +9083,12 @@
       <c r="Q108" s="38"/>
       <c r="R108" s="38"/>
       <c r="S108" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T108" s="38"/>
       <c r="U108" s="39"/>
       <c r="V108" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W108" s="38" t="s">
         <v>44</v>
@@ -9157,13 +9114,13 @@
         <v>45986</v>
       </c>
       <c r="G109" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H109" s="37" t="s">
+        <v>576</v>
+      </c>
+      <c r="I109" s="42" t="s">
         <v>577</v>
-      </c>
-      <c r="I109" s="42" t="s">
-        <v>578</v>
       </c>
       <c r="J109" s="38" t="s">
         <v>64</v>
@@ -9177,7 +9134,7 @@
         <v>64</v>
       </c>
       <c r="O109" s="38" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="P109" s="45" t="s">
         <v>64</v>
@@ -9185,12 +9142,12 @@
       <c r="Q109" s="38"/>
       <c r="R109" s="38"/>
       <c r="S109" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T109" s="38"/>
       <c r="U109" s="39"/>
       <c r="V109" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W109" s="38" t="s">
         <v>44</v>
@@ -9216,13 +9173,13 @@
         <v>45986</v>
       </c>
       <c r="G110" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H110" s="37" t="s">
+        <v>578</v>
+      </c>
+      <c r="I110" s="42" t="s">
         <v>579</v>
-      </c>
-      <c r="I110" s="42" t="s">
-        <v>580</v>
       </c>
       <c r="J110" s="38" t="s">
         <v>64</v>
@@ -9236,7 +9193,7 @@
         <v>64</v>
       </c>
       <c r="O110" s="38" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="P110" s="45" t="s">
         <v>64</v>
@@ -9244,12 +9201,12 @@
       <c r="Q110" s="38"/>
       <c r="R110" s="38"/>
       <c r="S110" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T110" s="38"/>
       <c r="U110" s="39"/>
       <c r="V110" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W110" s="38" t="s">
         <v>44</v>
@@ -9275,13 +9232,13 @@
         <v>45986</v>
       </c>
       <c r="G111" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H111" s="37" t="s">
+        <v>580</v>
+      </c>
+      <c r="I111" s="42" t="s">
         <v>581</v>
-      </c>
-      <c r="I111" s="42" t="s">
-        <v>582</v>
       </c>
       <c r="J111" s="38" t="s">
         <v>64</v>
@@ -9295,7 +9252,7 @@
         <v>64</v>
       </c>
       <c r="O111" s="38" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="P111" s="45" t="s">
         <v>64</v>
@@ -9303,12 +9260,12 @@
       <c r="Q111" s="38"/>
       <c r="R111" s="38"/>
       <c r="S111" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T111" s="38"/>
       <c r="U111" s="39"/>
       <c r="V111" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W111" s="38" t="s">
         <v>44</v>
@@ -9334,13 +9291,13 @@
         <v>45986</v>
       </c>
       <c r="G112" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H112" s="37" t="s">
+        <v>582</v>
+      </c>
+      <c r="I112" s="42" t="s">
         <v>583</v>
-      </c>
-      <c r="I112" s="42" t="s">
-        <v>584</v>
       </c>
       <c r="J112" s="38" t="s">
         <v>64</v>
@@ -9354,7 +9311,7 @@
         <v>64</v>
       </c>
       <c r="O112" s="38" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="P112" s="45" t="s">
         <v>64</v>
@@ -9362,12 +9319,12 @@
       <c r="Q112" s="38"/>
       <c r="R112" s="38"/>
       <c r="S112" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T112" s="38"/>
       <c r="U112" s="39"/>
       <c r="V112" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W112" s="38" t="s">
         <v>44</v>
@@ -9393,13 +9350,13 @@
         <v>45986</v>
       </c>
       <c r="G113" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H113" s="37" t="s">
+        <v>584</v>
+      </c>
+      <c r="I113" s="42" t="s">
         <v>585</v>
-      </c>
-      <c r="I113" s="42" t="s">
-        <v>586</v>
       </c>
       <c r="J113" s="38" t="s">
         <v>64</v>
@@ -9413,7 +9370,7 @@
         <v>64</v>
       </c>
       <c r="O113" s="38" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="P113" s="45" t="s">
         <v>64</v>
@@ -9421,12 +9378,12 @@
       <c r="Q113" s="38"/>
       <c r="R113" s="38"/>
       <c r="S113" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T113" s="38"/>
       <c r="U113" s="39"/>
       <c r="V113" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W113" s="38" t="s">
         <v>44</v>
@@ -9452,13 +9409,13 @@
         <v>45986</v>
       </c>
       <c r="G114" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H114" s="37" t="s">
+        <v>586</v>
+      </c>
+      <c r="I114" s="42" t="s">
         <v>587</v>
-      </c>
-      <c r="I114" s="42" t="s">
-        <v>588</v>
       </c>
       <c r="J114" s="38" t="s">
         <v>64</v>
@@ -9472,7 +9429,7 @@
         <v>64</v>
       </c>
       <c r="O114" s="38" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="P114" s="45" t="s">
         <v>64</v>
@@ -9480,12 +9437,12 @@
       <c r="Q114" s="38"/>
       <c r="R114" s="38"/>
       <c r="S114" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T114" s="38"/>
       <c r="U114" s="39"/>
       <c r="V114" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W114" s="38" t="s">
         <v>44</v>
@@ -9511,13 +9468,13 @@
         <v>45986</v>
       </c>
       <c r="G115" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H115" s="37" t="s">
+        <v>588</v>
+      </c>
+      <c r="I115" s="42" t="s">
         <v>589</v>
-      </c>
-      <c r="I115" s="42" t="s">
-        <v>590</v>
       </c>
       <c r="J115" s="38" t="s">
         <v>64</v>
@@ -9531,7 +9488,7 @@
         <v>64</v>
       </c>
       <c r="O115" s="38" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="P115" s="45" t="s">
         <v>64</v>
@@ -9539,12 +9496,12 @@
       <c r="Q115" s="38"/>
       <c r="R115" s="38"/>
       <c r="S115" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T115" s="38"/>
       <c r="U115" s="39"/>
       <c r="V115" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W115" s="38" t="s">
         <v>44</v>
@@ -9570,13 +9527,13 @@
         <v>45985</v>
       </c>
       <c r="G116" s="37" t="s">
+        <v>485</v>
+      </c>
+      <c r="H116" s="37" t="s">
         <v>486</v>
       </c>
-      <c r="H116" s="37" t="s">
+      <c r="I116" s="42" t="s">
         <v>487</v>
-      </c>
-      <c r="I116" s="42" t="s">
-        <v>488</v>
       </c>
       <c r="J116" s="38" t="s">
         <v>64</v>
@@ -9590,7 +9547,7 @@
         <v>64</v>
       </c>
       <c r="O116" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P116" s="45" t="s">
         <v>64</v>
@@ -9598,12 +9555,12 @@
       <c r="Q116" s="38"/>
       <c r="R116" s="38"/>
       <c r="S116" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T116" s="38"/>
       <c r="U116" s="39"/>
       <c r="V116" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W116" s="38" t="s">
         <v>44</v>
@@ -9629,13 +9586,13 @@
         <v>45985</v>
       </c>
       <c r="G117" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H117" s="37" t="s">
+        <v>488</v>
+      </c>
+      <c r="I117" s="42" t="s">
         <v>489</v>
-      </c>
-      <c r="I117" s="42" t="s">
-        <v>490</v>
       </c>
       <c r="J117" s="38" t="s">
         <v>64</v>
@@ -9649,7 +9606,7 @@
         <v>64</v>
       </c>
       <c r="O117" s="38" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="P117" s="45" t="s">
         <v>64</v>
@@ -9657,12 +9614,12 @@
       <c r="Q117" s="38"/>
       <c r="R117" s="38"/>
       <c r="S117" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T117" s="38"/>
       <c r="U117" s="39"/>
       <c r="V117" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W117" s="38" t="s">
         <v>44</v>
@@ -9688,13 +9645,13 @@
         <v>45985</v>
       </c>
       <c r="G118" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H118" s="37" t="s">
+        <v>490</v>
+      </c>
+      <c r="I118" s="42" t="s">
         <v>491</v>
-      </c>
-      <c r="I118" s="42" t="s">
-        <v>492</v>
       </c>
       <c r="J118" s="38" t="s">
         <v>64</v>
@@ -9708,7 +9665,7 @@
         <v>64</v>
       </c>
       <c r="O118" s="38" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="P118" s="45" t="s">
         <v>64</v>
@@ -9716,12 +9673,12 @@
       <c r="Q118" s="38"/>
       <c r="R118" s="38"/>
       <c r="S118" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T118" s="38"/>
       <c r="U118" s="39"/>
       <c r="V118" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W118" s="38" t="s">
         <v>44</v>
@@ -9747,13 +9704,13 @@
         <v>45985</v>
       </c>
       <c r="G119" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H119" s="37" t="s">
+        <v>492</v>
+      </c>
+      <c r="I119" s="42" t="s">
         <v>493</v>
-      </c>
-      <c r="I119" s="42" t="s">
-        <v>494</v>
       </c>
       <c r="J119" s="38" t="s">
         <v>64</v>
@@ -9767,7 +9724,7 @@
         <v>64</v>
       </c>
       <c r="O119" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="P119" s="45" t="s">
         <v>64</v>
@@ -9775,12 +9732,12 @@
       <c r="Q119" s="38"/>
       <c r="R119" s="38"/>
       <c r="S119" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T119" s="38"/>
       <c r="U119" s="39"/>
       <c r="V119" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W119" s="38" t="s">
         <v>44</v>
@@ -9806,13 +9763,13 @@
         <v>45985</v>
       </c>
       <c r="G120" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H120" s="37" t="s">
+        <v>495</v>
+      </c>
+      <c r="I120" s="42" t="s">
         <v>496</v>
-      </c>
-      <c r="I120" s="42" t="s">
-        <v>497</v>
       </c>
       <c r="J120" s="38" t="s">
         <v>64</v>
@@ -9826,7 +9783,7 @@
         <v>64</v>
       </c>
       <c r="O120" s="38" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="P120" s="45" t="s">
         <v>64</v>
@@ -9834,12 +9791,12 @@
       <c r="Q120" s="38"/>
       <c r="R120" s="38"/>
       <c r="S120" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T120" s="38"/>
       <c r="U120" s="39"/>
       <c r="V120" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W120" s="38" t="s">
         <v>44</v>
@@ -9865,13 +9822,13 @@
         <v>45985</v>
       </c>
       <c r="G121" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H121" s="37" t="s">
+        <v>497</v>
+      </c>
+      <c r="I121" s="42" t="s">
         <v>498</v>
-      </c>
-      <c r="I121" s="42" t="s">
-        <v>499</v>
       </c>
       <c r="J121" s="38" t="s">
         <v>64</v>
@@ -9885,7 +9842,7 @@
         <v>64</v>
       </c>
       <c r="O121" s="38" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="P121" s="45" t="s">
         <v>64</v>
@@ -9893,12 +9850,12 @@
       <c r="Q121" s="38"/>
       <c r="R121" s="38"/>
       <c r="S121" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T121" s="38"/>
       <c r="U121" s="39"/>
       <c r="V121" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W121" s="38" t="s">
         <v>44</v>
@@ -9924,13 +9881,13 @@
         <v>45985</v>
       </c>
       <c r="G122" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H122" s="37" t="s">
+        <v>499</v>
+      </c>
+      <c r="I122" s="42" t="s">
         <v>500</v>
-      </c>
-      <c r="I122" s="42" t="s">
-        <v>501</v>
       </c>
       <c r="J122" s="38" t="s">
         <v>64</v>
@@ -9944,7 +9901,7 @@
         <v>64</v>
       </c>
       <c r="O122" s="38" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="P122" s="45" t="s">
         <v>64</v>
@@ -9952,12 +9909,12 @@
       <c r="Q122" s="38"/>
       <c r="R122" s="38"/>
       <c r="S122" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T122" s="38"/>
       <c r="U122" s="39"/>
       <c r="V122" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W122" s="38" t="s">
         <v>44</v>
@@ -9983,13 +9940,13 @@
         <v>45985</v>
       </c>
       <c r="G123" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H123" s="37" t="s">
+        <v>501</v>
+      </c>
+      <c r="I123" s="42" t="s">
         <v>502</v>
-      </c>
-      <c r="I123" s="42" t="s">
-        <v>503</v>
       </c>
       <c r="J123" s="38" t="s">
         <v>64</v>
@@ -10003,7 +9960,7 @@
         <v>64</v>
       </c>
       <c r="O123" s="38" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="P123" s="45" t="s">
         <v>64</v>
@@ -10011,12 +9968,12 @@
       <c r="Q123" s="38"/>
       <c r="R123" s="38"/>
       <c r="S123" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T123" s="38"/>
       <c r="U123" s="39"/>
       <c r="V123" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W123" s="38" t="s">
         <v>44</v>
@@ -10042,13 +9999,13 @@
         <v>45985</v>
       </c>
       <c r="G124" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H124" s="37" t="s">
+        <v>503</v>
+      </c>
+      <c r="I124" s="42" t="s">
         <v>504</v>
-      </c>
-      <c r="I124" s="42" t="s">
-        <v>505</v>
       </c>
       <c r="J124" s="38" t="s">
         <v>64</v>
@@ -10062,7 +10019,7 @@
         <v>64</v>
       </c>
       <c r="O124" s="38" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="P124" s="45" t="s">
         <v>64</v>
@@ -10070,12 +10027,12 @@
       <c r="Q124" s="38"/>
       <c r="R124" s="38"/>
       <c r="S124" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T124" s="38"/>
       <c r="U124" s="39"/>
       <c r="V124" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W124" s="38" t="s">
         <v>44</v>
@@ -10101,13 +10058,13 @@
         <v>45985</v>
       </c>
       <c r="G125" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H125" s="37" t="s">
+        <v>505</v>
+      </c>
+      <c r="I125" s="42" t="s">
         <v>506</v>
-      </c>
-      <c r="I125" s="42" t="s">
-        <v>507</v>
       </c>
       <c r="J125" s="38" t="s">
         <v>64</v>
@@ -10121,7 +10078,7 @@
         <v>64</v>
       </c>
       <c r="O125" s="38" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="P125" s="45" t="s">
         <v>64</v>
@@ -10129,12 +10086,12 @@
       <c r="Q125" s="38"/>
       <c r="R125" s="38"/>
       <c r="S125" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T125" s="38"/>
       <c r="U125" s="39"/>
       <c r="V125" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W125" s="38" t="s">
         <v>44</v>
@@ -10160,13 +10117,13 @@
         <v>45985</v>
       </c>
       <c r="G126" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H126" s="37" t="s">
+        <v>507</v>
+      </c>
+      <c r="I126" s="42" t="s">
         <v>508</v>
-      </c>
-      <c r="I126" s="42" t="s">
-        <v>509</v>
       </c>
       <c r="J126" s="38" t="s">
         <v>64</v>
@@ -10180,7 +10137,7 @@
         <v>64</v>
       </c>
       <c r="O126" s="38" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="P126" s="45" t="s">
         <v>64</v>
@@ -10188,12 +10145,12 @@
       <c r="Q126" s="38"/>
       <c r="R126" s="38"/>
       <c r="S126" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T126" s="38"/>
       <c r="U126" s="39"/>
       <c r="V126" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W126" s="38" t="s">
         <v>44</v>
@@ -10219,13 +10176,13 @@
         <v>45985</v>
       </c>
       <c r="G127" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H127" s="37" t="s">
+        <v>516</v>
+      </c>
+      <c r="I127" s="42" t="s">
         <v>517</v>
-      </c>
-      <c r="I127" s="42" t="s">
-        <v>518</v>
       </c>
       <c r="J127" s="38" t="s">
         <v>64</v>
@@ -10239,7 +10196,7 @@
         <v>64</v>
       </c>
       <c r="O127" s="38" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="P127" s="45" t="s">
         <v>64</v>
@@ -10247,12 +10204,12 @@
       <c r="Q127" s="38"/>
       <c r="R127" s="38"/>
       <c r="S127" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T127" s="38"/>
       <c r="U127" s="39"/>
       <c r="V127" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W127" s="38" t="s">
         <v>44</v>
@@ -10278,13 +10235,13 @@
         <v>45985</v>
       </c>
       <c r="G128" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H128" s="37" t="s">
+        <v>518</v>
+      </c>
+      <c r="I128" s="42" t="s">
         <v>519</v>
-      </c>
-      <c r="I128" s="42" t="s">
-        <v>520</v>
       </c>
       <c r="J128" s="38" t="s">
         <v>64</v>
@@ -10298,7 +10255,7 @@
         <v>64</v>
       </c>
       <c r="O128" s="38" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="P128" s="45" t="s">
         <v>64</v>
@@ -10306,12 +10263,12 @@
       <c r="Q128" s="38"/>
       <c r="R128" s="38"/>
       <c r="S128" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T128" s="38"/>
       <c r="U128" s="39"/>
       <c r="V128" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W128" s="38" t="s">
         <v>44</v>
@@ -10337,13 +10294,13 @@
         <v>45985</v>
       </c>
       <c r="G129" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H129" s="37" t="s">
+        <v>520</v>
+      </c>
+      <c r="I129" s="42" t="s">
         <v>521</v>
-      </c>
-      <c r="I129" s="42" t="s">
-        <v>522</v>
       </c>
       <c r="J129" s="38" t="s">
         <v>64</v>
@@ -10357,7 +10314,7 @@
         <v>64</v>
       </c>
       <c r="O129" s="38" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="P129" s="45" t="s">
         <v>64</v>
@@ -10365,12 +10322,12 @@
       <c r="Q129" s="38"/>
       <c r="R129" s="38"/>
       <c r="S129" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T129" s="38"/>
       <c r="U129" s="39"/>
       <c r="V129" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W129" s="38" t="s">
         <v>44</v>
@@ -10396,13 +10353,13 @@
         <v>45985</v>
       </c>
       <c r="G130" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H130" s="37" t="s">
+        <v>522</v>
+      </c>
+      <c r="I130" s="42" t="s">
         <v>523</v>
-      </c>
-      <c r="I130" s="42" t="s">
-        <v>524</v>
       </c>
       <c r="J130" s="38" t="s">
         <v>64</v>
@@ -10416,7 +10373,7 @@
         <v>64</v>
       </c>
       <c r="O130" s="38" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="P130" s="45" t="s">
         <v>64</v>
@@ -10424,12 +10381,12 @@
       <c r="Q130" s="38"/>
       <c r="R130" s="38"/>
       <c r="S130" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T130" s="38"/>
       <c r="U130" s="39"/>
       <c r="V130" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W130" s="38" t="s">
         <v>44</v>
@@ -11750,13 +11707,13 @@
         <v>45985</v>
       </c>
       <c r="G166" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H166" s="37" t="s">
+        <v>528</v>
+      </c>
+      <c r="I166" s="42" t="s">
         <v>529</v>
-      </c>
-      <c r="I166" s="42" t="s">
-        <v>530</v>
       </c>
       <c r="J166" s="38" t="s">
         <v>64</v>
@@ -11797,13 +11754,13 @@
         <v>45985</v>
       </c>
       <c r="G167" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H167" s="37" t="s">
+        <v>530</v>
+      </c>
+      <c r="I167" s="42" t="s">
         <v>531</v>
-      </c>
-      <c r="I167" s="42" t="s">
-        <v>532</v>
       </c>
       <c r="J167" s="38" t="s">
         <v>64</v>
@@ -11847,10 +11804,10 @@
         <v>437</v>
       </c>
       <c r="H168" s="37" t="s">
+        <v>467</v>
+      </c>
+      <c r="I168" s="42" t="s">
         <v>468</v>
-      </c>
-      <c r="I168" s="42" t="s">
-        <v>469</v>
       </c>
       <c r="J168" s="38" t="s">
         <v>64</v>
@@ -11894,10 +11851,10 @@
         <v>437</v>
       </c>
       <c r="H169" s="37" t="s">
+        <v>469</v>
+      </c>
+      <c r="I169" s="42" t="s">
         <v>470</v>
-      </c>
-      <c r="I169" s="42" t="s">
-        <v>471</v>
       </c>
       <c r="J169" s="38" t="s">
         <v>64</v>
@@ -11975,13 +11932,13 @@
         <v>45986</v>
       </c>
       <c r="G171" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H171" s="37" t="s">
+        <v>609</v>
+      </c>
+      <c r="I171" s="42" t="s">
         <v>610</v>
-      </c>
-      <c r="I171" s="42" t="s">
-        <v>611</v>
       </c>
       <c r="J171" s="38" t="s">
         <v>64</v>
@@ -12022,13 +11979,13 @@
         <v>45986</v>
       </c>
       <c r="G172" s="37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H172" s="37" t="s">
+        <v>611</v>
+      </c>
+      <c r="I172" s="42" t="s">
         <v>612</v>
-      </c>
-      <c r="I172" s="42" t="s">
-        <v>613</v>
       </c>
       <c r="J172" s="38" t="s">
         <v>64</v>
@@ -12254,13 +12211,13 @@
         <v>45985</v>
       </c>
       <c r="G178" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H178" s="37" t="s">
+        <v>532</v>
+      </c>
+      <c r="I178" s="42" t="s">
         <v>533</v>
-      </c>
-      <c r="I178" s="42" t="s">
-        <v>534</v>
       </c>
       <c r="J178" s="38" t="s">
         <v>64</v>
@@ -12274,7 +12231,7 @@
         <v>64</v>
       </c>
       <c r="O178" s="35" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="P178" s="45" t="s">
         <v>64</v>
@@ -12282,12 +12239,12 @@
       <c r="Q178" s="38"/>
       <c r="R178" s="38"/>
       <c r="S178" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T178" s="38"/>
       <c r="U178" s="35"/>
       <c r="V178" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W178" s="35" t="s">
         <v>44</v>
@@ -12350,13 +12307,13 @@
         <v>45986</v>
       </c>
       <c r="G180" s="35" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H180" s="37" t="s">
+        <v>613</v>
+      </c>
+      <c r="I180" s="42" t="s">
         <v>614</v>
-      </c>
-      <c r="I180" s="42" t="s">
-        <v>615</v>
       </c>
       <c r="J180" s="38" t="s">
         <v>64</v>
@@ -12370,7 +12327,7 @@
         <v>64</v>
       </c>
       <c r="O180" s="38" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="P180" s="45" t="s">
         <v>64</v>
@@ -12378,12 +12335,12 @@
       <c r="Q180" s="38"/>
       <c r="R180" s="38"/>
       <c r="S180" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T180" s="38"/>
       <c r="U180" s="35"/>
       <c r="V180" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W180" s="35" t="s">
         <v>44</v>
@@ -12523,28 +12480,24 @@
         <v>437</v>
       </c>
       <c r="H184" s="35" t="s">
+        <v>471</v>
+      </c>
+      <c r="I184" s="35" t="s">
         <v>472</v>
       </c>
-      <c r="I184" s="35" t="s">
+      <c r="J184" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="K184" s="38"/>
+      <c r="L184" s="35"/>
+      <c r="M184" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="N184" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="O184" s="38" t="s">
         <v>473</v>
-      </c>
-      <c r="J184" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="K184" s="38" t="s">
-        <v>442</v>
-      </c>
-      <c r="L184" s="35" t="s">
-        <v>442</v>
-      </c>
-      <c r="M184" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="N184" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="O184" s="38" t="s">
-        <v>474</v>
       </c>
       <c r="P184" s="45" t="s">
         <v>64</v>
@@ -12552,12 +12505,12 @@
       <c r="Q184" s="38"/>
       <c r="R184" s="38"/>
       <c r="S184" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T184" s="38"/>
       <c r="U184" s="35"/>
       <c r="V184" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W184" s="35" t="s">
         <v>44</v>
@@ -12583,13 +12536,13 @@
         <v>45985</v>
       </c>
       <c r="G185" s="37" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H185" s="37" t="s">
+        <v>535</v>
+      </c>
+      <c r="I185" s="42" t="s">
         <v>536</v>
-      </c>
-      <c r="I185" s="42" t="s">
-        <v>537</v>
       </c>
       <c r="J185" s="38" t="s">
         <v>64</v>
@@ -12603,7 +12556,7 @@
         <v>64</v>
       </c>
       <c r="O185" s="35" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="P185" s="45" t="s">
         <v>64</v>
@@ -12611,12 +12564,12 @@
       <c r="Q185" s="38"/>
       <c r="R185" s="38"/>
       <c r="S185" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T185" s="38"/>
       <c r="U185" s="35"/>
       <c r="V185" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W185" s="35" t="s">
         <v>44</v>
@@ -12864,13 +12817,13 @@
         <v>45985</v>
       </c>
       <c r="G192" s="37" t="s">
+        <v>537</v>
+      </c>
+      <c r="H192" s="37" t="s">
         <v>538</v>
       </c>
-      <c r="H192" s="37" t="s">
+      <c r="I192" s="42" t="s">
         <v>539</v>
-      </c>
-      <c r="I192" s="42" t="s">
-        <v>540</v>
       </c>
       <c r="J192" s="38" t="s">
         <v>64</v>
@@ -12884,7 +12837,7 @@
         <v>64</v>
       </c>
       <c r="O192" s="38" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="P192" s="45" t="s">
         <v>64</v>
@@ -12892,12 +12845,12 @@
       <c r="Q192" s="38"/>
       <c r="R192" s="38"/>
       <c r="S192" s="45" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T192" s="38"/>
       <c r="U192" s="39"/>
       <c r="V192" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="W192" s="38" t="s">
         <v>44</v>

</xml_diff>